<commit_message>
updated a few tu texts
</commit_message>
<xml_diff>
--- a/check list.xlsx
+++ b/check list.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="293">
   <si>
     <t>ARMOR</t>
   </si>
@@ -890,13 +890,19 @@
   </si>
   <si>
     <t>SS checked</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>T5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1030,6 +1036,13 @@
       <color rgb="FFFF0000"/>
       <name val="Verdana"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1229,7 +1242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1469,6 +1482,12 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9007,8 +9026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="C118" sqref="C118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9604,7 +9623,9 @@
       <c r="B30" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="20"/>
+      <c r="C30" s="84" t="s">
+        <v>291</v>
+      </c>
       <c r="D30" s="20"/>
       <c r="E30" s="20"/>
       <c r="F30" s="20"/>
@@ -11206,7 +11227,9 @@
       <c r="H116" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="I116" s="20"/>
+      <c r="I116" s="84" t="s">
+        <v>291</v>
+      </c>
       <c r="J116" s="20"/>
       <c r="K116" s="20"/>
       <c r="L116" s="20"/>
@@ -11217,7 +11240,9 @@
       <c r="B117" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="C117" s="41"/>
+      <c r="C117" s="85" t="s">
+        <v>292</v>
+      </c>
       <c r="D117" s="41"/>
       <c r="E117" s="39"/>
       <c r="F117" s="39"/>

</xml_diff>

<commit_message>
Tu / SU page
SU -> changed the block on shield back to what it was as informed by
Quiri
TU -> updated a few more of items
</commit_message>
<xml_diff>
--- a/check list.xlsx
+++ b/check list.xlsx
@@ -9053,8 +9053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G79" workbookViewId="0">
-      <selection activeCell="K101" sqref="K101"/>
+    <sheetView tabSelected="1" topLeftCell="B134" workbookViewId="0">
+      <selection activeCell="D149" sqref="D149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9062,9 +9062,14 @@
     <col min="1" max="1" width="21.7109375" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="4" max="5" width="12.5703125" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="19" customWidth="1"/>
     <col min="9" max="9" width="17.85546875" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" customWidth="1"/>
     <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9548,7 +9553,7 @@
       <c r="L24" s="20"/>
       <c r="M24" s="58"/>
     </row>
-    <row r="25" spans="1:13" ht="26.25" thickBot="1">
+    <row r="25" spans="1:13" ht="19.5" customHeight="1" thickBot="1">
       <c r="A25" s="58"/>
       <c r="B25" s="19" t="s">
         <v>23</v>
@@ -9561,7 +9566,7 @@
       <c r="H25" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="I25" s="20"/>
+      <c r="I25" s="73"/>
       <c r="J25" s="20"/>
       <c r="K25" s="20"/>
       <c r="L25" s="73"/>
@@ -10105,7 +10110,7 @@
       <c r="B55" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="C55" s="20"/>
+      <c r="C55" s="73"/>
       <c r="D55" s="20"/>
       <c r="E55" s="20"/>
       <c r="F55" s="20"/>
@@ -10294,7 +10299,7 @@
       <c r="B66" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="C66" s="20"/>
+      <c r="C66" s="73"/>
       <c r="D66" s="20"/>
       <c r="E66" s="20"/>
       <c r="F66" s="20"/>
@@ -10440,7 +10445,7 @@
       <c r="B74" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="C74" s="20"/>
+      <c r="C74" s="73"/>
       <c r="D74" s="20"/>
       <c r="E74" s="20"/>
       <c r="F74" s="20"/>
@@ -10608,7 +10613,7 @@
       <c r="H82" s="19" t="s">
         <v>184</v>
       </c>
-      <c r="I82" s="20"/>
+      <c r="I82" s="73"/>
       <c r="J82" s="20"/>
       <c r="K82" s="20"/>
       <c r="L82" s="73"/>
@@ -10779,7 +10784,7 @@
       <c r="H91" s="19" t="s">
         <v>193</v>
       </c>
-      <c r="I91" s="20"/>
+      <c r="I91" s="73"/>
       <c r="J91" s="73"/>
       <c r="K91" s="20"/>
       <c r="L91" s="20"/>
@@ -10866,7 +10871,7 @@
       <c r="B96" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="C96" s="20"/>
+      <c r="C96" s="73"/>
       <c r="D96" s="20"/>
       <c r="E96" s="20"/>
       <c r="F96" s="20"/>
@@ -11209,7 +11214,7 @@
       <c r="H113" s="19" t="s">
         <v>212</v>
       </c>
-      <c r="I113" s="20"/>
+      <c r="I113" s="73"/>
       <c r="J113" s="20"/>
       <c r="K113" s="20"/>
       <c r="L113" s="20"/>
@@ -11585,7 +11590,7 @@
       <c r="B133" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="C133" s="20"/>
+      <c r="C133" s="73"/>
       <c r="D133" s="20"/>
       <c r="E133" s="20"/>
       <c r="F133" s="20"/>
@@ -11617,7 +11622,7 @@
       <c r="M134" s="4"/>
       <c r="N134" s="4"/>
     </row>
-    <row r="135" spans="1:14" ht="52.5" thickBot="1">
+    <row r="135" spans="1:14" ht="27" thickBot="1">
       <c r="A135" s="58"/>
       <c r="B135" s="19" t="s">
         <v>127</v>
@@ -11919,7 +11924,7 @@
       <c r="M148" s="4"/>
       <c r="N148" s="4"/>
     </row>
-    <row r="149" spans="1:14" ht="52.5" thickBot="1">
+    <row r="149" spans="1:14" ht="27" thickBot="1">
       <c r="A149" s="58"/>
       <c r="B149" s="19" t="s">
         <v>140</v>
@@ -11954,7 +11959,7 @@
       <c r="B150" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="C150" s="20"/>
+      <c r="C150" s="73"/>
       <c r="D150" s="20"/>
       <c r="E150" s="20"/>
       <c r="F150" s="20"/>
@@ -12067,7 +12072,7 @@
       <c r="M155" s="4"/>
       <c r="N155" s="4"/>
     </row>
-    <row r="156" spans="1:14" ht="52.5" thickBot="1">
+    <row r="156" spans="1:14" ht="39.75" thickBot="1">
       <c r="A156" s="58"/>
       <c r="B156" s="58"/>
       <c r="C156" s="58"/>
@@ -12223,7 +12228,7 @@
       <c r="M162" s="4"/>
       <c r="N162" s="4"/>
     </row>
-    <row r="163" spans="1:14" ht="52.5" thickBot="1">
+    <row r="163" spans="1:14" ht="39.75" thickBot="1">
       <c r="A163" s="4"/>
       <c r="B163" s="4"/>
       <c r="C163" s="4"/>
@@ -12251,7 +12256,7 @@
       </c>
       <c r="N163" s="4"/>
     </row>
-    <row r="164" spans="1:14" ht="52.5" thickBot="1">
+    <row r="164" spans="1:14" ht="39.75" thickBot="1">
       <c r="A164" s="44" t="s">
         <v>276</v>
       </c>
@@ -12395,7 +12400,7 @@
       <c r="M170" s="4"/>
       <c r="N170" s="4"/>
     </row>
-    <row r="171" spans="1:14" ht="52.5" thickBot="1">
+    <row r="171" spans="1:14" ht="27" thickBot="1">
       <c r="A171" s="4"/>
       <c r="B171" s="5" t="s">
         <v>282</v>

</xml_diff>

<commit_message>
tu page/ su page / updated readme
tu page :
updated many tu items stats
-
SU page :
Removed durability from indestr items
TU+SU page:
removed "durability" from all throw weapons and Indetr items (Javelin,
Pilum, Short Spear, Glaive, Throwing Spear, Throwing Knife, Flying
Knife, Balanced Knife, Throwing Axe, Balanced Axe, Maiden Javelin). If
any other weapon also don't show durability in game then do tell /
update docs.
None of the TU armors have Indestr bonus so only these weapons lost
durability in tu.
</commit_message>
<xml_diff>
--- a/check list.xlsx
+++ b/check list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Blank checklist (SU-TU)" sheetId="2" r:id="rId1"/>
@@ -691,9 +691,6 @@
     <t>Horned Helm</t>
   </si>
   <si>
-    <t>Assult Helmet</t>
-  </si>
-  <si>
     <t>Avenger Guard</t>
   </si>
   <si>
@@ -914,6 +911,9 @@
   </si>
   <si>
     <t>Ring of the five</t>
+  </si>
+  <si>
+    <t>Assault Helmet</t>
   </si>
 </sst>
 </file>
@@ -1493,6 +1493,9 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1521,9 +1524,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1822,8 +1822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N153"/>
   <sheetViews>
-    <sheetView topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+    <sheetView topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="I122" sqref="I122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1863,7 +1863,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="56" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>1</v>
@@ -1879,7 +1879,7 @@
         <v>147</v>
       </c>
       <c r="I2" s="56" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J2" s="14" t="s">
         <v>1</v>
@@ -2295,7 +2295,7 @@
         <v>24</v>
       </c>
       <c r="C24" s="56" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D24" s="26" t="s">
         <v>1</v>
@@ -2362,13 +2362,13 @@
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
       <c r="G27" s="7"/>
-      <c r="H27" s="80" t="s">
+      <c r="H27" s="81" t="s">
         <v>171</v>
       </c>
-      <c r="I27" s="80"/>
-      <c r="J27" s="80"/>
-      <c r="K27" s="80"/>
-      <c r="L27" s="80"/>
+      <c r="I27" s="81"/>
+      <c r="J27" s="81"/>
+      <c r="K27" s="81"/>
+      <c r="L27" s="81"/>
       <c r="M27" s="7"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1">
@@ -2426,7 +2426,7 @@
         <v>30</v>
       </c>
       <c r="C31" s="56" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D31" s="26" t="s">
         <v>1</v>
@@ -2523,13 +2523,13 @@
       <c r="E36" s="20"/>
       <c r="F36" s="29"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="80" t="s">
+      <c r="H36" s="81" t="s">
         <v>172</v>
       </c>
-      <c r="I36" s="80"/>
-      <c r="J36" s="80"/>
-      <c r="K36" s="80"/>
-      <c r="L36" s="80"/>
+      <c r="I36" s="81"/>
+      <c r="J36" s="81"/>
+      <c r="K36" s="81"/>
+      <c r="L36" s="81"/>
       <c r="M36" s="7"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
@@ -2553,7 +2553,7 @@
         <v>36</v>
       </c>
       <c r="C38" s="56" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>1</v>
@@ -2678,7 +2678,7 @@
         <v>42</v>
       </c>
       <c r="C45" s="56" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D45" s="14" t="s">
         <v>1</v>
@@ -2690,13 +2690,13 @@
         <v>3</v>
       </c>
       <c r="G45" s="7"/>
-      <c r="H45" s="80" t="s">
+      <c r="H45" s="81" t="s">
         <v>173</v>
       </c>
-      <c r="I45" s="80"/>
-      <c r="J45" s="80"/>
-      <c r="K45" s="80"/>
-      <c r="L45" s="80"/>
+      <c r="I45" s="81"/>
+      <c r="J45" s="81"/>
+      <c r="K45" s="81"/>
+      <c r="L45" s="81"/>
       <c r="M45" s="7"/>
     </row>
     <row r="46" spans="1:13" ht="15.75" thickBot="1">
@@ -2845,13 +2845,13 @@
       <c r="E54" s="39"/>
       <c r="F54" s="39"/>
       <c r="G54" s="7"/>
-      <c r="H54" s="80" t="s">
+      <c r="H54" s="81" t="s">
         <v>174</v>
       </c>
-      <c r="I54" s="80"/>
-      <c r="J54" s="80"/>
-      <c r="K54" s="80"/>
-      <c r="L54" s="80"/>
+      <c r="I54" s="81"/>
+      <c r="J54" s="81"/>
+      <c r="K54" s="81"/>
+      <c r="L54" s="81"/>
       <c r="M54" s="7"/>
     </row>
     <row r="55" spans="1:13" ht="15.75" thickBot="1">
@@ -3000,13 +3000,13 @@
       <c r="E63" s="20"/>
       <c r="F63" s="20"/>
       <c r="G63" s="7"/>
-      <c r="H63" s="80" t="s">
+      <c r="H63" s="81" t="s">
         <v>175</v>
       </c>
-      <c r="I63" s="80"/>
-      <c r="J63" s="80"/>
-      <c r="K63" s="80"/>
-      <c r="L63" s="80"/>
+      <c r="I63" s="81"/>
+      <c r="J63" s="81"/>
+      <c r="K63" s="81"/>
+      <c r="L63" s="81"/>
       <c r="M63" s="7"/>
     </row>
     <row r="64" spans="1:13" ht="15.75" thickBot="1">
@@ -3142,7 +3142,7 @@
         <v>176</v>
       </c>
       <c r="I71" s="56" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J71" s="14" t="s">
         <v>1</v>
@@ -3576,7 +3576,7 @@
     <row r="94" spans="1:13" ht="15.75" thickBot="1">
       <c r="A94" s="7"/>
       <c r="B94" s="19" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C94" s="20"/>
       <c r="D94" s="20"/>
@@ -3727,7 +3727,7 @@
         <v>97</v>
       </c>
       <c r="C102" s="56" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D102" s="14" t="s">
         <v>1</v>
@@ -3740,10 +3740,10 @@
       </c>
       <c r="G102" s="7"/>
       <c r="H102" s="13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I102" s="56" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J102" s="14" t="s">
         <v>1</v>
@@ -4128,7 +4128,7 @@
       <c r="F122" s="20"/>
       <c r="G122" s="7"/>
       <c r="H122" s="19" t="s">
-        <v>224</v>
+        <v>298</v>
       </c>
       <c r="I122" s="20"/>
       <c r="J122" s="20"/>
@@ -4147,7 +4147,7 @@
       <c r="F123" s="20"/>
       <c r="G123" s="7"/>
       <c r="H123" s="19" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I123" s="20"/>
       <c r="J123" s="20"/>
@@ -4166,7 +4166,7 @@
       <c r="F124" s="20"/>
       <c r="G124" s="7"/>
       <c r="H124" s="19" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I124" s="20"/>
       <c r="J124" s="20"/>
@@ -4185,7 +4185,7 @@
       <c r="F125" s="39"/>
       <c r="G125" s="7"/>
       <c r="H125" s="19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I125" s="20"/>
       <c r="J125" s="20"/>
@@ -4204,7 +4204,7 @@
       <c r="F126" s="20"/>
       <c r="G126" s="7"/>
       <c r="H126" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I126" s="20"/>
       <c r="J126" s="20"/>
@@ -4223,7 +4223,7 @@
       <c r="F127" s="20"/>
       <c r="G127" s="7"/>
       <c r="H127" s="19" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I127" s="20"/>
       <c r="J127" s="20"/>
@@ -4242,7 +4242,7 @@
       <c r="F128" s="41"/>
       <c r="G128" s="7"/>
       <c r="H128" s="19" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I128" s="20"/>
       <c r="J128" s="20"/>
@@ -4261,7 +4261,7 @@
       <c r="F129" s="20"/>
       <c r="G129" s="7"/>
       <c r="H129" s="19" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I129" s="20"/>
       <c r="J129" s="20"/>
@@ -4280,7 +4280,7 @@
       <c r="F130" s="20"/>
       <c r="G130" s="7"/>
       <c r="H130" s="19" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I130" s="20"/>
       <c r="J130" s="20"/>
@@ -4315,11 +4315,11 @@
       <c r="E132" s="20"/>
       <c r="F132" s="20"/>
       <c r="G132" s="7"/>
-      <c r="H132" s="79"/>
-      <c r="I132" s="79"/>
-      <c r="J132" s="79"/>
-      <c r="K132" s="79"/>
-      <c r="L132" s="79"/>
+      <c r="H132" s="80"/>
+      <c r="I132" s="80"/>
+      <c r="J132" s="80"/>
+      <c r="K132" s="80"/>
+      <c r="L132" s="80"/>
       <c r="M132" s="7"/>
     </row>
     <row r="133" spans="1:14" ht="18" thickBot="1">
@@ -4464,7 +4464,7 @@
         <v>135</v>
       </c>
       <c r="C141" s="56" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D141" s="14" t="s">
         <v>1</v>
@@ -4730,29 +4730,29 @@
     <row r="2" spans="1:8" ht="37.5" customHeight="1" thickBot="1">
       <c r="A2" s="4"/>
       <c r="B2" s="44" t="s">
+        <v>233</v>
+      </c>
+      <c r="C2" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="D2" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="E2" s="45" t="s">
         <v>236</v>
       </c>
-      <c r="E2" s="45" t="s">
+      <c r="F2" s="45" t="s">
         <v>237</v>
       </c>
-      <c r="F2" s="45" t="s">
+      <c r="G2" s="45" t="s">
         <v>238</v>
-      </c>
-      <c r="G2" s="45" t="s">
-        <v>239</v>
       </c>
       <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1">
       <c r="A3" s="4"/>
       <c r="B3" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -4764,7 +4764,7 @@
     <row r="4" spans="1:8" ht="15.75" thickBot="1">
       <c r="A4" s="4"/>
       <c r="B4" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -4776,7 +4776,7 @@
     <row r="5" spans="1:8" ht="15.75" thickBot="1">
       <c r="A5" s="4"/>
       <c r="B5" s="51" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -4788,7 +4788,7 @@
     <row r="6" spans="1:8" ht="15.75" thickBot="1">
       <c r="A6" s="4"/>
       <c r="B6" s="52" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C6" s="54"/>
       <c r="D6" s="54"/>
@@ -4800,7 +4800,7 @@
     <row r="7" spans="1:8" ht="15.75" thickBot="1">
       <c r="A7" s="4"/>
       <c r="B7" s="53" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C7" s="54"/>
       <c r="D7" s="54"/>
@@ -4822,29 +4822,29 @@
     <row r="9" spans="1:8" ht="30.75" customHeight="1" thickBot="1">
       <c r="A9" s="4"/>
       <c r="B9" s="44" t="s">
+        <v>245</v>
+      </c>
+      <c r="C9" s="45" t="s">
         <v>246</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="D9" s="45" t="s">
         <v>247</v>
       </c>
-      <c r="D9" s="45" t="s">
+      <c r="E9" s="45" t="s">
         <v>248</v>
       </c>
-      <c r="E9" s="45" t="s">
+      <c r="F9" s="45" t="s">
         <v>249</v>
       </c>
-      <c r="F9" s="45" t="s">
+      <c r="G9" s="45" t="s">
         <v>250</v>
-      </c>
-      <c r="G9" s="45" t="s">
-        <v>251</v>
       </c>
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1">
       <c r="A10" s="4"/>
       <c r="B10" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -4856,7 +4856,7 @@
     <row r="11" spans="1:8" ht="15.75" thickBot="1">
       <c r="A11" s="4"/>
       <c r="B11" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -4868,7 +4868,7 @@
     <row r="12" spans="1:8" ht="15.75" thickBot="1">
       <c r="A12" s="4"/>
       <c r="B12" s="51" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -4880,7 +4880,7 @@
     <row r="13" spans="1:8" ht="15.75" thickBot="1">
       <c r="A13" s="4"/>
       <c r="B13" s="51" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -4892,7 +4892,7 @@
     <row r="14" spans="1:8" ht="15.75" thickBot="1">
       <c r="A14" s="4"/>
       <c r="B14" s="57" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -4914,29 +4914,29 @@
     <row r="16" spans="1:8" ht="27" thickBot="1">
       <c r="A16" s="4"/>
       <c r="B16" s="44" t="s">
+        <v>251</v>
+      </c>
+      <c r="C16" s="45" t="s">
         <v>252</v>
       </c>
-      <c r="C16" s="45" t="s">
+      <c r="D16" s="45" t="s">
         <v>253</v>
       </c>
-      <c r="D16" s="45" t="s">
+      <c r="E16" s="45" t="s">
         <v>254</v>
       </c>
-      <c r="E16" s="45" t="s">
+      <c r="F16" s="45" t="s">
         <v>255</v>
       </c>
-      <c r="F16" s="45" t="s">
+      <c r="G16" s="45" t="s">
         <v>256</v>
-      </c>
-      <c r="G16" s="45" t="s">
-        <v>257</v>
       </c>
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" thickBot="1">
       <c r="A17" s="4"/>
       <c r="B17" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -4948,7 +4948,7 @@
     <row r="18" spans="1:8" ht="15.75" thickBot="1">
       <c r="A18" s="4"/>
       <c r="B18" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -4960,7 +4960,7 @@
     <row r="19" spans="1:8" ht="15.75" thickBot="1">
       <c r="A19" s="4"/>
       <c r="B19" s="51" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -4972,7 +4972,7 @@
     <row r="20" spans="1:8" ht="15.75" thickBot="1">
       <c r="A20" s="4"/>
       <c r="B20" s="51" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -4984,7 +4984,7 @@
     <row r="21" spans="1:8" ht="15.75" thickBot="1">
       <c r="A21" s="4"/>
       <c r="B21" s="57" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -5006,29 +5006,29 @@
     <row r="23" spans="1:8" ht="45" customHeight="1" thickBot="1">
       <c r="A23" s="4"/>
       <c r="B23" s="44" t="s">
+        <v>257</v>
+      </c>
+      <c r="C23" s="45" t="s">
         <v>258</v>
       </c>
-      <c r="C23" s="45" t="s">
+      <c r="D23" s="45" t="s">
         <v>259</v>
       </c>
-      <c r="D23" s="45" t="s">
+      <c r="E23" s="45" t="s">
         <v>260</v>
       </c>
-      <c r="E23" s="45" t="s">
+      <c r="F23" s="45" t="s">
         <v>261</v>
       </c>
-      <c r="F23" s="45" t="s">
+      <c r="G23" s="45" t="s">
         <v>262</v>
-      </c>
-      <c r="G23" s="45" t="s">
-        <v>263</v>
       </c>
       <c r="H23" s="4"/>
     </row>
     <row r="24" spans="1:8" ht="15.75" thickBot="1">
       <c r="A24" s="4"/>
       <c r="B24" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -5040,7 +5040,7 @@
     <row r="25" spans="1:8" ht="15.75" thickBot="1">
       <c r="A25" s="4"/>
       <c r="B25" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -5052,7 +5052,7 @@
     <row r="26" spans="1:8" ht="15.75" thickBot="1">
       <c r="A26" s="4"/>
       <c r="B26" s="51" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -5064,7 +5064,7 @@
     <row r="27" spans="1:8" ht="15.75" thickBot="1">
       <c r="A27" s="4"/>
       <c r="B27" s="51" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -5076,7 +5076,7 @@
     <row r="28" spans="1:8" ht="15.75" thickBot="1">
       <c r="A28" s="4"/>
       <c r="B28" s="57" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -5098,29 +5098,29 @@
     <row r="30" spans="1:8" ht="39.75" thickBot="1">
       <c r="A30" s="4"/>
       <c r="B30" s="44" t="s">
+        <v>263</v>
+      </c>
+      <c r="C30" s="45" t="s">
         <v>264</v>
       </c>
-      <c r="C30" s="45" t="s">
+      <c r="D30" s="45" t="s">
         <v>265</v>
       </c>
-      <c r="D30" s="45" t="s">
+      <c r="E30" s="45" t="s">
         <v>266</v>
       </c>
-      <c r="E30" s="45" t="s">
+      <c r="F30" s="45" t="s">
         <v>267</v>
       </c>
-      <c r="F30" s="45" t="s">
+      <c r="G30" s="45" t="s">
         <v>268</v>
-      </c>
-      <c r="G30" s="45" t="s">
-        <v>269</v>
       </c>
       <c r="H30" s="4"/>
     </row>
     <row r="31" spans="1:8" ht="15.75" thickBot="1">
       <c r="A31" s="4"/>
       <c r="B31" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -5132,7 +5132,7 @@
     <row r="32" spans="1:8" ht="15.75" thickBot="1">
       <c r="A32" s="4"/>
       <c r="B32" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -5144,7 +5144,7 @@
     <row r="33" spans="1:8" ht="15.75" thickBot="1">
       <c r="A33" s="4"/>
       <c r="B33" s="51" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
@@ -5156,7 +5156,7 @@
     <row r="34" spans="1:8" ht="15.75" thickBot="1">
       <c r="A34" s="4"/>
       <c r="B34" s="51" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -5168,7 +5168,7 @@
     <row r="35" spans="1:8" ht="15.75" thickBot="1">
       <c r="A35" s="4"/>
       <c r="B35" s="57" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -5190,29 +5190,29 @@
     <row r="37" spans="1:8" ht="35.25" thickBot="1">
       <c r="A37" s="4"/>
       <c r="B37" s="44" t="s">
+        <v>269</v>
+      </c>
+      <c r="C37" s="45" t="s">
         <v>270</v>
       </c>
-      <c r="C37" s="45" t="s">
+      <c r="D37" s="45" t="s">
         <v>271</v>
       </c>
-      <c r="D37" s="45" t="s">
+      <c r="E37" s="45" t="s">
         <v>272</v>
       </c>
-      <c r="E37" s="45" t="s">
+      <c r="F37" s="45" t="s">
         <v>273</v>
       </c>
-      <c r="F37" s="45" t="s">
+      <c r="G37" s="45" t="s">
         <v>274</v>
-      </c>
-      <c r="G37" s="45" t="s">
-        <v>275</v>
       </c>
       <c r="H37" s="4"/>
     </row>
     <row r="38" spans="1:8" ht="15.75" thickBot="1">
       <c r="A38" s="4"/>
       <c r="B38" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -5224,7 +5224,7 @@
     <row r="39" spans="1:8" ht="15.75" thickBot="1">
       <c r="A39" s="4"/>
       <c r="B39" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -5236,7 +5236,7 @@
     <row r="40" spans="1:8" ht="15.75" thickBot="1">
       <c r="A40" s="4"/>
       <c r="B40" s="51" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -5248,7 +5248,7 @@
     <row r="41" spans="1:8" ht="15.75" thickBot="1">
       <c r="A41" s="4"/>
       <c r="B41" s="51" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
@@ -5260,7 +5260,7 @@
     <row r="42" spans="1:8" ht="15.75" thickBot="1">
       <c r="A42" s="4"/>
       <c r="B42" s="57" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -5282,29 +5282,29 @@
     <row r="44" spans="1:8" ht="39.75" thickBot="1">
       <c r="A44" s="4"/>
       <c r="B44" s="44" t="s">
+        <v>275</v>
+      </c>
+      <c r="C44" s="45" t="s">
         <v>276</v>
       </c>
-      <c r="C44" s="45" t="s">
+      <c r="D44" s="45" t="s">
         <v>277</v>
       </c>
-      <c r="D44" s="45" t="s">
+      <c r="E44" s="45" t="s">
         <v>278</v>
       </c>
-      <c r="E44" s="45" t="s">
+      <c r="F44" s="45" t="s">
         <v>279</v>
       </c>
-      <c r="F44" s="45" t="s">
+      <c r="G44" s="45" t="s">
         <v>280</v>
-      </c>
-      <c r="G44" s="45" t="s">
-        <v>281</v>
       </c>
       <c r="H44" s="4"/>
     </row>
     <row r="45" spans="1:8" ht="15.75" thickBot="1">
       <c r="A45" s="4"/>
       <c r="B45" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -5316,7 +5316,7 @@
     <row r="46" spans="1:8" ht="15.75" thickBot="1">
       <c r="A46" s="4"/>
       <c r="B46" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -5328,7 +5328,7 @@
     <row r="47" spans="1:8" ht="15" customHeight="1" thickBot="1">
       <c r="A47" s="4"/>
       <c r="B47" s="51" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
@@ -5340,7 +5340,7 @@
     <row r="48" spans="1:8" ht="15.75" thickBot="1">
       <c r="A48" s="4"/>
       <c r="B48" s="51" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
@@ -5352,7 +5352,7 @@
     <row r="49" spans="1:8" ht="15.75" thickBot="1">
       <c r="A49" s="4"/>
       <c r="B49" s="57" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -5374,19 +5374,19 @@
     <row r="51" spans="1:8" ht="39.75" thickBot="1">
       <c r="A51" s="4"/>
       <c r="B51" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="C51" s="45" t="s">
         <v>282</v>
       </c>
-      <c r="C51" s="45" t="s">
+      <c r="D51" s="45" t="s">
         <v>283</v>
       </c>
-      <c r="D51" s="45" t="s">
+      <c r="E51" s="45" t="s">
         <v>284</v>
       </c>
-      <c r="E51" s="45" t="s">
+      <c r="F51" s="45" t="s">
         <v>285</v>
-      </c>
-      <c r="F51" s="45" t="s">
-        <v>286</v>
       </c>
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
@@ -5394,7 +5394,7 @@
     <row r="52" spans="1:8" ht="15.75" thickBot="1">
       <c r="A52" s="4"/>
       <c r="B52" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
@@ -5406,7 +5406,7 @@
     <row r="53" spans="1:8" ht="15.75" thickBot="1">
       <c r="A53" s="4"/>
       <c r="B53" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
@@ -5418,7 +5418,7 @@
     <row r="54" spans="1:8" ht="15.75" thickBot="1">
       <c r="A54" s="4"/>
       <c r="B54" s="51" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
@@ -5430,7 +5430,7 @@
     <row r="55" spans="1:8" ht="15.75" thickBot="1">
       <c r="A55" s="4"/>
       <c r="B55" s="51" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
@@ -5442,7 +5442,7 @@
     <row r="56" spans="1:8" ht="15.75" thickBot="1">
       <c r="A56" s="4"/>
       <c r="B56" s="57" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -5470,8 +5470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q190"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98"/>
+    <sheetView topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="D129" sqref="D129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5566,7 +5566,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="59" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>1</v>
@@ -5582,7 +5582,7 @@
         <v>147</v>
       </c>
       <c r="I5" s="59" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J5" s="14" t="s">
         <v>1</v>
@@ -5998,7 +5998,7 @@
         <v>24</v>
       </c>
       <c r="C27" s="59" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D27" s="26" t="s">
         <v>1</v>
@@ -6065,13 +6065,13 @@
       <c r="E30" s="20"/>
       <c r="F30" s="20"/>
       <c r="G30" s="58"/>
-      <c r="H30" s="81" t="s">
+      <c r="H30" s="82" t="s">
         <v>171</v>
       </c>
-      <c r="I30" s="82"/>
-      <c r="J30" s="82"/>
-      <c r="K30" s="82"/>
-      <c r="L30" s="83"/>
+      <c r="I30" s="83"/>
+      <c r="J30" s="83"/>
+      <c r="K30" s="83"/>
+      <c r="L30" s="84"/>
       <c r="M30" s="58"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1">
@@ -6129,7 +6129,7 @@
         <v>30</v>
       </c>
       <c r="C34" s="59" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D34" s="26" t="s">
         <v>1</v>
@@ -6226,13 +6226,13 @@
       <c r="E39" s="20"/>
       <c r="F39" s="62"/>
       <c r="G39" s="58"/>
-      <c r="H39" s="81" t="s">
+      <c r="H39" s="82" t="s">
         <v>172</v>
       </c>
-      <c r="I39" s="82"/>
-      <c r="J39" s="82"/>
-      <c r="K39" s="82"/>
-      <c r="L39" s="83"/>
+      <c r="I39" s="83"/>
+      <c r="J39" s="83"/>
+      <c r="K39" s="83"/>
+      <c r="L39" s="84"/>
       <c r="M39" s="58"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" thickBot="1">
@@ -6256,7 +6256,7 @@
         <v>36</v>
       </c>
       <c r="C41" s="59" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>1</v>
@@ -6381,7 +6381,7 @@
         <v>42</v>
       </c>
       <c r="C48" s="59" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D48" s="14" t="s">
         <v>1</v>
@@ -6393,13 +6393,13 @@
         <v>3</v>
       </c>
       <c r="G48" s="58"/>
-      <c r="H48" s="81" t="s">
+      <c r="H48" s="82" t="s">
         <v>173</v>
       </c>
-      <c r="I48" s="82"/>
-      <c r="J48" s="82"/>
-      <c r="K48" s="82"/>
-      <c r="L48" s="83"/>
+      <c r="I48" s="83"/>
+      <c r="J48" s="83"/>
+      <c r="K48" s="83"/>
+      <c r="L48" s="84"/>
       <c r="M48" s="58"/>
     </row>
     <row r="49" spans="1:13" ht="15.75" thickBot="1">
@@ -6548,13 +6548,13 @@
       <c r="E57" s="39"/>
       <c r="F57" s="39"/>
       <c r="G57" s="58"/>
-      <c r="H57" s="81" t="s">
+      <c r="H57" s="82" t="s">
         <v>174</v>
       </c>
-      <c r="I57" s="82"/>
-      <c r="J57" s="82"/>
-      <c r="K57" s="82"/>
-      <c r="L57" s="83"/>
+      <c r="I57" s="83"/>
+      <c r="J57" s="83"/>
+      <c r="K57" s="83"/>
+      <c r="L57" s="84"/>
       <c r="M57" s="58"/>
     </row>
     <row r="58" spans="1:13" ht="15.75" thickBot="1">
@@ -6703,13 +6703,13 @@
       <c r="E66" s="20"/>
       <c r="F66" s="20"/>
       <c r="G66" s="58"/>
-      <c r="H66" s="81" t="s">
+      <c r="H66" s="82" t="s">
         <v>175</v>
       </c>
-      <c r="I66" s="82"/>
-      <c r="J66" s="82"/>
-      <c r="K66" s="82"/>
-      <c r="L66" s="83"/>
+      <c r="I66" s="83"/>
+      <c r="J66" s="83"/>
+      <c r="K66" s="83"/>
+      <c r="L66" s="84"/>
       <c r="M66" s="58"/>
     </row>
     <row r="67" spans="1:13" ht="15.75" thickBot="1">
@@ -6845,7 +6845,7 @@
         <v>176</v>
       </c>
       <c r="I74" s="59" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J74" s="14" t="s">
         <v>1</v>
@@ -7279,7 +7279,7 @@
     <row r="97" spans="1:13" ht="15.75" thickBot="1">
       <c r="A97" s="58"/>
       <c r="B97" s="19" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C97" s="20"/>
       <c r="D97" s="20"/>
@@ -7430,7 +7430,7 @@
         <v>97</v>
       </c>
       <c r="C105" s="59" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D105" s="14" t="s">
         <v>1</v>
@@ -7443,10 +7443,10 @@
       </c>
       <c r="G105" s="58"/>
       <c r="H105" s="13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I105" s="59" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J105" s="14" t="s">
         <v>1</v>
@@ -7831,7 +7831,7 @@
       <c r="F125" s="20"/>
       <c r="G125" s="58"/>
       <c r="H125" s="19" t="s">
-        <v>224</v>
+        <v>298</v>
       </c>
       <c r="I125" s="20"/>
       <c r="J125" s="20"/>
@@ -7850,7 +7850,7 @@
       <c r="F126" s="20"/>
       <c r="G126" s="58"/>
       <c r="H126" s="19" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I126" s="20"/>
       <c r="J126" s="20"/>
@@ -7869,7 +7869,7 @@
       <c r="F127" s="20"/>
       <c r="G127" s="58"/>
       <c r="H127" s="19" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I127" s="20"/>
       <c r="J127" s="20"/>
@@ -7888,7 +7888,7 @@
       <c r="F128" s="39"/>
       <c r="G128" s="58"/>
       <c r="H128" s="19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I128" s="20"/>
       <c r="J128" s="20"/>
@@ -7907,7 +7907,7 @@
       <c r="F129" s="20"/>
       <c r="G129" s="58"/>
       <c r="H129" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I129" s="20"/>
       <c r="J129" s="20"/>
@@ -7926,7 +7926,7 @@
       <c r="F130" s="20"/>
       <c r="G130" s="58"/>
       <c r="H130" s="19" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I130" s="20"/>
       <c r="J130" s="20"/>
@@ -7945,7 +7945,7 @@
       <c r="F131" s="41"/>
       <c r="G131" s="58"/>
       <c r="H131" s="19" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I131" s="20"/>
       <c r="J131" s="20"/>
@@ -7964,7 +7964,7 @@
       <c r="F132" s="20"/>
       <c r="G132" s="58"/>
       <c r="H132" s="19" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I132" s="20"/>
       <c r="J132" s="20"/>
@@ -7983,7 +7983,7 @@
       <c r="F133" s="20"/>
       <c r="G133" s="58"/>
       <c r="H133" s="19" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I133" s="20"/>
       <c r="J133" s="20"/>
@@ -8020,22 +8020,22 @@
       <c r="F135" s="20"/>
       <c r="G135" s="4"/>
       <c r="H135" s="44" t="s">
+        <v>233</v>
+      </c>
+      <c r="I135" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="I135" s="45" t="s">
+      <c r="J135" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="J135" s="45" t="s">
+      <c r="K135" s="45" t="s">
         <v>236</v>
       </c>
-      <c r="K135" s="45" t="s">
+      <c r="L135" s="45" t="s">
         <v>237</v>
       </c>
-      <c r="L135" s="45" t="s">
+      <c r="M135" s="45" t="s">
         <v>238</v>
-      </c>
-      <c r="M135" s="45" t="s">
-        <v>239</v>
       </c>
       <c r="N135" s="4"/>
     </row>
@@ -8050,7 +8050,7 @@
       <c r="F136" s="40"/>
       <c r="G136" s="4"/>
       <c r="H136" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I136" s="3"/>
       <c r="J136" s="3"/>
@@ -8070,7 +8070,7 @@
       <c r="F137" s="20"/>
       <c r="G137" s="4"/>
       <c r="H137" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I137" s="3"/>
       <c r="J137" s="3"/>
@@ -8090,7 +8090,7 @@
       <c r="F138" s="20"/>
       <c r="G138" s="4"/>
       <c r="H138" s="51" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I138" s="3"/>
       <c r="J138" s="3"/>
@@ -8110,7 +8110,7 @@
       <c r="F139" s="20"/>
       <c r="G139" s="4"/>
       <c r="H139" s="52" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I139" s="54"/>
       <c r="J139" s="54"/>
@@ -8130,7 +8130,7 @@
       <c r="F140" s="20"/>
       <c r="G140" s="4"/>
       <c r="H140" s="53" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I140" s="54"/>
       <c r="J140" s="54"/>
@@ -8168,22 +8168,22 @@
       <c r="F142" s="62"/>
       <c r="G142" s="4"/>
       <c r="H142" s="44" t="s">
+        <v>245</v>
+      </c>
+      <c r="I142" s="45" t="s">
         <v>246</v>
       </c>
-      <c r="I142" s="45" t="s">
+      <c r="J142" s="45" t="s">
         <v>247</v>
       </c>
-      <c r="J142" s="45" t="s">
+      <c r="K142" s="45" t="s">
         <v>248</v>
       </c>
-      <c r="K142" s="45" t="s">
+      <c r="L142" s="45" t="s">
         <v>249</v>
       </c>
-      <c r="L142" s="45" t="s">
+      <c r="M142" s="45" t="s">
         <v>250</v>
-      </c>
-      <c r="M142" s="45" t="s">
-        <v>251</v>
       </c>
       <c r="N142" s="4"/>
     </row>
@@ -8196,7 +8196,7 @@
       <c r="F143" s="58"/>
       <c r="G143" s="4"/>
       <c r="H143" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I143" s="3"/>
       <c r="J143" s="3"/>
@@ -8211,7 +8211,7 @@
         <v>135</v>
       </c>
       <c r="C144" s="59" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D144" s="14" t="s">
         <v>1</v>
@@ -8224,7 +8224,7 @@
       </c>
       <c r="G144" s="4"/>
       <c r="H144" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I144" s="3"/>
       <c r="J144" s="3"/>
@@ -8244,7 +8244,7 @@
       <c r="F145" s="20"/>
       <c r="G145" s="4"/>
       <c r="H145" s="51" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I145" s="3"/>
       <c r="J145" s="3"/>
@@ -8264,7 +8264,7 @@
       <c r="F146" s="20"/>
       <c r="G146" s="4"/>
       <c r="H146" s="51" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I146" s="3"/>
       <c r="J146" s="3"/>
@@ -8284,7 +8284,7 @@
       <c r="F147" s="20"/>
       <c r="G147" s="4"/>
       <c r="H147" s="57" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I147" s="2"/>
       <c r="J147" s="2"/>
@@ -8322,22 +8322,22 @@
       <c r="F149" s="20"/>
       <c r="G149" s="4"/>
       <c r="H149" s="44" t="s">
+        <v>251</v>
+      </c>
+      <c r="I149" s="45" t="s">
         <v>252</v>
       </c>
-      <c r="I149" s="45" t="s">
+      <c r="J149" s="45" t="s">
         <v>253</v>
       </c>
-      <c r="J149" s="45" t="s">
+      <c r="K149" s="45" t="s">
         <v>254</v>
       </c>
-      <c r="K149" s="45" t="s">
+      <c r="L149" s="45" t="s">
         <v>255</v>
       </c>
-      <c r="L149" s="45" t="s">
+      <c r="M149" s="45" t="s">
         <v>256</v>
-      </c>
-      <c r="M149" s="45" t="s">
-        <v>257</v>
       </c>
       <c r="N149" s="4"/>
     </row>
@@ -8352,7 +8352,7 @@
       <c r="F150" s="20"/>
       <c r="G150" s="4"/>
       <c r="H150" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I150" s="3"/>
       <c r="J150" s="3"/>
@@ -8372,7 +8372,7 @@
       <c r="F151" s="20"/>
       <c r="G151" s="4"/>
       <c r="H151" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I151" s="3"/>
       <c r="J151" s="3"/>
@@ -8392,7 +8392,7 @@
       <c r="F152" s="20"/>
       <c r="G152" s="4"/>
       <c r="H152" s="51" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I152" s="3"/>
       <c r="J152" s="3"/>
@@ -8412,7 +8412,7 @@
       <c r="F153" s="20"/>
       <c r="G153" s="4"/>
       <c r="H153" s="51" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I153" s="3"/>
       <c r="J153" s="3"/>
@@ -8432,7 +8432,7 @@
       <c r="F154" s="20"/>
       <c r="G154" s="4"/>
       <c r="H154" s="57" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I154" s="2"/>
       <c r="J154" s="2"/>
@@ -8468,47 +8468,47 @@
       <c r="F156" s="58"/>
       <c r="G156" s="4"/>
       <c r="H156" s="44" t="s">
+        <v>257</v>
+      </c>
+      <c r="I156" s="45" t="s">
         <v>258</v>
       </c>
-      <c r="I156" s="45" t="s">
+      <c r="J156" s="45" t="s">
         <v>259</v>
       </c>
-      <c r="J156" s="45" t="s">
+      <c r="K156" s="45" t="s">
         <v>260</v>
       </c>
-      <c r="K156" s="45" t="s">
+      <c r="L156" s="45" t="s">
         <v>261</v>
       </c>
-      <c r="L156" s="45" t="s">
+      <c r="M156" s="45" t="s">
         <v>262</v>
-      </c>
-      <c r="M156" s="45" t="s">
-        <v>263</v>
       </c>
       <c r="N156" s="4"/>
     </row>
     <row r="157" spans="1:14" ht="39.75" thickBot="1">
       <c r="A157" s="44" t="s">
+        <v>269</v>
+      </c>
+      <c r="B157" s="45" t="s">
         <v>270</v>
       </c>
-      <c r="B157" s="45" t="s">
+      <c r="C157" s="45" t="s">
         <v>271</v>
       </c>
-      <c r="C157" s="45" t="s">
+      <c r="D157" s="45" t="s">
         <v>272</v>
       </c>
-      <c r="D157" s="45" t="s">
+      <c r="E157" s="45" t="s">
         <v>273</v>
       </c>
-      <c r="E157" s="45" t="s">
+      <c r="F157" s="45" t="s">
         <v>274</v>
-      </c>
-      <c r="F157" s="45" t="s">
-        <v>275</v>
       </c>
       <c r="G157" s="4"/>
       <c r="H157" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I157" s="3"/>
       <c r="J157" s="3"/>
@@ -8519,7 +8519,7 @@
     </row>
     <row r="158" spans="1:14" ht="15.75" thickBot="1">
       <c r="A158" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B158" s="3"/>
       <c r="C158" s="3"/>
@@ -8528,7 +8528,7 @@
       <c r="F158" s="3"/>
       <c r="G158" s="4"/>
       <c r="H158" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I158" s="3"/>
       <c r="J158" s="3"/>
@@ -8539,7 +8539,7 @@
     </row>
     <row r="159" spans="1:14" ht="15.75" thickBot="1">
       <c r="A159" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B159" s="3"/>
       <c r="C159" s="3"/>
@@ -8548,7 +8548,7 @@
       <c r="F159" s="3"/>
       <c r="G159" s="4"/>
       <c r="H159" s="51" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I159" s="3"/>
       <c r="J159" s="3"/>
@@ -8559,7 +8559,7 @@
     </row>
     <row r="160" spans="1:14" ht="15.75" thickBot="1">
       <c r="A160" s="51" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B160" s="3"/>
       <c r="C160" s="3"/>
@@ -8568,7 +8568,7 @@
       <c r="F160" s="3"/>
       <c r="G160" s="4"/>
       <c r="H160" s="51" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I160" s="3"/>
       <c r="J160" s="3"/>
@@ -8579,7 +8579,7 @@
     </row>
     <row r="161" spans="1:14" ht="15.75" thickBot="1">
       <c r="A161" s="51" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B161" s="3"/>
       <c r="C161" s="3"/>
@@ -8588,7 +8588,7 @@
       <c r="F161" s="3"/>
       <c r="G161" s="4"/>
       <c r="H161" s="57" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I161" s="2"/>
       <c r="J161" s="2"/>
@@ -8599,7 +8599,7 @@
     </row>
     <row r="162" spans="1:14" ht="15.75" thickBot="1">
       <c r="A162" s="57" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B162" s="2"/>
       <c r="C162" s="2"/>
@@ -8624,47 +8624,47 @@
       <c r="F163" s="4"/>
       <c r="G163" s="4"/>
       <c r="H163" s="44" t="s">
+        <v>263</v>
+      </c>
+      <c r="I163" s="45" t="s">
         <v>264</v>
       </c>
-      <c r="I163" s="45" t="s">
+      <c r="J163" s="45" t="s">
         <v>265</v>
       </c>
-      <c r="J163" s="45" t="s">
+      <c r="K163" s="45" t="s">
         <v>266</v>
       </c>
-      <c r="K163" s="45" t="s">
+      <c r="L163" s="45" t="s">
         <v>267</v>
       </c>
-      <c r="L163" s="45" t="s">
+      <c r="M163" s="45" t="s">
         <v>268</v>
-      </c>
-      <c r="M163" s="45" t="s">
-        <v>269</v>
       </c>
       <c r="N163" s="4"/>
     </row>
     <row r="164" spans="1:14" ht="52.5" thickBot="1">
       <c r="A164" s="44" t="s">
+        <v>275</v>
+      </c>
+      <c r="B164" s="45" t="s">
         <v>276</v>
       </c>
-      <c r="B164" s="45" t="s">
+      <c r="C164" s="45" t="s">
         <v>277</v>
       </c>
-      <c r="C164" s="45" t="s">
+      <c r="D164" s="45" t="s">
         <v>278</v>
       </c>
-      <c r="D164" s="45" t="s">
+      <c r="E164" s="45" t="s">
         <v>279</v>
       </c>
-      <c r="E164" s="45" t="s">
+      <c r="F164" s="45" t="s">
         <v>280</v>
-      </c>
-      <c r="F164" s="45" t="s">
-        <v>281</v>
       </c>
       <c r="G164" s="4"/>
       <c r="H164" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I164" s="3"/>
       <c r="J164" s="3"/>
@@ -8675,7 +8675,7 @@
     </row>
     <row r="165" spans="1:14" ht="15.75" thickBot="1">
       <c r="A165" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B165" s="3"/>
       <c r="C165" s="3"/>
@@ -8684,7 +8684,7 @@
       <c r="F165" s="3"/>
       <c r="G165" s="4"/>
       <c r="H165" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I165" s="3"/>
       <c r="J165" s="3"/>
@@ -8695,7 +8695,7 @@
     </row>
     <row r="166" spans="1:14" ht="15.75" thickBot="1">
       <c r="A166" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B166" s="3"/>
       <c r="C166" s="3"/>
@@ -8704,7 +8704,7 @@
       <c r="F166" s="3"/>
       <c r="G166" s="4"/>
       <c r="H166" s="51" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I166" s="3"/>
       <c r="J166" s="3"/>
@@ -8715,7 +8715,7 @@
     </row>
     <row r="167" spans="1:14" ht="15.75" thickBot="1">
       <c r="A167" s="51" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B167" s="3"/>
       <c r="C167" s="3"/>
@@ -8724,7 +8724,7 @@
       <c r="F167" s="3"/>
       <c r="G167" s="4"/>
       <c r="H167" s="51" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I167" s="3"/>
       <c r="J167" s="3"/>
@@ -8735,7 +8735,7 @@
     </row>
     <row r="168" spans="1:14" ht="15.75" thickBot="1">
       <c r="A168" s="51" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B168" s="3"/>
       <c r="C168" s="3"/>
@@ -8744,7 +8744,7 @@
       <c r="F168" s="3"/>
       <c r="G168" s="4"/>
       <c r="H168" s="57" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I168" s="2"/>
       <c r="J168" s="2"/>
@@ -8755,7 +8755,7 @@
     </row>
     <row r="169" spans="1:14" ht="15.75" thickBot="1">
       <c r="A169" s="57" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B169" s="2"/>
       <c r="C169" s="2"/>
@@ -8790,19 +8790,19 @@
     <row r="171" spans="1:14" ht="52.5" thickBot="1">
       <c r="A171" s="4"/>
       <c r="B171" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="C171" s="45" t="s">
         <v>282</v>
       </c>
-      <c r="C171" s="45" t="s">
+      <c r="D171" s="45" t="s">
         <v>283</v>
       </c>
-      <c r="D171" s="45" t="s">
+      <c r="E171" s="45" t="s">
         <v>284</v>
       </c>
-      <c r="E171" s="45" t="s">
+      <c r="F171" s="45" t="s">
         <v>285</v>
-      </c>
-      <c r="F171" s="45" t="s">
-        <v>286</v>
       </c>
       <c r="G171" s="4"/>
       <c r="H171" s="4"/>
@@ -8816,7 +8816,7 @@
     <row r="172" spans="1:14" ht="15.75" thickBot="1">
       <c r="A172" s="4"/>
       <c r="B172" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C172" s="3"/>
       <c r="D172" s="3"/>
@@ -8834,7 +8834,7 @@
     <row r="173" spans="1:14" ht="15.75" thickBot="1">
       <c r="A173" s="4"/>
       <c r="B173" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C173" s="3"/>
       <c r="D173" s="3"/>
@@ -8852,7 +8852,7 @@
     <row r="174" spans="1:14" ht="15.75" thickBot="1">
       <c r="A174" s="4"/>
       <c r="B174" s="51" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C174" s="3"/>
       <c r="D174" s="3"/>
@@ -8870,7 +8870,7 @@
     <row r="175" spans="1:14" ht="15.75" thickBot="1">
       <c r="A175" s="4"/>
       <c r="B175" s="51" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C175" s="3"/>
       <c r="D175" s="3"/>
@@ -8888,7 +8888,7 @@
     <row r="176" spans="1:14" ht="15.75" thickBot="1">
       <c r="A176" s="4"/>
       <c r="B176" s="57" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C176" s="2"/>
       <c r="D176" s="2"/>
@@ -9066,8 +9066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="D123" sqref="D123"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9087,61 +9087,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="23.25" customHeight="1">
-      <c r="A1" s="86" t="s">
-        <v>287</v>
-      </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="86"/>
-      <c r="L1" s="86"/>
-      <c r="M1" s="86"/>
+      <c r="A1" s="87" t="s">
+        <v>286</v>
+      </c>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="87"/>
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
+      <c r="M1" s="87"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1">
-      <c r="A2" s="86"/>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
+      <c r="A2" s="87"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="87"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="87"/>
+      <c r="L2" s="87"/>
+      <c r="M2" s="87"/>
       <c r="N2" s="1"/>
       <c r="O2" s="69"/>
       <c r="P2" s="70" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="Q2" s="1"/>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1">
-      <c r="A3" s="86"/>
-      <c r="B3" s="86"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="86"/>
-      <c r="K3" s="86"/>
-      <c r="L3" s="86"/>
-      <c r="M3" s="86"/>
+      <c r="A3" s="87"/>
+      <c r="B3" s="87"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="87"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -9164,7 +9164,7 @@
       <c r="N4" s="1"/>
       <c r="O4" s="71"/>
       <c r="P4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="Q4" s="1"/>
     </row>
@@ -9174,7 +9174,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="59" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>1</v>
@@ -9190,7 +9190,7 @@
         <v>147</v>
       </c>
       <c r="I5" s="59" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J5" s="14" t="s">
         <v>1</v>
@@ -9209,7 +9209,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="72" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D6" s="72"/>
       <c r="E6" s="73"/>
@@ -9313,7 +9313,7 @@
       <c r="H11" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="I11" s="20"/>
+      <c r="I11" s="73"/>
       <c r="J11" s="20"/>
       <c r="K11" s="20"/>
       <c r="L11" s="73"/>
@@ -9436,7 +9436,7 @@
     <row r="18" spans="1:13" ht="15.75" thickBot="1">
       <c r="A18" s="58"/>
       <c r="B18" s="19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C18" s="72"/>
       <c r="D18" s="20"/>
@@ -9608,7 +9608,7 @@
         <v>24</v>
       </c>
       <c r="C27" s="59" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D27" s="26" t="s">
         <v>1</v>
@@ -9623,7 +9623,7 @@
       <c r="H27" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="I27" s="20"/>
+      <c r="I27" s="73"/>
       <c r="J27" s="20"/>
       <c r="K27" s="20"/>
       <c r="L27" s="20"/>
@@ -9634,7 +9634,7 @@
       <c r="B28" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="20"/>
+      <c r="C28" s="73"/>
       <c r="D28" s="73"/>
       <c r="E28" s="73"/>
       <c r="F28" s="20"/>
@@ -9671,19 +9671,19 @@
         <v>27</v>
       </c>
       <c r="C30" s="75" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D30" s="20"/>
       <c r="E30" s="73"/>
       <c r="F30" s="20"/>
       <c r="G30" s="58"/>
-      <c r="H30" s="81" t="s">
+      <c r="H30" s="82" t="s">
         <v>171</v>
       </c>
-      <c r="I30" s="82"/>
-      <c r="J30" s="82"/>
-      <c r="K30" s="82"/>
-      <c r="L30" s="83"/>
+      <c r="I30" s="83"/>
+      <c r="J30" s="83"/>
+      <c r="K30" s="83"/>
+      <c r="L30" s="84"/>
       <c r="M30" s="58"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1">
@@ -9697,7 +9697,7 @@
       <c r="F31" s="20"/>
       <c r="G31" s="58"/>
       <c r="H31" s="77" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I31" s="63"/>
       <c r="J31" s="63"/>
@@ -9743,7 +9743,7 @@
         <v>30</v>
       </c>
       <c r="C34" s="59" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D34" s="26" t="s">
         <v>1</v>
@@ -9840,13 +9840,13 @@
       <c r="E39" s="73"/>
       <c r="F39" s="62"/>
       <c r="G39" s="58"/>
-      <c r="H39" s="81" t="s">
+      <c r="H39" s="82" t="s">
         <v>172</v>
       </c>
-      <c r="I39" s="82"/>
-      <c r="J39" s="82"/>
-      <c r="K39" s="82"/>
-      <c r="L39" s="83"/>
+      <c r="I39" s="83"/>
+      <c r="J39" s="83"/>
+      <c r="K39" s="83"/>
+      <c r="L39" s="84"/>
       <c r="M39" s="58"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" thickBot="1">
@@ -9870,7 +9870,7 @@
         <v>36</v>
       </c>
       <c r="C41" s="59" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>1</v>
@@ -9995,7 +9995,7 @@
         <v>42</v>
       </c>
       <c r="C48" s="59" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D48" s="14" t="s">
         <v>1</v>
@@ -10007,13 +10007,13 @@
         <v>3</v>
       </c>
       <c r="G48" s="58"/>
-      <c r="H48" s="81" t="s">
+      <c r="H48" s="82" t="s">
         <v>173</v>
       </c>
-      <c r="I48" s="82"/>
-      <c r="J48" s="82"/>
-      <c r="K48" s="82"/>
-      <c r="L48" s="83"/>
+      <c r="I48" s="83"/>
+      <c r="J48" s="83"/>
+      <c r="K48" s="83"/>
+      <c r="L48" s="84"/>
       <c r="M48" s="58"/>
     </row>
     <row r="49" spans="1:13" ht="15.75" thickBot="1">
@@ -10074,7 +10074,9 @@
       </c>
       <c r="C52" s="20"/>
       <c r="D52" s="73"/>
-      <c r="E52" s="20"/>
+      <c r="E52" s="73">
+        <v>0</v>
+      </c>
       <c r="F52" s="20"/>
       <c r="G52" s="58"/>
       <c r="H52" s="20"/>
@@ -10162,13 +10164,13 @@
       <c r="E57" s="39"/>
       <c r="F57" s="74"/>
       <c r="G57" s="58"/>
-      <c r="H57" s="81" t="s">
+      <c r="H57" s="82" t="s">
         <v>174</v>
       </c>
-      <c r="I57" s="82"/>
-      <c r="J57" s="82"/>
-      <c r="K57" s="82"/>
-      <c r="L57" s="83"/>
+      <c r="I57" s="83"/>
+      <c r="J57" s="83"/>
+      <c r="K57" s="83"/>
+      <c r="L57" s="84"/>
       <c r="M57" s="58"/>
     </row>
     <row r="58" spans="1:13" ht="15.75" thickBot="1">
@@ -10317,13 +10319,13 @@
       <c r="E66" s="20"/>
       <c r="F66" s="20"/>
       <c r="G66" s="58"/>
-      <c r="H66" s="81" t="s">
+      <c r="H66" s="82" t="s">
         <v>175</v>
       </c>
-      <c r="I66" s="82"/>
-      <c r="J66" s="82"/>
-      <c r="K66" s="82"/>
-      <c r="L66" s="83"/>
+      <c r="I66" s="83"/>
+      <c r="J66" s="83"/>
+      <c r="K66" s="83"/>
+      <c r="L66" s="84"/>
       <c r="M66" s="58"/>
     </row>
     <row r="67" spans="1:13" ht="15.75" thickBot="1">
@@ -10337,14 +10339,14 @@
       <c r="F67" s="73"/>
       <c r="G67" s="58"/>
       <c r="H67" s="77" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I67" s="63"/>
       <c r="J67" s="63"/>
-      <c r="K67" s="87" t="s">
-        <v>294</v>
-      </c>
-      <c r="L67" s="88"/>
+      <c r="K67" s="88" t="s">
+        <v>293</v>
+      </c>
+      <c r="L67" s="89"/>
       <c r="M67" s="58"/>
     </row>
     <row r="68" spans="1:13" ht="15.75" thickBot="1">
@@ -10358,14 +10360,14 @@
       <c r="F68" s="20"/>
       <c r="G68" s="58"/>
       <c r="H68" s="77" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="I68" s="63"/>
       <c r="J68" s="63"/>
-      <c r="K68" s="87" t="s">
-        <v>295</v>
-      </c>
-      <c r="L68" s="88"/>
+      <c r="K68" s="88" t="s">
+        <v>294</v>
+      </c>
+      <c r="L68" s="89"/>
       <c r="M68" s="58"/>
     </row>
     <row r="69" spans="1:13" ht="15.75" thickBot="1">
@@ -10381,8 +10383,8 @@
       <c r="H69" s="20"/>
       <c r="I69" s="20"/>
       <c r="J69" s="20"/>
-      <c r="K69" s="84"/>
-      <c r="L69" s="85"/>
+      <c r="K69" s="85"/>
+      <c r="L69" s="86"/>
       <c r="M69" s="58"/>
     </row>
     <row r="70" spans="1:13" ht="15.75" thickBot="1">
@@ -10398,8 +10400,8 @@
       <c r="H70" s="20"/>
       <c r="I70" s="20"/>
       <c r="J70" s="20"/>
-      <c r="K70" s="84"/>
-      <c r="L70" s="85"/>
+      <c r="K70" s="85"/>
+      <c r="L70" s="86"/>
       <c r="M70" s="58"/>
     </row>
     <row r="71" spans="1:13" ht="15.75" thickBot="1">
@@ -10415,8 +10417,8 @@
       <c r="H71" s="20"/>
       <c r="I71" s="20"/>
       <c r="J71" s="20"/>
-      <c r="K71" s="84"/>
-      <c r="L71" s="85"/>
+      <c r="K71" s="85"/>
+      <c r="L71" s="86"/>
       <c r="M71" s="58"/>
     </row>
     <row r="72" spans="1:13" ht="15.75" thickBot="1">
@@ -10432,8 +10434,8 @@
       <c r="H72" s="20"/>
       <c r="I72" s="20"/>
       <c r="J72" s="20"/>
-      <c r="K72" s="84"/>
-      <c r="L72" s="85"/>
+      <c r="K72" s="85"/>
+      <c r="L72" s="86"/>
       <c r="M72" s="58"/>
     </row>
     <row r="73" spans="1:13" ht="15.75" thickBot="1">
@@ -10467,7 +10469,7 @@
         <v>176</v>
       </c>
       <c r="I74" s="59" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J74" s="14" t="s">
         <v>1</v>
@@ -10752,7 +10754,7 @@
         <v>83</v>
       </c>
       <c r="C89" s="20"/>
-      <c r="D89" s="89"/>
+      <c r="D89" s="79"/>
       <c r="E89" s="73"/>
       <c r="F89" s="73"/>
       <c r="G89" s="58"/>
@@ -10901,7 +10903,7 @@
     <row r="97" spans="1:13" ht="15.75" thickBot="1">
       <c r="A97" s="58"/>
       <c r="B97" s="19" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C97" s="73"/>
       <c r="D97" s="20"/>
@@ -11052,7 +11054,7 @@
         <v>97</v>
       </c>
       <c r="C105" s="59" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D105" s="14" t="s">
         <v>1</v>
@@ -11065,10 +11067,10 @@
       </c>
       <c r="G105" s="58"/>
       <c r="H105" s="13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I105" s="59" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J105" s="14" t="s">
         <v>1</v>
@@ -11285,7 +11287,7 @@
         <v>215</v>
       </c>
       <c r="I116" s="75" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J116" s="20"/>
       <c r="K116" s="20"/>
@@ -11298,7 +11300,7 @@
         <v>109</v>
       </c>
       <c r="C117" s="76" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D117" s="41"/>
       <c r="E117" s="39"/>
@@ -11457,7 +11459,7 @@
       <c r="F125" s="20"/>
       <c r="G125" s="58"/>
       <c r="H125" s="19" t="s">
-        <v>224</v>
+        <v>298</v>
       </c>
       <c r="I125" s="73"/>
       <c r="J125" s="20"/>
@@ -11476,7 +11478,7 @@
       <c r="F126" s="20"/>
       <c r="G126" s="58"/>
       <c r="H126" s="19" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I126" s="20"/>
       <c r="J126" s="20"/>
@@ -11495,7 +11497,7 @@
       <c r="F127" s="20"/>
       <c r="G127" s="58"/>
       <c r="H127" s="19" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I127" s="20"/>
       <c r="J127" s="20"/>
@@ -11514,7 +11516,7 @@
       <c r="F128" s="39"/>
       <c r="G128" s="58"/>
       <c r="H128" s="19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I128" s="20"/>
       <c r="J128" s="20"/>
@@ -11533,7 +11535,7 @@
       <c r="F129" s="20"/>
       <c r="G129" s="58"/>
       <c r="H129" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I129" s="20"/>
       <c r="J129" s="20"/>
@@ -11552,7 +11554,7 @@
       <c r="F130" s="20"/>
       <c r="G130" s="58"/>
       <c r="H130" s="19" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I130" s="73"/>
       <c r="J130" s="73"/>
@@ -11571,7 +11573,7 @@
       <c r="F131" s="41"/>
       <c r="G131" s="58"/>
       <c r="H131" s="19" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I131" s="20"/>
       <c r="J131" s="20"/>
@@ -11590,7 +11592,7 @@
       <c r="F132" s="20"/>
       <c r="G132" s="58"/>
       <c r="H132" s="19" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I132" s="20"/>
       <c r="J132" s="20"/>
@@ -11609,7 +11611,7 @@
       <c r="F133" s="20"/>
       <c r="G133" s="58"/>
       <c r="H133" s="19" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I133" s="20"/>
       <c r="J133" s="73"/>
@@ -11646,22 +11648,22 @@
       <c r="F135" s="20"/>
       <c r="G135" s="4"/>
       <c r="H135" s="44" t="s">
+        <v>233</v>
+      </c>
+      <c r="I135" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="I135" s="45" t="s">
+      <c r="J135" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="J135" s="45" t="s">
+      <c r="K135" s="45" t="s">
         <v>236</v>
       </c>
-      <c r="K135" s="45" t="s">
+      <c r="L135" s="45" t="s">
         <v>237</v>
       </c>
-      <c r="L135" s="45" t="s">
+      <c r="M135" s="45" t="s">
         <v>238</v>
-      </c>
-      <c r="M135" s="45" t="s">
-        <v>239</v>
       </c>
       <c r="N135" s="4"/>
     </row>
@@ -11676,7 +11678,7 @@
       <c r="F136" s="78"/>
       <c r="G136" s="4"/>
       <c r="H136" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I136" s="3"/>
       <c r="J136" s="3"/>
@@ -11696,7 +11698,7 @@
       <c r="F137" s="20"/>
       <c r="G137" s="4"/>
       <c r="H137" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I137" s="3"/>
       <c r="J137" s="3"/>
@@ -11716,7 +11718,7 @@
       <c r="F138" s="20"/>
       <c r="G138" s="4"/>
       <c r="H138" s="51" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I138" s="3"/>
       <c r="J138" s="3"/>
@@ -11736,7 +11738,7 @@
       <c r="F139" s="20"/>
       <c r="G139" s="4"/>
       <c r="H139" s="52" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I139" s="54"/>
       <c r="J139" s="54"/>
@@ -11756,7 +11758,7 @@
       <c r="F140" s="20"/>
       <c r="G140" s="4"/>
       <c r="H140" s="53" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I140" s="54"/>
       <c r="J140" s="54"/>
@@ -11794,22 +11796,22 @@
       <c r="F142" s="62"/>
       <c r="G142" s="4"/>
       <c r="H142" s="44" t="s">
+        <v>245</v>
+      </c>
+      <c r="I142" s="45" t="s">
         <v>246</v>
       </c>
-      <c r="I142" s="45" t="s">
+      <c r="J142" s="45" t="s">
         <v>247</v>
       </c>
-      <c r="J142" s="45" t="s">
+      <c r="K142" s="45" t="s">
         <v>248</v>
       </c>
-      <c r="K142" s="45" t="s">
+      <c r="L142" s="45" t="s">
         <v>249</v>
       </c>
-      <c r="L142" s="45" t="s">
+      <c r="M142" s="45" t="s">
         <v>250</v>
-      </c>
-      <c r="M142" s="45" t="s">
-        <v>251</v>
       </c>
       <c r="N142" s="4"/>
     </row>
@@ -11822,7 +11824,7 @@
       <c r="F143" s="58"/>
       <c r="G143" s="4"/>
       <c r="H143" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I143" s="3"/>
       <c r="J143" s="3"/>
@@ -11837,7 +11839,7 @@
         <v>135</v>
       </c>
       <c r="C144" s="59" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D144" s="14" t="s">
         <v>1</v>
@@ -11850,7 +11852,7 @@
       </c>
       <c r="G144" s="4"/>
       <c r="H144" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I144" s="3"/>
       <c r="J144" s="3"/>
@@ -11870,7 +11872,7 @@
       <c r="F145" s="20"/>
       <c r="G145" s="4"/>
       <c r="H145" s="51" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I145" s="3"/>
       <c r="J145" s="3"/>
@@ -11890,7 +11892,7 @@
       <c r="F146" s="20"/>
       <c r="G146" s="4"/>
       <c r="H146" s="51" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I146" s="3"/>
       <c r="J146" s="3"/>
@@ -11910,7 +11912,7 @@
       <c r="F147" s="20"/>
       <c r="G147" s="4"/>
       <c r="H147" s="57" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I147" s="2"/>
       <c r="J147" s="2"/>
@@ -11948,22 +11950,22 @@
       <c r="F149" s="20"/>
       <c r="G149" s="4"/>
       <c r="H149" s="44" t="s">
+        <v>251</v>
+      </c>
+      <c r="I149" s="45" t="s">
         <v>252</v>
       </c>
-      <c r="I149" s="45" t="s">
+      <c r="J149" s="45" t="s">
         <v>253</v>
       </c>
-      <c r="J149" s="45" t="s">
+      <c r="K149" s="45" t="s">
         <v>254</v>
       </c>
-      <c r="K149" s="45" t="s">
+      <c r="L149" s="45" t="s">
         <v>255</v>
       </c>
-      <c r="L149" s="45" t="s">
+      <c r="M149" s="45" t="s">
         <v>256</v>
-      </c>
-      <c r="M149" s="45" t="s">
-        <v>257</v>
       </c>
       <c r="N149" s="4"/>
     </row>
@@ -11978,7 +11980,7 @@
       <c r="F150" s="73"/>
       <c r="G150" s="4"/>
       <c r="H150" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I150" s="3"/>
       <c r="J150" s="3"/>
@@ -11998,7 +12000,7 @@
       <c r="F151" s="20"/>
       <c r="G151" s="4"/>
       <c r="H151" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I151" s="3"/>
       <c r="J151" s="3"/>
@@ -12018,7 +12020,7 @@
       <c r="F152" s="73"/>
       <c r="G152" s="4"/>
       <c r="H152" s="51" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I152" s="3"/>
       <c r="J152" s="3"/>
@@ -12038,7 +12040,7 @@
       <c r="F153" s="20"/>
       <c r="G153" s="4"/>
       <c r="H153" s="51" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I153" s="3"/>
       <c r="J153" s="3"/>
@@ -12058,7 +12060,7 @@
       <c r="F154" s="20"/>
       <c r="G154" s="4"/>
       <c r="H154" s="57" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I154" s="2"/>
       <c r="J154" s="2"/>
@@ -12094,47 +12096,47 @@
       <c r="F156" s="58"/>
       <c r="G156" s="4"/>
       <c r="H156" s="44" t="s">
+        <v>257</v>
+      </c>
+      <c r="I156" s="45" t="s">
         <v>258</v>
       </c>
-      <c r="I156" s="45" t="s">
+      <c r="J156" s="45" t="s">
         <v>259</v>
       </c>
-      <c r="J156" s="45" t="s">
+      <c r="K156" s="45" t="s">
         <v>260</v>
       </c>
-      <c r="K156" s="45" t="s">
+      <c r="L156" s="45" t="s">
         <v>261</v>
       </c>
-      <c r="L156" s="45" t="s">
+      <c r="M156" s="45" t="s">
         <v>262</v>
-      </c>
-      <c r="M156" s="45" t="s">
-        <v>263</v>
       </c>
       <c r="N156" s="4"/>
     </row>
     <row r="157" spans="1:14" ht="27" thickBot="1">
       <c r="A157" s="44" t="s">
+        <v>269</v>
+      </c>
+      <c r="B157" s="45" t="s">
         <v>270</v>
       </c>
-      <c r="B157" s="45" t="s">
+      <c r="C157" s="45" t="s">
         <v>271</v>
       </c>
-      <c r="C157" s="45" t="s">
+      <c r="D157" s="45" t="s">
         <v>272</v>
       </c>
-      <c r="D157" s="45" t="s">
+      <c r="E157" s="45" t="s">
         <v>273</v>
       </c>
-      <c r="E157" s="45" t="s">
+      <c r="F157" s="45" t="s">
         <v>274</v>
-      </c>
-      <c r="F157" s="45" t="s">
-        <v>275</v>
       </c>
       <c r="G157" s="4"/>
       <c r="H157" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I157" s="3"/>
       <c r="J157" s="3"/>
@@ -12145,7 +12147,7 @@
     </row>
     <row r="158" spans="1:14" ht="15.75" thickBot="1">
       <c r="A158" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B158" s="3"/>
       <c r="C158" s="3"/>
@@ -12154,7 +12156,7 @@
       <c r="F158" s="3"/>
       <c r="G158" s="4"/>
       <c r="H158" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I158" s="3"/>
       <c r="J158" s="3"/>
@@ -12165,7 +12167,7 @@
     </row>
     <row r="159" spans="1:14" ht="15.75" thickBot="1">
       <c r="A159" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B159" s="3"/>
       <c r="C159" s="3"/>
@@ -12174,7 +12176,7 @@
       <c r="F159" s="3"/>
       <c r="G159" s="4"/>
       <c r="H159" s="51" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I159" s="3"/>
       <c r="J159" s="3"/>
@@ -12185,7 +12187,7 @@
     </row>
     <row r="160" spans="1:14" ht="15.75" thickBot="1">
       <c r="A160" s="51" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B160" s="3"/>
       <c r="C160" s="3"/>
@@ -12194,7 +12196,7 @@
       <c r="F160" s="3"/>
       <c r="G160" s="4"/>
       <c r="H160" s="51" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I160" s="3"/>
       <c r="J160" s="3"/>
@@ -12205,7 +12207,7 @@
     </row>
     <row r="161" spans="1:14" ht="15.75" thickBot="1">
       <c r="A161" s="51" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B161" s="3"/>
       <c r="C161" s="3"/>
@@ -12214,7 +12216,7 @@
       <c r="F161" s="3"/>
       <c r="G161" s="4"/>
       <c r="H161" s="57" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I161" s="2"/>
       <c r="J161" s="2"/>
@@ -12225,7 +12227,7 @@
     </row>
     <row r="162" spans="1:14" ht="15.75" thickBot="1">
       <c r="A162" s="57" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B162" s="2"/>
       <c r="C162" s="2"/>
@@ -12250,47 +12252,47 @@
       <c r="F163" s="4"/>
       <c r="G163" s="4"/>
       <c r="H163" s="44" t="s">
+        <v>263</v>
+      </c>
+      <c r="I163" s="45" t="s">
         <v>264</v>
       </c>
-      <c r="I163" s="45" t="s">
+      <c r="J163" s="45" t="s">
         <v>265</v>
       </c>
-      <c r="J163" s="45" t="s">
+      <c r="K163" s="45" t="s">
         <v>266</v>
       </c>
-      <c r="K163" s="45" t="s">
+      <c r="L163" s="45" t="s">
         <v>267</v>
       </c>
-      <c r="L163" s="45" t="s">
+      <c r="M163" s="45" t="s">
         <v>268</v>
-      </c>
-      <c r="M163" s="45" t="s">
-        <v>269</v>
       </c>
       <c r="N163" s="4"/>
     </row>
     <row r="164" spans="1:14" ht="39.75" thickBot="1">
       <c r="A164" s="44" t="s">
+        <v>275</v>
+      </c>
+      <c r="B164" s="45" t="s">
         <v>276</v>
       </c>
-      <c r="B164" s="45" t="s">
+      <c r="C164" s="45" t="s">
         <v>277</v>
       </c>
-      <c r="C164" s="45" t="s">
+      <c r="D164" s="45" t="s">
         <v>278</v>
       </c>
-      <c r="D164" s="45" t="s">
+      <c r="E164" s="45" t="s">
         <v>279</v>
       </c>
-      <c r="E164" s="45" t="s">
+      <c r="F164" s="45" t="s">
         <v>280</v>
-      </c>
-      <c r="F164" s="45" t="s">
-        <v>281</v>
       </c>
       <c r="G164" s="4"/>
       <c r="H164" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I164" s="3"/>
       <c r="J164" s="3"/>
@@ -12301,7 +12303,7 @@
     </row>
     <row r="165" spans="1:14" ht="15.75" thickBot="1">
       <c r="A165" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B165" s="3"/>
       <c r="C165" s="3"/>
@@ -12310,7 +12312,7 @@
       <c r="F165" s="3"/>
       <c r="G165" s="4"/>
       <c r="H165" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I165" s="3"/>
       <c r="J165" s="3"/>
@@ -12321,7 +12323,7 @@
     </row>
     <row r="166" spans="1:14" ht="15.75" thickBot="1">
       <c r="A166" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B166" s="3"/>
       <c r="C166" s="3"/>
@@ -12330,7 +12332,7 @@
       <c r="F166" s="3"/>
       <c r="G166" s="4"/>
       <c r="H166" s="51" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I166" s="3"/>
       <c r="J166" s="3"/>
@@ -12341,7 +12343,7 @@
     </row>
     <row r="167" spans="1:14" ht="15.75" thickBot="1">
       <c r="A167" s="51" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B167" s="3"/>
       <c r="C167" s="3"/>
@@ -12350,7 +12352,7 @@
       <c r="F167" s="3"/>
       <c r="G167" s="4"/>
       <c r="H167" s="51" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I167" s="3"/>
       <c r="J167" s="3"/>
@@ -12361,7 +12363,7 @@
     </row>
     <row r="168" spans="1:14" ht="15.75" thickBot="1">
       <c r="A168" s="51" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B168" s="3"/>
       <c r="C168" s="3"/>
@@ -12370,7 +12372,7 @@
       <c r="F168" s="3"/>
       <c r="G168" s="4"/>
       <c r="H168" s="57" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I168" s="2"/>
       <c r="J168" s="2"/>
@@ -12381,7 +12383,7 @@
     </row>
     <row r="169" spans="1:14" ht="15.75" thickBot="1">
       <c r="A169" s="57" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B169" s="2"/>
       <c r="C169" s="2"/>
@@ -12416,19 +12418,19 @@
     <row r="171" spans="1:14" ht="27" thickBot="1">
       <c r="A171" s="4"/>
       <c r="B171" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="C171" s="45" t="s">
         <v>282</v>
       </c>
-      <c r="C171" s="45" t="s">
+      <c r="D171" s="45" t="s">
         <v>283</v>
       </c>
-      <c r="D171" s="45" t="s">
+      <c r="E171" s="45" t="s">
         <v>284</v>
       </c>
-      <c r="E171" s="45" t="s">
+      <c r="F171" s="45" t="s">
         <v>285</v>
-      </c>
-      <c r="F171" s="45" t="s">
-        <v>286</v>
       </c>
       <c r="G171" s="4"/>
       <c r="H171" s="4"/>
@@ -12442,7 +12444,7 @@
     <row r="172" spans="1:14" ht="15.75" thickBot="1">
       <c r="A172" s="4"/>
       <c r="B172" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C172" s="3"/>
       <c r="D172" s="3"/>
@@ -12460,7 +12462,7 @@
     <row r="173" spans="1:14" ht="15.75" thickBot="1">
       <c r="A173" s="4"/>
       <c r="B173" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C173" s="3"/>
       <c r="D173" s="3"/>
@@ -12478,7 +12480,7 @@
     <row r="174" spans="1:14" ht="15.75" thickBot="1">
       <c r="A174" s="4"/>
       <c r="B174" s="51" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C174" s="3"/>
       <c r="D174" s="3"/>
@@ -12496,7 +12498,7 @@
     <row r="175" spans="1:14" ht="15.75" thickBot="1">
       <c r="A175" s="4"/>
       <c r="B175" s="51" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C175" s="3"/>
       <c r="D175" s="3"/>
@@ -12514,7 +12516,7 @@
     <row r="176" spans="1:14" ht="15.75" thickBot="1">
       <c r="A176" s="4"/>
       <c r="B176" s="57" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C176" s="2"/>
       <c r="D176" s="2"/>

</xml_diff>

<commit_message>
stats on su updated
SU page: updated stats on many items
proc_item file : removed a ctc from sssu short bow
</commit_message>
<xml_diff>
--- a/check list.xlsx
+++ b/check list.xlsx
@@ -1518,6 +1518,12 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1546,12 +1552,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2390,13 +2390,13 @@
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
       <c r="G27" s="7"/>
-      <c r="H27" s="85" t="s">
+      <c r="H27" s="87" t="s">
         <v>171</v>
       </c>
-      <c r="I27" s="85"/>
-      <c r="J27" s="85"/>
-      <c r="K27" s="85"/>
-      <c r="L27" s="85"/>
+      <c r="I27" s="87"/>
+      <c r="J27" s="87"/>
+      <c r="K27" s="87"/>
+      <c r="L27" s="87"/>
       <c r="M27" s="7"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1">
@@ -2551,13 +2551,13 @@
       <c r="E36" s="20"/>
       <c r="F36" s="29"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="85" t="s">
+      <c r="H36" s="87" t="s">
         <v>172</v>
       </c>
-      <c r="I36" s="85"/>
-      <c r="J36" s="85"/>
-      <c r="K36" s="85"/>
-      <c r="L36" s="85"/>
+      <c r="I36" s="87"/>
+      <c r="J36" s="87"/>
+      <c r="K36" s="87"/>
+      <c r="L36" s="87"/>
       <c r="M36" s="7"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
@@ -2718,13 +2718,13 @@
         <v>3</v>
       </c>
       <c r="G45" s="7"/>
-      <c r="H45" s="85" t="s">
+      <c r="H45" s="87" t="s">
         <v>173</v>
       </c>
-      <c r="I45" s="85"/>
-      <c r="J45" s="85"/>
-      <c r="K45" s="85"/>
-      <c r="L45" s="85"/>
+      <c r="I45" s="87"/>
+      <c r="J45" s="87"/>
+      <c r="K45" s="87"/>
+      <c r="L45" s="87"/>
       <c r="M45" s="7"/>
     </row>
     <row r="46" spans="1:13" ht="15.75" thickBot="1">
@@ -2873,13 +2873,13 @@
       <c r="E54" s="39"/>
       <c r="F54" s="39"/>
       <c r="G54" s="7"/>
-      <c r="H54" s="85" t="s">
+      <c r="H54" s="87" t="s">
         <v>174</v>
       </c>
-      <c r="I54" s="85"/>
-      <c r="J54" s="85"/>
-      <c r="K54" s="85"/>
-      <c r="L54" s="85"/>
+      <c r="I54" s="87"/>
+      <c r="J54" s="87"/>
+      <c r="K54" s="87"/>
+      <c r="L54" s="87"/>
       <c r="M54" s="7"/>
     </row>
     <row r="55" spans="1:13" ht="15.75" thickBot="1">
@@ -3028,13 +3028,13 @@
       <c r="E63" s="20"/>
       <c r="F63" s="20"/>
       <c r="G63" s="7"/>
-      <c r="H63" s="85" t="s">
+      <c r="H63" s="87" t="s">
         <v>175</v>
       </c>
-      <c r="I63" s="85"/>
-      <c r="J63" s="85"/>
-      <c r="K63" s="85"/>
-      <c r="L63" s="85"/>
+      <c r="I63" s="87"/>
+      <c r="J63" s="87"/>
+      <c r="K63" s="87"/>
+      <c r="L63" s="87"/>
       <c r="M63" s="7"/>
     </row>
     <row r="64" spans="1:13" ht="15.75" thickBot="1">
@@ -4343,11 +4343,11 @@
       <c r="E132" s="20"/>
       <c r="F132" s="20"/>
       <c r="G132" s="7"/>
-      <c r="H132" s="84"/>
-      <c r="I132" s="84"/>
-      <c r="J132" s="84"/>
-      <c r="K132" s="84"/>
-      <c r="L132" s="84"/>
+      <c r="H132" s="86"/>
+      <c r="I132" s="86"/>
+      <c r="J132" s="86"/>
+      <c r="K132" s="86"/>
+      <c r="L132" s="86"/>
       <c r="M132" s="7"/>
     </row>
     <row r="133" spans="1:14" ht="18" thickBot="1">
@@ -6093,13 +6093,13 @@
       <c r="E30" s="20"/>
       <c r="F30" s="20"/>
       <c r="G30" s="58"/>
-      <c r="H30" s="86" t="s">
+      <c r="H30" s="88" t="s">
         <v>171</v>
       </c>
-      <c r="I30" s="87"/>
-      <c r="J30" s="87"/>
-      <c r="K30" s="87"/>
-      <c r="L30" s="88"/>
+      <c r="I30" s="89"/>
+      <c r="J30" s="89"/>
+      <c r="K30" s="89"/>
+      <c r="L30" s="90"/>
       <c r="M30" s="58"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1">
@@ -6254,13 +6254,13 @@
       <c r="E39" s="20"/>
       <c r="F39" s="62"/>
       <c r="G39" s="58"/>
-      <c r="H39" s="86" t="s">
+      <c r="H39" s="88" t="s">
         <v>172</v>
       </c>
-      <c r="I39" s="87"/>
-      <c r="J39" s="87"/>
-      <c r="K39" s="87"/>
-      <c r="L39" s="88"/>
+      <c r="I39" s="89"/>
+      <c r="J39" s="89"/>
+      <c r="K39" s="89"/>
+      <c r="L39" s="90"/>
       <c r="M39" s="58"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" thickBot="1">
@@ -6421,13 +6421,13 @@
         <v>3</v>
       </c>
       <c r="G48" s="58"/>
-      <c r="H48" s="86" t="s">
+      <c r="H48" s="88" t="s">
         <v>173</v>
       </c>
-      <c r="I48" s="87"/>
-      <c r="J48" s="87"/>
-      <c r="K48" s="87"/>
-      <c r="L48" s="88"/>
+      <c r="I48" s="89"/>
+      <c r="J48" s="89"/>
+      <c r="K48" s="89"/>
+      <c r="L48" s="90"/>
       <c r="M48" s="58"/>
     </row>
     <row r="49" spans="1:13" ht="15.75" thickBot="1">
@@ -6576,13 +6576,13 @@
       <c r="E57" s="39"/>
       <c r="F57" s="39"/>
       <c r="G57" s="58"/>
-      <c r="H57" s="86" t="s">
+      <c r="H57" s="88" t="s">
         <v>174</v>
       </c>
-      <c r="I57" s="87"/>
-      <c r="J57" s="87"/>
-      <c r="K57" s="87"/>
-      <c r="L57" s="88"/>
+      <c r="I57" s="89"/>
+      <c r="J57" s="89"/>
+      <c r="K57" s="89"/>
+      <c r="L57" s="90"/>
       <c r="M57" s="58"/>
     </row>
     <row r="58" spans="1:13" ht="15.75" thickBot="1">
@@ -6731,13 +6731,13 @@
       <c r="E66" s="20"/>
       <c r="F66" s="20"/>
       <c r="G66" s="58"/>
-      <c r="H66" s="86" t="s">
+      <c r="H66" s="88" t="s">
         <v>175</v>
       </c>
-      <c r="I66" s="87"/>
-      <c r="J66" s="87"/>
-      <c r="K66" s="87"/>
-      <c r="L66" s="88"/>
+      <c r="I66" s="89"/>
+      <c r="J66" s="89"/>
+      <c r="K66" s="89"/>
+      <c r="L66" s="90"/>
       <c r="M66" s="58"/>
     </row>
     <row r="67" spans="1:13" ht="15.75" thickBot="1">
@@ -9094,8 +9094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="E88" sqref="E88"/>
+    <sheetView tabSelected="1" topLeftCell="G2" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9114,40 +9114,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="23.25" customHeight="1">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="93" t="s">
         <v>286</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
-      <c r="J1" s="91"/>
-      <c r="K1" s="91"/>
-      <c r="L1" s="91"/>
-      <c r="M1" s="91"/>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
+      <c r="J1" s="93"/>
+      <c r="K1" s="93"/>
+      <c r="L1" s="93"/>
+      <c r="M1" s="93"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1">
-      <c r="A2" s="91"/>
-      <c r="B2" s="91"/>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="91"/>
-      <c r="L2" s="91"/>
-      <c r="M2" s="91"/>
+      <c r="A2" s="93"/>
+      <c r="B2" s="93"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
+      <c r="K2" s="93"/>
+      <c r="L2" s="93"/>
+      <c r="M2" s="93"/>
       <c r="N2" s="1"/>
       <c r="O2" s="69"/>
       <c r="P2" s="70" t="s">
@@ -9156,19 +9156,19 @@
       <c r="Q2" s="1"/>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1">
-      <c r="A3" s="91"/>
-      <c r="B3" s="91"/>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
+      <c r="A3" s="93"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -9248,7 +9248,7 @@
       <c r="I6" s="20"/>
       <c r="J6" s="80"/>
       <c r="K6" s="73"/>
-      <c r="L6" s="80"/>
+      <c r="L6" s="73"/>
       <c r="M6" s="58"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1">
@@ -9278,7 +9278,7 @@
       <c r="C8" s="20"/>
       <c r="D8" s="73"/>
       <c r="E8" s="73"/>
-      <c r="F8" s="80"/>
+      <c r="F8" s="73"/>
       <c r="G8" s="58"/>
       <c r="H8" s="19" t="s">
         <v>150</v>
@@ -9333,7 +9333,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="20"/>
-      <c r="D11" s="80"/>
+      <c r="D11" s="73"/>
       <c r="E11" s="73"/>
       <c r="F11" s="20"/>
       <c r="G11" s="58"/>
@@ -9373,7 +9373,7 @@
       <c r="C13" s="20"/>
       <c r="D13" s="20"/>
       <c r="E13" s="20"/>
-      <c r="F13" s="80"/>
+      <c r="F13" s="73"/>
       <c r="G13" s="58"/>
       <c r="H13" s="19" t="s">
         <v>155</v>
@@ -9455,7 +9455,7 @@
         <v>159</v>
       </c>
       <c r="I17" s="20"/>
-      <c r="J17" s="80"/>
+      <c r="J17" s="73"/>
       <c r="K17" s="20"/>
       <c r="L17" s="20"/>
       <c r="M17" s="58"/>
@@ -9514,7 +9514,7 @@
       <c r="I20" s="20"/>
       <c r="J20" s="73"/>
       <c r="K20" s="73"/>
-      <c r="L20" s="80"/>
+      <c r="L20" s="73"/>
       <c r="M20" s="58"/>
     </row>
     <row r="21" spans="1:13" ht="15.75" thickBot="1">
@@ -9544,7 +9544,7 @@
       <c r="C22" s="20"/>
       <c r="D22" s="73"/>
       <c r="E22" s="20"/>
-      <c r="F22" s="80"/>
+      <c r="F22" s="73"/>
       <c r="G22" s="58"/>
       <c r="H22" s="19" t="s">
         <v>164</v>
@@ -9624,7 +9624,7 @@
         <v>168</v>
       </c>
       <c r="I26" s="73"/>
-      <c r="J26" s="80"/>
+      <c r="J26" s="73"/>
       <c r="K26" s="20"/>
       <c r="L26" s="20"/>
       <c r="M26" s="58"/>
@@ -9653,7 +9653,7 @@
       <c r="I27" s="73"/>
       <c r="J27" s="20"/>
       <c r="K27" s="73"/>
-      <c r="L27" s="80"/>
+      <c r="L27" s="73"/>
       <c r="M27" s="58"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1">
@@ -9704,13 +9704,13 @@
       <c r="E30" s="73"/>
       <c r="F30" s="20"/>
       <c r="G30" s="58"/>
-      <c r="H30" s="86" t="s">
+      <c r="H30" s="88" t="s">
         <v>171</v>
       </c>
-      <c r="I30" s="87"/>
-      <c r="J30" s="87"/>
-      <c r="K30" s="87"/>
-      <c r="L30" s="88"/>
+      <c r="I30" s="89"/>
+      <c r="J30" s="89"/>
+      <c r="K30" s="89"/>
+      <c r="L30" s="90"/>
       <c r="M30" s="58"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1">
@@ -9867,13 +9867,13 @@
       <c r="E39" s="73"/>
       <c r="F39" s="62"/>
       <c r="G39" s="58"/>
-      <c r="H39" s="86" t="s">
+      <c r="H39" s="88" t="s">
         <v>172</v>
       </c>
-      <c r="I39" s="87"/>
-      <c r="J39" s="87"/>
-      <c r="K39" s="87"/>
-      <c r="L39" s="88"/>
+      <c r="I39" s="89"/>
+      <c r="J39" s="89"/>
+      <c r="K39" s="89"/>
+      <c r="L39" s="90"/>
       <c r="M39" s="58"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" thickBot="1">
@@ -10034,13 +10034,13 @@
         <v>3</v>
       </c>
       <c r="G48" s="58"/>
-      <c r="H48" s="86" t="s">
+      <c r="H48" s="88" t="s">
         <v>173</v>
       </c>
-      <c r="I48" s="87"/>
-      <c r="J48" s="87"/>
-      <c r="K48" s="87"/>
-      <c r="L48" s="88"/>
+      <c r="I48" s="89"/>
+      <c r="J48" s="89"/>
+      <c r="K48" s="89"/>
+      <c r="L48" s="90"/>
       <c r="M48" s="58"/>
     </row>
     <row r="49" spans="1:13" ht="15.75" thickBot="1">
@@ -10189,13 +10189,13 @@
       <c r="E57" s="81"/>
       <c r="F57" s="74"/>
       <c r="G57" s="58"/>
-      <c r="H57" s="86" t="s">
+      <c r="H57" s="88" t="s">
         <v>174</v>
       </c>
-      <c r="I57" s="87"/>
-      <c r="J57" s="87"/>
-      <c r="K57" s="87"/>
-      <c r="L57" s="88"/>
+      <c r="I57" s="89"/>
+      <c r="J57" s="89"/>
+      <c r="K57" s="89"/>
+      <c r="L57" s="90"/>
       <c r="M57" s="58"/>
     </row>
     <row r="58" spans="1:13" ht="15.75" thickBot="1">
@@ -10344,13 +10344,13 @@
       <c r="E66" s="80"/>
       <c r="F66" s="20"/>
       <c r="G66" s="58"/>
-      <c r="H66" s="86" t="s">
+      <c r="H66" s="88" t="s">
         <v>175</v>
       </c>
-      <c r="I66" s="87"/>
-      <c r="J66" s="87"/>
-      <c r="K66" s="87"/>
-      <c r="L66" s="88"/>
+      <c r="I66" s="89"/>
+      <c r="J66" s="89"/>
+      <c r="K66" s="89"/>
+      <c r="L66" s="90"/>
       <c r="M66" s="58"/>
     </row>
     <row r="67" spans="1:13" ht="15.75" thickBot="1">
@@ -10368,10 +10368,10 @@
       </c>
       <c r="I67" s="63"/>
       <c r="J67" s="63"/>
-      <c r="K67" s="92" t="s">
+      <c r="K67" s="94" t="s">
         <v>292</v>
       </c>
-      <c r="L67" s="93"/>
+      <c r="L67" s="95"/>
       <c r="M67" s="58"/>
     </row>
     <row r="68" spans="1:13" ht="15.75" thickBot="1">
@@ -10389,10 +10389,10 @@
       </c>
       <c r="I68" s="63"/>
       <c r="J68" s="63"/>
-      <c r="K68" s="92" t="s">
+      <c r="K68" s="94" t="s">
         <v>293</v>
       </c>
-      <c r="L68" s="93"/>
+      <c r="L68" s="95"/>
       <c r="M68" s="58"/>
     </row>
     <row r="69" spans="1:13" ht="15.75" thickBot="1">
@@ -10402,14 +10402,14 @@
       </c>
       <c r="C69" s="20"/>
       <c r="D69" s="73"/>
-      <c r="E69" s="80"/>
+      <c r="E69" s="73"/>
       <c r="F69" s="20"/>
       <c r="G69" s="58"/>
       <c r="H69" s="20"/>
       <c r="I69" s="20"/>
       <c r="J69" s="20"/>
-      <c r="K69" s="89"/>
-      <c r="L69" s="90"/>
+      <c r="K69" s="91"/>
+      <c r="L69" s="92"/>
       <c r="M69" s="58"/>
     </row>
     <row r="70" spans="1:13" ht="15.75" thickBot="1">
@@ -10425,8 +10425,8 @@
       <c r="H70" s="20"/>
       <c r="I70" s="20"/>
       <c r="J70" s="20"/>
-      <c r="K70" s="89"/>
-      <c r="L70" s="90"/>
+      <c r="K70" s="91"/>
+      <c r="L70" s="92"/>
       <c r="M70" s="58"/>
     </row>
     <row r="71" spans="1:13" ht="15.75" thickBot="1">
@@ -10442,8 +10442,8 @@
       <c r="H71" s="20"/>
       <c r="I71" s="20"/>
       <c r="J71" s="20"/>
-      <c r="K71" s="89"/>
-      <c r="L71" s="90"/>
+      <c r="K71" s="91"/>
+      <c r="L71" s="92"/>
       <c r="M71" s="58"/>
     </row>
     <row r="72" spans="1:13" ht="15.75" thickBot="1">
@@ -10459,8 +10459,8 @@
       <c r="H72" s="20"/>
       <c r="I72" s="20"/>
       <c r="J72" s="20"/>
-      <c r="K72" s="89"/>
-      <c r="L72" s="90"/>
+      <c r="K72" s="91"/>
+      <c r="L72" s="92"/>
       <c r="M72" s="58"/>
     </row>
     <row r="73" spans="1:13" ht="15.75" thickBot="1">
@@ -10550,7 +10550,7 @@
       <c r="B77" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="C77" s="94"/>
+      <c r="C77" s="84"/>
       <c r="D77" s="41"/>
       <c r="E77" s="39"/>
       <c r="F77" s="39"/>
@@ -10589,7 +10589,7 @@
         <v>73</v>
       </c>
       <c r="C79" s="20"/>
-      <c r="D79" s="80"/>
+      <c r="D79" s="73"/>
       <c r="E79" s="20"/>
       <c r="F79" s="20"/>
       <c r="G79" s="58"/>
@@ -10636,8 +10636,8 @@
       </c>
       <c r="I81" s="20"/>
       <c r="J81" s="20"/>
-      <c r="K81" s="80"/>
-      <c r="L81" s="80"/>
+      <c r="K81" s="73"/>
+      <c r="L81" s="73"/>
       <c r="M81" s="58"/>
     </row>
     <row r="82" spans="1:13" ht="15.75" thickBot="1">
@@ -10760,8 +10760,8 @@
         <v>82</v>
       </c>
       <c r="C88" s="73"/>
-      <c r="D88" s="95"/>
-      <c r="E88" s="80"/>
+      <c r="D88" s="85"/>
+      <c r="E88" s="73"/>
       <c r="F88" s="20"/>
       <c r="G88" s="58"/>
       <c r="H88" s="19" t="s">
@@ -10932,14 +10932,14 @@
       </c>
       <c r="C97" s="73"/>
       <c r="D97" s="80"/>
-      <c r="E97" s="80"/>
+      <c r="E97" s="73"/>
       <c r="F97" s="20"/>
       <c r="G97" s="58"/>
       <c r="H97" s="19" t="s">
         <v>199</v>
       </c>
       <c r="I97" s="20"/>
-      <c r="J97" s="80"/>
+      <c r="J97" s="73"/>
       <c r="K97" s="20"/>
       <c r="L97" s="20"/>
       <c r="M97" s="58"/>
@@ -10970,7 +10970,7 @@
       </c>
       <c r="C99" s="80"/>
       <c r="D99" s="80"/>
-      <c r="E99" s="80"/>
+      <c r="E99" s="73"/>
       <c r="F99" s="20"/>
       <c r="G99" s="58"/>
       <c r="H99" s="19" t="s">
@@ -11015,7 +11015,7 @@
         <v>202</v>
       </c>
       <c r="I101" s="20"/>
-      <c r="J101" s="80"/>
+      <c r="J101" s="73"/>
       <c r="K101" s="73"/>
       <c r="L101" s="80"/>
       <c r="M101" s="58"/>
@@ -11422,7 +11422,7 @@
         <v>114</v>
       </c>
       <c r="C122" s="20"/>
-      <c r="D122" s="80"/>
+      <c r="D122" s="73"/>
       <c r="E122" s="20"/>
       <c r="F122" s="20"/>
       <c r="G122" s="58"/>
@@ -11450,7 +11450,7 @@
       </c>
       <c r="I123" s="20"/>
       <c r="J123" s="20"/>
-      <c r="K123" s="80"/>
+      <c r="K123" s="73"/>
       <c r="L123" s="20"/>
       <c r="M123" s="58"/>
     </row>
@@ -11535,7 +11535,7 @@
       <c r="B128" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="C128" s="94"/>
+      <c r="C128" s="84"/>
       <c r="D128" s="82"/>
       <c r="E128" s="74"/>
       <c r="F128" s="39"/>
@@ -12040,7 +12040,7 @@
         <v>143</v>
       </c>
       <c r="C152" s="73"/>
-      <c r="D152" s="80"/>
+      <c r="D152" s="73"/>
       <c r="E152" s="20"/>
       <c r="F152" s="73"/>
       <c r="G152" s="4"/>
@@ -12100,7 +12100,7 @@
         <v>146</v>
       </c>
       <c r="C155" s="20"/>
-      <c r="D155" s="80"/>
+      <c r="D155" s="73"/>
       <c r="E155" s="20"/>
       <c r="F155" s="62"/>
       <c r="G155" s="4"/>

</xml_diff>

<commit_message>
updates and shit bro
</commit_message>
<xml_diff>
--- a/check list.xlsx
+++ b/check list.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="302">
   <si>
     <t>ARMOR</t>
   </si>
@@ -917,13 +917,19 @@
   </si>
   <si>
     <t>Clasped Orb</t>
+  </si>
+  <si>
+    <t>Hammerspace</t>
+  </si>
+  <si>
+    <t>Lammergeier</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1075,6 +1081,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF111111"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
       <color rgb="FF111111"/>
       <name val="Verdana"/>
       <family val="2"/>
@@ -1277,7 +1290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1509,12 +1522,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1552,6 +1559,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2390,13 +2409,13 @@
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
       <c r="G27" s="7"/>
-      <c r="H27" s="87" t="s">
+      <c r="H27" s="85" t="s">
         <v>171</v>
       </c>
-      <c r="I27" s="87"/>
-      <c r="J27" s="87"/>
-      <c r="K27" s="87"/>
-      <c r="L27" s="87"/>
+      <c r="I27" s="85"/>
+      <c r="J27" s="85"/>
+      <c r="K27" s="85"/>
+      <c r="L27" s="85"/>
       <c r="M27" s="7"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1">
@@ -2551,13 +2570,13 @@
       <c r="E36" s="20"/>
       <c r="F36" s="29"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="87" t="s">
+      <c r="H36" s="85" t="s">
         <v>172</v>
       </c>
-      <c r="I36" s="87"/>
-      <c r="J36" s="87"/>
-      <c r="K36" s="87"/>
-      <c r="L36" s="87"/>
+      <c r="I36" s="85"/>
+      <c r="J36" s="85"/>
+      <c r="K36" s="85"/>
+      <c r="L36" s="85"/>
       <c r="M36" s="7"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
@@ -2718,13 +2737,13 @@
         <v>3</v>
       </c>
       <c r="G45" s="7"/>
-      <c r="H45" s="87" t="s">
+      <c r="H45" s="85" t="s">
         <v>173</v>
       </c>
-      <c r="I45" s="87"/>
-      <c r="J45" s="87"/>
-      <c r="K45" s="87"/>
-      <c r="L45" s="87"/>
+      <c r="I45" s="85"/>
+      <c r="J45" s="85"/>
+      <c r="K45" s="85"/>
+      <c r="L45" s="85"/>
       <c r="M45" s="7"/>
     </row>
     <row r="46" spans="1:13" ht="15.75" thickBot="1">
@@ -2873,13 +2892,13 @@
       <c r="E54" s="39"/>
       <c r="F54" s="39"/>
       <c r="G54" s="7"/>
-      <c r="H54" s="87" t="s">
+      <c r="H54" s="85" t="s">
         <v>174</v>
       </c>
-      <c r="I54" s="87"/>
-      <c r="J54" s="87"/>
-      <c r="K54" s="87"/>
-      <c r="L54" s="87"/>
+      <c r="I54" s="85"/>
+      <c r="J54" s="85"/>
+      <c r="K54" s="85"/>
+      <c r="L54" s="85"/>
       <c r="M54" s="7"/>
     </row>
     <row r="55" spans="1:13" ht="15.75" thickBot="1">
@@ -3028,13 +3047,13 @@
       <c r="E63" s="20"/>
       <c r="F63" s="20"/>
       <c r="G63" s="7"/>
-      <c r="H63" s="87" t="s">
+      <c r="H63" s="85" t="s">
         <v>175</v>
       </c>
-      <c r="I63" s="87"/>
-      <c r="J63" s="87"/>
-      <c r="K63" s="87"/>
-      <c r="L63" s="87"/>
+      <c r="I63" s="85"/>
+      <c r="J63" s="85"/>
+      <c r="K63" s="85"/>
+      <c r="L63" s="85"/>
       <c r="M63" s="7"/>
     </row>
     <row r="64" spans="1:13" ht="15.75" thickBot="1">
@@ -4343,11 +4362,11 @@
       <c r="E132" s="20"/>
       <c r="F132" s="20"/>
       <c r="G132" s="7"/>
-      <c r="H132" s="86"/>
-      <c r="I132" s="86"/>
-      <c r="J132" s="86"/>
-      <c r="K132" s="86"/>
-      <c r="L132" s="86"/>
+      <c r="H132" s="84"/>
+      <c r="I132" s="84"/>
+      <c r="J132" s="84"/>
+      <c r="K132" s="84"/>
+      <c r="L132" s="84"/>
       <c r="M132" s="7"/>
     </row>
     <row r="133" spans="1:14" ht="18" thickBot="1">
@@ -6093,13 +6112,13 @@
       <c r="E30" s="20"/>
       <c r="F30" s="20"/>
       <c r="G30" s="58"/>
-      <c r="H30" s="88" t="s">
+      <c r="H30" s="86" t="s">
         <v>171</v>
       </c>
-      <c r="I30" s="89"/>
-      <c r="J30" s="89"/>
-      <c r="K30" s="89"/>
-      <c r="L30" s="90"/>
+      <c r="I30" s="87"/>
+      <c r="J30" s="87"/>
+      <c r="K30" s="87"/>
+      <c r="L30" s="88"/>
       <c r="M30" s="58"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1">
@@ -6254,13 +6273,13 @@
       <c r="E39" s="20"/>
       <c r="F39" s="62"/>
       <c r="G39" s="58"/>
-      <c r="H39" s="88" t="s">
+      <c r="H39" s="86" t="s">
         <v>172</v>
       </c>
-      <c r="I39" s="89"/>
-      <c r="J39" s="89"/>
-      <c r="K39" s="89"/>
-      <c r="L39" s="90"/>
+      <c r="I39" s="87"/>
+      <c r="J39" s="87"/>
+      <c r="K39" s="87"/>
+      <c r="L39" s="88"/>
       <c r="M39" s="58"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" thickBot="1">
@@ -6421,13 +6440,13 @@
         <v>3</v>
       </c>
       <c r="G48" s="58"/>
-      <c r="H48" s="88" t="s">
+      <c r="H48" s="86" t="s">
         <v>173</v>
       </c>
-      <c r="I48" s="89"/>
-      <c r="J48" s="89"/>
-      <c r="K48" s="89"/>
-      <c r="L48" s="90"/>
+      <c r="I48" s="87"/>
+      <c r="J48" s="87"/>
+      <c r="K48" s="87"/>
+      <c r="L48" s="88"/>
       <c r="M48" s="58"/>
     </row>
     <row r="49" spans="1:13" ht="15.75" thickBot="1">
@@ -6576,13 +6595,13 @@
       <c r="E57" s="39"/>
       <c r="F57" s="39"/>
       <c r="G57" s="58"/>
-      <c r="H57" s="88" t="s">
+      <c r="H57" s="86" t="s">
         <v>174</v>
       </c>
-      <c r="I57" s="89"/>
-      <c r="J57" s="89"/>
-      <c r="K57" s="89"/>
-      <c r="L57" s="90"/>
+      <c r="I57" s="87"/>
+      <c r="J57" s="87"/>
+      <c r="K57" s="87"/>
+      <c r="L57" s="88"/>
       <c r="M57" s="58"/>
     </row>
     <row r="58" spans="1:13" ht="15.75" thickBot="1">
@@ -6731,13 +6750,13 @@
       <c r="E66" s="20"/>
       <c r="F66" s="20"/>
       <c r="G66" s="58"/>
-      <c r="H66" s="88" t="s">
+      <c r="H66" s="86" t="s">
         <v>175</v>
       </c>
-      <c r="I66" s="89"/>
-      <c r="J66" s="89"/>
-      <c r="K66" s="89"/>
-      <c r="L66" s="90"/>
+      <c r="I66" s="87"/>
+      <c r="J66" s="87"/>
+      <c r="K66" s="87"/>
+      <c r="L66" s="88"/>
       <c r="M66" s="58"/>
     </row>
     <row r="67" spans="1:13" ht="15.75" thickBot="1">
@@ -9094,8 +9113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G2" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="B74" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9114,40 +9133,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="23.25" customHeight="1">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="91" t="s">
         <v>286</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="93"/>
-      <c r="I1" s="93"/>
-      <c r="J1" s="93"/>
-      <c r="K1" s="93"/>
-      <c r="L1" s="93"/>
-      <c r="M1" s="93"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="91"/>
+      <c r="L1" s="91"/>
+      <c r="M1" s="91"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1">
-      <c r="A2" s="93"/>
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="93"/>
-      <c r="I2" s="93"/>
-      <c r="J2" s="93"/>
-      <c r="K2" s="93"/>
-      <c r="L2" s="93"/>
-      <c r="M2" s="93"/>
+      <c r="A2" s="91"/>
+      <c r="B2" s="91"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="91"/>
+      <c r="M2" s="91"/>
       <c r="N2" s="1"/>
       <c r="O2" s="69"/>
       <c r="P2" s="70" t="s">
@@ -9156,19 +9175,19 @@
       <c r="Q2" s="1"/>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1">
-      <c r="A3" s="93"/>
-      <c r="B3" s="93"/>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
+      <c r="A3" s="91"/>
+      <c r="B3" s="91"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -9246,7 +9265,7 @@
         <v>148</v>
       </c>
       <c r="I6" s="20"/>
-      <c r="J6" s="80"/>
+      <c r="J6" s="73"/>
       <c r="K6" s="73"/>
       <c r="L6" s="73"/>
       <c r="M6" s="58"/>
@@ -9258,7 +9277,7 @@
       </c>
       <c r="C7" s="39"/>
       <c r="D7" s="74"/>
-      <c r="E7" s="81"/>
+      <c r="E7" s="74"/>
       <c r="F7" s="39"/>
       <c r="G7" s="58"/>
       <c r="H7" s="19" t="s">
@@ -9314,7 +9333,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="20"/>
-      <c r="D10" s="80"/>
+      <c r="D10" s="73"/>
       <c r="E10" s="73"/>
       <c r="F10" s="20"/>
       <c r="G10" s="58"/>
@@ -9323,7 +9342,7 @@
       </c>
       <c r="I10" s="20"/>
       <c r="J10" s="20"/>
-      <c r="K10" s="80"/>
+      <c r="K10" s="73"/>
       <c r="L10" s="20"/>
       <c r="M10" s="58"/>
     </row>
@@ -9352,7 +9371,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="20"/>
-      <c r="D12" s="80"/>
+      <c r="D12" s="73"/>
       <c r="E12" s="73"/>
       <c r="F12" s="20"/>
       <c r="G12" s="58"/>
@@ -9361,7 +9380,7 @@
       </c>
       <c r="I12" s="20"/>
       <c r="J12" s="73"/>
-      <c r="K12" s="80"/>
+      <c r="K12" s="73"/>
       <c r="L12" s="20"/>
       <c r="M12" s="58"/>
     </row>
@@ -9410,14 +9429,14 @@
       </c>
       <c r="C15" s="73"/>
       <c r="D15" s="20"/>
-      <c r="E15" s="80"/>
+      <c r="E15" s="73"/>
       <c r="F15" s="20"/>
       <c r="G15" s="58"/>
       <c r="H15" s="19" t="s">
         <v>157</v>
       </c>
       <c r="I15" s="20"/>
-      <c r="J15" s="80"/>
+      <c r="J15" s="73"/>
       <c r="K15" s="73"/>
       <c r="L15" s="20"/>
       <c r="M15" s="58"/>
@@ -9704,13 +9723,13 @@
       <c r="E30" s="73"/>
       <c r="F30" s="20"/>
       <c r="G30" s="58"/>
-      <c r="H30" s="88" t="s">
+      <c r="H30" s="86" t="s">
         <v>171</v>
       </c>
-      <c r="I30" s="89"/>
-      <c r="J30" s="89"/>
-      <c r="K30" s="89"/>
-      <c r="L30" s="90"/>
+      <c r="I30" s="87"/>
+      <c r="J30" s="87"/>
+      <c r="K30" s="87"/>
+      <c r="L30" s="88"/>
       <c r="M30" s="58"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1">
@@ -9867,13 +9886,13 @@
       <c r="E39" s="73"/>
       <c r="F39" s="62"/>
       <c r="G39" s="58"/>
-      <c r="H39" s="88" t="s">
+      <c r="H39" s="86" t="s">
         <v>172</v>
       </c>
-      <c r="I39" s="89"/>
-      <c r="J39" s="89"/>
-      <c r="K39" s="89"/>
-      <c r="L39" s="90"/>
+      <c r="I39" s="87"/>
+      <c r="J39" s="87"/>
+      <c r="K39" s="87"/>
+      <c r="L39" s="88"/>
       <c r="M39" s="58"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" thickBot="1">
@@ -9939,7 +9958,7 @@
         <v>38</v>
       </c>
       <c r="C43" s="20"/>
-      <c r="D43" s="80"/>
+      <c r="D43" s="73"/>
       <c r="E43" s="20"/>
       <c r="F43" s="20"/>
       <c r="G43" s="58"/>
@@ -10034,13 +10053,13 @@
         <v>3</v>
       </c>
       <c r="G48" s="58"/>
-      <c r="H48" s="88" t="s">
+      <c r="H48" s="86" t="s">
         <v>173</v>
       </c>
-      <c r="I48" s="89"/>
-      <c r="J48" s="89"/>
-      <c r="K48" s="89"/>
-      <c r="L48" s="90"/>
+      <c r="I48" s="87"/>
+      <c r="J48" s="87"/>
+      <c r="K48" s="87"/>
+      <c r="L48" s="88"/>
       <c r="M48" s="58"/>
     </row>
     <row r="49" spans="1:13" ht="15.75" thickBot="1">
@@ -10082,7 +10101,7 @@
       <c r="B51" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C51" s="20"/>
+      <c r="C51" s="80"/>
       <c r="D51" s="73"/>
       <c r="E51" s="20"/>
       <c r="F51" s="20"/>
@@ -10117,7 +10136,7 @@
         <v>47</v>
       </c>
       <c r="C53" s="73"/>
-      <c r="D53" s="80"/>
+      <c r="D53" s="73"/>
       <c r="E53" s="20"/>
       <c r="F53" s="20"/>
       <c r="G53" s="58"/>
@@ -10168,7 +10187,7 @@
         <v>50</v>
       </c>
       <c r="C56" s="20"/>
-      <c r="D56" s="80"/>
+      <c r="D56" s="73"/>
       <c r="E56" s="20"/>
       <c r="F56" s="20"/>
       <c r="G56" s="58"/>
@@ -10186,16 +10205,16 @@
       </c>
       <c r="C57" s="39"/>
       <c r="D57" s="74"/>
-      <c r="E57" s="81"/>
+      <c r="E57" s="74"/>
       <c r="F57" s="74"/>
       <c r="G57" s="58"/>
-      <c r="H57" s="88" t="s">
+      <c r="H57" s="86" t="s">
         <v>174</v>
       </c>
-      <c r="I57" s="89"/>
-      <c r="J57" s="89"/>
-      <c r="K57" s="89"/>
-      <c r="L57" s="90"/>
+      <c r="I57" s="87"/>
+      <c r="J57" s="87"/>
+      <c r="K57" s="87"/>
+      <c r="L57" s="88"/>
       <c r="M57" s="58"/>
     </row>
     <row r="58" spans="1:13" ht="15.75" thickBot="1">
@@ -10341,16 +10360,16 @@
       </c>
       <c r="C66" s="73"/>
       <c r="D66" s="80"/>
-      <c r="E66" s="80"/>
+      <c r="E66" s="73"/>
       <c r="F66" s="20"/>
       <c r="G66" s="58"/>
-      <c r="H66" s="88" t="s">
+      <c r="H66" s="86" t="s">
         <v>175</v>
       </c>
-      <c r="I66" s="89"/>
-      <c r="J66" s="89"/>
-      <c r="K66" s="89"/>
-      <c r="L66" s="90"/>
+      <c r="I66" s="87"/>
+      <c r="J66" s="87"/>
+      <c r="K66" s="87"/>
+      <c r="L66" s="88"/>
       <c r="M66" s="58"/>
     </row>
     <row r="67" spans="1:13" ht="15.75" thickBot="1">
@@ -10360,7 +10379,7 @@
       </c>
       <c r="C67" s="20"/>
       <c r="D67" s="73"/>
-      <c r="E67" s="80"/>
+      <c r="E67" s="73"/>
       <c r="F67" s="73"/>
       <c r="G67" s="58"/>
       <c r="H67" s="77" t="s">
@@ -10368,10 +10387,10 @@
       </c>
       <c r="I67" s="63"/>
       <c r="J67" s="63"/>
-      <c r="K67" s="94" t="s">
+      <c r="K67" s="92" t="s">
         <v>292</v>
       </c>
-      <c r="L67" s="95"/>
+      <c r="L67" s="93"/>
       <c r="M67" s="58"/>
     </row>
     <row r="68" spans="1:13" ht="15.75" thickBot="1">
@@ -10389,10 +10408,10 @@
       </c>
       <c r="I68" s="63"/>
       <c r="J68" s="63"/>
-      <c r="K68" s="94" t="s">
+      <c r="K68" s="92" t="s">
         <v>293</v>
       </c>
-      <c r="L68" s="95"/>
+      <c r="L68" s="93"/>
       <c r="M68" s="58"/>
     </row>
     <row r="69" spans="1:13" ht="15.75" thickBot="1">
@@ -10408,8 +10427,10 @@
       <c r="H69" s="20"/>
       <c r="I69" s="20"/>
       <c r="J69" s="20"/>
-      <c r="K69" s="91"/>
-      <c r="L69" s="92"/>
+      <c r="K69" s="94" t="s">
+        <v>300</v>
+      </c>
+      <c r="L69" s="95"/>
       <c r="M69" s="58"/>
     </row>
     <row r="70" spans="1:13" ht="15.75" thickBot="1">
@@ -10425,8 +10446,10 @@
       <c r="H70" s="20"/>
       <c r="I70" s="20"/>
       <c r="J70" s="20"/>
-      <c r="K70" s="91"/>
-      <c r="L70" s="92"/>
+      <c r="K70" s="94" t="s">
+        <v>301</v>
+      </c>
+      <c r="L70" s="95"/>
       <c r="M70" s="58"/>
     </row>
     <row r="71" spans="1:13" ht="15.75" thickBot="1">
@@ -10435,15 +10458,15 @@
         <v>65</v>
       </c>
       <c r="C71" s="20"/>
-      <c r="D71" s="80"/>
+      <c r="D71" s="73"/>
       <c r="E71" s="73"/>
       <c r="F71" s="73"/>
       <c r="G71" s="58"/>
       <c r="H71" s="20"/>
       <c r="I71" s="20"/>
       <c r="J71" s="20"/>
-      <c r="K71" s="91"/>
-      <c r="L71" s="92"/>
+      <c r="K71" s="89"/>
+      <c r="L71" s="90"/>
       <c r="M71" s="58"/>
     </row>
     <row r="72" spans="1:13" ht="15.75" thickBot="1">
@@ -10459,8 +10482,8 @@
       <c r="H72" s="20"/>
       <c r="I72" s="20"/>
       <c r="J72" s="20"/>
-      <c r="K72" s="91"/>
-      <c r="L72" s="92"/>
+      <c r="K72" s="89"/>
+      <c r="L72" s="90"/>
       <c r="M72" s="58"/>
     </row>
     <row r="73" spans="1:13" ht="15.75" thickBot="1">
@@ -10532,7 +10555,7 @@
         <v>70</v>
       </c>
       <c r="C76" s="20"/>
-      <c r="D76" s="80"/>
+      <c r="D76" s="73"/>
       <c r="E76" s="20"/>
       <c r="F76" s="20"/>
       <c r="G76" s="58"/>
@@ -10541,7 +10564,7 @@
       </c>
       <c r="I76" s="20"/>
       <c r="J76" s="20"/>
-      <c r="K76" s="80"/>
+      <c r="K76" s="73"/>
       <c r="L76" s="20"/>
       <c r="M76" s="58"/>
     </row>
@@ -10550,7 +10573,7 @@
       <c r="B77" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="C77" s="84"/>
+      <c r="C77" s="82"/>
       <c r="D77" s="41"/>
       <c r="E77" s="39"/>
       <c r="F77" s="39"/>
@@ -10578,7 +10601,7 @@
         <v>180</v>
       </c>
       <c r="I78" s="20"/>
-      <c r="J78" s="80"/>
+      <c r="J78" s="73"/>
       <c r="K78" s="20"/>
       <c r="L78" s="20"/>
       <c r="M78" s="58"/>
@@ -10645,7 +10668,7 @@
       <c r="B82" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="C82" s="20"/>
+      <c r="C82" s="80"/>
       <c r="D82" s="20"/>
       <c r="E82" s="20"/>
       <c r="F82" s="20"/>
@@ -10760,7 +10783,7 @@
         <v>82</v>
       </c>
       <c r="C88" s="73"/>
-      <c r="D88" s="85"/>
+      <c r="D88" s="83"/>
       <c r="E88" s="73"/>
       <c r="F88" s="20"/>
       <c r="G88" s="58"/>
@@ -10799,7 +10822,7 @@
       </c>
       <c r="C90" s="39"/>
       <c r="D90" s="74"/>
-      <c r="E90" s="81"/>
+      <c r="E90" s="74"/>
       <c r="F90" s="41"/>
       <c r="G90" s="58"/>
       <c r="H90" s="19" t="s">
@@ -10873,7 +10896,7 @@
       <c r="B94" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="C94" s="20"/>
+      <c r="C94" s="80"/>
       <c r="D94" s="73"/>
       <c r="E94" s="20"/>
       <c r="F94" s="20"/>
@@ -10931,7 +10954,7 @@
         <v>295</v>
       </c>
       <c r="C97" s="73"/>
-      <c r="D97" s="80"/>
+      <c r="D97" s="73"/>
       <c r="E97" s="73"/>
       <c r="F97" s="20"/>
       <c r="G97" s="58"/>
@@ -11017,7 +11040,7 @@
       <c r="I101" s="20"/>
       <c r="J101" s="73"/>
       <c r="K101" s="73"/>
-      <c r="L101" s="80"/>
+      <c r="L101" s="73"/>
       <c r="M101" s="58"/>
     </row>
     <row r="102" spans="1:13" ht="15.75" thickBot="1">
@@ -11028,7 +11051,7 @@
       <c r="C102" s="20"/>
       <c r="D102" s="73"/>
       <c r="E102" s="73"/>
-      <c r="F102" s="80"/>
+      <c r="F102" s="73"/>
       <c r="G102" s="58"/>
       <c r="H102" s="19" t="s">
         <v>203</v>
@@ -11045,7 +11068,7 @@
         <v>96</v>
       </c>
       <c r="C103" s="20"/>
-      <c r="D103" s="80"/>
+      <c r="D103" s="73"/>
       <c r="E103" s="20"/>
       <c r="F103" s="62"/>
       <c r="G103" s="58"/>
@@ -11123,7 +11146,7 @@
       </c>
       <c r="I106" s="20"/>
       <c r="J106" s="73"/>
-      <c r="K106" s="80"/>
+      <c r="K106" s="73"/>
       <c r="L106" s="20"/>
       <c r="M106" s="58"/>
     </row>
@@ -11152,7 +11175,7 @@
         <v>100</v>
       </c>
       <c r="C108" s="20"/>
-      <c r="D108" s="80"/>
+      <c r="D108" s="73"/>
       <c r="E108" s="20"/>
       <c r="F108" s="20"/>
       <c r="G108" s="58"/>
@@ -11198,7 +11221,7 @@
         <v>209</v>
       </c>
       <c r="I110" s="20"/>
-      <c r="J110" s="80"/>
+      <c r="J110" s="96"/>
       <c r="K110" s="20"/>
       <c r="L110" s="20"/>
       <c r="M110" s="58"/>
@@ -11304,7 +11327,7 @@
         <v>108</v>
       </c>
       <c r="C116" s="20"/>
-      <c r="D116" s="80"/>
+      <c r="D116" s="73"/>
       <c r="E116" s="20"/>
       <c r="F116" s="20"/>
       <c r="G116" s="58"/>
@@ -11481,7 +11504,7 @@
       <c r="C125" s="20"/>
       <c r="D125" s="73"/>
       <c r="E125" s="73"/>
-      <c r="F125" s="80"/>
+      <c r="F125" s="73"/>
       <c r="G125" s="58"/>
       <c r="H125" s="19" t="s">
         <v>297</v>
@@ -11535,8 +11558,8 @@
       <c r="B128" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="C128" s="84"/>
-      <c r="D128" s="82"/>
+      <c r="C128" s="82"/>
+      <c r="D128" s="97"/>
       <c r="E128" s="74"/>
       <c r="F128" s="39"/>
       <c r="G128" s="58"/>
@@ -11620,7 +11643,7 @@
         <v>230</v>
       </c>
       <c r="I132" s="20"/>
-      <c r="J132" s="80"/>
+      <c r="J132" s="73"/>
       <c r="K132" s="20"/>
       <c r="L132" s="20"/>
       <c r="M132" s="58"/>
@@ -11798,7 +11821,7 @@
         <v>133</v>
       </c>
       <c r="C141" s="20"/>
-      <c r="D141" s="80"/>
+      <c r="D141" s="73"/>
       <c r="E141" s="20"/>
       <c r="F141" s="73"/>
       <c r="G141" s="4"/>
@@ -11970,7 +11993,7 @@
         <v>140</v>
       </c>
       <c r="C149" s="73"/>
-      <c r="D149" s="80"/>
+      <c r="D149" s="73"/>
       <c r="E149" s="20"/>
       <c r="F149" s="20"/>
       <c r="G149" s="4"/>
@@ -12141,7 +12164,7 @@
       <c r="N156" s="4"/>
     </row>
     <row r="157" spans="1:14" ht="27" thickBot="1">
-      <c r="A157" s="83" t="s">
+      <c r="A157" s="81" t="s">
         <v>269</v>
       </c>
       <c r="B157" s="45" t="s">

</xml_diff>

<commit_message>
another update walking by, nothing to see
</commit_message>
<xml_diff>
--- a/check list.xlsx
+++ b/check list.xlsx
@@ -1290,7 +1290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1507,9 +1507,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1529,6 +1526,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1565,12 +1577,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2409,13 +2415,13 @@
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
       <c r="G27" s="7"/>
-      <c r="H27" s="85" t="s">
+      <c r="H27" s="89" t="s">
         <v>171</v>
       </c>
-      <c r="I27" s="85"/>
-      <c r="J27" s="85"/>
-      <c r="K27" s="85"/>
-      <c r="L27" s="85"/>
+      <c r="I27" s="89"/>
+      <c r="J27" s="89"/>
+      <c r="K27" s="89"/>
+      <c r="L27" s="89"/>
       <c r="M27" s="7"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1">
@@ -2570,13 +2576,13 @@
       <c r="E36" s="20"/>
       <c r="F36" s="29"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="85" t="s">
+      <c r="H36" s="89" t="s">
         <v>172</v>
       </c>
-      <c r="I36" s="85"/>
-      <c r="J36" s="85"/>
-      <c r="K36" s="85"/>
-      <c r="L36" s="85"/>
+      <c r="I36" s="89"/>
+      <c r="J36" s="89"/>
+      <c r="K36" s="89"/>
+      <c r="L36" s="89"/>
       <c r="M36" s="7"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
@@ -2737,13 +2743,13 @@
         <v>3</v>
       </c>
       <c r="G45" s="7"/>
-      <c r="H45" s="85" t="s">
+      <c r="H45" s="89" t="s">
         <v>173</v>
       </c>
-      <c r="I45" s="85"/>
-      <c r="J45" s="85"/>
-      <c r="K45" s="85"/>
-      <c r="L45" s="85"/>
+      <c r="I45" s="89"/>
+      <c r="J45" s="89"/>
+      <c r="K45" s="89"/>
+      <c r="L45" s="89"/>
       <c r="M45" s="7"/>
     </row>
     <row r="46" spans="1:13" ht="15.75" thickBot="1">
@@ -2892,13 +2898,13 @@
       <c r="E54" s="39"/>
       <c r="F54" s="39"/>
       <c r="G54" s="7"/>
-      <c r="H54" s="85" t="s">
+      <c r="H54" s="89" t="s">
         <v>174</v>
       </c>
-      <c r="I54" s="85"/>
-      <c r="J54" s="85"/>
-      <c r="K54" s="85"/>
-      <c r="L54" s="85"/>
+      <c r="I54" s="89"/>
+      <c r="J54" s="89"/>
+      <c r="K54" s="89"/>
+      <c r="L54" s="89"/>
       <c r="M54" s="7"/>
     </row>
     <row r="55" spans="1:13" ht="15.75" thickBot="1">
@@ -3047,13 +3053,13 @@
       <c r="E63" s="20"/>
       <c r="F63" s="20"/>
       <c r="G63" s="7"/>
-      <c r="H63" s="85" t="s">
+      <c r="H63" s="89" t="s">
         <v>175</v>
       </c>
-      <c r="I63" s="85"/>
-      <c r="J63" s="85"/>
-      <c r="K63" s="85"/>
-      <c r="L63" s="85"/>
+      <c r="I63" s="89"/>
+      <c r="J63" s="89"/>
+      <c r="K63" s="89"/>
+      <c r="L63" s="89"/>
       <c r="M63" s="7"/>
     </row>
     <row r="64" spans="1:13" ht="15.75" thickBot="1">
@@ -4362,11 +4368,11 @@
       <c r="E132" s="20"/>
       <c r="F132" s="20"/>
       <c r="G132" s="7"/>
-      <c r="H132" s="84"/>
-      <c r="I132" s="84"/>
-      <c r="J132" s="84"/>
-      <c r="K132" s="84"/>
-      <c r="L132" s="84"/>
+      <c r="H132" s="88"/>
+      <c r="I132" s="88"/>
+      <c r="J132" s="88"/>
+      <c r="K132" s="88"/>
+      <c r="L132" s="88"/>
       <c r="M132" s="7"/>
     </row>
     <row r="133" spans="1:14" ht="18" thickBot="1">
@@ -6112,13 +6118,13 @@
       <c r="E30" s="20"/>
       <c r="F30" s="20"/>
       <c r="G30" s="58"/>
-      <c r="H30" s="86" t="s">
+      <c r="H30" s="90" t="s">
         <v>171</v>
       </c>
-      <c r="I30" s="87"/>
-      <c r="J30" s="87"/>
-      <c r="K30" s="87"/>
-      <c r="L30" s="88"/>
+      <c r="I30" s="91"/>
+      <c r="J30" s="91"/>
+      <c r="K30" s="91"/>
+      <c r="L30" s="92"/>
       <c r="M30" s="58"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1">
@@ -6273,13 +6279,13 @@
       <c r="E39" s="20"/>
       <c r="F39" s="62"/>
       <c r="G39" s="58"/>
-      <c r="H39" s="86" t="s">
+      <c r="H39" s="90" t="s">
         <v>172</v>
       </c>
-      <c r="I39" s="87"/>
-      <c r="J39" s="87"/>
-      <c r="K39" s="87"/>
-      <c r="L39" s="88"/>
+      <c r="I39" s="91"/>
+      <c r="J39" s="91"/>
+      <c r="K39" s="91"/>
+      <c r="L39" s="92"/>
       <c r="M39" s="58"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" thickBot="1">
@@ -6440,13 +6446,13 @@
         <v>3</v>
       </c>
       <c r="G48" s="58"/>
-      <c r="H48" s="86" t="s">
+      <c r="H48" s="90" t="s">
         <v>173</v>
       </c>
-      <c r="I48" s="87"/>
-      <c r="J48" s="87"/>
-      <c r="K48" s="87"/>
-      <c r="L48" s="88"/>
+      <c r="I48" s="91"/>
+      <c r="J48" s="91"/>
+      <c r="K48" s="91"/>
+      <c r="L48" s="92"/>
       <c r="M48" s="58"/>
     </row>
     <row r="49" spans="1:13" ht="15.75" thickBot="1">
@@ -6595,13 +6601,13 @@
       <c r="E57" s="39"/>
       <c r="F57" s="39"/>
       <c r="G57" s="58"/>
-      <c r="H57" s="86" t="s">
+      <c r="H57" s="90" t="s">
         <v>174</v>
       </c>
-      <c r="I57" s="87"/>
-      <c r="J57" s="87"/>
-      <c r="K57" s="87"/>
-      <c r="L57" s="88"/>
+      <c r="I57" s="91"/>
+      <c r="J57" s="91"/>
+      <c r="K57" s="91"/>
+      <c r="L57" s="92"/>
       <c r="M57" s="58"/>
     </row>
     <row r="58" spans="1:13" ht="15.75" thickBot="1">
@@ -6750,13 +6756,13 @@
       <c r="E66" s="20"/>
       <c r="F66" s="20"/>
       <c r="G66" s="58"/>
-      <c r="H66" s="86" t="s">
+      <c r="H66" s="90" t="s">
         <v>175</v>
       </c>
-      <c r="I66" s="87"/>
-      <c r="J66" s="87"/>
-      <c r="K66" s="87"/>
-      <c r="L66" s="88"/>
+      <c r="I66" s="91"/>
+      <c r="J66" s="91"/>
+      <c r="K66" s="91"/>
+      <c r="L66" s="92"/>
       <c r="M66" s="58"/>
     </row>
     <row r="67" spans="1:13" ht="15.75" thickBot="1">
@@ -9113,8 +9119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B74" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView tabSelected="1" topLeftCell="B110" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D121" sqref="D121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9133,40 +9139,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="23.25" customHeight="1">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="95" t="s">
         <v>286</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
-      <c r="J1" s="91"/>
-      <c r="K1" s="91"/>
-      <c r="L1" s="91"/>
-      <c r="M1" s="91"/>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="95"/>
+      <c r="J1" s="95"/>
+      <c r="K1" s="95"/>
+      <c r="L1" s="95"/>
+      <c r="M1" s="95"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1">
-      <c r="A2" s="91"/>
-      <c r="B2" s="91"/>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="91"/>
-      <c r="L2" s="91"/>
-      <c r="M2" s="91"/>
+      <c r="A2" s="95"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
       <c r="N2" s="1"/>
       <c r="O2" s="69"/>
       <c r="P2" s="70" t="s">
@@ -9175,19 +9181,19 @@
       <c r="Q2" s="1"/>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1">
-      <c r="A3" s="91"/>
-      <c r="B3" s="91"/>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
+      <c r="A3" s="95"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="95"/>
+      <c r="L3" s="95"/>
+      <c r="M3" s="95"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -9259,12 +9265,12 @@
       </c>
       <c r="D6" s="72"/>
       <c r="E6" s="73"/>
-      <c r="F6" s="20"/>
+      <c r="F6" s="79"/>
       <c r="G6" s="58"/>
       <c r="H6" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="I6" s="20"/>
+      <c r="I6" s="79"/>
       <c r="J6" s="73"/>
       <c r="K6" s="73"/>
       <c r="L6" s="73"/>
@@ -9332,7 +9338,7 @@
       <c r="B10" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="20"/>
+      <c r="C10" s="79"/>
       <c r="D10" s="73"/>
       <c r="E10" s="73"/>
       <c r="F10" s="20"/>
@@ -9408,7 +9414,7 @@
       <c r="B14" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="20"/>
+      <c r="C14" s="79"/>
       <c r="D14" s="73"/>
       <c r="E14" s="20"/>
       <c r="F14" s="20"/>
@@ -9446,7 +9452,7 @@
       <c r="B16" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="20"/>
+      <c r="C16" s="79"/>
       <c r="D16" s="20"/>
       <c r="E16" s="73"/>
       <c r="F16" s="20"/>
@@ -9492,7 +9498,7 @@
       <c r="H18" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="I18" s="80"/>
+      <c r="I18" s="79"/>
       <c r="J18" s="73"/>
       <c r="K18" s="20"/>
       <c r="L18" s="20"/>
@@ -9549,8 +9555,8 @@
       <c r="H21" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="I21" s="80"/>
-      <c r="J21" s="80"/>
+      <c r="I21" s="79"/>
+      <c r="J21" s="73"/>
       <c r="K21" s="20"/>
       <c r="L21" s="20"/>
       <c r="M21" s="58"/>
@@ -9579,7 +9585,7 @@
       <c r="B23" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="20"/>
+      <c r="C23" s="79"/>
       <c r="D23" s="73"/>
       <c r="E23" s="20"/>
       <c r="F23" s="20"/>
@@ -9612,12 +9618,12 @@
       <c r="L24" s="20"/>
       <c r="M24" s="58"/>
     </row>
-    <row r="25" spans="1:13" ht="19.5" customHeight="1" thickBot="1">
+    <row r="25" spans="1:13" ht="26.25" thickBot="1">
       <c r="A25" s="58"/>
       <c r="B25" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="20"/>
+      <c r="C25" s="79"/>
       <c r="D25" s="20"/>
       <c r="E25" s="20"/>
       <c r="F25" s="20"/>
@@ -9683,7 +9689,7 @@
       <c r="C28" s="73"/>
       <c r="D28" s="73"/>
       <c r="E28" s="73"/>
-      <c r="F28" s="80"/>
+      <c r="F28" s="73"/>
       <c r="G28" s="58"/>
       <c r="H28" s="19" t="s">
         <v>170</v>
@@ -9701,7 +9707,7 @@
       </c>
       <c r="C29" s="20"/>
       <c r="D29" s="20"/>
-      <c r="E29" s="80"/>
+      <c r="E29" s="73"/>
       <c r="F29" s="20"/>
       <c r="G29" s="58"/>
       <c r="H29" s="58"/>
@@ -9716,20 +9722,20 @@
       <c r="B30" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="75" t="s">
+      <c r="C30" s="86" t="s">
         <v>288</v>
       </c>
       <c r="D30" s="20"/>
       <c r="E30" s="73"/>
       <c r="F30" s="20"/>
       <c r="G30" s="58"/>
-      <c r="H30" s="86" t="s">
+      <c r="H30" s="90" t="s">
         <v>171</v>
       </c>
-      <c r="I30" s="87"/>
-      <c r="J30" s="87"/>
-      <c r="K30" s="87"/>
-      <c r="L30" s="88"/>
+      <c r="I30" s="91"/>
+      <c r="J30" s="91"/>
+      <c r="K30" s="91"/>
+      <c r="L30" s="92"/>
       <c r="M30" s="58"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1">
@@ -9742,7 +9748,7 @@
       <c r="E31" s="20"/>
       <c r="F31" s="20"/>
       <c r="G31" s="58"/>
-      <c r="H31" s="77" t="s">
+      <c r="H31" s="76" t="s">
         <v>296</v>
       </c>
       <c r="I31" s="63"/>
@@ -9756,7 +9762,7 @@
       <c r="B32" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="20"/>
+      <c r="C32" s="79"/>
       <c r="D32" s="20"/>
       <c r="E32" s="73"/>
       <c r="F32" s="20"/>
@@ -9886,13 +9892,13 @@
       <c r="E39" s="73"/>
       <c r="F39" s="62"/>
       <c r="G39" s="58"/>
-      <c r="H39" s="86" t="s">
+      <c r="H39" s="90" t="s">
         <v>172</v>
       </c>
-      <c r="I39" s="87"/>
-      <c r="J39" s="87"/>
-      <c r="K39" s="87"/>
-      <c r="L39" s="88"/>
+      <c r="I39" s="91"/>
+      <c r="J39" s="91"/>
+      <c r="K39" s="91"/>
+      <c r="L39" s="92"/>
       <c r="M39" s="58"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" thickBot="1">
@@ -9974,7 +9980,7 @@
       <c r="B44" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="C44" s="20"/>
+      <c r="C44" s="79"/>
       <c r="D44" s="20"/>
       <c r="E44" s="20"/>
       <c r="F44" s="20"/>
@@ -10009,7 +10015,7 @@
         <v>41</v>
       </c>
       <c r="C46" s="73"/>
-      <c r="D46" s="20"/>
+      <c r="D46" s="79"/>
       <c r="E46" s="20"/>
       <c r="F46" s="62"/>
       <c r="G46" s="58"/>
@@ -10053,13 +10059,13 @@
         <v>3</v>
       </c>
       <c r="G48" s="58"/>
-      <c r="H48" s="86" t="s">
+      <c r="H48" s="90" t="s">
         <v>173</v>
       </c>
-      <c r="I48" s="87"/>
-      <c r="J48" s="87"/>
-      <c r="K48" s="87"/>
-      <c r="L48" s="88"/>
+      <c r="I48" s="91"/>
+      <c r="J48" s="91"/>
+      <c r="K48" s="91"/>
+      <c r="L48" s="92"/>
       <c r="M48" s="58"/>
     </row>
     <row r="49" spans="1:13" ht="15.75" thickBot="1">
@@ -10070,7 +10076,7 @@
       <c r="C49" s="73"/>
       <c r="D49" s="73"/>
       <c r="E49" s="20"/>
-      <c r="F49" s="80"/>
+      <c r="F49" s="73"/>
       <c r="G49" s="58"/>
       <c r="H49" s="63"/>
       <c r="I49" s="63"/>
@@ -10101,7 +10107,7 @@
       <c r="B51" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C51" s="80"/>
+      <c r="C51" s="79"/>
       <c r="D51" s="73"/>
       <c r="E51" s="20"/>
       <c r="F51" s="20"/>
@@ -10118,10 +10124,10 @@
       <c r="B52" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="C52" s="20"/>
+      <c r="C52" s="79"/>
       <c r="D52" s="73"/>
       <c r="E52" s="73"/>
-      <c r="F52" s="80"/>
+      <c r="F52" s="73"/>
       <c r="G52" s="58"/>
       <c r="H52" s="20"/>
       <c r="I52" s="20"/>
@@ -10152,7 +10158,7 @@
       <c r="B54" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C54" s="20"/>
+      <c r="C54" s="79"/>
       <c r="D54" s="73"/>
       <c r="E54" s="73"/>
       <c r="F54" s="20"/>
@@ -10203,18 +10209,18 @@
       <c r="B57" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="C57" s="39"/>
+      <c r="C57" s="85"/>
       <c r="D57" s="74"/>
       <c r="E57" s="74"/>
       <c r="F57" s="74"/>
       <c r="G57" s="58"/>
-      <c r="H57" s="86" t="s">
+      <c r="H57" s="90" t="s">
         <v>174</v>
       </c>
-      <c r="I57" s="87"/>
-      <c r="J57" s="87"/>
-      <c r="K57" s="87"/>
-      <c r="L57" s="88"/>
+      <c r="I57" s="91"/>
+      <c r="J57" s="91"/>
+      <c r="K57" s="91"/>
+      <c r="L57" s="92"/>
       <c r="M57" s="58"/>
     </row>
     <row r="58" spans="1:13" ht="15.75" thickBot="1">
@@ -10256,7 +10262,7 @@
       <c r="B60" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C60" s="80"/>
+      <c r="C60" s="79"/>
       <c r="D60" s="20"/>
       <c r="E60" s="20"/>
       <c r="F60" s="20"/>
@@ -10293,7 +10299,7 @@
       <c r="C62" s="73"/>
       <c r="D62" s="73"/>
       <c r="E62" s="73"/>
-      <c r="F62" s="80"/>
+      <c r="F62" s="73"/>
       <c r="G62" s="58"/>
       <c r="H62" s="20"/>
       <c r="I62" s="20"/>
@@ -10341,7 +10347,7 @@
       <c r="B65" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="C65" s="20"/>
+      <c r="C65" s="79"/>
       <c r="D65" s="73"/>
       <c r="E65" s="73"/>
       <c r="F65" s="73"/>
@@ -10359,17 +10365,17 @@
         <v>60</v>
       </c>
       <c r="C66" s="73"/>
-      <c r="D66" s="80"/>
+      <c r="D66" s="82"/>
       <c r="E66" s="73"/>
       <c r="F66" s="20"/>
       <c r="G66" s="58"/>
-      <c r="H66" s="86" t="s">
+      <c r="H66" s="90" t="s">
         <v>175</v>
       </c>
-      <c r="I66" s="87"/>
-      <c r="J66" s="87"/>
-      <c r="K66" s="87"/>
-      <c r="L66" s="88"/>
+      <c r="I66" s="91"/>
+      <c r="J66" s="91"/>
+      <c r="K66" s="91"/>
+      <c r="L66" s="92"/>
       <c r="M66" s="58"/>
     </row>
     <row r="67" spans="1:13" ht="15.75" thickBot="1">
@@ -10377,20 +10383,20 @@
       <c r="B67" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C67" s="20"/>
+      <c r="C67" s="79"/>
       <c r="D67" s="73"/>
       <c r="E67" s="73"/>
       <c r="F67" s="73"/>
       <c r="G67" s="58"/>
-      <c r="H67" s="77" t="s">
+      <c r="H67" s="76" t="s">
         <v>290</v>
       </c>
       <c r="I67" s="63"/>
       <c r="J67" s="63"/>
-      <c r="K67" s="92" t="s">
+      <c r="K67" s="96" t="s">
         <v>292</v>
       </c>
-      <c r="L67" s="93"/>
+      <c r="L67" s="97"/>
       <c r="M67" s="58"/>
     </row>
     <row r="68" spans="1:13" ht="15.75" thickBot="1">
@@ -10403,15 +10409,15 @@
       <c r="E68" s="73"/>
       <c r="F68" s="20"/>
       <c r="G68" s="58"/>
-      <c r="H68" s="77" t="s">
+      <c r="H68" s="76" t="s">
         <v>291</v>
       </c>
       <c r="I68" s="63"/>
       <c r="J68" s="63"/>
-      <c r="K68" s="92" t="s">
+      <c r="K68" s="96" t="s">
         <v>293</v>
       </c>
-      <c r="L68" s="93"/>
+      <c r="L68" s="97"/>
       <c r="M68" s="58"/>
     </row>
     <row r="69" spans="1:13" ht="15.75" thickBot="1">
@@ -10422,15 +10428,15 @@
       <c r="C69" s="20"/>
       <c r="D69" s="73"/>
       <c r="E69" s="73"/>
-      <c r="F69" s="20"/>
+      <c r="F69" s="79"/>
       <c r="G69" s="58"/>
       <c r="H69" s="20"/>
       <c r="I69" s="20"/>
       <c r="J69" s="20"/>
-      <c r="K69" s="94" t="s">
+      <c r="K69" s="98" t="s">
         <v>300</v>
       </c>
-      <c r="L69" s="95"/>
+      <c r="L69" s="99"/>
       <c r="M69" s="58"/>
     </row>
     <row r="70" spans="1:13" ht="15.75" thickBot="1">
@@ -10440,16 +10446,16 @@
       </c>
       <c r="C70" s="20"/>
       <c r="D70" s="73"/>
-      <c r="E70" s="78"/>
+      <c r="E70" s="77"/>
       <c r="F70" s="20"/>
       <c r="G70" s="58"/>
       <c r="H70" s="20"/>
       <c r="I70" s="20"/>
       <c r="J70" s="20"/>
-      <c r="K70" s="94" t="s">
+      <c r="K70" s="98" t="s">
         <v>301</v>
       </c>
-      <c r="L70" s="95"/>
+      <c r="L70" s="99"/>
       <c r="M70" s="58"/>
     </row>
     <row r="71" spans="1:13" ht="15.75" thickBot="1">
@@ -10457,7 +10463,7 @@
       <c r="B71" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C71" s="20"/>
+      <c r="C71" s="79"/>
       <c r="D71" s="73"/>
       <c r="E71" s="73"/>
       <c r="F71" s="73"/>
@@ -10465,8 +10471,8 @@
       <c r="H71" s="20"/>
       <c r="I71" s="20"/>
       <c r="J71" s="20"/>
-      <c r="K71" s="89"/>
-      <c r="L71" s="90"/>
+      <c r="K71" s="93"/>
+      <c r="L71" s="94"/>
       <c r="M71" s="58"/>
     </row>
     <row r="72" spans="1:13" ht="15.75" thickBot="1">
@@ -10477,13 +10483,13 @@
       <c r="C72" s="73"/>
       <c r="D72" s="20"/>
       <c r="E72" s="73"/>
-      <c r="F72" s="20"/>
+      <c r="F72" s="79"/>
       <c r="G72" s="58"/>
       <c r="H72" s="20"/>
       <c r="I72" s="20"/>
       <c r="J72" s="20"/>
-      <c r="K72" s="89"/>
-      <c r="L72" s="90"/>
+      <c r="K72" s="93"/>
+      <c r="L72" s="94"/>
       <c r="M72" s="58"/>
     </row>
     <row r="73" spans="1:13" ht="15.75" thickBot="1">
@@ -10573,7 +10579,7 @@
       <c r="B77" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="C77" s="82"/>
+      <c r="C77" s="81"/>
       <c r="D77" s="41"/>
       <c r="E77" s="39"/>
       <c r="F77" s="39"/>
@@ -10668,7 +10674,7 @@
       <c r="B82" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="C82" s="80"/>
+      <c r="C82" s="79"/>
       <c r="D82" s="20"/>
       <c r="E82" s="20"/>
       <c r="F82" s="20"/>
@@ -10696,7 +10702,7 @@
         <v>185</v>
       </c>
       <c r="I83" s="20"/>
-      <c r="J83" s="80"/>
+      <c r="J83" s="73"/>
       <c r="K83" s="20"/>
       <c r="L83" s="20"/>
       <c r="M83" s="58"/>
@@ -10706,7 +10712,7 @@
       <c r="B84" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="C84" s="20"/>
+      <c r="C84" s="79"/>
       <c r="D84" s="20"/>
       <c r="E84" s="73"/>
       <c r="F84" s="20"/>
@@ -10744,7 +10750,7 @@
       <c r="B86" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="C86" s="20"/>
+      <c r="C86" s="79"/>
       <c r="D86" s="20"/>
       <c r="E86" s="20"/>
       <c r="F86" s="20"/>
@@ -10763,7 +10769,7 @@
       <c r="B87" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="C87" s="20"/>
+      <c r="C87" s="79"/>
       <c r="D87" s="20"/>
       <c r="E87" s="20"/>
       <c r="F87" s="20"/>
@@ -10783,7 +10789,7 @@
         <v>82</v>
       </c>
       <c r="C88" s="73"/>
-      <c r="D88" s="83"/>
+      <c r="D88" s="82"/>
       <c r="E88" s="73"/>
       <c r="F88" s="20"/>
       <c r="G88" s="58"/>
@@ -10802,7 +10808,7 @@
         <v>83</v>
       </c>
       <c r="C89" s="20"/>
-      <c r="D89" s="79"/>
+      <c r="D89" s="78"/>
       <c r="E89" s="73"/>
       <c r="F89" s="73"/>
       <c r="G89" s="58"/>
@@ -10820,7 +10826,7 @@
       <c r="B90" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="C90" s="39"/>
+      <c r="C90" s="85"/>
       <c r="D90" s="74"/>
       <c r="E90" s="74"/>
       <c r="F90" s="41"/>
@@ -10877,9 +10883,9 @@
       <c r="B93" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="C93" s="20"/>
+      <c r="C93" s="79"/>
       <c r="D93" s="20"/>
-      <c r="E93" s="80"/>
+      <c r="E93" s="73"/>
       <c r="F93" s="20"/>
       <c r="G93" s="58"/>
       <c r="H93" s="19" t="s">
@@ -10896,7 +10902,7 @@
       <c r="B94" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="C94" s="80"/>
+      <c r="C94" s="79"/>
       <c r="D94" s="73"/>
       <c r="E94" s="20"/>
       <c r="F94" s="20"/>
@@ -10923,7 +10929,7 @@
       <c r="H95" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="I95" s="20"/>
+      <c r="I95" s="79"/>
       <c r="J95" s="73"/>
       <c r="K95" s="20"/>
       <c r="L95" s="20"/>
@@ -10991,8 +10997,8 @@
       <c r="B99" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="C99" s="80"/>
-      <c r="D99" s="80"/>
+      <c r="C99" s="79"/>
+      <c r="D99" s="73"/>
       <c r="E99" s="73"/>
       <c r="F99" s="20"/>
       <c r="G99" s="58"/>
@@ -11010,7 +11016,7 @@
       <c r="B100" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="C100" s="39"/>
+      <c r="C100" s="85"/>
       <c r="D100" s="74"/>
       <c r="E100" s="39"/>
       <c r="F100" s="41"/>
@@ -11018,7 +11024,7 @@
       <c r="H100" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="I100" s="20"/>
+      <c r="I100" s="79"/>
       <c r="J100" s="73"/>
       <c r="K100" s="20"/>
       <c r="L100" s="20"/>
@@ -11030,7 +11036,7 @@
         <v>299</v>
       </c>
       <c r="C101" s="20"/>
-      <c r="D101" s="80"/>
+      <c r="D101" s="73"/>
       <c r="E101" s="20"/>
       <c r="F101" s="20"/>
       <c r="G101" s="58"/>
@@ -11067,7 +11073,7 @@
       <c r="B103" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="C103" s="20"/>
+      <c r="C103" s="79"/>
       <c r="D103" s="73"/>
       <c r="E103" s="20"/>
       <c r="F103" s="62"/>
@@ -11221,7 +11227,7 @@
         <v>209</v>
       </c>
       <c r="I110" s="20"/>
-      <c r="J110" s="96"/>
+      <c r="J110" s="83"/>
       <c r="K110" s="20"/>
       <c r="L110" s="20"/>
       <c r="M110" s="58"/>
@@ -11337,7 +11343,7 @@
       <c r="I116" s="75" t="s">
         <v>288</v>
       </c>
-      <c r="J116" s="20"/>
+      <c r="J116" s="79"/>
       <c r="K116" s="20"/>
       <c r="L116" s="20"/>
       <c r="M116" s="58"/>
@@ -11347,7 +11353,7 @@
       <c r="B117" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="C117" s="76" t="s">
+      <c r="C117" s="87" t="s">
         <v>289</v>
       </c>
       <c r="D117" s="41"/>
@@ -11395,7 +11401,7 @@
       <c r="H119" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="I119" s="20"/>
+      <c r="I119" s="79"/>
       <c r="J119" s="73"/>
       <c r="K119" s="20"/>
       <c r="L119" s="20"/>
@@ -11414,7 +11420,7 @@
       <c r="H120" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="I120" s="20"/>
+      <c r="I120" s="79"/>
       <c r="J120" s="20"/>
       <c r="K120" s="42"/>
       <c r="L120" s="20"/>
@@ -11426,14 +11432,14 @@
         <v>113</v>
       </c>
       <c r="C121" s="20"/>
-      <c r="D121" s="80"/>
+      <c r="D121" s="73"/>
       <c r="E121" s="73"/>
       <c r="F121" s="20"/>
       <c r="G121" s="58"/>
       <c r="H121" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="I121" s="20"/>
+      <c r="I121" s="79"/>
       <c r="J121" s="20"/>
       <c r="K121" s="20"/>
       <c r="L121" s="20"/>
@@ -11463,7 +11469,7 @@
       <c r="B123" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="C123" s="20"/>
+      <c r="C123" s="79"/>
       <c r="D123" s="73"/>
       <c r="E123" s="73"/>
       <c r="F123" s="20"/>
@@ -11501,7 +11507,7 @@
       <c r="B125" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="C125" s="20"/>
+      <c r="C125" s="79"/>
       <c r="D125" s="73"/>
       <c r="E125" s="73"/>
       <c r="F125" s="73"/>
@@ -11558,8 +11564,8 @@
       <c r="B128" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="C128" s="82"/>
-      <c r="D128" s="97"/>
+      <c r="C128" s="81"/>
+      <c r="D128" s="84"/>
       <c r="E128" s="74"/>
       <c r="F128" s="39"/>
       <c r="G128" s="58"/>
@@ -11577,7 +11583,7 @@
       <c r="B129" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="C129" s="20"/>
+      <c r="C129" s="79"/>
       <c r="D129" s="73"/>
       <c r="E129" s="20"/>
       <c r="F129" s="20"/>
@@ -11606,7 +11612,7 @@
       </c>
       <c r="I130" s="73"/>
       <c r="J130" s="73"/>
-      <c r="K130" s="20"/>
+      <c r="K130" s="79"/>
       <c r="L130" s="20"/>
       <c r="M130" s="58"/>
     </row>
@@ -11615,7 +11621,7 @@
       <c r="B131" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="C131" s="39"/>
+      <c r="C131" s="85"/>
       <c r="D131" s="74"/>
       <c r="E131" s="74"/>
       <c r="F131" s="41"/>
@@ -11634,7 +11640,7 @@
       <c r="B132" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="C132" s="20"/>
+      <c r="C132" s="79"/>
       <c r="D132" s="73"/>
       <c r="E132" s="20"/>
       <c r="F132" s="20"/>
@@ -11661,9 +11667,9 @@
       <c r="H133" s="19" t="s">
         <v>231</v>
       </c>
-      <c r="I133" s="20"/>
+      <c r="I133" s="79"/>
       <c r="J133" s="73"/>
-      <c r="K133" s="20"/>
+      <c r="K133" s="79"/>
       <c r="L133" s="62"/>
       <c r="M133" s="58"/>
     </row>
@@ -11672,7 +11678,7 @@
       <c r="B134" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="C134" s="20"/>
+      <c r="C134" s="79"/>
       <c r="D134" s="73"/>
       <c r="E134" s="20"/>
       <c r="F134" s="20"/>
@@ -11723,7 +11729,7 @@
       <c r="C136" s="73"/>
       <c r="D136" s="73"/>
       <c r="E136" s="73"/>
-      <c r="F136" s="78"/>
+      <c r="F136" s="77"/>
       <c r="G136" s="4"/>
       <c r="H136" s="51" t="s">
         <v>239</v>
@@ -11760,7 +11766,7 @@
       <c r="B138" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="C138" s="20"/>
+      <c r="C138" s="79"/>
       <c r="D138" s="20"/>
       <c r="E138" s="20"/>
       <c r="F138" s="20"/>
@@ -12164,7 +12170,7 @@
       <c r="N156" s="4"/>
     </row>
     <row r="157" spans="1:14" ht="27" thickBot="1">
-      <c r="A157" s="81" t="s">
+      <c r="A157" s="80" t="s">
         <v>269</v>
       </c>
       <c r="B157" s="45" t="s">

</xml_diff>

<commit_message>
more items updated on both pages
</commit_message>
<xml_diff>
--- a/check list.xlsx
+++ b/check list.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="313">
   <si>
     <t>ARMOR</t>
   </si>
@@ -923,6 +923,39 @@
   </si>
   <si>
     <t>Lammergeier</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Demonstone Blood</t>
+  </si>
+  <si>
+    <t>Black Dwarf</t>
+  </si>
+  <si>
+    <t>Death Ward</t>
+  </si>
+  <si>
+    <t>Dragon's Egg</t>
+  </si>
+  <si>
+    <t>Lamen of the Archbishop</t>
+  </si>
+  <si>
+    <t>Heavenstone</t>
+  </si>
+  <si>
+    <t>Klaatu Barada Nikto</t>
+  </si>
+  <si>
+    <t>Myokai's path</t>
+  </si>
+  <si>
+    <t>Gallowlaugh</t>
+  </si>
+  <si>
+    <t>Seal of the Nephalem Kings</t>
   </si>
 </sst>
 </file>
@@ -1290,7 +1323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1522,9 +1555,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1535,12 +1565,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1577,6 +1601,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2415,13 +2445,13 @@
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
       <c r="G27" s="7"/>
-      <c r="H27" s="89" t="s">
+      <c r="H27" s="86" t="s">
         <v>171</v>
       </c>
-      <c r="I27" s="89"/>
-      <c r="J27" s="89"/>
-      <c r="K27" s="89"/>
-      <c r="L27" s="89"/>
+      <c r="I27" s="86"/>
+      <c r="J27" s="86"/>
+      <c r="K27" s="86"/>
+      <c r="L27" s="86"/>
       <c r="M27" s="7"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1">
@@ -2576,13 +2606,13 @@
       <c r="E36" s="20"/>
       <c r="F36" s="29"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="89" t="s">
+      <c r="H36" s="86" t="s">
         <v>172</v>
       </c>
-      <c r="I36" s="89"/>
-      <c r="J36" s="89"/>
-      <c r="K36" s="89"/>
-      <c r="L36" s="89"/>
+      <c r="I36" s="86"/>
+      <c r="J36" s="86"/>
+      <c r="K36" s="86"/>
+      <c r="L36" s="86"/>
       <c r="M36" s="7"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
@@ -2743,13 +2773,13 @@
         <v>3</v>
       </c>
       <c r="G45" s="7"/>
-      <c r="H45" s="89" t="s">
+      <c r="H45" s="86" t="s">
         <v>173</v>
       </c>
-      <c r="I45" s="89"/>
-      <c r="J45" s="89"/>
-      <c r="K45" s="89"/>
-      <c r="L45" s="89"/>
+      <c r="I45" s="86"/>
+      <c r="J45" s="86"/>
+      <c r="K45" s="86"/>
+      <c r="L45" s="86"/>
       <c r="M45" s="7"/>
     </row>
     <row r="46" spans="1:13" ht="15.75" thickBot="1">
@@ -2898,13 +2928,13 @@
       <c r="E54" s="39"/>
       <c r="F54" s="39"/>
       <c r="G54" s="7"/>
-      <c r="H54" s="89" t="s">
+      <c r="H54" s="86" t="s">
         <v>174</v>
       </c>
-      <c r="I54" s="89"/>
-      <c r="J54" s="89"/>
-      <c r="K54" s="89"/>
-      <c r="L54" s="89"/>
+      <c r="I54" s="86"/>
+      <c r="J54" s="86"/>
+      <c r="K54" s="86"/>
+      <c r="L54" s="86"/>
       <c r="M54" s="7"/>
     </row>
     <row r="55" spans="1:13" ht="15.75" thickBot="1">
@@ -3053,13 +3083,13 @@
       <c r="E63" s="20"/>
       <c r="F63" s="20"/>
       <c r="G63" s="7"/>
-      <c r="H63" s="89" t="s">
+      <c r="H63" s="86" t="s">
         <v>175</v>
       </c>
-      <c r="I63" s="89"/>
-      <c r="J63" s="89"/>
-      <c r="K63" s="89"/>
-      <c r="L63" s="89"/>
+      <c r="I63" s="86"/>
+      <c r="J63" s="86"/>
+      <c r="K63" s="86"/>
+      <c r="L63" s="86"/>
       <c r="M63" s="7"/>
     </row>
     <row r="64" spans="1:13" ht="15.75" thickBot="1">
@@ -4368,11 +4398,11 @@
       <c r="E132" s="20"/>
       <c r="F132" s="20"/>
       <c r="G132" s="7"/>
-      <c r="H132" s="88"/>
-      <c r="I132" s="88"/>
-      <c r="J132" s="88"/>
-      <c r="K132" s="88"/>
-      <c r="L132" s="88"/>
+      <c r="H132" s="85"/>
+      <c r="I132" s="85"/>
+      <c r="J132" s="85"/>
+      <c r="K132" s="85"/>
+      <c r="L132" s="85"/>
       <c r="M132" s="7"/>
     </row>
     <row r="133" spans="1:14" ht="18" thickBot="1">
@@ -6118,13 +6148,13 @@
       <c r="E30" s="20"/>
       <c r="F30" s="20"/>
       <c r="G30" s="58"/>
-      <c r="H30" s="90" t="s">
+      <c r="H30" s="87" t="s">
         <v>171</v>
       </c>
-      <c r="I30" s="91"/>
-      <c r="J30" s="91"/>
-      <c r="K30" s="91"/>
-      <c r="L30" s="92"/>
+      <c r="I30" s="88"/>
+      <c r="J30" s="88"/>
+      <c r="K30" s="88"/>
+      <c r="L30" s="89"/>
       <c r="M30" s="58"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1">
@@ -6279,13 +6309,13 @@
       <c r="E39" s="20"/>
       <c r="F39" s="62"/>
       <c r="G39" s="58"/>
-      <c r="H39" s="90" t="s">
+      <c r="H39" s="87" t="s">
         <v>172</v>
       </c>
-      <c r="I39" s="91"/>
-      <c r="J39" s="91"/>
-      <c r="K39" s="91"/>
-      <c r="L39" s="92"/>
+      <c r="I39" s="88"/>
+      <c r="J39" s="88"/>
+      <c r="K39" s="88"/>
+      <c r="L39" s="89"/>
       <c r="M39" s="58"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" thickBot="1">
@@ -6446,13 +6476,13 @@
         <v>3</v>
       </c>
       <c r="G48" s="58"/>
-      <c r="H48" s="90" t="s">
+      <c r="H48" s="87" t="s">
         <v>173</v>
       </c>
-      <c r="I48" s="91"/>
-      <c r="J48" s="91"/>
-      <c r="K48" s="91"/>
-      <c r="L48" s="92"/>
+      <c r="I48" s="88"/>
+      <c r="J48" s="88"/>
+      <c r="K48" s="88"/>
+      <c r="L48" s="89"/>
       <c r="M48" s="58"/>
     </row>
     <row r="49" spans="1:13" ht="15.75" thickBot="1">
@@ -6601,13 +6631,13 @@
       <c r="E57" s="39"/>
       <c r="F57" s="39"/>
       <c r="G57" s="58"/>
-      <c r="H57" s="90" t="s">
+      <c r="H57" s="87" t="s">
         <v>174</v>
       </c>
-      <c r="I57" s="91"/>
-      <c r="J57" s="91"/>
-      <c r="K57" s="91"/>
-      <c r="L57" s="92"/>
+      <c r="I57" s="88"/>
+      <c r="J57" s="88"/>
+      <c r="K57" s="88"/>
+      <c r="L57" s="89"/>
       <c r="M57" s="58"/>
     </row>
     <row r="58" spans="1:13" ht="15.75" thickBot="1">
@@ -6756,13 +6786,13 @@
       <c r="E66" s="20"/>
       <c r="F66" s="20"/>
       <c r="G66" s="58"/>
-      <c r="H66" s="90" t="s">
+      <c r="H66" s="87" t="s">
         <v>175</v>
       </c>
-      <c r="I66" s="91"/>
-      <c r="J66" s="91"/>
-      <c r="K66" s="91"/>
-      <c r="L66" s="92"/>
+      <c r="I66" s="88"/>
+      <c r="J66" s="88"/>
+      <c r="K66" s="88"/>
+      <c r="L66" s="89"/>
       <c r="M66" s="58"/>
     </row>
     <row r="67" spans="1:13" ht="15.75" thickBot="1">
@@ -9119,8 +9149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B110" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D121" sqref="D121"/>
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C117" sqref="C117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9139,40 +9169,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="23.25" customHeight="1">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="92" t="s">
         <v>286</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
-      <c r="J1" s="95"/>
-      <c r="K1" s="95"/>
-      <c r="L1" s="95"/>
-      <c r="M1" s="95"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
+      <c r="L1" s="92"/>
+      <c r="M1" s="92"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1">
-      <c r="A2" s="95"/>
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
+      <c r="A2" s="92"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
       <c r="N2" s="1"/>
       <c r="O2" s="69"/>
       <c r="P2" s="70" t="s">
@@ -9181,19 +9211,19 @@
       <c r="Q2" s="1"/>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1">
-      <c r="A3" s="95"/>
-      <c r="B3" s="95"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="95"/>
-      <c r="I3" s="95"/>
-      <c r="J3" s="95"/>
-      <c r="K3" s="95"/>
-      <c r="L3" s="95"/>
-      <c r="M3" s="95"/>
+      <c r="A3" s="92"/>
+      <c r="B3" s="92"/>
+      <c r="C3" s="92"/>
+      <c r="D3" s="92"/>
+      <c r="E3" s="92"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="92"/>
+      <c r="J3" s="92"/>
+      <c r="K3" s="92"/>
+      <c r="L3" s="92"/>
+      <c r="M3" s="92"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -9265,12 +9295,12 @@
       </c>
       <c r="D6" s="72"/>
       <c r="E6" s="73"/>
-      <c r="F6" s="79"/>
+      <c r="F6" s="73"/>
       <c r="G6" s="58"/>
       <c r="H6" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="I6" s="79"/>
+      <c r="I6" s="73"/>
       <c r="J6" s="73"/>
       <c r="K6" s="73"/>
       <c r="L6" s="73"/>
@@ -9338,7 +9368,7 @@
       <c r="B10" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="79"/>
+      <c r="C10" s="73"/>
       <c r="D10" s="73"/>
       <c r="E10" s="73"/>
       <c r="F10" s="20"/>
@@ -9722,20 +9752,20 @@
       <c r="B30" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="86" t="s">
+      <c r="C30" s="72" t="s">
         <v>288</v>
       </c>
       <c r="D30" s="20"/>
       <c r="E30" s="73"/>
       <c r="F30" s="20"/>
       <c r="G30" s="58"/>
-      <c r="H30" s="90" t="s">
+      <c r="H30" s="87" t="s">
         <v>171</v>
       </c>
-      <c r="I30" s="91"/>
-      <c r="J30" s="91"/>
-      <c r="K30" s="91"/>
-      <c r="L30" s="92"/>
+      <c r="I30" s="88"/>
+      <c r="J30" s="88"/>
+      <c r="K30" s="88"/>
+      <c r="L30" s="89"/>
       <c r="M30" s="58"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1">
@@ -9762,19 +9792,21 @@
       <c r="B32" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="79"/>
+      <c r="C32" s="73"/>
       <c r="D32" s="20"/>
       <c r="E32" s="73"/>
       <c r="F32" s="20"/>
       <c r="G32" s="58"/>
-      <c r="H32" s="63"/>
+      <c r="H32" s="76" t="s">
+        <v>310</v>
+      </c>
       <c r="I32" s="63"/>
       <c r="J32" s="63"/>
       <c r="K32" s="63"/>
       <c r="L32" s="63"/>
       <c r="M32" s="58"/>
     </row>
-    <row r="33" spans="1:13" ht="15.75" thickBot="1">
+    <row r="33" spans="1:13" ht="26.25" thickBot="1">
       <c r="A33" s="58"/>
       <c r="B33" s="31"/>
       <c r="C33" s="32"/>
@@ -9782,7 +9814,9 @@
       <c r="E33" s="32"/>
       <c r="F33" s="32"/>
       <c r="G33" s="58"/>
-      <c r="H33" s="20"/>
+      <c r="H33" s="75" t="s">
+        <v>312</v>
+      </c>
       <c r="I33" s="20"/>
       <c r="J33" s="20"/>
       <c r="K33" s="20"/>
@@ -9836,7 +9870,7 @@
       <c r="B36" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="20"/>
+      <c r="C36" s="79"/>
       <c r="D36" s="20"/>
       <c r="E36" s="20"/>
       <c r="F36" s="20"/>
@@ -9892,13 +9926,13 @@
       <c r="E39" s="73"/>
       <c r="F39" s="62"/>
       <c r="G39" s="58"/>
-      <c r="H39" s="90" t="s">
+      <c r="H39" s="87" t="s">
         <v>172</v>
       </c>
-      <c r="I39" s="91"/>
-      <c r="J39" s="91"/>
-      <c r="K39" s="91"/>
-      <c r="L39" s="92"/>
+      <c r="I39" s="88"/>
+      <c r="J39" s="88"/>
+      <c r="K39" s="88"/>
+      <c r="L39" s="89"/>
       <c r="M39" s="58"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" thickBot="1">
@@ -9909,7 +9943,9 @@
       <c r="E40" s="65"/>
       <c r="F40" s="66"/>
       <c r="G40" s="58"/>
-      <c r="H40" s="63"/>
+      <c r="H40" s="76" t="s">
+        <v>304</v>
+      </c>
       <c r="I40" s="63"/>
       <c r="J40" s="63"/>
       <c r="K40" s="63"/>
@@ -9934,14 +9970,16 @@
         <v>3</v>
       </c>
       <c r="G41" s="58"/>
-      <c r="H41" s="63"/>
+      <c r="H41" s="76" t="s">
+        <v>305</v>
+      </c>
       <c r="I41" s="63"/>
       <c r="J41" s="63"/>
       <c r="K41" s="63"/>
       <c r="L41" s="63"/>
       <c r="M41" s="58"/>
     </row>
-    <row r="42" spans="1:13" ht="15.75" thickBot="1">
+    <row r="42" spans="1:13" ht="26.25" thickBot="1">
       <c r="A42" s="58"/>
       <c r="B42" s="38" t="s">
         <v>37</v>
@@ -9951,14 +9989,16 @@
       <c r="E42" s="74"/>
       <c r="F42" s="39"/>
       <c r="G42" s="58"/>
-      <c r="H42" s="20"/>
+      <c r="H42" s="75" t="s">
+        <v>307</v>
+      </c>
       <c r="I42" s="20"/>
       <c r="J42" s="20"/>
       <c r="K42" s="20"/>
       <c r="L42" s="20"/>
       <c r="M42" s="58"/>
     </row>
-    <row r="43" spans="1:13" ht="15.75" thickBot="1">
+    <row r="43" spans="1:13" ht="26.25" thickBot="1">
       <c r="A43" s="58"/>
       <c r="B43" s="19" t="s">
         <v>38</v>
@@ -9968,7 +10008,9 @@
       <c r="E43" s="20"/>
       <c r="F43" s="20"/>
       <c r="G43" s="58"/>
-      <c r="H43" s="20"/>
+      <c r="H43" s="75" t="s">
+        <v>309</v>
+      </c>
       <c r="I43" s="20"/>
       <c r="J43" s="20"/>
       <c r="K43" s="20"/>
@@ -9980,12 +10022,14 @@
       <c r="B44" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="C44" s="79"/>
+      <c r="C44" s="73"/>
       <c r="D44" s="20"/>
       <c r="E44" s="20"/>
       <c r="F44" s="20"/>
       <c r="G44" s="58"/>
-      <c r="H44" s="20"/>
+      <c r="H44" s="75" t="s">
+        <v>311</v>
+      </c>
       <c r="I44" s="20"/>
       <c r="J44" s="20"/>
       <c r="K44" s="20"/>
@@ -10015,7 +10059,7 @@
         <v>41</v>
       </c>
       <c r="C46" s="73"/>
-      <c r="D46" s="79"/>
+      <c r="D46" s="73"/>
       <c r="E46" s="20"/>
       <c r="F46" s="62"/>
       <c r="G46" s="58"/>
@@ -10059,13 +10103,13 @@
         <v>3</v>
       </c>
       <c r="G48" s="58"/>
-      <c r="H48" s="90" t="s">
+      <c r="H48" s="87" t="s">
         <v>173</v>
       </c>
-      <c r="I48" s="91"/>
-      <c r="J48" s="91"/>
-      <c r="K48" s="91"/>
-      <c r="L48" s="92"/>
+      <c r="I48" s="88"/>
+      <c r="J48" s="88"/>
+      <c r="K48" s="88"/>
+      <c r="L48" s="89"/>
       <c r="M48" s="58"/>
     </row>
     <row r="49" spans="1:13" ht="15.75" thickBot="1">
@@ -10078,7 +10122,9 @@
       <c r="E49" s="20"/>
       <c r="F49" s="73"/>
       <c r="G49" s="58"/>
-      <c r="H49" s="63"/>
+      <c r="H49" s="76" t="s">
+        <v>303</v>
+      </c>
       <c r="I49" s="63"/>
       <c r="J49" s="63"/>
       <c r="K49" s="63"/>
@@ -10095,7 +10141,9 @@
       <c r="E50" s="73"/>
       <c r="F50" s="20"/>
       <c r="G50" s="58"/>
-      <c r="H50" s="63"/>
+      <c r="H50" s="76" t="s">
+        <v>306</v>
+      </c>
       <c r="I50" s="63"/>
       <c r="J50" s="63"/>
       <c r="K50" s="63"/>
@@ -10107,12 +10155,14 @@
       <c r="B51" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C51" s="79"/>
+      <c r="C51" s="73"/>
       <c r="D51" s="73"/>
       <c r="E51" s="20"/>
       <c r="F51" s="20"/>
       <c r="G51" s="58"/>
-      <c r="H51" s="20"/>
+      <c r="H51" s="75" t="s">
+        <v>308</v>
+      </c>
       <c r="I51" s="20"/>
       <c r="J51" s="20"/>
       <c r="K51" s="20"/>
@@ -10124,7 +10174,7 @@
       <c r="B52" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="C52" s="79"/>
+      <c r="C52" s="73"/>
       <c r="D52" s="73"/>
       <c r="E52" s="73"/>
       <c r="F52" s="73"/>
@@ -10158,7 +10208,7 @@
       <c r="B54" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C54" s="79"/>
+      <c r="C54" s="73"/>
       <c r="D54" s="73"/>
       <c r="E54" s="73"/>
       <c r="F54" s="20"/>
@@ -10209,18 +10259,18 @@
       <c r="B57" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="C57" s="85"/>
+      <c r="C57" s="74"/>
       <c r="D57" s="74"/>
       <c r="E57" s="74"/>
       <c r="F57" s="74"/>
       <c r="G57" s="58"/>
-      <c r="H57" s="90" t="s">
+      <c r="H57" s="87" t="s">
         <v>174</v>
       </c>
-      <c r="I57" s="91"/>
-      <c r="J57" s="91"/>
-      <c r="K57" s="91"/>
-      <c r="L57" s="92"/>
+      <c r="I57" s="88"/>
+      <c r="J57" s="88"/>
+      <c r="K57" s="88"/>
+      <c r="L57" s="89"/>
       <c r="M57" s="58"/>
     </row>
     <row r="58" spans="1:13" ht="15.75" thickBot="1">
@@ -10262,7 +10312,7 @@
       <c r="B60" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C60" s="79"/>
+      <c r="C60" s="73"/>
       <c r="D60" s="20"/>
       <c r="E60" s="20"/>
       <c r="F60" s="20"/>
@@ -10365,17 +10415,17 @@
         <v>60</v>
       </c>
       <c r="C66" s="73"/>
-      <c r="D66" s="82"/>
+      <c r="D66" s="81"/>
       <c r="E66" s="73"/>
       <c r="F66" s="20"/>
       <c r="G66" s="58"/>
-      <c r="H66" s="90" t="s">
+      <c r="H66" s="87" t="s">
         <v>175</v>
       </c>
-      <c r="I66" s="91"/>
-      <c r="J66" s="91"/>
-      <c r="K66" s="91"/>
-      <c r="L66" s="92"/>
+      <c r="I66" s="88"/>
+      <c r="J66" s="88"/>
+      <c r="K66" s="88"/>
+      <c r="L66" s="89"/>
       <c r="M66" s="58"/>
     </row>
     <row r="67" spans="1:13" ht="15.75" thickBot="1">
@@ -10393,10 +10443,10 @@
       </c>
       <c r="I67" s="63"/>
       <c r="J67" s="63"/>
-      <c r="K67" s="96" t="s">
+      <c r="K67" s="93" t="s">
         <v>292</v>
       </c>
-      <c r="L67" s="97"/>
+      <c r="L67" s="94"/>
       <c r="M67" s="58"/>
     </row>
     <row r="68" spans="1:13" ht="15.75" thickBot="1">
@@ -10414,10 +10464,10 @@
       </c>
       <c r="I68" s="63"/>
       <c r="J68" s="63"/>
-      <c r="K68" s="96" t="s">
+      <c r="K68" s="93" t="s">
         <v>293</v>
       </c>
-      <c r="L68" s="97"/>
+      <c r="L68" s="94"/>
       <c r="M68" s="58"/>
     </row>
     <row r="69" spans="1:13" ht="15.75" thickBot="1">
@@ -10428,15 +10478,15 @@
       <c r="C69" s="20"/>
       <c r="D69" s="73"/>
       <c r="E69" s="73"/>
-      <c r="F69" s="79"/>
+      <c r="F69" s="73"/>
       <c r="G69" s="58"/>
       <c r="H69" s="20"/>
       <c r="I69" s="20"/>
       <c r="J69" s="20"/>
-      <c r="K69" s="98" t="s">
+      <c r="K69" s="95" t="s">
         <v>300</v>
       </c>
-      <c r="L69" s="99"/>
+      <c r="L69" s="96"/>
       <c r="M69" s="58"/>
     </row>
     <row r="70" spans="1:13" ht="15.75" thickBot="1">
@@ -10452,10 +10502,10 @@
       <c r="H70" s="20"/>
       <c r="I70" s="20"/>
       <c r="J70" s="20"/>
-      <c r="K70" s="98" t="s">
+      <c r="K70" s="95" t="s">
         <v>301</v>
       </c>
-      <c r="L70" s="99"/>
+      <c r="L70" s="96"/>
       <c r="M70" s="58"/>
     </row>
     <row r="71" spans="1:13" ht="15.75" thickBot="1">
@@ -10471,8 +10521,8 @@
       <c r="H71" s="20"/>
       <c r="I71" s="20"/>
       <c r="J71" s="20"/>
-      <c r="K71" s="93"/>
-      <c r="L71" s="94"/>
+      <c r="K71" s="90"/>
+      <c r="L71" s="91"/>
       <c r="M71" s="58"/>
     </row>
     <row r="72" spans="1:13" ht="15.75" thickBot="1">
@@ -10488,8 +10538,8 @@
       <c r="H72" s="20"/>
       <c r="I72" s="20"/>
       <c r="J72" s="20"/>
-      <c r="K72" s="93"/>
-      <c r="L72" s="94"/>
+      <c r="K72" s="90"/>
+      <c r="L72" s="91"/>
       <c r="M72" s="58"/>
     </row>
     <row r="73" spans="1:13" ht="15.75" thickBot="1">
@@ -10579,7 +10629,7 @@
       <c r="B77" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="C77" s="81"/>
+      <c r="C77" s="97"/>
       <c r="D77" s="41"/>
       <c r="E77" s="39"/>
       <c r="F77" s="39"/>
@@ -10663,7 +10713,7 @@
       <c r="H81" s="19" t="s">
         <v>183</v>
       </c>
-      <c r="I81" s="20"/>
+      <c r="I81" s="79"/>
       <c r="J81" s="20"/>
       <c r="K81" s="73"/>
       <c r="L81" s="73"/>
@@ -10674,7 +10724,7 @@
       <c r="B82" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="C82" s="79"/>
+      <c r="C82" s="73"/>
       <c r="D82" s="20"/>
       <c r="E82" s="20"/>
       <c r="F82" s="20"/>
@@ -10712,7 +10762,7 @@
       <c r="B84" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="C84" s="79"/>
+      <c r="C84" s="73"/>
       <c r="D84" s="20"/>
       <c r="E84" s="73"/>
       <c r="F84" s="20"/>
@@ -10750,7 +10800,7 @@
       <c r="B86" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="C86" s="79"/>
+      <c r="C86" s="73"/>
       <c r="D86" s="20"/>
       <c r="E86" s="20"/>
       <c r="F86" s="20"/>
@@ -10769,7 +10819,7 @@
       <c r="B87" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="C87" s="79"/>
+      <c r="C87" s="73"/>
       <c r="D87" s="20"/>
       <c r="E87" s="20"/>
       <c r="F87" s="20"/>
@@ -10789,7 +10839,7 @@
         <v>82</v>
       </c>
       <c r="C88" s="73"/>
-      <c r="D88" s="82"/>
+      <c r="D88" s="81"/>
       <c r="E88" s="73"/>
       <c r="F88" s="20"/>
       <c r="G88" s="58"/>
@@ -10826,7 +10876,7 @@
       <c r="B90" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="C90" s="85"/>
+      <c r="C90" s="74"/>
       <c r="D90" s="74"/>
       <c r="E90" s="74"/>
       <c r="F90" s="41"/>
@@ -10883,7 +10933,7 @@
       <c r="B93" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="C93" s="79"/>
+      <c r="C93" s="73"/>
       <c r="D93" s="20"/>
       <c r="E93" s="73"/>
       <c r="F93" s="20"/>
@@ -10902,7 +10952,7 @@
       <c r="B94" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="C94" s="79"/>
+      <c r="C94" s="73"/>
       <c r="D94" s="73"/>
       <c r="E94" s="20"/>
       <c r="F94" s="20"/>
@@ -10929,7 +10979,7 @@
       <c r="H95" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="I95" s="79"/>
+      <c r="I95" s="73"/>
       <c r="J95" s="73"/>
       <c r="K95" s="20"/>
       <c r="L95" s="20"/>
@@ -10997,7 +11047,7 @@
       <c r="B99" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="C99" s="79"/>
+      <c r="C99" s="73"/>
       <c r="D99" s="73"/>
       <c r="E99" s="73"/>
       <c r="F99" s="20"/>
@@ -11016,7 +11066,7 @@
       <c r="B100" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="C100" s="85"/>
+      <c r="C100" s="74"/>
       <c r="D100" s="74"/>
       <c r="E100" s="39"/>
       <c r="F100" s="41"/>
@@ -11024,7 +11074,7 @@
       <c r="H100" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="I100" s="79"/>
+      <c r="I100" s="73"/>
       <c r="J100" s="73"/>
       <c r="K100" s="20"/>
       <c r="L100" s="20"/>
@@ -11063,7 +11113,7 @@
         <v>203</v>
       </c>
       <c r="I102" s="72"/>
-      <c r="J102" s="73"/>
+      <c r="J102" s="81"/>
       <c r="K102" s="20"/>
       <c r="L102" s="20"/>
       <c r="M102" s="58"/>
@@ -11227,7 +11277,7 @@
         <v>209</v>
       </c>
       <c r="I110" s="20"/>
-      <c r="J110" s="83"/>
+      <c r="J110" s="82"/>
       <c r="K110" s="20"/>
       <c r="L110" s="20"/>
       <c r="M110" s="58"/>
@@ -11294,7 +11344,9 @@
       <c r="B114" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="C114" s="20"/>
+      <c r="C114" s="79" t="s">
+        <v>302</v>
+      </c>
       <c r="D114" s="73"/>
       <c r="E114" s="20"/>
       <c r="F114" s="20"/>
@@ -11343,7 +11395,7 @@
       <c r="I116" s="75" t="s">
         <v>288</v>
       </c>
-      <c r="J116" s="79"/>
+      <c r="J116" s="73"/>
       <c r="K116" s="20"/>
       <c r="L116" s="20"/>
       <c r="M116" s="58"/>
@@ -11353,7 +11405,7 @@
       <c r="B117" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="C117" s="87" t="s">
+      <c r="C117" s="98" t="s">
         <v>289</v>
       </c>
       <c r="D117" s="41"/>
@@ -11439,7 +11491,7 @@
       <c r="H121" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="I121" s="79"/>
+      <c r="I121" s="73"/>
       <c r="J121" s="20"/>
       <c r="K121" s="20"/>
       <c r="L121" s="20"/>
@@ -11507,7 +11559,7 @@
       <c r="B125" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="C125" s="79"/>
+      <c r="C125" s="73"/>
       <c r="D125" s="73"/>
       <c r="E125" s="73"/>
       <c r="F125" s="73"/>
@@ -11564,8 +11616,8 @@
       <c r="B128" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="C128" s="81"/>
-      <c r="D128" s="84"/>
+      <c r="C128" s="97"/>
+      <c r="D128" s="83"/>
       <c r="E128" s="74"/>
       <c r="F128" s="39"/>
       <c r="G128" s="58"/>
@@ -11583,7 +11635,7 @@
       <c r="B129" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="C129" s="79"/>
+      <c r="C129" s="73"/>
       <c r="D129" s="73"/>
       <c r="E129" s="20"/>
       <c r="F129" s="20"/>
@@ -11621,7 +11673,7 @@
       <c r="B131" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="C131" s="85"/>
+      <c r="C131" s="84"/>
       <c r="D131" s="74"/>
       <c r="E131" s="74"/>
       <c r="F131" s="41"/>
@@ -11667,9 +11719,9 @@
       <c r="H133" s="19" t="s">
         <v>231</v>
       </c>
-      <c r="I133" s="79"/>
+      <c r="I133" s="73"/>
       <c r="J133" s="73"/>
-      <c r="K133" s="79"/>
+      <c r="K133" s="73"/>
       <c r="L133" s="62"/>
       <c r="M133" s="58"/>
     </row>
@@ -11678,7 +11730,7 @@
       <c r="B134" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="C134" s="79"/>
+      <c r="C134" s="73"/>
       <c r="D134" s="73"/>
       <c r="E134" s="20"/>
       <c r="F134" s="20"/>
@@ -11766,7 +11818,7 @@
       <c r="B138" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="C138" s="79"/>
+      <c r="C138" s="73"/>
       <c r="D138" s="20"/>
       <c r="E138" s="20"/>
       <c r="F138" s="20"/>
@@ -12128,7 +12180,7 @@
       <c r="B155" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="C155" s="20"/>
+      <c r="C155" s="79"/>
       <c r="D155" s="73"/>
       <c r="E155" s="20"/>
       <c r="F155" s="62"/>

</xml_diff>

<commit_message>
few more items done
i have ran out of items pics so now updates will be of few items at a
time
</commit_message>
<xml_diff>
--- a/check list.xlsx
+++ b/check list.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="315">
   <si>
     <t>ARMOR</t>
   </si>
@@ -956,6 +956,12 @@
   </si>
   <si>
     <t>Seal of the Nephalem Kings</t>
+  </si>
+  <si>
+    <t>kingsport' signal</t>
+  </si>
+  <si>
+    <t>Hangman</t>
   </si>
 </sst>
 </file>
@@ -1549,9 +1555,6 @@
     <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1564,7 +1567,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1603,10 +1609,10 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -9149,8 +9155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C117" sqref="C117"/>
+    <sheetView tabSelected="1" topLeftCell="F29" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9444,7 +9450,7 @@
       <c r="B14" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="79"/>
+      <c r="C14" s="73"/>
       <c r="D14" s="73"/>
       <c r="E14" s="20"/>
       <c r="F14" s="20"/>
@@ -9482,10 +9488,10 @@
       <c r="B16" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="79"/>
+      <c r="C16" s="73"/>
       <c r="D16" s="20"/>
       <c r="E16" s="73"/>
-      <c r="F16" s="20"/>
+      <c r="F16" s="73"/>
       <c r="G16" s="58"/>
       <c r="H16" s="19" t="s">
         <v>158</v>
@@ -9528,7 +9534,7 @@
       <c r="H18" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="I18" s="79"/>
+      <c r="I18" s="80"/>
       <c r="J18" s="73"/>
       <c r="K18" s="20"/>
       <c r="L18" s="20"/>
@@ -9585,7 +9591,7 @@
       <c r="H21" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="I21" s="79"/>
+      <c r="I21" s="80"/>
       <c r="J21" s="73"/>
       <c r="K21" s="20"/>
       <c r="L21" s="20"/>
@@ -9615,7 +9621,7 @@
       <c r="B23" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="79"/>
+      <c r="C23" s="80"/>
       <c r="D23" s="73"/>
       <c r="E23" s="20"/>
       <c r="F23" s="20"/>
@@ -9653,7 +9659,7 @@
       <c r="B25" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="79"/>
+      <c r="C25" s="80"/>
       <c r="D25" s="20"/>
       <c r="E25" s="20"/>
       <c r="F25" s="20"/>
@@ -9870,7 +9876,7 @@
       <c r="B36" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="79"/>
+      <c r="C36" s="73"/>
       <c r="D36" s="20"/>
       <c r="E36" s="20"/>
       <c r="F36" s="20"/>
@@ -9984,7 +9990,7 @@
       <c r="B42" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="C42" s="39"/>
+      <c r="C42" s="74"/>
       <c r="D42" s="74"/>
       <c r="E42" s="74"/>
       <c r="F42" s="39"/>
@@ -10046,7 +10052,9 @@
       <c r="E45" s="20"/>
       <c r="F45" s="73"/>
       <c r="G45" s="58"/>
-      <c r="H45" s="20"/>
+      <c r="H45" s="75" t="s">
+        <v>314</v>
+      </c>
       <c r="I45" s="20"/>
       <c r="J45" s="20"/>
       <c r="K45" s="20"/>
@@ -10397,7 +10405,7 @@
       <c r="B65" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="C65" s="79"/>
+      <c r="C65" s="73"/>
       <c r="D65" s="73"/>
       <c r="E65" s="73"/>
       <c r="F65" s="73"/>
@@ -10415,7 +10423,7 @@
         <v>60</v>
       </c>
       <c r="C66" s="73"/>
-      <c r="D66" s="81"/>
+      <c r="D66" s="80"/>
       <c r="E66" s="73"/>
       <c r="F66" s="20"/>
       <c r="G66" s="58"/>
@@ -10433,7 +10441,7 @@
       <c r="B67" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C67" s="79"/>
+      <c r="C67" s="73"/>
       <c r="D67" s="73"/>
       <c r="E67" s="73"/>
       <c r="F67" s="73"/>
@@ -10480,7 +10488,9 @@
       <c r="E69" s="73"/>
       <c r="F69" s="73"/>
       <c r="G69" s="58"/>
-      <c r="H69" s="20"/>
+      <c r="H69" s="75" t="s">
+        <v>313</v>
+      </c>
       <c r="I69" s="20"/>
       <c r="J69" s="20"/>
       <c r="K69" s="95" t="s">
@@ -10513,7 +10523,7 @@
       <c r="B71" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C71" s="79"/>
+      <c r="C71" s="73"/>
       <c r="D71" s="73"/>
       <c r="E71" s="73"/>
       <c r="F71" s="73"/>
@@ -10533,7 +10543,7 @@
       <c r="C72" s="73"/>
       <c r="D72" s="20"/>
       <c r="E72" s="73"/>
-      <c r="F72" s="79"/>
+      <c r="F72" s="97"/>
       <c r="G72" s="58"/>
       <c r="H72" s="20"/>
       <c r="I72" s="20"/>
@@ -10629,7 +10639,7 @@
       <c r="B77" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="C77" s="97"/>
+      <c r="C77" s="83"/>
       <c r="D77" s="41"/>
       <c r="E77" s="39"/>
       <c r="F77" s="39"/>
@@ -10713,7 +10723,7 @@
       <c r="H81" s="19" t="s">
         <v>183</v>
       </c>
-      <c r="I81" s="79"/>
+      <c r="I81" s="73"/>
       <c r="J81" s="20"/>
       <c r="K81" s="73"/>
       <c r="L81" s="73"/>
@@ -10839,7 +10849,7 @@
         <v>82</v>
       </c>
       <c r="C88" s="73"/>
-      <c r="D88" s="81"/>
+      <c r="D88" s="80"/>
       <c r="E88" s="73"/>
       <c r="F88" s="20"/>
       <c r="G88" s="58"/>
@@ -11113,7 +11123,7 @@
         <v>203</v>
       </c>
       <c r="I102" s="72"/>
-      <c r="J102" s="81"/>
+      <c r="J102" s="80"/>
       <c r="K102" s="20"/>
       <c r="L102" s="20"/>
       <c r="M102" s="58"/>
@@ -11123,7 +11133,7 @@
       <c r="B103" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="C103" s="79"/>
+      <c r="C103" s="73"/>
       <c r="D103" s="73"/>
       <c r="E103" s="20"/>
       <c r="F103" s="62"/>
@@ -11277,7 +11287,7 @@
         <v>209</v>
       </c>
       <c r="I110" s="20"/>
-      <c r="J110" s="82"/>
+      <c r="J110" s="81"/>
       <c r="K110" s="20"/>
       <c r="L110" s="20"/>
       <c r="M110" s="58"/>
@@ -11344,7 +11354,7 @@
       <c r="B114" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="C114" s="79" t="s">
+      <c r="C114" s="73" t="s">
         <v>302</v>
       </c>
       <c r="D114" s="73"/>
@@ -11405,7 +11415,7 @@
       <c r="B117" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="C117" s="98" t="s">
+      <c r="C117" s="84" t="s">
         <v>289</v>
       </c>
       <c r="D117" s="41"/>
@@ -11453,7 +11463,7 @@
       <c r="H119" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="I119" s="79"/>
+      <c r="I119" s="80"/>
       <c r="J119" s="73"/>
       <c r="K119" s="20"/>
       <c r="L119" s="20"/>
@@ -11464,7 +11474,7 @@
       <c r="B120" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="C120" s="20"/>
+      <c r="C120" s="73"/>
       <c r="D120" s="73"/>
       <c r="E120" s="20"/>
       <c r="F120" s="73"/>
@@ -11472,7 +11482,7 @@
       <c r="H120" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="I120" s="79"/>
+      <c r="I120" s="80"/>
       <c r="J120" s="20"/>
       <c r="K120" s="42"/>
       <c r="L120" s="20"/>
@@ -11521,7 +11531,7 @@
       <c r="B123" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="C123" s="79"/>
+      <c r="C123" s="73"/>
       <c r="D123" s="73"/>
       <c r="E123" s="73"/>
       <c r="F123" s="20"/>
@@ -11579,7 +11589,7 @@
         <v>118</v>
       </c>
       <c r="C126" s="20"/>
-      <c r="D126" s="20"/>
+      <c r="D126" s="73"/>
       <c r="E126" s="20"/>
       <c r="F126" s="20"/>
       <c r="G126" s="58"/>
@@ -11616,8 +11626,8 @@
       <c r="B128" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="C128" s="97"/>
-      <c r="D128" s="83"/>
+      <c r="C128" s="83"/>
+      <c r="D128" s="82"/>
       <c r="E128" s="74"/>
       <c r="F128" s="39"/>
       <c r="G128" s="58"/>
@@ -11664,7 +11674,7 @@
       </c>
       <c r="I130" s="73"/>
       <c r="J130" s="73"/>
-      <c r="K130" s="79"/>
+      <c r="K130" s="97"/>
       <c r="L130" s="20"/>
       <c r="M130" s="58"/>
     </row>
@@ -11673,7 +11683,7 @@
       <c r="B131" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="C131" s="84"/>
+      <c r="C131" s="98"/>
       <c r="D131" s="74"/>
       <c r="E131" s="74"/>
       <c r="F131" s="41"/>
@@ -11692,7 +11702,7 @@
       <c r="B132" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="C132" s="79"/>
+      <c r="C132" s="73"/>
       <c r="D132" s="73"/>
       <c r="E132" s="20"/>
       <c r="F132" s="20"/>
@@ -12180,7 +12190,7 @@
       <c r="B155" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="C155" s="79"/>
+      <c r="C155" s="73"/>
       <c r="D155" s="73"/>
       <c r="E155" s="20"/>
       <c r="F155" s="62"/>
@@ -12222,7 +12232,7 @@
       <c r="N156" s="4"/>
     </row>
     <row r="157" spans="1:14" ht="27" thickBot="1">
-      <c r="A157" s="80" t="s">
+      <c r="A157" s="79" t="s">
         <v>269</v>
       </c>
       <c r="B157" s="45" t="s">

</xml_diff>

<commit_message>
loads more items done in SU page
updated proc su diadem in proc_item
</commit_message>
<xml_diff>
--- a/check list.xlsx
+++ b/check list.xlsx
@@ -1329,7 +1329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1573,6 +1573,15 @@
     <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1607,12 +1616,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2451,13 +2454,13 @@
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
       <c r="G27" s="7"/>
-      <c r="H27" s="86" t="s">
+      <c r="H27" s="89" t="s">
         <v>171</v>
       </c>
-      <c r="I27" s="86"/>
-      <c r="J27" s="86"/>
-      <c r="K27" s="86"/>
-      <c r="L27" s="86"/>
+      <c r="I27" s="89"/>
+      <c r="J27" s="89"/>
+      <c r="K27" s="89"/>
+      <c r="L27" s="89"/>
       <c r="M27" s="7"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1">
@@ -2612,13 +2615,13 @@
       <c r="E36" s="20"/>
       <c r="F36" s="29"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="86" t="s">
+      <c r="H36" s="89" t="s">
         <v>172</v>
       </c>
-      <c r="I36" s="86"/>
-      <c r="J36" s="86"/>
-      <c r="K36" s="86"/>
-      <c r="L36" s="86"/>
+      <c r="I36" s="89"/>
+      <c r="J36" s="89"/>
+      <c r="K36" s="89"/>
+      <c r="L36" s="89"/>
       <c r="M36" s="7"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
@@ -2779,13 +2782,13 @@
         <v>3</v>
       </c>
       <c r="G45" s="7"/>
-      <c r="H45" s="86" t="s">
+      <c r="H45" s="89" t="s">
         <v>173</v>
       </c>
-      <c r="I45" s="86"/>
-      <c r="J45" s="86"/>
-      <c r="K45" s="86"/>
-      <c r="L45" s="86"/>
+      <c r="I45" s="89"/>
+      <c r="J45" s="89"/>
+      <c r="K45" s="89"/>
+      <c r="L45" s="89"/>
       <c r="M45" s="7"/>
     </row>
     <row r="46" spans="1:13" ht="15.75" thickBot="1">
@@ -2934,13 +2937,13 @@
       <c r="E54" s="39"/>
       <c r="F54" s="39"/>
       <c r="G54" s="7"/>
-      <c r="H54" s="86" t="s">
+      <c r="H54" s="89" t="s">
         <v>174</v>
       </c>
-      <c r="I54" s="86"/>
-      <c r="J54" s="86"/>
-      <c r="K54" s="86"/>
-      <c r="L54" s="86"/>
+      <c r="I54" s="89"/>
+      <c r="J54" s="89"/>
+      <c r="K54" s="89"/>
+      <c r="L54" s="89"/>
       <c r="M54" s="7"/>
     </row>
     <row r="55" spans="1:13" ht="15.75" thickBot="1">
@@ -3089,13 +3092,13 @@
       <c r="E63" s="20"/>
       <c r="F63" s="20"/>
       <c r="G63" s="7"/>
-      <c r="H63" s="86" t="s">
+      <c r="H63" s="89" t="s">
         <v>175</v>
       </c>
-      <c r="I63" s="86"/>
-      <c r="J63" s="86"/>
-      <c r="K63" s="86"/>
-      <c r="L63" s="86"/>
+      <c r="I63" s="89"/>
+      <c r="J63" s="89"/>
+      <c r="K63" s="89"/>
+      <c r="L63" s="89"/>
       <c r="M63" s="7"/>
     </row>
     <row r="64" spans="1:13" ht="15.75" thickBot="1">
@@ -4404,11 +4407,11 @@
       <c r="E132" s="20"/>
       <c r="F132" s="20"/>
       <c r="G132" s="7"/>
-      <c r="H132" s="85"/>
-      <c r="I132" s="85"/>
-      <c r="J132" s="85"/>
-      <c r="K132" s="85"/>
-      <c r="L132" s="85"/>
+      <c r="H132" s="88"/>
+      <c r="I132" s="88"/>
+      <c r="J132" s="88"/>
+      <c r="K132" s="88"/>
+      <c r="L132" s="88"/>
       <c r="M132" s="7"/>
     </row>
     <row r="133" spans="1:14" ht="18" thickBot="1">
@@ -6154,13 +6157,13 @@
       <c r="E30" s="20"/>
       <c r="F30" s="20"/>
       <c r="G30" s="58"/>
-      <c r="H30" s="87" t="s">
+      <c r="H30" s="90" t="s">
         <v>171</v>
       </c>
-      <c r="I30" s="88"/>
-      <c r="J30" s="88"/>
-      <c r="K30" s="88"/>
-      <c r="L30" s="89"/>
+      <c r="I30" s="91"/>
+      <c r="J30" s="91"/>
+      <c r="K30" s="91"/>
+      <c r="L30" s="92"/>
       <c r="M30" s="58"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1">
@@ -6315,13 +6318,13 @@
       <c r="E39" s="20"/>
       <c r="F39" s="62"/>
       <c r="G39" s="58"/>
-      <c r="H39" s="87" t="s">
+      <c r="H39" s="90" t="s">
         <v>172</v>
       </c>
-      <c r="I39" s="88"/>
-      <c r="J39" s="88"/>
-      <c r="K39" s="88"/>
-      <c r="L39" s="89"/>
+      <c r="I39" s="91"/>
+      <c r="J39" s="91"/>
+      <c r="K39" s="91"/>
+      <c r="L39" s="92"/>
       <c r="M39" s="58"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" thickBot="1">
@@ -6482,13 +6485,13 @@
         <v>3</v>
       </c>
       <c r="G48" s="58"/>
-      <c r="H48" s="87" t="s">
+      <c r="H48" s="90" t="s">
         <v>173</v>
       </c>
-      <c r="I48" s="88"/>
-      <c r="J48" s="88"/>
-      <c r="K48" s="88"/>
-      <c r="L48" s="89"/>
+      <c r="I48" s="91"/>
+      <c r="J48" s="91"/>
+      <c r="K48" s="91"/>
+      <c r="L48" s="92"/>
       <c r="M48" s="58"/>
     </row>
     <row r="49" spans="1:13" ht="15.75" thickBot="1">
@@ -6637,13 +6640,13 @@
       <c r="E57" s="39"/>
       <c r="F57" s="39"/>
       <c r="G57" s="58"/>
-      <c r="H57" s="87" t="s">
+      <c r="H57" s="90" t="s">
         <v>174</v>
       </c>
-      <c r="I57" s="88"/>
-      <c r="J57" s="88"/>
-      <c r="K57" s="88"/>
-      <c r="L57" s="89"/>
+      <c r="I57" s="91"/>
+      <c r="J57" s="91"/>
+      <c r="K57" s="91"/>
+      <c r="L57" s="92"/>
       <c r="M57" s="58"/>
     </row>
     <row r="58" spans="1:13" ht="15.75" thickBot="1">
@@ -6792,13 +6795,13 @@
       <c r="E66" s="20"/>
       <c r="F66" s="20"/>
       <c r="G66" s="58"/>
-      <c r="H66" s="87" t="s">
+      <c r="H66" s="90" t="s">
         <v>175</v>
       </c>
-      <c r="I66" s="88"/>
-      <c r="J66" s="88"/>
-      <c r="K66" s="88"/>
-      <c r="L66" s="89"/>
+      <c r="I66" s="91"/>
+      <c r="J66" s="91"/>
+      <c r="K66" s="91"/>
+      <c r="L66" s="92"/>
       <c r="M66" s="58"/>
     </row>
     <row r="67" spans="1:13" ht="15.75" thickBot="1">
@@ -9155,8 +9158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F29" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J107" sqref="J107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9175,40 +9178,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="23.25" customHeight="1">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="95" t="s">
         <v>286</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
-      <c r="J1" s="92"/>
-      <c r="K1" s="92"/>
-      <c r="L1" s="92"/>
-      <c r="M1" s="92"/>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="95"/>
+      <c r="J1" s="95"/>
+      <c r="K1" s="95"/>
+      <c r="L1" s="95"/>
+      <c r="M1" s="95"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1">
-      <c r="A2" s="92"/>
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
+      <c r="A2" s="95"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
       <c r="N2" s="1"/>
       <c r="O2" s="69"/>
       <c r="P2" s="70" t="s">
@@ -9217,19 +9220,19 @@
       <c r="Q2" s="1"/>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1">
-      <c r="A3" s="92"/>
-      <c r="B3" s="92"/>
-      <c r="C3" s="92"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="92"/>
-      <c r="H3" s="92"/>
-      <c r="I3" s="92"/>
-      <c r="J3" s="92"/>
-      <c r="K3" s="92"/>
-      <c r="L3" s="92"/>
-      <c r="M3" s="92"/>
+      <c r="A3" s="95"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="95"/>
+      <c r="L3" s="95"/>
+      <c r="M3" s="95"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -9320,7 +9323,7 @@
       <c r="C7" s="39"/>
       <c r="D7" s="74"/>
       <c r="E7" s="74"/>
-      <c r="F7" s="39"/>
+      <c r="F7" s="74"/>
       <c r="G7" s="58"/>
       <c r="H7" s="19" t="s">
         <v>149</v>
@@ -9328,7 +9331,7 @@
       <c r="I7" s="20"/>
       <c r="J7" s="73"/>
       <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
+      <c r="L7" s="73"/>
       <c r="M7" s="58"/>
     </row>
     <row r="8" spans="1:17" ht="26.25" thickBot="1">
@@ -9346,8 +9349,8 @@
       </c>
       <c r="I8" s="73"/>
       <c r="J8" s="73"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
+      <c r="K8" s="73"/>
+      <c r="L8" s="73"/>
       <c r="M8" s="58"/>
     </row>
     <row r="9" spans="1:17" ht="15.75" thickBot="1">
@@ -9383,9 +9386,9 @@
         <v>152</v>
       </c>
       <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
+      <c r="J10" s="73"/>
       <c r="K10" s="73"/>
-      <c r="L10" s="20"/>
+      <c r="L10" s="73"/>
       <c r="M10" s="58"/>
     </row>
     <row r="11" spans="1:17" ht="15.75" thickBot="1">
@@ -9432,7 +9435,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
+      <c r="D13" s="73"/>
       <c r="E13" s="20"/>
       <c r="F13" s="73"/>
       <c r="G13" s="58"/>
@@ -9499,7 +9502,7 @@
       <c r="I16" s="73"/>
       <c r="J16" s="73"/>
       <c r="K16" s="73"/>
-      <c r="L16" s="20"/>
+      <c r="L16" s="73"/>
       <c r="M16" s="58"/>
     </row>
     <row r="17" spans="1:13" ht="26.25" thickBot="1">
@@ -9509,8 +9512,8 @@
       </c>
       <c r="C17" s="73"/>
       <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="73"/>
       <c r="G17" s="58"/>
       <c r="H17" s="19" t="s">
         <v>159</v>
@@ -9536,7 +9539,7 @@
       </c>
       <c r="I18" s="80"/>
       <c r="J18" s="73"/>
-      <c r="K18" s="20"/>
+      <c r="K18" s="73"/>
       <c r="L18" s="20"/>
       <c r="M18" s="58"/>
     </row>
@@ -9565,7 +9568,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
+      <c r="D20" s="73"/>
       <c r="E20" s="20"/>
       <c r="F20" s="20"/>
       <c r="G20" s="58"/>
@@ -9668,7 +9671,7 @@
         <v>167</v>
       </c>
       <c r="I25" s="73"/>
-      <c r="J25" s="20"/>
+      <c r="J25" s="73"/>
       <c r="K25" s="20"/>
       <c r="L25" s="73"/>
       <c r="M25" s="58"/>
@@ -9686,7 +9689,7 @@
       </c>
       <c r="I26" s="73"/>
       <c r="J26" s="73"/>
-      <c r="K26" s="20"/>
+      <c r="K26" s="73"/>
       <c r="L26" s="20"/>
       <c r="M26" s="58"/>
     </row>
@@ -9731,7 +9734,7 @@
         <v>170</v>
       </c>
       <c r="I28" s="20"/>
-      <c r="J28" s="20"/>
+      <c r="J28" s="73"/>
       <c r="K28" s="20"/>
       <c r="L28" s="62"/>
       <c r="M28" s="58"/>
@@ -9765,13 +9768,13 @@
       <c r="E30" s="73"/>
       <c r="F30" s="20"/>
       <c r="G30" s="58"/>
-      <c r="H30" s="87" t="s">
+      <c r="H30" s="90" t="s">
         <v>171</v>
       </c>
-      <c r="I30" s="88"/>
-      <c r="J30" s="88"/>
-      <c r="K30" s="88"/>
-      <c r="L30" s="89"/>
+      <c r="I30" s="91"/>
+      <c r="J30" s="91"/>
+      <c r="K30" s="91"/>
+      <c r="L30" s="92"/>
       <c r="M30" s="58"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1">
@@ -9877,7 +9880,7 @@
         <v>32</v>
       </c>
       <c r="C36" s="73"/>
-      <c r="D36" s="20"/>
+      <c r="D36" s="73"/>
       <c r="E36" s="20"/>
       <c r="F36" s="20"/>
       <c r="G36" s="58"/>
@@ -9894,8 +9897,8 @@
         <v>33</v>
       </c>
       <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20"/>
+      <c r="D37" s="73"/>
+      <c r="E37" s="73"/>
       <c r="F37" s="20"/>
       <c r="G37" s="58"/>
       <c r="H37" s="20"/>
@@ -9911,9 +9914,9 @@
         <v>34</v>
       </c>
       <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
+      <c r="D38" s="73"/>
+      <c r="E38" s="73"/>
+      <c r="F38" s="73"/>
       <c r="G38" s="58"/>
       <c r="H38" s="34"/>
       <c r="I38" s="34"/>
@@ -9928,17 +9931,17 @@
         <v>35</v>
       </c>
       <c r="C39" s="73"/>
-      <c r="D39" s="20"/>
+      <c r="D39" s="73"/>
       <c r="E39" s="73"/>
       <c r="F39" s="62"/>
       <c r="G39" s="58"/>
-      <c r="H39" s="87" t="s">
+      <c r="H39" s="90" t="s">
         <v>172</v>
       </c>
-      <c r="I39" s="88"/>
-      <c r="J39" s="88"/>
-      <c r="K39" s="88"/>
-      <c r="L39" s="89"/>
+      <c r="I39" s="91"/>
+      <c r="J39" s="91"/>
+      <c r="K39" s="91"/>
+      <c r="L39" s="92"/>
       <c r="M39" s="58"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" thickBot="1">
@@ -10029,7 +10032,7 @@
         <v>39</v>
       </c>
       <c r="C44" s="73"/>
-      <c r="D44" s="20"/>
+      <c r="D44" s="73"/>
       <c r="E44" s="20"/>
       <c r="F44" s="20"/>
       <c r="G44" s="58"/>
@@ -10111,13 +10114,13 @@
         <v>3</v>
       </c>
       <c r="G48" s="58"/>
-      <c r="H48" s="87" t="s">
+      <c r="H48" s="90" t="s">
         <v>173</v>
       </c>
-      <c r="I48" s="88"/>
-      <c r="J48" s="88"/>
-      <c r="K48" s="88"/>
-      <c r="L48" s="89"/>
+      <c r="I48" s="91"/>
+      <c r="J48" s="91"/>
+      <c r="K48" s="91"/>
+      <c r="L48" s="92"/>
       <c r="M48" s="58"/>
     </row>
     <row r="49" spans="1:13" ht="15.75" thickBot="1">
@@ -10127,7 +10130,7 @@
       </c>
       <c r="C49" s="73"/>
       <c r="D49" s="73"/>
-      <c r="E49" s="20"/>
+      <c r="E49" s="73"/>
       <c r="F49" s="73"/>
       <c r="G49" s="58"/>
       <c r="H49" s="76" t="s">
@@ -10165,7 +10168,7 @@
       </c>
       <c r="C51" s="73"/>
       <c r="D51" s="73"/>
-      <c r="E51" s="20"/>
+      <c r="E51" s="73"/>
       <c r="F51" s="20"/>
       <c r="G51" s="58"/>
       <c r="H51" s="75" t="s">
@@ -10252,7 +10255,7 @@
       </c>
       <c r="C56" s="20"/>
       <c r="D56" s="73"/>
-      <c r="E56" s="20"/>
+      <c r="E56" s="73"/>
       <c r="F56" s="20"/>
       <c r="G56" s="58"/>
       <c r="H56" s="58"/>
@@ -10272,13 +10275,13 @@
       <c r="E57" s="74"/>
       <c r="F57" s="74"/>
       <c r="G57" s="58"/>
-      <c r="H57" s="87" t="s">
+      <c r="H57" s="90" t="s">
         <v>174</v>
       </c>
-      <c r="I57" s="88"/>
-      <c r="J57" s="88"/>
-      <c r="K57" s="88"/>
-      <c r="L57" s="89"/>
+      <c r="I57" s="91"/>
+      <c r="J57" s="91"/>
+      <c r="K57" s="91"/>
+      <c r="L57" s="92"/>
       <c r="M57" s="58"/>
     </row>
     <row r="58" spans="1:13" ht="15.75" thickBot="1">
@@ -10288,7 +10291,7 @@
       </c>
       <c r="C58" s="20"/>
       <c r="D58" s="73"/>
-      <c r="E58" s="20"/>
+      <c r="E58" s="73"/>
       <c r="F58" s="20"/>
       <c r="G58" s="58"/>
       <c r="H58" s="63"/>
@@ -10306,7 +10309,7 @@
       <c r="C59" s="39"/>
       <c r="D59" s="74"/>
       <c r="E59" s="74"/>
-      <c r="F59" s="39"/>
+      <c r="F59" s="74"/>
       <c r="G59" s="58"/>
       <c r="H59" s="63"/>
       <c r="I59" s="63"/>
@@ -10338,7 +10341,7 @@
         <v>55</v>
       </c>
       <c r="C61" s="73"/>
-      <c r="D61" s="20"/>
+      <c r="D61" s="73"/>
       <c r="E61" s="20"/>
       <c r="F61" s="73"/>
       <c r="G61" s="58"/>
@@ -10390,7 +10393,7 @@
       </c>
       <c r="C64" s="20"/>
       <c r="D64" s="73"/>
-      <c r="E64" s="20"/>
+      <c r="E64" s="73"/>
       <c r="F64" s="20"/>
       <c r="G64" s="58"/>
       <c r="H64" s="20"/>
@@ -10425,15 +10428,15 @@
       <c r="C66" s="73"/>
       <c r="D66" s="80"/>
       <c r="E66" s="73"/>
-      <c r="F66" s="20"/>
+      <c r="F66" s="73"/>
       <c r="G66" s="58"/>
-      <c r="H66" s="87" t="s">
+      <c r="H66" s="90" t="s">
         <v>175</v>
       </c>
-      <c r="I66" s="88"/>
-      <c r="J66" s="88"/>
-      <c r="K66" s="88"/>
-      <c r="L66" s="89"/>
+      <c r="I66" s="91"/>
+      <c r="J66" s="91"/>
+      <c r="K66" s="91"/>
+      <c r="L66" s="92"/>
       <c r="M66" s="58"/>
     </row>
     <row r="67" spans="1:13" ht="15.75" thickBot="1">
@@ -10451,10 +10454,10 @@
       </c>
       <c r="I67" s="63"/>
       <c r="J67" s="63"/>
-      <c r="K67" s="93" t="s">
+      <c r="K67" s="96" t="s">
         <v>292</v>
       </c>
-      <c r="L67" s="94"/>
+      <c r="L67" s="97"/>
       <c r="M67" s="58"/>
     </row>
     <row r="68" spans="1:13" ht="15.75" thickBot="1">
@@ -10472,10 +10475,10 @@
       </c>
       <c r="I68" s="63"/>
       <c r="J68" s="63"/>
-      <c r="K68" s="93" t="s">
+      <c r="K68" s="96" t="s">
         <v>293</v>
       </c>
-      <c r="L68" s="94"/>
+      <c r="L68" s="97"/>
       <c r="M68" s="58"/>
     </row>
     <row r="69" spans="1:13" ht="15.75" thickBot="1">
@@ -10493,10 +10496,10 @@
       </c>
       <c r="I69" s="20"/>
       <c r="J69" s="20"/>
-      <c r="K69" s="95" t="s">
+      <c r="K69" s="98" t="s">
         <v>300</v>
       </c>
-      <c r="L69" s="96"/>
+      <c r="L69" s="99"/>
       <c r="M69" s="58"/>
     </row>
     <row r="70" spans="1:13" ht="15.75" thickBot="1">
@@ -10512,10 +10515,10 @@
       <c r="H70" s="20"/>
       <c r="I70" s="20"/>
       <c r="J70" s="20"/>
-      <c r="K70" s="95" t="s">
+      <c r="K70" s="98" t="s">
         <v>301</v>
       </c>
-      <c r="L70" s="96"/>
+      <c r="L70" s="99"/>
       <c r="M70" s="58"/>
     </row>
     <row r="71" spans="1:13" ht="15.75" thickBot="1">
@@ -10531,8 +10534,8 @@
       <c r="H71" s="20"/>
       <c r="I71" s="20"/>
       <c r="J71" s="20"/>
-      <c r="K71" s="90"/>
-      <c r="L71" s="91"/>
+      <c r="K71" s="93"/>
+      <c r="L71" s="94"/>
       <c r="M71" s="58"/>
     </row>
     <row r="72" spans="1:13" ht="15.75" thickBot="1">
@@ -10543,13 +10546,13 @@
       <c r="C72" s="73"/>
       <c r="D72" s="20"/>
       <c r="E72" s="73"/>
-      <c r="F72" s="97"/>
+      <c r="F72" s="85"/>
       <c r="G72" s="58"/>
       <c r="H72" s="20"/>
       <c r="I72" s="20"/>
       <c r="J72" s="20"/>
-      <c r="K72" s="90"/>
-      <c r="L72" s="91"/>
+      <c r="K72" s="93"/>
+      <c r="L72" s="94"/>
       <c r="M72" s="58"/>
     </row>
     <row r="73" spans="1:13" ht="15.75" thickBot="1">
@@ -10559,8 +10562,8 @@
       </c>
       <c r="C73" s="73"/>
       <c r="D73" s="73"/>
-      <c r="E73" s="20"/>
-      <c r="F73" s="20"/>
+      <c r="E73" s="73"/>
+      <c r="F73" s="73"/>
       <c r="G73" s="58"/>
       <c r="H73" s="58"/>
       <c r="I73" s="58"/>
@@ -10577,7 +10580,7 @@
       <c r="C74" s="73"/>
       <c r="D74" s="20"/>
       <c r="E74" s="20"/>
-      <c r="F74" s="20"/>
+      <c r="F74" s="73"/>
       <c r="G74" s="58"/>
       <c r="H74" s="13" t="s">
         <v>176</v>
@@ -10611,7 +10614,7 @@
       </c>
       <c r="I75" s="20"/>
       <c r="J75" s="73"/>
-      <c r="K75" s="20"/>
+      <c r="K75" s="73"/>
       <c r="L75" s="20"/>
       <c r="M75" s="58"/>
     </row>
@@ -10640,7 +10643,7 @@
         <v>71</v>
       </c>
       <c r="C77" s="83"/>
-      <c r="D77" s="41"/>
+      <c r="D77" s="83"/>
       <c r="E77" s="39"/>
       <c r="F77" s="39"/>
       <c r="G77" s="58"/>
@@ -10669,7 +10672,7 @@
       <c r="I78" s="20"/>
       <c r="J78" s="73"/>
       <c r="K78" s="20"/>
-      <c r="L78" s="20"/>
+      <c r="L78" s="73"/>
       <c r="M78" s="58"/>
     </row>
     <row r="79" spans="1:13" ht="15.75" thickBot="1">
@@ -10679,7 +10682,7 @@
       </c>
       <c r="C79" s="20"/>
       <c r="D79" s="73"/>
-      <c r="E79" s="20"/>
+      <c r="E79" s="73"/>
       <c r="F79" s="20"/>
       <c r="G79" s="58"/>
       <c r="H79" s="19" t="s">
@@ -10698,7 +10701,7 @@
       </c>
       <c r="C80" s="20"/>
       <c r="D80" s="20"/>
-      <c r="E80" s="20"/>
+      <c r="E80" s="73"/>
       <c r="F80" s="20"/>
       <c r="G80" s="58"/>
       <c r="H80" s="19" t="s">
@@ -10724,7 +10727,7 @@
         <v>183</v>
       </c>
       <c r="I81" s="73"/>
-      <c r="J81" s="20"/>
+      <c r="J81" s="73"/>
       <c r="K81" s="73"/>
       <c r="L81" s="73"/>
       <c r="M81" s="58"/>
@@ -10736,7 +10739,7 @@
       </c>
       <c r="C82" s="73"/>
       <c r="D82" s="20"/>
-      <c r="E82" s="20"/>
+      <c r="E82" s="73"/>
       <c r="F82" s="20"/>
       <c r="G82" s="58"/>
       <c r="H82" s="19" t="s">
@@ -10783,7 +10786,7 @@
       <c r="I84" s="20"/>
       <c r="J84" s="73"/>
       <c r="K84" s="20"/>
-      <c r="L84" s="20"/>
+      <c r="L84" s="73"/>
       <c r="M84" s="58"/>
     </row>
     <row r="85" spans="1:13" ht="15.75" thickBot="1">
@@ -10819,7 +10822,7 @@
         <v>188</v>
       </c>
       <c r="I86" s="20"/>
-      <c r="J86" s="20"/>
+      <c r="J86" s="73"/>
       <c r="K86" s="73"/>
       <c r="L86" s="20"/>
       <c r="M86" s="58"/>
@@ -10830,7 +10833,7 @@
         <v>81</v>
       </c>
       <c r="C87" s="73"/>
-      <c r="D87" s="20"/>
+      <c r="D87" s="73"/>
       <c r="E87" s="20"/>
       <c r="F87" s="20"/>
       <c r="G87" s="58"/>
@@ -10915,7 +10918,7 @@
       </c>
       <c r="I91" s="73"/>
       <c r="J91" s="73"/>
-      <c r="K91" s="20"/>
+      <c r="K91" s="73"/>
       <c r="L91" s="20"/>
       <c r="M91" s="58"/>
     </row>
@@ -10991,7 +10994,7 @@
       </c>
       <c r="I95" s="73"/>
       <c r="J95" s="73"/>
-      <c r="K95" s="20"/>
+      <c r="K95" s="73"/>
       <c r="L95" s="20"/>
       <c r="M95" s="58"/>
     </row>
@@ -11022,7 +11025,7 @@
       <c r="C97" s="73"/>
       <c r="D97" s="73"/>
       <c r="E97" s="73"/>
-      <c r="F97" s="20"/>
+      <c r="F97" s="73"/>
       <c r="G97" s="58"/>
       <c r="H97" s="19" t="s">
         <v>199</v>
@@ -11039,7 +11042,7 @@
         <v>91</v>
       </c>
       <c r="C98" s="20"/>
-      <c r="D98" s="20"/>
+      <c r="D98" s="73"/>
       <c r="E98" s="20"/>
       <c r="F98" s="20"/>
       <c r="G98" s="58"/>
@@ -11048,7 +11051,7 @@
       </c>
       <c r="I98" s="20"/>
       <c r="J98" s="20"/>
-      <c r="K98" s="20"/>
+      <c r="K98" s="73"/>
       <c r="L98" s="20"/>
       <c r="M98" s="58"/>
     </row>
@@ -11086,7 +11089,7 @@
       </c>
       <c r="I100" s="73"/>
       <c r="J100" s="73"/>
-      <c r="K100" s="20"/>
+      <c r="K100" s="73"/>
       <c r="L100" s="20"/>
       <c r="M100" s="58"/>
     </row>
@@ -11142,7 +11145,7 @@
         <v>204</v>
       </c>
       <c r="I103" s="20"/>
-      <c r="J103" s="20"/>
+      <c r="J103" s="73"/>
       <c r="K103" s="20"/>
       <c r="L103" s="62"/>
       <c r="M103" s="58"/>
@@ -11230,7 +11233,7 @@
         <v>206</v>
       </c>
       <c r="I107" s="20"/>
-      <c r="J107" s="20"/>
+      <c r="J107" s="73"/>
       <c r="K107" s="20"/>
       <c r="L107" s="20"/>
       <c r="M107" s="58"/>
@@ -11242,7 +11245,7 @@
       </c>
       <c r="C108" s="20"/>
       <c r="D108" s="73"/>
-      <c r="E108" s="20"/>
+      <c r="E108" s="73"/>
       <c r="F108" s="20"/>
       <c r="G108" s="58"/>
       <c r="H108" s="19" t="s">
@@ -11289,7 +11292,7 @@
       <c r="I110" s="20"/>
       <c r="J110" s="81"/>
       <c r="K110" s="20"/>
-      <c r="L110" s="20"/>
+      <c r="L110" s="73"/>
       <c r="M110" s="58"/>
     </row>
     <row r="111" spans="1:13" ht="15.75" thickBot="1">
@@ -11319,7 +11322,7 @@
       <c r="C112" s="20"/>
       <c r="D112" s="73"/>
       <c r="E112" s="73"/>
-      <c r="F112" s="20"/>
+      <c r="F112" s="73"/>
       <c r="G112" s="58"/>
       <c r="H112" s="19" t="s">
         <v>211</v>
@@ -11338,14 +11341,14 @@
       <c r="C113" s="20"/>
       <c r="D113" s="73"/>
       <c r="E113" s="20"/>
-      <c r="F113" s="20"/>
+      <c r="F113" s="73"/>
       <c r="G113" s="58"/>
       <c r="H113" s="19" t="s">
         <v>212</v>
       </c>
       <c r="I113" s="73"/>
       <c r="J113" s="20"/>
-      <c r="K113" s="20"/>
+      <c r="K113" s="73"/>
       <c r="L113" s="20"/>
       <c r="M113" s="58"/>
     </row>
@@ -11377,16 +11380,16 @@
       </c>
       <c r="C115" s="20"/>
       <c r="D115" s="73"/>
-      <c r="E115" s="20"/>
+      <c r="E115" s="73"/>
       <c r="F115" s="20"/>
       <c r="G115" s="58"/>
       <c r="H115" s="19" t="s">
         <v>214</v>
       </c>
       <c r="I115" s="20"/>
-      <c r="J115" s="20"/>
+      <c r="J115" s="73"/>
       <c r="K115" s="20"/>
-      <c r="L115" s="20"/>
+      <c r="L115" s="73"/>
       <c r="M115" s="58"/>
     </row>
     <row r="116" spans="1:13" ht="15.75" thickBot="1">
@@ -11419,7 +11422,7 @@
         <v>289</v>
       </c>
       <c r="D117" s="41"/>
-      <c r="E117" s="39"/>
+      <c r="E117" s="74"/>
       <c r="F117" s="39"/>
       <c r="G117" s="58"/>
       <c r="H117" s="19" t="s">
@@ -11438,7 +11441,7 @@
       </c>
       <c r="C118" s="20"/>
       <c r="D118" s="73"/>
-      <c r="E118" s="20"/>
+      <c r="E118" s="73"/>
       <c r="F118" s="20"/>
       <c r="G118" s="58"/>
       <c r="H118" s="19" t="s">
@@ -11458,7 +11461,7 @@
       <c r="C119" s="20"/>
       <c r="D119" s="73"/>
       <c r="E119" s="73"/>
-      <c r="F119" s="20"/>
+      <c r="F119" s="73"/>
       <c r="G119" s="58"/>
       <c r="H119" s="19" t="s">
         <v>218</v>
@@ -11466,7 +11469,7 @@
       <c r="I119" s="80"/>
       <c r="J119" s="73"/>
       <c r="K119" s="20"/>
-      <c r="L119" s="20"/>
+      <c r="L119" s="73"/>
       <c r="M119" s="58"/>
     </row>
     <row r="120" spans="1:13" ht="15.75" thickBot="1">
@@ -11476,14 +11479,14 @@
       </c>
       <c r="C120" s="73"/>
       <c r="D120" s="73"/>
-      <c r="E120" s="20"/>
+      <c r="E120" s="73"/>
       <c r="F120" s="73"/>
       <c r="G120" s="58"/>
       <c r="H120" s="19" t="s">
         <v>219</v>
       </c>
       <c r="I120" s="80"/>
-      <c r="J120" s="20"/>
+      <c r="J120" s="73"/>
       <c r="K120" s="42"/>
       <c r="L120" s="20"/>
       <c r="M120" s="58"/>
@@ -11578,8 +11581,8 @@
         <v>297</v>
       </c>
       <c r="I125" s="73"/>
-      <c r="J125" s="20"/>
-      <c r="K125" s="20"/>
+      <c r="J125" s="73"/>
+      <c r="K125" s="73"/>
       <c r="L125" s="20"/>
       <c r="M125" s="58"/>
     </row>
@@ -11617,8 +11620,8 @@
       </c>
       <c r="I127" s="20"/>
       <c r="J127" s="20"/>
-      <c r="K127" s="20"/>
-      <c r="L127" s="20"/>
+      <c r="K127" s="73"/>
+      <c r="L127" s="73"/>
       <c r="M127" s="58"/>
     </row>
     <row r="128" spans="1:13" ht="15.75" thickBot="1">
@@ -11636,7 +11639,7 @@
       </c>
       <c r="I128" s="20"/>
       <c r="J128" s="20"/>
-      <c r="K128" s="20"/>
+      <c r="K128" s="73"/>
       <c r="L128" s="20"/>
       <c r="M128" s="58"/>
     </row>
@@ -11654,7 +11657,7 @@
         <v>227</v>
       </c>
       <c r="I129" s="20"/>
-      <c r="J129" s="20"/>
+      <c r="J129" s="73"/>
       <c r="K129" s="20"/>
       <c r="L129" s="20"/>
       <c r="M129" s="58"/>
@@ -11666,7 +11669,7 @@
       </c>
       <c r="C130" s="20"/>
       <c r="D130" s="73"/>
-      <c r="E130" s="20"/>
+      <c r="E130" s="73"/>
       <c r="F130" s="20"/>
       <c r="G130" s="58"/>
       <c r="H130" s="19" t="s">
@@ -11674,7 +11677,7 @@
       </c>
       <c r="I130" s="73"/>
       <c r="J130" s="73"/>
-      <c r="K130" s="97"/>
+      <c r="K130" s="85"/>
       <c r="L130" s="20"/>
       <c r="M130" s="58"/>
     </row>
@@ -11683,7 +11686,7 @@
       <c r="B131" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="C131" s="98"/>
+      <c r="C131" s="86"/>
       <c r="D131" s="74"/>
       <c r="E131" s="74"/>
       <c r="F131" s="41"/>
@@ -11693,7 +11696,7 @@
       </c>
       <c r="I131" s="20"/>
       <c r="J131" s="20"/>
-      <c r="K131" s="20"/>
+      <c r="K131" s="73"/>
       <c r="L131" s="20"/>
       <c r="M131" s="58"/>
     </row>
@@ -11704,7 +11707,7 @@
       </c>
       <c r="C132" s="73"/>
       <c r="D132" s="73"/>
-      <c r="E132" s="20"/>
+      <c r="E132" s="73"/>
       <c r="F132" s="20"/>
       <c r="G132" s="58"/>
       <c r="H132" s="19" t="s">
@@ -11829,7 +11832,7 @@
         <v>130</v>
       </c>
       <c r="C138" s="73"/>
-      <c r="D138" s="20"/>
+      <c r="D138" s="73"/>
       <c r="E138" s="20"/>
       <c r="F138" s="20"/>
       <c r="G138" s="4"/>
@@ -11908,7 +11911,7 @@
       </c>
       <c r="C142" s="20"/>
       <c r="D142" s="20"/>
-      <c r="E142" s="20"/>
+      <c r="E142" s="73"/>
       <c r="F142" s="62"/>
       <c r="G142" s="4"/>
       <c r="H142" s="44" t="s">
@@ -11984,7 +11987,7 @@
       </c>
       <c r="C145" s="73"/>
       <c r="D145" s="73"/>
-      <c r="E145" s="20"/>
+      <c r="E145" s="73"/>
       <c r="F145" s="20"/>
       <c r="G145" s="4"/>
       <c r="H145" s="51" t="s">
@@ -12003,8 +12006,8 @@
         <v>137</v>
       </c>
       <c r="C146" s="20"/>
-      <c r="D146" s="20"/>
-      <c r="E146" s="20"/>
+      <c r="D146" s="73"/>
+      <c r="E146" s="73"/>
       <c r="F146" s="73"/>
       <c r="G146" s="4"/>
       <c r="H146" s="51" t="s">
@@ -12024,7 +12027,7 @@
       </c>
       <c r="C147" s="20"/>
       <c r="D147" s="73"/>
-      <c r="E147" s="20"/>
+      <c r="E147" s="73"/>
       <c r="F147" s="20"/>
       <c r="G147" s="4"/>
       <c r="H147" s="57" t="s">
@@ -12044,7 +12047,7 @@
       </c>
       <c r="C148" s="73"/>
       <c r="D148" s="73"/>
-      <c r="E148" s="20"/>
+      <c r="E148" s="73"/>
       <c r="F148" s="20"/>
       <c r="G148" s="4"/>
       <c r="H148" s="4"/>
@@ -12151,7 +12154,7 @@
         <v>144</v>
       </c>
       <c r="C153" s="20"/>
-      <c r="D153" s="20"/>
+      <c r="D153" s="73"/>
       <c r="E153" s="20"/>
       <c r="F153" s="20"/>
       <c r="G153" s="4"/>
@@ -12193,7 +12196,7 @@
       <c r="C155" s="73"/>
       <c r="D155" s="73"/>
       <c r="E155" s="20"/>
-      <c r="F155" s="62"/>
+      <c r="F155" s="87"/>
       <c r="G155" s="4"/>
       <c r="H155" s="4"/>
       <c r="I155" s="4"/>

</xml_diff>

<commit_message>
items updated / readme
also added a suggestion in readme
</commit_message>
<xml_diff>
--- a/check list.xlsx
+++ b/check list.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1116" uniqueCount="324">
   <si>
     <t>ARMOR</t>
   </si>
@@ -607,9 +607,6 @@
     <t>Demon Head</t>
   </si>
   <si>
-    <t>Zombie Heard</t>
-  </si>
-  <si>
     <t>Unraveller Head</t>
   </si>
   <si>
@@ -986,6 +983,12 @@
   </si>
   <si>
     <t>Asheara's Cateye</t>
+  </si>
+  <si>
+    <t>Zombie Head</t>
+  </si>
+  <si>
+    <t>Beads of the Snake Queen</t>
   </si>
 </sst>
 </file>
@@ -1353,7 +1356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1643,6 +1646,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1941,8 +1947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N153"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="F77" workbookViewId="0">
+      <selection activeCell="I91" sqref="I91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1982,7 +1988,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="56" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>1</v>
@@ -1998,7 +2004,7 @@
         <v>146</v>
       </c>
       <c r="I2" s="56" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J2" s="14" t="s">
         <v>1</v>
@@ -2261,7 +2267,7 @@
     <row r="16" spans="1:13" ht="15.75" thickBot="1">
       <c r="A16" s="7"/>
       <c r="B16" s="17" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
@@ -2414,7 +2420,7 @@
         <v>23</v>
       </c>
       <c r="C24" s="56" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D24" s="26" t="s">
         <v>1</v>
@@ -2545,7 +2551,7 @@
         <v>29</v>
       </c>
       <c r="C31" s="56" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D31" s="26" t="s">
         <v>1</v>
@@ -2672,7 +2678,7 @@
         <v>35</v>
       </c>
       <c r="C38" s="56" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>1</v>
@@ -2797,7 +2803,7 @@
         <v>41</v>
       </c>
       <c r="C45" s="56" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D45" s="14" t="s">
         <v>1</v>
@@ -3261,7 +3267,7 @@
         <v>175</v>
       </c>
       <c r="I71" s="56" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J71" s="14" t="s">
         <v>1</v>
@@ -3665,7 +3671,7 @@
       <c r="F92" s="20"/>
       <c r="G92" s="7"/>
       <c r="H92" s="19" t="s">
-        <v>196</v>
+        <v>322</v>
       </c>
       <c r="I92" s="20"/>
       <c r="J92" s="20"/>
@@ -3684,7 +3690,7 @@
       <c r="F93" s="20"/>
       <c r="G93" s="7"/>
       <c r="H93" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I93" s="20"/>
       <c r="J93" s="20"/>
@@ -3695,7 +3701,7 @@
     <row r="94" spans="1:13" ht="15.75" thickBot="1">
       <c r="A94" s="7"/>
       <c r="B94" s="19" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C94" s="20"/>
       <c r="D94" s="20"/>
@@ -3703,7 +3709,7 @@
       <c r="F94" s="20"/>
       <c r="G94" s="7"/>
       <c r="H94" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I94" s="20"/>
       <c r="J94" s="20"/>
@@ -3741,7 +3747,7 @@
       <c r="F96" s="20"/>
       <c r="G96" s="7"/>
       <c r="H96" s="19" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I96" s="20"/>
       <c r="J96" s="20"/>
@@ -3760,7 +3766,7 @@
       <c r="F97" s="41"/>
       <c r="G97" s="7"/>
       <c r="H97" s="19" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I97" s="20"/>
       <c r="J97" s="20"/>
@@ -3779,7 +3785,7 @@
       <c r="F98" s="20"/>
       <c r="G98" s="7"/>
       <c r="H98" s="19" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I98" s="20"/>
       <c r="J98" s="20"/>
@@ -3798,7 +3804,7 @@
       <c r="F99" s="20"/>
       <c r="G99" s="7"/>
       <c r="H99" s="19" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I99" s="20"/>
       <c r="J99" s="20"/>
@@ -3817,7 +3823,7 @@
       <c r="F100" s="29"/>
       <c r="G100" s="7"/>
       <c r="H100" s="19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I100" s="20"/>
       <c r="J100" s="20"/>
@@ -3846,7 +3852,7 @@
         <v>96</v>
       </c>
       <c r="C102" s="56" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D102" s="14" t="s">
         <v>1</v>
@@ -3859,10 +3865,10 @@
       </c>
       <c r="G102" s="7"/>
       <c r="H102" s="13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I102" s="56" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J102" s="14" t="s">
         <v>1</v>
@@ -3886,7 +3892,7 @@
       <c r="F103" s="20"/>
       <c r="G103" s="7"/>
       <c r="H103" s="19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I103" s="20"/>
       <c r="J103" s="20"/>
@@ -3905,7 +3911,7 @@
       <c r="F104" s="20"/>
       <c r="G104" s="7"/>
       <c r="H104" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I104" s="20"/>
       <c r="J104" s="20"/>
@@ -3924,7 +3930,7 @@
       <c r="F105" s="20"/>
       <c r="G105" s="7"/>
       <c r="H105" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I105" s="20"/>
       <c r="J105" s="20"/>
@@ -3943,7 +3949,7 @@
       <c r="F106" s="20"/>
       <c r="G106" s="7"/>
       <c r="H106" s="19" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I106" s="20"/>
       <c r="J106" s="20"/>
@@ -3962,7 +3968,7 @@
       <c r="F107" s="20"/>
       <c r="G107" s="7"/>
       <c r="H107" s="19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I107" s="20"/>
       <c r="J107" s="20"/>
@@ -3981,7 +3987,7 @@
       <c r="F108" s="20"/>
       <c r="G108" s="7"/>
       <c r="H108" s="19" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I108" s="20"/>
       <c r="J108" s="20"/>
@@ -4000,7 +4006,7 @@
       <c r="F109" s="20"/>
       <c r="G109" s="7"/>
       <c r="H109" s="19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I109" s="20"/>
       <c r="J109" s="20"/>
@@ -4019,7 +4025,7 @@
       <c r="F110" s="20"/>
       <c r="G110" s="7"/>
       <c r="H110" s="19" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I110" s="20"/>
       <c r="J110" s="20"/>
@@ -4038,7 +4044,7 @@
       <c r="F111" s="20"/>
       <c r="G111" s="7"/>
       <c r="H111" s="19" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I111" s="20"/>
       <c r="J111" s="20"/>
@@ -4057,7 +4063,7 @@
       <c r="F112" s="20"/>
       <c r="G112" s="7"/>
       <c r="H112" s="19" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I112" s="20"/>
       <c r="J112" s="20"/>
@@ -4076,7 +4082,7 @@
       <c r="F113" s="20"/>
       <c r="G113" s="7"/>
       <c r="H113" s="19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I113" s="20"/>
       <c r="J113" s="20"/>
@@ -4095,7 +4101,7 @@
       <c r="F114" s="39"/>
       <c r="G114" s="7"/>
       <c r="H114" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I114" s="20"/>
       <c r="J114" s="20"/>
@@ -4114,7 +4120,7 @@
       <c r="F115" s="20"/>
       <c r="G115" s="7"/>
       <c r="H115" s="19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I115" s="20"/>
       <c r="J115" s="20"/>
@@ -4133,7 +4139,7 @@
       <c r="F116" s="20"/>
       <c r="G116" s="7"/>
       <c r="H116" s="19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I116" s="20"/>
       <c r="J116" s="20"/>
@@ -4152,7 +4158,7 @@
       <c r="F117" s="20"/>
       <c r="G117" s="7"/>
       <c r="H117" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I117" s="20"/>
       <c r="J117" s="20"/>
@@ -4171,7 +4177,7 @@
       <c r="F118" s="20"/>
       <c r="G118" s="7"/>
       <c r="H118" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I118" s="20"/>
       <c r="J118" s="20"/>
@@ -4190,7 +4196,7 @@
       <c r="F119" s="20"/>
       <c r="G119" s="7"/>
       <c r="H119" s="19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I119" s="20"/>
       <c r="J119" s="20"/>
@@ -4209,7 +4215,7 @@
       <c r="F120" s="20"/>
       <c r="G120" s="7"/>
       <c r="H120" s="19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I120" s="20"/>
       <c r="J120" s="20"/>
@@ -4228,7 +4234,7 @@
       <c r="F121" s="20"/>
       <c r="G121" s="7"/>
       <c r="H121" s="19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I121" s="20"/>
       <c r="J121" s="20"/>
@@ -4247,7 +4253,7 @@
       <c r="F122" s="20"/>
       <c r="G122" s="7"/>
       <c r="H122" s="19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I122" s="20"/>
       <c r="J122" s="20"/>
@@ -4266,7 +4272,7 @@
       <c r="F123" s="20"/>
       <c r="G123" s="7"/>
       <c r="H123" s="19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I123" s="20"/>
       <c r="J123" s="20"/>
@@ -4285,7 +4291,7 @@
       <c r="F124" s="20"/>
       <c r="G124" s="7"/>
       <c r="H124" s="19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I124" s="20"/>
       <c r="J124" s="20"/>
@@ -4304,7 +4310,7 @@
       <c r="F125" s="39"/>
       <c r="G125" s="7"/>
       <c r="H125" s="19" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I125" s="20"/>
       <c r="J125" s="20"/>
@@ -4323,7 +4329,7 @@
       <c r="F126" s="20"/>
       <c r="G126" s="7"/>
       <c r="H126" s="19" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I126" s="20"/>
       <c r="J126" s="20"/>
@@ -4342,7 +4348,7 @@
       <c r="F127" s="20"/>
       <c r="G127" s="7"/>
       <c r="H127" s="19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I127" s="20"/>
       <c r="J127" s="20"/>
@@ -4361,7 +4367,7 @@
       <c r="F128" s="41"/>
       <c r="G128" s="7"/>
       <c r="H128" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I128" s="20"/>
       <c r="J128" s="20"/>
@@ -4380,7 +4386,7 @@
       <c r="F129" s="20"/>
       <c r="G129" s="7"/>
       <c r="H129" s="19" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I129" s="20"/>
       <c r="J129" s="20"/>
@@ -4399,7 +4405,7 @@
       <c r="F130" s="20"/>
       <c r="G130" s="7"/>
       <c r="H130" s="19" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I130" s="20"/>
       <c r="J130" s="20"/>
@@ -4583,7 +4589,7 @@
         <v>134</v>
       </c>
       <c r="C141" s="56" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D141" s="14" t="s">
         <v>1</v>
@@ -4849,29 +4855,29 @@
     <row r="2" spans="1:8" ht="37.5" customHeight="1" thickBot="1">
       <c r="A2" s="4"/>
       <c r="B2" s="44" t="s">
+        <v>231</v>
+      </c>
+      <c r="C2" s="45" t="s">
         <v>232</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="D2" s="45" t="s">
         <v>233</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="E2" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="E2" s="45" t="s">
+      <c r="F2" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="F2" s="45" t="s">
+      <c r="G2" s="45" t="s">
         <v>236</v>
-      </c>
-      <c r="G2" s="45" t="s">
-        <v>237</v>
       </c>
       <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1">
       <c r="A3" s="4"/>
       <c r="B3" s="51" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -4883,7 +4889,7 @@
     <row r="4" spans="1:8" ht="15.75" thickBot="1">
       <c r="A4" s="4"/>
       <c r="B4" s="51" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -4895,7 +4901,7 @@
     <row r="5" spans="1:8" ht="15.75" thickBot="1">
       <c r="A5" s="4"/>
       <c r="B5" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -4907,7 +4913,7 @@
     <row r="6" spans="1:8" ht="15.75" thickBot="1">
       <c r="A6" s="4"/>
       <c r="B6" s="52" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C6" s="54"/>
       <c r="D6" s="54"/>
@@ -4919,7 +4925,7 @@
     <row r="7" spans="1:8" ht="15.75" thickBot="1">
       <c r="A7" s="4"/>
       <c r="B7" s="53" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C7" s="54"/>
       <c r="D7" s="54"/>
@@ -4941,29 +4947,29 @@
     <row r="9" spans="1:8" ht="30.75" customHeight="1" thickBot="1">
       <c r="A9" s="4"/>
       <c r="B9" s="44" t="s">
+        <v>243</v>
+      </c>
+      <c r="C9" s="45" t="s">
         <v>244</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="D9" s="45" t="s">
         <v>245</v>
       </c>
-      <c r="D9" s="45" t="s">
+      <c r="E9" s="45" t="s">
         <v>246</v>
       </c>
-      <c r="E9" s="45" t="s">
+      <c r="F9" s="45" t="s">
         <v>247</v>
       </c>
-      <c r="F9" s="45" t="s">
+      <c r="G9" s="45" t="s">
         <v>248</v>
-      </c>
-      <c r="G9" s="45" t="s">
-        <v>249</v>
       </c>
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1">
       <c r="A10" s="4"/>
       <c r="B10" s="51" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -4975,7 +4981,7 @@
     <row r="11" spans="1:8" ht="15.75" thickBot="1">
       <c r="A11" s="4"/>
       <c r="B11" s="51" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -4987,7 +4993,7 @@
     <row r="12" spans="1:8" ht="15.75" thickBot="1">
       <c r="A12" s="4"/>
       <c r="B12" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -4999,7 +5005,7 @@
     <row r="13" spans="1:8" ht="15.75" thickBot="1">
       <c r="A13" s="4"/>
       <c r="B13" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -5011,7 +5017,7 @@
     <row r="14" spans="1:8" ht="15.75" thickBot="1">
       <c r="A14" s="4"/>
       <c r="B14" s="57" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -5033,29 +5039,29 @@
     <row r="16" spans="1:8" ht="27" thickBot="1">
       <c r="A16" s="4"/>
       <c r="B16" s="44" t="s">
+        <v>249</v>
+      </c>
+      <c r="C16" s="45" t="s">
         <v>250</v>
       </c>
-      <c r="C16" s="45" t="s">
+      <c r="D16" s="45" t="s">
         <v>251</v>
       </c>
-      <c r="D16" s="45" t="s">
+      <c r="E16" s="45" t="s">
         <v>252</v>
       </c>
-      <c r="E16" s="45" t="s">
+      <c r="F16" s="45" t="s">
         <v>253</v>
       </c>
-      <c r="F16" s="45" t="s">
+      <c r="G16" s="45" t="s">
         <v>254</v>
-      </c>
-      <c r="G16" s="45" t="s">
-        <v>255</v>
       </c>
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" thickBot="1">
       <c r="A17" s="4"/>
       <c r="B17" s="51" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -5067,7 +5073,7 @@
     <row r="18" spans="1:8" ht="15.75" thickBot="1">
       <c r="A18" s="4"/>
       <c r="B18" s="51" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -5079,7 +5085,7 @@
     <row r="19" spans="1:8" ht="15.75" thickBot="1">
       <c r="A19" s="4"/>
       <c r="B19" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -5091,7 +5097,7 @@
     <row r="20" spans="1:8" ht="15.75" thickBot="1">
       <c r="A20" s="4"/>
       <c r="B20" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -5103,7 +5109,7 @@
     <row r="21" spans="1:8" ht="15.75" thickBot="1">
       <c r="A21" s="4"/>
       <c r="B21" s="57" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -5125,29 +5131,29 @@
     <row r="23" spans="1:8" ht="45" customHeight="1" thickBot="1">
       <c r="A23" s="4"/>
       <c r="B23" s="44" t="s">
+        <v>255</v>
+      </c>
+      <c r="C23" s="45" t="s">
         <v>256</v>
       </c>
-      <c r="C23" s="45" t="s">
+      <c r="D23" s="45" t="s">
         <v>257</v>
       </c>
-      <c r="D23" s="45" t="s">
+      <c r="E23" s="45" t="s">
         <v>258</v>
       </c>
-      <c r="E23" s="45" t="s">
+      <c r="F23" s="45" t="s">
         <v>259</v>
       </c>
-      <c r="F23" s="45" t="s">
+      <c r="G23" s="45" t="s">
         <v>260</v>
-      </c>
-      <c r="G23" s="45" t="s">
-        <v>261</v>
       </c>
       <c r="H23" s="4"/>
     </row>
     <row r="24" spans="1:8" ht="15.75" thickBot="1">
       <c r="A24" s="4"/>
       <c r="B24" s="51" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -5159,7 +5165,7 @@
     <row r="25" spans="1:8" ht="15.75" thickBot="1">
       <c r="A25" s="4"/>
       <c r="B25" s="51" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -5171,7 +5177,7 @@
     <row r="26" spans="1:8" ht="15.75" thickBot="1">
       <c r="A26" s="4"/>
       <c r="B26" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -5183,7 +5189,7 @@
     <row r="27" spans="1:8" ht="15.75" thickBot="1">
       <c r="A27" s="4"/>
       <c r="B27" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -5195,7 +5201,7 @@
     <row r="28" spans="1:8" ht="15.75" thickBot="1">
       <c r="A28" s="4"/>
       <c r="B28" s="57" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -5217,29 +5223,29 @@
     <row r="30" spans="1:8" ht="39.75" thickBot="1">
       <c r="A30" s="4"/>
       <c r="B30" s="44" t="s">
+        <v>261</v>
+      </c>
+      <c r="C30" s="45" t="s">
         <v>262</v>
       </c>
-      <c r="C30" s="45" t="s">
+      <c r="D30" s="45" t="s">
         <v>263</v>
       </c>
-      <c r="D30" s="45" t="s">
+      <c r="E30" s="45" t="s">
         <v>264</v>
       </c>
-      <c r="E30" s="45" t="s">
+      <c r="F30" s="45" t="s">
         <v>265</v>
       </c>
-      <c r="F30" s="45" t="s">
+      <c r="G30" s="45" t="s">
         <v>266</v>
-      </c>
-      <c r="G30" s="45" t="s">
-        <v>267</v>
       </c>
       <c r="H30" s="4"/>
     </row>
     <row r="31" spans="1:8" ht="15.75" thickBot="1">
       <c r="A31" s="4"/>
       <c r="B31" s="51" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -5251,7 +5257,7 @@
     <row r="32" spans="1:8" ht="15.75" thickBot="1">
       <c r="A32" s="4"/>
       <c r="B32" s="51" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -5263,7 +5269,7 @@
     <row r="33" spans="1:8" ht="15.75" thickBot="1">
       <c r="A33" s="4"/>
       <c r="B33" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
@@ -5275,7 +5281,7 @@
     <row r="34" spans="1:8" ht="15.75" thickBot="1">
       <c r="A34" s="4"/>
       <c r="B34" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -5287,7 +5293,7 @@
     <row r="35" spans="1:8" ht="15.75" thickBot="1">
       <c r="A35" s="4"/>
       <c r="B35" s="57" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -5309,29 +5315,29 @@
     <row r="37" spans="1:8" ht="35.25" thickBot="1">
       <c r="A37" s="4"/>
       <c r="B37" s="44" t="s">
+        <v>267</v>
+      </c>
+      <c r="C37" s="45" t="s">
         <v>268</v>
       </c>
-      <c r="C37" s="45" t="s">
+      <c r="D37" s="45" t="s">
         <v>269</v>
       </c>
-      <c r="D37" s="45" t="s">
+      <c r="E37" s="45" t="s">
         <v>270</v>
       </c>
-      <c r="E37" s="45" t="s">
+      <c r="F37" s="45" t="s">
         <v>271</v>
       </c>
-      <c r="F37" s="45" t="s">
+      <c r="G37" s="45" t="s">
         <v>272</v>
-      </c>
-      <c r="G37" s="45" t="s">
-        <v>273</v>
       </c>
       <c r="H37" s="4"/>
     </row>
     <row r="38" spans="1:8" ht="15.75" thickBot="1">
       <c r="A38" s="4"/>
       <c r="B38" s="51" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -5343,7 +5349,7 @@
     <row r="39" spans="1:8" ht="15.75" thickBot="1">
       <c r="A39" s="4"/>
       <c r="B39" s="51" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -5355,7 +5361,7 @@
     <row r="40" spans="1:8" ht="15.75" thickBot="1">
       <c r="A40" s="4"/>
       <c r="B40" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -5367,7 +5373,7 @@
     <row r="41" spans="1:8" ht="15.75" thickBot="1">
       <c r="A41" s="4"/>
       <c r="B41" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
@@ -5379,7 +5385,7 @@
     <row r="42" spans="1:8" ht="15.75" thickBot="1">
       <c r="A42" s="4"/>
       <c r="B42" s="57" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -5401,29 +5407,29 @@
     <row r="44" spans="1:8" ht="39.75" thickBot="1">
       <c r="A44" s="4"/>
       <c r="B44" s="44" t="s">
+        <v>273</v>
+      </c>
+      <c r="C44" s="45" t="s">
         <v>274</v>
       </c>
-      <c r="C44" s="45" t="s">
+      <c r="D44" s="45" t="s">
         <v>275</v>
       </c>
-      <c r="D44" s="45" t="s">
+      <c r="E44" s="45" t="s">
         <v>276</v>
       </c>
-      <c r="E44" s="45" t="s">
+      <c r="F44" s="45" t="s">
         <v>277</v>
       </c>
-      <c r="F44" s="45" t="s">
+      <c r="G44" s="45" t="s">
         <v>278</v>
-      </c>
-      <c r="G44" s="45" t="s">
-        <v>279</v>
       </c>
       <c r="H44" s="4"/>
     </row>
     <row r="45" spans="1:8" ht="15.75" thickBot="1">
       <c r="A45" s="4"/>
       <c r="B45" s="51" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -5435,7 +5441,7 @@
     <row r="46" spans="1:8" ht="15.75" thickBot="1">
       <c r="A46" s="4"/>
       <c r="B46" s="51" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -5447,7 +5453,7 @@
     <row r="47" spans="1:8" ht="15" customHeight="1" thickBot="1">
       <c r="A47" s="4"/>
       <c r="B47" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
@@ -5459,7 +5465,7 @@
     <row r="48" spans="1:8" ht="15.75" thickBot="1">
       <c r="A48" s="4"/>
       <c r="B48" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
@@ -5471,7 +5477,7 @@
     <row r="49" spans="1:8" ht="15.75" thickBot="1">
       <c r="A49" s="4"/>
       <c r="B49" s="57" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -5493,19 +5499,19 @@
     <row r="51" spans="1:8" ht="39.75" thickBot="1">
       <c r="A51" s="4"/>
       <c r="B51" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="C51" s="45" t="s">
         <v>280</v>
       </c>
-      <c r="C51" s="45" t="s">
+      <c r="D51" s="45" t="s">
         <v>281</v>
       </c>
-      <c r="D51" s="45" t="s">
+      <c r="E51" s="45" t="s">
         <v>282</v>
       </c>
-      <c r="E51" s="45" t="s">
+      <c r="F51" s="45" t="s">
         <v>283</v>
-      </c>
-      <c r="F51" s="45" t="s">
-        <v>284</v>
       </c>
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
@@ -5513,7 +5519,7 @@
     <row r="52" spans="1:8" ht="15.75" thickBot="1">
       <c r="A52" s="4"/>
       <c r="B52" s="51" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
@@ -5525,7 +5531,7 @@
     <row r="53" spans="1:8" ht="15.75" thickBot="1">
       <c r="A53" s="4"/>
       <c r="B53" s="51" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
@@ -5537,7 +5543,7 @@
     <row r="54" spans="1:8" ht="15.75" thickBot="1">
       <c r="A54" s="4"/>
       <c r="B54" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
@@ -5549,7 +5555,7 @@
     <row r="55" spans="1:8" ht="15.75" thickBot="1">
       <c r="A55" s="4"/>
       <c r="B55" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
@@ -5561,7 +5567,7 @@
     <row r="56" spans="1:8" ht="15.75" thickBot="1">
       <c r="A56" s="4"/>
       <c r="B56" s="57" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -5589,8 +5595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q190"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="E91" workbookViewId="0">
+      <selection activeCell="H96" sqref="H96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5685,7 +5691,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="59" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>1</v>
@@ -5701,7 +5707,7 @@
         <v>146</v>
       </c>
       <c r="I5" s="59" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J5" s="14" t="s">
         <v>1</v>
@@ -5964,7 +5970,7 @@
     <row r="19" spans="1:13" ht="15.75" thickBot="1">
       <c r="A19" s="58"/>
       <c r="B19" s="19" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C19" s="20"/>
       <c r="D19" s="20"/>
@@ -6117,7 +6123,7 @@
         <v>23</v>
       </c>
       <c r="C27" s="59" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D27" s="26" t="s">
         <v>1</v>
@@ -6248,7 +6254,7 @@
         <v>29</v>
       </c>
       <c r="C34" s="59" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D34" s="26" t="s">
         <v>1</v>
@@ -6375,7 +6381,7 @@
         <v>35</v>
       </c>
       <c r="C41" s="59" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>1</v>
@@ -6500,7 +6506,7 @@
         <v>41</v>
       </c>
       <c r="C48" s="59" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D48" s="14" t="s">
         <v>1</v>
@@ -6964,7 +6970,7 @@
         <v>175</v>
       </c>
       <c r="I74" s="59" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J74" s="14" t="s">
         <v>1</v>
@@ -7368,7 +7374,7 @@
       <c r="F95" s="20"/>
       <c r="G95" s="58"/>
       <c r="H95" s="19" t="s">
-        <v>196</v>
+        <v>322</v>
       </c>
       <c r="I95" s="20"/>
       <c r="J95" s="20"/>
@@ -7387,7 +7393,7 @@
       <c r="F96" s="20"/>
       <c r="G96" s="58"/>
       <c r="H96" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I96" s="20"/>
       <c r="J96" s="20"/>
@@ -7398,7 +7404,7 @@
     <row r="97" spans="1:13" ht="15.75" thickBot="1">
       <c r="A97" s="58"/>
       <c r="B97" s="19" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C97" s="20"/>
       <c r="D97" s="20"/>
@@ -7406,7 +7412,7 @@
       <c r="F97" s="20"/>
       <c r="G97" s="58"/>
       <c r="H97" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I97" s="20"/>
       <c r="J97" s="20"/>
@@ -7444,7 +7450,7 @@
       <c r="F99" s="20"/>
       <c r="G99" s="58"/>
       <c r="H99" s="19" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I99" s="20"/>
       <c r="J99" s="20"/>
@@ -7463,7 +7469,7 @@
       <c r="F100" s="41"/>
       <c r="G100" s="58"/>
       <c r="H100" s="19" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I100" s="20"/>
       <c r="J100" s="20"/>
@@ -7482,7 +7488,7 @@
       <c r="F101" s="20"/>
       <c r="G101" s="58"/>
       <c r="H101" s="19" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I101" s="20"/>
       <c r="J101" s="20"/>
@@ -7501,7 +7507,7 @@
       <c r="F102" s="20"/>
       <c r="G102" s="58"/>
       <c r="H102" s="19" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I102" s="20"/>
       <c r="J102" s="20"/>
@@ -7520,7 +7526,7 @@
       <c r="F103" s="62"/>
       <c r="G103" s="58"/>
       <c r="H103" s="19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I103" s="20"/>
       <c r="J103" s="20"/>
@@ -7549,7 +7555,7 @@
         <v>96</v>
       </c>
       <c r="C105" s="59" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D105" s="14" t="s">
         <v>1</v>
@@ -7562,10 +7568,10 @@
       </c>
       <c r="G105" s="58"/>
       <c r="H105" s="13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I105" s="59" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J105" s="14" t="s">
         <v>1</v>
@@ -7589,7 +7595,7 @@
       <c r="F106" s="20"/>
       <c r="G106" s="58"/>
       <c r="H106" s="19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I106" s="20"/>
       <c r="J106" s="20"/>
@@ -7608,7 +7614,7 @@
       <c r="F107" s="20"/>
       <c r="G107" s="58"/>
       <c r="H107" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I107" s="20"/>
       <c r="J107" s="20"/>
@@ -7627,7 +7633,7 @@
       <c r="F108" s="20"/>
       <c r="G108" s="58"/>
       <c r="H108" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I108" s="20"/>
       <c r="J108" s="20"/>
@@ -7646,7 +7652,7 @@
       <c r="F109" s="20"/>
       <c r="G109" s="58"/>
       <c r="H109" s="19" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I109" s="20"/>
       <c r="J109" s="20"/>
@@ -7665,7 +7671,7 @@
       <c r="F110" s="20"/>
       <c r="G110" s="58"/>
       <c r="H110" s="19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I110" s="20"/>
       <c r="J110" s="20"/>
@@ -7684,7 +7690,7 @@
       <c r="F111" s="20"/>
       <c r="G111" s="58"/>
       <c r="H111" s="19" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I111" s="20"/>
       <c r="J111" s="20"/>
@@ -7703,7 +7709,7 @@
       <c r="F112" s="20"/>
       <c r="G112" s="58"/>
       <c r="H112" s="19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I112" s="20"/>
       <c r="J112" s="20"/>
@@ -7722,7 +7728,7 @@
       <c r="F113" s="20"/>
       <c r="G113" s="58"/>
       <c r="H113" s="19" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I113" s="20"/>
       <c r="J113" s="20"/>
@@ -7741,7 +7747,7 @@
       <c r="F114" s="20"/>
       <c r="G114" s="58"/>
       <c r="H114" s="19" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I114" s="20"/>
       <c r="J114" s="20"/>
@@ -7760,7 +7766,7 @@
       <c r="F115" s="20"/>
       <c r="G115" s="58"/>
       <c r="H115" s="19" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I115" s="20"/>
       <c r="J115" s="20"/>
@@ -7779,7 +7785,7 @@
       <c r="F116" s="20"/>
       <c r="G116" s="58"/>
       <c r="H116" s="19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I116" s="20"/>
       <c r="J116" s="20"/>
@@ -7798,7 +7804,7 @@
       <c r="F117" s="39"/>
       <c r="G117" s="58"/>
       <c r="H117" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I117" s="20"/>
       <c r="J117" s="20"/>
@@ -7817,7 +7823,7 @@
       <c r="F118" s="20"/>
       <c r="G118" s="58"/>
       <c r="H118" s="19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I118" s="20"/>
       <c r="J118" s="20"/>
@@ -7836,7 +7842,7 @@
       <c r="F119" s="20"/>
       <c r="G119" s="58"/>
       <c r="H119" s="19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I119" s="20"/>
       <c r="J119" s="20"/>
@@ -7855,7 +7861,7 @@
       <c r="F120" s="20"/>
       <c r="G120" s="58"/>
       <c r="H120" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I120" s="20"/>
       <c r="J120" s="20"/>
@@ -7874,7 +7880,7 @@
       <c r="F121" s="20"/>
       <c r="G121" s="58"/>
       <c r="H121" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I121" s="20"/>
       <c r="J121" s="20"/>
@@ -7893,7 +7899,7 @@
       <c r="F122" s="20"/>
       <c r="G122" s="58"/>
       <c r="H122" s="19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I122" s="20"/>
       <c r="J122" s="20"/>
@@ -7912,7 +7918,7 @@
       <c r="F123" s="20"/>
       <c r="G123" s="58"/>
       <c r="H123" s="19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I123" s="20"/>
       <c r="J123" s="20"/>
@@ -7931,7 +7937,7 @@
       <c r="F124" s="20"/>
       <c r="G124" s="58"/>
       <c r="H124" s="19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I124" s="20"/>
       <c r="J124" s="20"/>
@@ -7950,7 +7956,7 @@
       <c r="F125" s="20"/>
       <c r="G125" s="58"/>
       <c r="H125" s="19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I125" s="20"/>
       <c r="J125" s="20"/>
@@ -7969,7 +7975,7 @@
       <c r="F126" s="20"/>
       <c r="G126" s="58"/>
       <c r="H126" s="19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I126" s="20"/>
       <c r="J126" s="20"/>
@@ -7988,7 +7994,7 @@
       <c r="F127" s="20"/>
       <c r="G127" s="58"/>
       <c r="H127" s="19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I127" s="20"/>
       <c r="J127" s="20"/>
@@ -8007,7 +8013,7 @@
       <c r="F128" s="39"/>
       <c r="G128" s="58"/>
       <c r="H128" s="19" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I128" s="20"/>
       <c r="J128" s="20"/>
@@ -8026,7 +8032,7 @@
       <c r="F129" s="20"/>
       <c r="G129" s="58"/>
       <c r="H129" s="19" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I129" s="20"/>
       <c r="J129" s="20"/>
@@ -8045,7 +8051,7 @@
       <c r="F130" s="20"/>
       <c r="G130" s="58"/>
       <c r="H130" s="19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I130" s="20"/>
       <c r="J130" s="20"/>
@@ -8064,7 +8070,7 @@
       <c r="F131" s="41"/>
       <c r="G131" s="58"/>
       <c r="H131" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I131" s="20"/>
       <c r="J131" s="20"/>
@@ -8083,7 +8089,7 @@
       <c r="F132" s="20"/>
       <c r="G132" s="58"/>
       <c r="H132" s="19" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I132" s="20"/>
       <c r="J132" s="20"/>
@@ -8102,7 +8108,7 @@
       <c r="F133" s="20"/>
       <c r="G133" s="58"/>
       <c r="H133" s="19" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I133" s="20"/>
       <c r="J133" s="20"/>
@@ -8139,22 +8145,22 @@
       <c r="F135" s="20"/>
       <c r="G135" s="4"/>
       <c r="H135" s="44" t="s">
+        <v>231</v>
+      </c>
+      <c r="I135" s="45" t="s">
         <v>232</v>
       </c>
-      <c r="I135" s="45" t="s">
+      <c r="J135" s="45" t="s">
         <v>233</v>
       </c>
-      <c r="J135" s="45" t="s">
+      <c r="K135" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="K135" s="45" t="s">
+      <c r="L135" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="L135" s="45" t="s">
+      <c r="M135" s="45" t="s">
         <v>236</v>
-      </c>
-      <c r="M135" s="45" t="s">
-        <v>237</v>
       </c>
       <c r="N135" s="4"/>
     </row>
@@ -8169,7 +8175,7 @@
       <c r="F136" s="40"/>
       <c r="G136" s="4"/>
       <c r="H136" s="51" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I136" s="3"/>
       <c r="J136" s="3"/>
@@ -8189,7 +8195,7 @@
       <c r="F137" s="20"/>
       <c r="G137" s="4"/>
       <c r="H137" s="51" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I137" s="3"/>
       <c r="J137" s="3"/>
@@ -8209,7 +8215,7 @@
       <c r="F138" s="20"/>
       <c r="G138" s="4"/>
       <c r="H138" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I138" s="3"/>
       <c r="J138" s="3"/>
@@ -8229,7 +8235,7 @@
       <c r="F139" s="20"/>
       <c r="G139" s="4"/>
       <c r="H139" s="52" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I139" s="54"/>
       <c r="J139" s="54"/>
@@ -8249,7 +8255,7 @@
       <c r="F140" s="20"/>
       <c r="G140" s="4"/>
       <c r="H140" s="53" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I140" s="54"/>
       <c r="J140" s="54"/>
@@ -8287,22 +8293,22 @@
       <c r="F142" s="62"/>
       <c r="G142" s="4"/>
       <c r="H142" s="44" t="s">
+        <v>243</v>
+      </c>
+      <c r="I142" s="45" t="s">
         <v>244</v>
       </c>
-      <c r="I142" s="45" t="s">
+      <c r="J142" s="45" t="s">
         <v>245</v>
       </c>
-      <c r="J142" s="45" t="s">
+      <c r="K142" s="45" t="s">
         <v>246</v>
       </c>
-      <c r="K142" s="45" t="s">
+      <c r="L142" s="45" t="s">
         <v>247</v>
       </c>
-      <c r="L142" s="45" t="s">
+      <c r="M142" s="45" t="s">
         <v>248</v>
-      </c>
-      <c r="M142" s="45" t="s">
-        <v>249</v>
       </c>
       <c r="N142" s="4"/>
     </row>
@@ -8315,7 +8321,7 @@
       <c r="F143" s="58"/>
       <c r="G143" s="4"/>
       <c r="H143" s="51" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I143" s="3"/>
       <c r="J143" s="3"/>
@@ -8330,7 +8336,7 @@
         <v>134</v>
       </c>
       <c r="C144" s="59" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D144" s="14" t="s">
         <v>1</v>
@@ -8343,7 +8349,7 @@
       </c>
       <c r="G144" s="4"/>
       <c r="H144" s="51" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I144" s="3"/>
       <c r="J144" s="3"/>
@@ -8363,7 +8369,7 @@
       <c r="F145" s="20"/>
       <c r="G145" s="4"/>
       <c r="H145" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I145" s="3"/>
       <c r="J145" s="3"/>
@@ -8383,7 +8389,7 @@
       <c r="F146" s="20"/>
       <c r="G146" s="4"/>
       <c r="H146" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I146" s="3"/>
       <c r="J146" s="3"/>
@@ -8403,7 +8409,7 @@
       <c r="F147" s="20"/>
       <c r="G147" s="4"/>
       <c r="H147" s="57" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I147" s="2"/>
       <c r="J147" s="2"/>
@@ -8441,22 +8447,22 @@
       <c r="F149" s="20"/>
       <c r="G149" s="4"/>
       <c r="H149" s="44" t="s">
+        <v>249</v>
+      </c>
+      <c r="I149" s="45" t="s">
         <v>250</v>
       </c>
-      <c r="I149" s="45" t="s">
+      <c r="J149" s="45" t="s">
         <v>251</v>
       </c>
-      <c r="J149" s="45" t="s">
+      <c r="K149" s="45" t="s">
         <v>252</v>
       </c>
-      <c r="K149" s="45" t="s">
+      <c r="L149" s="45" t="s">
         <v>253</v>
       </c>
-      <c r="L149" s="45" t="s">
+      <c r="M149" s="45" t="s">
         <v>254</v>
-      </c>
-      <c r="M149" s="45" t="s">
-        <v>255</v>
       </c>
       <c r="N149" s="4"/>
     </row>
@@ -8471,7 +8477,7 @@
       <c r="F150" s="20"/>
       <c r="G150" s="4"/>
       <c r="H150" s="51" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I150" s="3"/>
       <c r="J150" s="3"/>
@@ -8491,7 +8497,7 @@
       <c r="F151" s="20"/>
       <c r="G151" s="4"/>
       <c r="H151" s="51" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I151" s="3"/>
       <c r="J151" s="3"/>
@@ -8511,7 +8517,7 @@
       <c r="F152" s="20"/>
       <c r="G152" s="4"/>
       <c r="H152" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I152" s="3"/>
       <c r="J152" s="3"/>
@@ -8531,7 +8537,7 @@
       <c r="F153" s="20"/>
       <c r="G153" s="4"/>
       <c r="H153" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I153" s="3"/>
       <c r="J153" s="3"/>
@@ -8551,7 +8557,7 @@
       <c r="F154" s="20"/>
       <c r="G154" s="4"/>
       <c r="H154" s="57" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I154" s="2"/>
       <c r="J154" s="2"/>
@@ -8587,47 +8593,47 @@
       <c r="F156" s="58"/>
       <c r="G156" s="4"/>
       <c r="H156" s="44" t="s">
+        <v>255</v>
+      </c>
+      <c r="I156" s="45" t="s">
         <v>256</v>
       </c>
-      <c r="I156" s="45" t="s">
+      <c r="J156" s="45" t="s">
         <v>257</v>
       </c>
-      <c r="J156" s="45" t="s">
+      <c r="K156" s="45" t="s">
         <v>258</v>
       </c>
-      <c r="K156" s="45" t="s">
+      <c r="L156" s="45" t="s">
         <v>259</v>
       </c>
-      <c r="L156" s="45" t="s">
+      <c r="M156" s="45" t="s">
         <v>260</v>
-      </c>
-      <c r="M156" s="45" t="s">
-        <v>261</v>
       </c>
       <c r="N156" s="4"/>
     </row>
     <row r="157" spans="1:14" ht="39.75" thickBot="1">
       <c r="A157" s="44" t="s">
+        <v>267</v>
+      </c>
+      <c r="B157" s="45" t="s">
         <v>268</v>
       </c>
-      <c r="B157" s="45" t="s">
+      <c r="C157" s="45" t="s">
         <v>269</v>
       </c>
-      <c r="C157" s="45" t="s">
+      <c r="D157" s="45" t="s">
         <v>270</v>
       </c>
-      <c r="D157" s="45" t="s">
+      <c r="E157" s="45" t="s">
         <v>271</v>
       </c>
-      <c r="E157" s="45" t="s">
+      <c r="F157" s="45" t="s">
         <v>272</v>
-      </c>
-      <c r="F157" s="45" t="s">
-        <v>273</v>
       </c>
       <c r="G157" s="4"/>
       <c r="H157" s="51" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I157" s="3"/>
       <c r="J157" s="3"/>
@@ -8638,7 +8644,7 @@
     </row>
     <row r="158" spans="1:14" ht="15.75" thickBot="1">
       <c r="A158" s="51" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B158" s="3"/>
       <c r="C158" s="3"/>
@@ -8647,7 +8653,7 @@
       <c r="F158" s="3"/>
       <c r="G158" s="4"/>
       <c r="H158" s="51" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I158" s="3"/>
       <c r="J158" s="3"/>
@@ -8658,7 +8664,7 @@
     </row>
     <row r="159" spans="1:14" ht="15.75" thickBot="1">
       <c r="A159" s="51" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B159" s="3"/>
       <c r="C159" s="3"/>
@@ -8667,7 +8673,7 @@
       <c r="F159" s="3"/>
       <c r="G159" s="4"/>
       <c r="H159" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I159" s="3"/>
       <c r="J159" s="3"/>
@@ -8678,7 +8684,7 @@
     </row>
     <row r="160" spans="1:14" ht="15.75" thickBot="1">
       <c r="A160" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B160" s="3"/>
       <c r="C160" s="3"/>
@@ -8687,7 +8693,7 @@
       <c r="F160" s="3"/>
       <c r="G160" s="4"/>
       <c r="H160" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I160" s="3"/>
       <c r="J160" s="3"/>
@@ -8698,7 +8704,7 @@
     </row>
     <row r="161" spans="1:14" ht="15.75" thickBot="1">
       <c r="A161" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B161" s="3"/>
       <c r="C161" s="3"/>
@@ -8707,7 +8713,7 @@
       <c r="F161" s="3"/>
       <c r="G161" s="4"/>
       <c r="H161" s="57" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I161" s="2"/>
       <c r="J161" s="2"/>
@@ -8718,7 +8724,7 @@
     </row>
     <row r="162" spans="1:14" ht="15.75" thickBot="1">
       <c r="A162" s="57" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B162" s="2"/>
       <c r="C162" s="2"/>
@@ -8743,47 +8749,47 @@
       <c r="F163" s="4"/>
       <c r="G163" s="4"/>
       <c r="H163" s="44" t="s">
+        <v>261</v>
+      </c>
+      <c r="I163" s="45" t="s">
         <v>262</v>
       </c>
-      <c r="I163" s="45" t="s">
+      <c r="J163" s="45" t="s">
         <v>263</v>
       </c>
-      <c r="J163" s="45" t="s">
+      <c r="K163" s="45" t="s">
         <v>264</v>
       </c>
-      <c r="K163" s="45" t="s">
+      <c r="L163" s="45" t="s">
         <v>265</v>
       </c>
-      <c r="L163" s="45" t="s">
+      <c r="M163" s="45" t="s">
         <v>266</v>
-      </c>
-      <c r="M163" s="45" t="s">
-        <v>267</v>
       </c>
       <c r="N163" s="4"/>
     </row>
     <row r="164" spans="1:14" ht="52.5" thickBot="1">
       <c r="A164" s="44" t="s">
+        <v>273</v>
+      </c>
+      <c r="B164" s="45" t="s">
         <v>274</v>
       </c>
-      <c r="B164" s="45" t="s">
+      <c r="C164" s="45" t="s">
         <v>275</v>
       </c>
-      <c r="C164" s="45" t="s">
+      <c r="D164" s="45" t="s">
         <v>276</v>
       </c>
-      <c r="D164" s="45" t="s">
+      <c r="E164" s="45" t="s">
         <v>277</v>
       </c>
-      <c r="E164" s="45" t="s">
+      <c r="F164" s="45" t="s">
         <v>278</v>
-      </c>
-      <c r="F164" s="45" t="s">
-        <v>279</v>
       </c>
       <c r="G164" s="4"/>
       <c r="H164" s="51" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I164" s="3"/>
       <c r="J164" s="3"/>
@@ -8794,7 +8800,7 @@
     </row>
     <row r="165" spans="1:14" ht="15.75" thickBot="1">
       <c r="A165" s="51" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B165" s="3"/>
       <c r="C165" s="3"/>
@@ -8803,7 +8809,7 @@
       <c r="F165" s="3"/>
       <c r="G165" s="4"/>
       <c r="H165" s="51" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I165" s="3"/>
       <c r="J165" s="3"/>
@@ -8814,7 +8820,7 @@
     </row>
     <row r="166" spans="1:14" ht="15.75" thickBot="1">
       <c r="A166" s="51" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B166" s="3"/>
       <c r="C166" s="3"/>
@@ -8823,7 +8829,7 @@
       <c r="F166" s="3"/>
       <c r="G166" s="4"/>
       <c r="H166" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I166" s="3"/>
       <c r="J166" s="3"/>
@@ -8834,7 +8840,7 @@
     </row>
     <row r="167" spans="1:14" ht="15.75" thickBot="1">
       <c r="A167" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B167" s="3"/>
       <c r="C167" s="3"/>
@@ -8843,7 +8849,7 @@
       <c r="F167" s="3"/>
       <c r="G167" s="4"/>
       <c r="H167" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I167" s="3"/>
       <c r="J167" s="3"/>
@@ -8854,7 +8860,7 @@
     </row>
     <row r="168" spans="1:14" ht="15.75" thickBot="1">
       <c r="A168" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B168" s="3"/>
       <c r="C168" s="3"/>
@@ -8863,7 +8869,7 @@
       <c r="F168" s="3"/>
       <c r="G168" s="4"/>
       <c r="H168" s="57" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I168" s="2"/>
       <c r="J168" s="2"/>
@@ -8874,7 +8880,7 @@
     </row>
     <row r="169" spans="1:14" ht="15.75" thickBot="1">
       <c r="A169" s="57" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B169" s="2"/>
       <c r="C169" s="2"/>
@@ -8909,19 +8915,19 @@
     <row r="171" spans="1:14" ht="52.5" thickBot="1">
       <c r="A171" s="4"/>
       <c r="B171" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="C171" s="45" t="s">
         <v>280</v>
       </c>
-      <c r="C171" s="45" t="s">
+      <c r="D171" s="45" t="s">
         <v>281</v>
       </c>
-      <c r="D171" s="45" t="s">
+      <c r="E171" s="45" t="s">
         <v>282</v>
       </c>
-      <c r="E171" s="45" t="s">
+      <c r="F171" s="45" t="s">
         <v>283</v>
-      </c>
-      <c r="F171" s="45" t="s">
-        <v>284</v>
       </c>
       <c r="G171" s="4"/>
       <c r="H171" s="4"/>
@@ -8935,7 +8941,7 @@
     <row r="172" spans="1:14" ht="15.75" thickBot="1">
       <c r="A172" s="4"/>
       <c r="B172" s="51" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C172" s="3"/>
       <c r="D172" s="3"/>
@@ -8953,7 +8959,7 @@
     <row r="173" spans="1:14" ht="15.75" thickBot="1">
       <c r="A173" s="4"/>
       <c r="B173" s="51" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C173" s="3"/>
       <c r="D173" s="3"/>
@@ -8971,7 +8977,7 @@
     <row r="174" spans="1:14" ht="15.75" thickBot="1">
       <c r="A174" s="4"/>
       <c r="B174" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C174" s="3"/>
       <c r="D174" s="3"/>
@@ -8989,7 +8995,7 @@
     <row r="175" spans="1:14" ht="15.75" thickBot="1">
       <c r="A175" s="4"/>
       <c r="B175" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C175" s="3"/>
       <c r="D175" s="3"/>
@@ -9007,7 +9013,7 @@
     <row r="176" spans="1:14" ht="15.75" thickBot="1">
       <c r="A176" s="4"/>
       <c r="B176" s="57" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C176" s="2"/>
       <c r="D176" s="2"/>
@@ -9185,8 +9191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K89" sqref="K89"/>
+    <sheetView tabSelected="1" topLeftCell="G29" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9207,7 +9213,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="23.25" customHeight="1">
       <c r="A1" s="98" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B1" s="98"/>
       <c r="C1" s="98"/>
@@ -9243,7 +9249,7 @@
       <c r="N2" s="1"/>
       <c r="O2" s="69"/>
       <c r="P2" s="70" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="Q2" s="1"/>
     </row>
@@ -9283,7 +9289,7 @@
       <c r="N4" s="1"/>
       <c r="O4" s="71"/>
       <c r="P4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="Q4" s="1"/>
     </row>
@@ -9293,7 +9299,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="59" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>1</v>
@@ -9309,7 +9315,7 @@
         <v>146</v>
       </c>
       <c r="I5" s="59" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J5" s="14" t="s">
         <v>1</v>
@@ -9328,7 +9334,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="72" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D6" s="72"/>
       <c r="E6" s="73"/>
@@ -9386,7 +9392,7 @@
       <c r="B9" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="20"/>
+      <c r="C9" s="73"/>
       <c r="D9" s="73"/>
       <c r="E9" s="73"/>
       <c r="F9" s="20"/>
@@ -9413,7 +9419,7 @@
       <c r="H10" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="I10" s="20"/>
+      <c r="I10" s="73"/>
       <c r="J10" s="73"/>
       <c r="K10" s="73"/>
       <c r="L10" s="73"/>
@@ -9424,7 +9430,7 @@
       <c r="B11" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="20"/>
+      <c r="C11" s="73"/>
       <c r="D11" s="73"/>
       <c r="E11" s="73"/>
       <c r="F11" s="20"/>
@@ -9555,7 +9561,7 @@
     <row r="18" spans="1:13" ht="15.75" thickBot="1">
       <c r="A18" s="58"/>
       <c r="B18" s="19" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C18" s="72"/>
       <c r="D18" s="73"/>
@@ -9574,7 +9580,7 @@
     <row r="19" spans="1:13" ht="15.75" thickBot="1">
       <c r="A19" s="58"/>
       <c r="B19" s="19" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C19" s="20"/>
       <c r="D19" s="73"/>
@@ -9727,7 +9733,7 @@
         <v>23</v>
       </c>
       <c r="C27" s="59" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D27" s="26" t="s">
         <v>1</v>
@@ -9790,7 +9796,7 @@
         <v>26</v>
       </c>
       <c r="C30" s="72" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D30" s="73"/>
       <c r="E30" s="73"/>
@@ -9816,7 +9822,7 @@
       <c r="F31" s="20"/>
       <c r="G31" s="58"/>
       <c r="H31" s="76" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I31" s="63"/>
       <c r="J31" s="63"/>
@@ -9835,7 +9841,7 @@
       <c r="F32" s="20"/>
       <c r="G32" s="58"/>
       <c r="H32" s="76" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I32" s="63"/>
       <c r="J32" s="63"/>
@@ -9852,7 +9858,7 @@
       <c r="F33" s="32"/>
       <c r="G33" s="58"/>
       <c r="H33" s="75" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I33" s="20"/>
       <c r="J33" s="20"/>
@@ -9866,7 +9872,7 @@
         <v>29</v>
       </c>
       <c r="C34" s="59" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D34" s="26" t="s">
         <v>1</v>
@@ -9879,7 +9885,7 @@
       </c>
       <c r="G34" s="58"/>
       <c r="H34" s="75" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="I34" s="20"/>
       <c r="J34" s="20"/>
@@ -9898,7 +9904,7 @@
       <c r="F35" s="20"/>
       <c r="G35" s="58"/>
       <c r="H35" s="75" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I35" s="20"/>
       <c r="J35" s="20"/>
@@ -9976,7 +9982,7 @@
       <c r="L39" s="93"/>
       <c r="M39" s="58"/>
     </row>
-    <row r="40" spans="1:13" ht="15.75" thickBot="1">
+    <row r="40" spans="1:13" ht="30.75" thickBot="1">
       <c r="A40" s="58"/>
       <c r="B40" s="64"/>
       <c r="C40" s="65"/>
@@ -9985,9 +9991,11 @@
       <c r="F40" s="66"/>
       <c r="G40" s="58"/>
       <c r="H40" s="76" t="s">
-        <v>303</v>
-      </c>
-      <c r="I40" s="63"/>
+        <v>302</v>
+      </c>
+      <c r="I40" s="76" t="s">
+        <v>323</v>
+      </c>
       <c r="J40" s="63"/>
       <c r="K40" s="63"/>
       <c r="L40" s="63"/>
@@ -9999,7 +10007,7 @@
         <v>35</v>
       </c>
       <c r="C41" s="59" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>1</v>
@@ -10012,7 +10020,7 @@
       </c>
       <c r="G41" s="58"/>
       <c r="H41" s="76" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I41" s="63"/>
       <c r="J41" s="63"/>
@@ -10031,7 +10039,7 @@
       <c r="F42" s="74"/>
       <c r="G42" s="58"/>
       <c r="H42" s="75" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I42" s="20"/>
       <c r="J42" s="20"/>
@@ -10050,7 +10058,7 @@
       <c r="F43" s="20"/>
       <c r="G43" s="58"/>
       <c r="H43" s="75" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I43" s="20"/>
       <c r="J43" s="20"/>
@@ -10069,7 +10077,7 @@
       <c r="F44" s="20"/>
       <c r="G44" s="58"/>
       <c r="H44" s="75" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I44" s="20"/>
       <c r="J44" s="20"/>
@@ -10077,7 +10085,7 @@
       <c r="L44" s="20"/>
       <c r="M44" s="58"/>
     </row>
-    <row r="45" spans="1:13" ht="26.25" thickBot="1">
+    <row r="45" spans="1:13" ht="15.75" thickBot="1">
       <c r="A45" s="58"/>
       <c r="B45" s="19" t="s">
         <v>39</v>
@@ -10088,7 +10096,7 @@
       <c r="F45" s="73"/>
       <c r="G45" s="58"/>
       <c r="H45" s="75" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I45" s="20"/>
       <c r="J45" s="20"/>
@@ -10107,7 +10115,7 @@
       <c r="F46" s="62"/>
       <c r="G46" s="58"/>
       <c r="H46" s="75" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I46" s="20"/>
       <c r="J46" s="20"/>
@@ -10136,7 +10144,7 @@
         <v>41</v>
       </c>
       <c r="C48" s="59" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D48" s="14" t="s">
         <v>1</v>
@@ -10168,7 +10176,7 @@
       <c r="F49" s="73"/>
       <c r="G49" s="58"/>
       <c r="H49" s="76" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I49" s="63"/>
       <c r="J49" s="63"/>
@@ -10187,7 +10195,7 @@
       <c r="F50" s="20"/>
       <c r="G50" s="58"/>
       <c r="H50" s="76" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I50" s="63"/>
       <c r="J50" s="63"/>
@@ -10206,7 +10214,7 @@
       <c r="F51" s="20"/>
       <c r="G51" s="58"/>
       <c r="H51" s="75" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I51" s="20"/>
       <c r="J51" s="20"/>
@@ -10225,7 +10233,7 @@
       <c r="F52" s="73"/>
       <c r="G52" s="58"/>
       <c r="H52" s="75" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="I52" s="20"/>
       <c r="J52" s="20"/>
@@ -10244,7 +10252,7 @@
       <c r="F53" s="20"/>
       <c r="G53" s="58"/>
       <c r="H53" s="75" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I53" s="20"/>
       <c r="J53" s="20"/>
@@ -10263,7 +10271,7 @@
       <c r="F54" s="73"/>
       <c r="G54" s="58"/>
       <c r="H54" s="75" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I54" s="20"/>
       <c r="J54" s="20"/>
@@ -10490,12 +10498,12 @@
       <c r="F67" s="73"/>
       <c r="G67" s="58"/>
       <c r="H67" s="76" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I67" s="63"/>
       <c r="J67" s="63"/>
       <c r="K67" s="99" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="L67" s="100"/>
       <c r="M67" s="58"/>
@@ -10511,12 +10519,12 @@
       <c r="F68" s="73"/>
       <c r="G68" s="58"/>
       <c r="H68" s="76" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I68" s="63"/>
       <c r="J68" s="63"/>
       <c r="K68" s="99" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L68" s="100"/>
       <c r="M68" s="58"/>
@@ -10532,12 +10540,12 @@
       <c r="F69" s="73"/>
       <c r="G69" s="58"/>
       <c r="H69" s="75" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I69" s="20"/>
       <c r="J69" s="20"/>
       <c r="K69" s="94" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L69" s="95"/>
       <c r="M69" s="58"/>
@@ -10547,18 +10555,18 @@
       <c r="B70" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="C70" s="20"/>
+      <c r="C70" s="73"/>
       <c r="D70" s="73"/>
       <c r="E70" s="77"/>
       <c r="F70" s="20"/>
       <c r="G70" s="58"/>
       <c r="H70" s="75" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="I70" s="20"/>
       <c r="J70" s="20"/>
       <c r="K70" s="94" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L70" s="95"/>
       <c r="M70" s="58"/>
@@ -10577,7 +10585,7 @@
       <c r="I71" s="20"/>
       <c r="J71" s="20"/>
       <c r="K71" s="94" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L71" s="95"/>
       <c r="M71" s="58"/>
@@ -10630,7 +10638,7 @@
         <v>175</v>
       </c>
       <c r="I74" s="59" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J74" s="14" t="s">
         <v>1</v>
@@ -10713,7 +10721,7 @@
       <c r="H78" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="I78" s="20"/>
+      <c r="I78" s="73"/>
       <c r="J78" s="73"/>
       <c r="K78" s="73"/>
       <c r="L78" s="73"/>
@@ -10732,7 +10740,7 @@
       <c r="H79" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="I79" s="20"/>
+      <c r="I79" s="73"/>
       <c r="J79" s="73"/>
       <c r="K79" s="73"/>
       <c r="L79" s="73"/>
@@ -10743,7 +10751,7 @@
       <c r="B80" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="C80" s="20"/>
+      <c r="C80" s="73"/>
       <c r="D80" s="73"/>
       <c r="E80" s="73"/>
       <c r="F80" s="20"/>
@@ -10762,7 +10770,7 @@
       <c r="B81" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="C81" s="20"/>
+      <c r="C81" s="73"/>
       <c r="D81" s="73"/>
       <c r="E81" s="73"/>
       <c r="F81" s="20"/>
@@ -10971,7 +10979,7 @@
       <c r="B92" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="C92" s="20"/>
+      <c r="C92" s="73"/>
       <c r="D92" s="73"/>
       <c r="E92" s="20"/>
       <c r="F92" s="20"/>
@@ -11034,12 +11042,12 @@
       <c r="F95" s="73"/>
       <c r="G95" s="58"/>
       <c r="H95" s="19" t="s">
-        <v>196</v>
+        <v>322</v>
       </c>
       <c r="I95" s="73"/>
       <c r="J95" s="73"/>
       <c r="K95" s="73"/>
-      <c r="L95" s="20"/>
+      <c r="L95" s="73"/>
       <c r="M95" s="58"/>
     </row>
     <row r="96" spans="1:13" ht="15.75" thickBot="1">
@@ -11053,7 +11061,7 @@
       <c r="F96" s="73"/>
       <c r="G96" s="58"/>
       <c r="H96" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I96" s="20"/>
       <c r="J96" s="20"/>
@@ -11064,7 +11072,7 @@
     <row r="97" spans="1:13" ht="15.75" thickBot="1">
       <c r="A97" s="58"/>
       <c r="B97" s="19" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C97" s="73"/>
       <c r="D97" s="73"/>
@@ -11072,7 +11080,7 @@
       <c r="F97" s="73"/>
       <c r="G97" s="58"/>
       <c r="H97" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I97" s="20"/>
       <c r="J97" s="73"/>
@@ -11110,7 +11118,7 @@
       <c r="F99" s="73"/>
       <c r="G99" s="58"/>
       <c r="H99" s="19" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I99" s="20"/>
       <c r="J99" s="73"/>
@@ -11129,7 +11137,7 @@
       <c r="F100" s="83"/>
       <c r="G100" s="58"/>
       <c r="H100" s="19" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I100" s="73"/>
       <c r="J100" s="73"/>
@@ -11140,7 +11148,7 @@
     <row r="101" spans="1:13" ht="15.75" thickBot="1">
       <c r="A101" s="58"/>
       <c r="B101" s="19" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C101" s="20"/>
       <c r="D101" s="73"/>
@@ -11148,7 +11156,7 @@
       <c r="F101" s="20"/>
       <c r="G101" s="58"/>
       <c r="H101" s="19" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I101" s="20"/>
       <c r="J101" s="73"/>
@@ -11167,7 +11175,7 @@
       <c r="F102" s="73"/>
       <c r="G102" s="58"/>
       <c r="H102" s="19" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I102" s="72"/>
       <c r="J102" s="73"/>
@@ -11186,7 +11194,7 @@
       <c r="F103" s="87"/>
       <c r="G103" s="58"/>
       <c r="H103" s="19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I103" s="20"/>
       <c r="J103" s="73"/>
@@ -11215,7 +11223,7 @@
         <v>96</v>
       </c>
       <c r="C105" s="59" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D105" s="14" t="s">
         <v>1</v>
@@ -11228,10 +11236,10 @@
       </c>
       <c r="G105" s="58"/>
       <c r="H105" s="13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I105" s="59" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J105" s="14" t="s">
         <v>1</v>
@@ -11255,7 +11263,7 @@
       <c r="F106" s="20"/>
       <c r="G106" s="58"/>
       <c r="H106" s="19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I106" s="73"/>
       <c r="J106" s="73"/>
@@ -11274,7 +11282,7 @@
       <c r="F107" s="73"/>
       <c r="G107" s="58"/>
       <c r="H107" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I107" s="20"/>
       <c r="J107" s="73"/>
@@ -11293,7 +11301,7 @@
       <c r="F108" s="73"/>
       <c r="G108" s="58"/>
       <c r="H108" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I108" s="72"/>
       <c r="J108" s="20"/>
@@ -11312,9 +11320,9 @@
       <c r="F109" s="73"/>
       <c r="G109" s="58"/>
       <c r="H109" s="19" t="s">
-        <v>207</v>
-      </c>
-      <c r="I109" s="20"/>
+        <v>206</v>
+      </c>
+      <c r="I109" s="73"/>
       <c r="J109" s="20"/>
       <c r="K109" s="73"/>
       <c r="L109" s="20"/>
@@ -11331,11 +11339,11 @@
       <c r="F110" s="20"/>
       <c r="G110" s="58"/>
       <c r="H110" s="19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I110" s="20"/>
       <c r="J110" s="81"/>
-      <c r="K110" s="20"/>
+      <c r="K110" s="73"/>
       <c r="L110" s="73"/>
       <c r="M110" s="58"/>
     </row>
@@ -11350,7 +11358,7 @@
       <c r="F111" s="73"/>
       <c r="G111" s="58"/>
       <c r="H111" s="19" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I111" s="20"/>
       <c r="J111" s="73"/>
@@ -11369,7 +11377,7 @@
       <c r="F112" s="73"/>
       <c r="G112" s="58"/>
       <c r="H112" s="19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I112" s="20"/>
       <c r="J112" s="73"/>
@@ -11388,7 +11396,7 @@
       <c r="F113" s="73"/>
       <c r="G113" s="58"/>
       <c r="H113" s="19" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I113" s="73"/>
       <c r="J113" s="20"/>
@@ -11402,14 +11410,14 @@
         <v>105</v>
       </c>
       <c r="C114" s="73" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D114" s="73"/>
       <c r="E114" s="20"/>
       <c r="F114" s="20"/>
       <c r="G114" s="58"/>
       <c r="H114" s="19" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I114" s="73"/>
       <c r="J114" s="73"/>
@@ -11428,7 +11436,7 @@
       <c r="F115" s="20"/>
       <c r="G115" s="58"/>
       <c r="H115" s="19" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I115" s="20"/>
       <c r="J115" s="73"/>
@@ -11447,10 +11455,10 @@
       <c r="F116" s="73"/>
       <c r="G116" s="58"/>
       <c r="H116" s="19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I116" s="75" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J116" s="73"/>
       <c r="K116" s="20"/>
@@ -11463,14 +11471,14 @@
         <v>108</v>
       </c>
       <c r="C117" s="84" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D117" s="41"/>
       <c r="E117" s="74"/>
       <c r="F117" s="74"/>
       <c r="G117" s="58"/>
       <c r="H117" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I117" s="73"/>
       <c r="J117" s="73"/>
@@ -11489,7 +11497,7 @@
       <c r="F118" s="20"/>
       <c r="G118" s="58"/>
       <c r="H118" s="19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I118" s="20"/>
       <c r="J118" s="20"/>
@@ -11508,7 +11516,7 @@
       <c r="F119" s="73"/>
       <c r="G119" s="58"/>
       <c r="H119" s="19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I119" s="80"/>
       <c r="J119" s="73"/>
@@ -11527,11 +11535,11 @@
       <c r="F120" s="73"/>
       <c r="G120" s="58"/>
       <c r="H120" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I120" s="80"/>
       <c r="J120" s="73"/>
-      <c r="K120" s="42"/>
+      <c r="K120" s="101"/>
       <c r="L120" s="73"/>
       <c r="M120" s="58"/>
     </row>
@@ -11546,7 +11554,7 @@
       <c r="F121" s="20"/>
       <c r="G121" s="58"/>
       <c r="H121" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I121" s="73"/>
       <c r="J121" s="73"/>
@@ -11565,11 +11573,11 @@
       <c r="F122" s="73"/>
       <c r="G122" s="58"/>
       <c r="H122" s="19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I122" s="73"/>
       <c r="J122" s="73"/>
-      <c r="K122" s="20"/>
+      <c r="K122" s="73"/>
       <c r="L122" s="20"/>
       <c r="M122" s="58"/>
     </row>
@@ -11584,9 +11592,9 @@
       <c r="F123" s="73"/>
       <c r="G123" s="58"/>
       <c r="H123" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="I123" s="20"/>
+        <v>220</v>
+      </c>
+      <c r="I123" s="73"/>
       <c r="J123" s="20"/>
       <c r="K123" s="73"/>
       <c r="L123" s="20"/>
@@ -11603,7 +11611,7 @@
       <c r="F124" s="20"/>
       <c r="G124" s="58"/>
       <c r="H124" s="19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I124" s="73"/>
       <c r="J124" s="73"/>
@@ -11622,7 +11630,7 @@
       <c r="F125" s="73"/>
       <c r="G125" s="58"/>
       <c r="H125" s="19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I125" s="73"/>
       <c r="J125" s="73"/>
@@ -11641,7 +11649,7 @@
       <c r="F126" s="20"/>
       <c r="G126" s="58"/>
       <c r="H126" s="19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I126" s="20"/>
       <c r="J126" s="20"/>
@@ -11660,7 +11668,7 @@
       <c r="F127" s="73"/>
       <c r="G127" s="58"/>
       <c r="H127" s="19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I127" s="20"/>
       <c r="J127" s="73"/>
@@ -11679,7 +11687,7 @@
       <c r="F128" s="39"/>
       <c r="G128" s="58"/>
       <c r="H128" s="19" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I128" s="20"/>
       <c r="J128" s="73"/>
@@ -11698,7 +11706,7 @@
       <c r="F129" s="73"/>
       <c r="G129" s="58"/>
       <c r="H129" s="19" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I129" s="20"/>
       <c r="J129" s="73"/>
@@ -11711,18 +11719,18 @@
       <c r="B130" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="C130" s="20"/>
+      <c r="C130" s="73"/>
       <c r="D130" s="73"/>
       <c r="E130" s="73"/>
       <c r="F130" s="20"/>
       <c r="G130" s="58"/>
       <c r="H130" s="19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I130" s="73"/>
       <c r="J130" s="73"/>
       <c r="K130" s="85"/>
-      <c r="L130" s="20"/>
+      <c r="L130" s="73"/>
       <c r="M130" s="58"/>
     </row>
     <row r="131" spans="1:14" ht="15.75" thickBot="1">
@@ -11736,7 +11744,7 @@
       <c r="F131" s="41"/>
       <c r="G131" s="58"/>
       <c r="H131" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I131" s="20"/>
       <c r="J131" s="73"/>
@@ -11755,7 +11763,7 @@
       <c r="F132" s="20"/>
       <c r="G132" s="58"/>
       <c r="H132" s="19" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I132" s="20"/>
       <c r="J132" s="73"/>
@@ -11774,7 +11782,7 @@
       <c r="F133" s="20"/>
       <c r="G133" s="58"/>
       <c r="H133" s="19" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I133" s="73"/>
       <c r="J133" s="73"/>
@@ -11811,22 +11819,22 @@
       <c r="F135" s="20"/>
       <c r="G135" s="4"/>
       <c r="H135" s="44" t="s">
+        <v>231</v>
+      </c>
+      <c r="I135" s="45" t="s">
         <v>232</v>
       </c>
-      <c r="I135" s="45" t="s">
+      <c r="J135" s="45" t="s">
         <v>233</v>
       </c>
-      <c r="J135" s="45" t="s">
+      <c r="K135" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="K135" s="45" t="s">
+      <c r="L135" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="L135" s="45" t="s">
+      <c r="M135" s="45" t="s">
         <v>236</v>
-      </c>
-      <c r="M135" s="45" t="s">
-        <v>237</v>
       </c>
       <c r="N135" s="4"/>
     </row>
@@ -11841,7 +11849,7 @@
       <c r="F136" s="77"/>
       <c r="G136" s="4"/>
       <c r="H136" s="51" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I136" s="3"/>
       <c r="J136" s="3"/>
@@ -11861,7 +11869,7 @@
       <c r="F137" s="20"/>
       <c r="G137" s="4"/>
       <c r="H137" s="51" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I137" s="3"/>
       <c r="J137" s="3"/>
@@ -11881,7 +11889,7 @@
       <c r="F138" s="73"/>
       <c r="G138" s="4"/>
       <c r="H138" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I138" s="3"/>
       <c r="J138" s="3"/>
@@ -11901,7 +11909,7 @@
       <c r="F139" s="20"/>
       <c r="G139" s="4"/>
       <c r="H139" s="52" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I139" s="54"/>
       <c r="J139" s="54"/>
@@ -11921,7 +11929,7 @@
       <c r="F140" s="73"/>
       <c r="G140" s="4"/>
       <c r="H140" s="53" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I140" s="54"/>
       <c r="J140" s="54"/>
@@ -11959,22 +11967,22 @@
       <c r="F142" s="87"/>
       <c r="G142" s="4"/>
       <c r="H142" s="44" t="s">
+        <v>243</v>
+      </c>
+      <c r="I142" s="45" t="s">
         <v>244</v>
       </c>
-      <c r="I142" s="45" t="s">
+      <c r="J142" s="45" t="s">
         <v>245</v>
       </c>
-      <c r="J142" s="45" t="s">
+      <c r="K142" s="45" t="s">
         <v>246</v>
       </c>
-      <c r="K142" s="45" t="s">
+      <c r="L142" s="45" t="s">
         <v>247</v>
       </c>
-      <c r="L142" s="45" t="s">
+      <c r="M142" s="45" t="s">
         <v>248</v>
-      </c>
-      <c r="M142" s="45" t="s">
-        <v>249</v>
       </c>
       <c r="N142" s="4"/>
     </row>
@@ -11987,7 +11995,7 @@
       <c r="F143" s="58"/>
       <c r="G143" s="4"/>
       <c r="H143" s="51" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I143" s="3"/>
       <c r="J143" s="3"/>
@@ -12002,7 +12010,7 @@
         <v>134</v>
       </c>
       <c r="C144" s="59" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D144" s="14" t="s">
         <v>1</v>
@@ -12015,7 +12023,7 @@
       </c>
       <c r="G144" s="4"/>
       <c r="H144" s="51" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I144" s="3"/>
       <c r="J144" s="3"/>
@@ -12035,7 +12043,7 @@
       <c r="F145" s="73"/>
       <c r="G145" s="4"/>
       <c r="H145" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I145" s="3"/>
       <c r="J145" s="3"/>
@@ -12055,7 +12063,7 @@
       <c r="F146" s="73"/>
       <c r="G146" s="4"/>
       <c r="H146" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I146" s="3"/>
       <c r="J146" s="3"/>
@@ -12075,7 +12083,7 @@
       <c r="F147" s="73"/>
       <c r="G147" s="4"/>
       <c r="H147" s="57" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I147" s="2"/>
       <c r="J147" s="2"/>
@@ -12113,22 +12121,22 @@
       <c r="F149" s="73"/>
       <c r="G149" s="4"/>
       <c r="H149" s="44" t="s">
+        <v>249</v>
+      </c>
+      <c r="I149" s="45" t="s">
         <v>250</v>
       </c>
-      <c r="I149" s="45" t="s">
+      <c r="J149" s="45" t="s">
         <v>251</v>
       </c>
-      <c r="J149" s="45" t="s">
+      <c r="K149" s="45" t="s">
         <v>252</v>
       </c>
-      <c r="K149" s="45" t="s">
+      <c r="L149" s="45" t="s">
         <v>253</v>
       </c>
-      <c r="L149" s="45" t="s">
+      <c r="M149" s="45" t="s">
         <v>254</v>
-      </c>
-      <c r="M149" s="45" t="s">
-        <v>255</v>
       </c>
       <c r="N149" s="4"/>
     </row>
@@ -12143,7 +12151,7 @@
       <c r="F150" s="73"/>
       <c r="G150" s="4"/>
       <c r="H150" s="51" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I150" s="3"/>
       <c r="J150" s="3"/>
@@ -12163,7 +12171,7 @@
       <c r="F151" s="73"/>
       <c r="G151" s="4"/>
       <c r="H151" s="51" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I151" s="3"/>
       <c r="J151" s="3"/>
@@ -12183,7 +12191,7 @@
       <c r="F152" s="73"/>
       <c r="G152" s="4"/>
       <c r="H152" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I152" s="3"/>
       <c r="J152" s="3"/>
@@ -12203,7 +12211,7 @@
       <c r="F153" s="73"/>
       <c r="G153" s="4"/>
       <c r="H153" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I153" s="3"/>
       <c r="J153" s="3"/>
@@ -12223,7 +12231,7 @@
       <c r="F154" s="20"/>
       <c r="G154" s="4"/>
       <c r="H154" s="57" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I154" s="2"/>
       <c r="J154" s="2"/>
@@ -12259,47 +12267,47 @@
       <c r="F156" s="58"/>
       <c r="G156" s="4"/>
       <c r="H156" s="44" t="s">
+        <v>255</v>
+      </c>
+      <c r="I156" s="45" t="s">
         <v>256</v>
       </c>
-      <c r="I156" s="45" t="s">
+      <c r="J156" s="45" t="s">
         <v>257</v>
       </c>
-      <c r="J156" s="45" t="s">
+      <c r="K156" s="45" t="s">
         <v>258</v>
       </c>
-      <c r="K156" s="45" t="s">
+      <c r="L156" s="45" t="s">
         <v>259</v>
       </c>
-      <c r="L156" s="45" t="s">
+      <c r="M156" s="45" t="s">
         <v>260</v>
-      </c>
-      <c r="M156" s="45" t="s">
-        <v>261</v>
       </c>
       <c r="N156" s="4"/>
     </row>
     <row r="157" spans="1:14" ht="27" thickBot="1">
       <c r="A157" s="79" t="s">
+        <v>267</v>
+      </c>
+      <c r="B157" s="45" t="s">
         <v>268</v>
       </c>
-      <c r="B157" s="45" t="s">
+      <c r="C157" s="45" t="s">
         <v>269</v>
       </c>
-      <c r="C157" s="45" t="s">
+      <c r="D157" s="45" t="s">
         <v>270</v>
       </c>
-      <c r="D157" s="45" t="s">
+      <c r="E157" s="45" t="s">
         <v>271</v>
       </c>
-      <c r="E157" s="45" t="s">
+      <c r="F157" s="45" t="s">
         <v>272</v>
-      </c>
-      <c r="F157" s="45" t="s">
-        <v>273</v>
       </c>
       <c r="G157" s="4"/>
       <c r="H157" s="51" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I157" s="3"/>
       <c r="J157" s="3"/>
@@ -12310,7 +12318,7 @@
     </row>
     <row r="158" spans="1:14" ht="15.75" thickBot="1">
       <c r="A158" s="51" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B158" s="3"/>
       <c r="C158" s="3"/>
@@ -12319,7 +12327,7 @@
       <c r="F158" s="3"/>
       <c r="G158" s="4"/>
       <c r="H158" s="51" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I158" s="3"/>
       <c r="J158" s="3"/>
@@ -12330,7 +12338,7 @@
     </row>
     <row r="159" spans="1:14" ht="15.75" thickBot="1">
       <c r="A159" s="51" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B159" s="3"/>
       <c r="C159" s="3"/>
@@ -12339,7 +12347,7 @@
       <c r="F159" s="3"/>
       <c r="G159" s="4"/>
       <c r="H159" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I159" s="3"/>
       <c r="J159" s="3"/>
@@ -12350,7 +12358,7 @@
     </row>
     <row r="160" spans="1:14" ht="15.75" thickBot="1">
       <c r="A160" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B160" s="3"/>
       <c r="C160" s="3"/>
@@ -12359,7 +12367,7 @@
       <c r="F160" s="3"/>
       <c r="G160" s="4"/>
       <c r="H160" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I160" s="3"/>
       <c r="J160" s="3"/>
@@ -12370,7 +12378,7 @@
     </row>
     <row r="161" spans="1:14" ht="15.75" thickBot="1">
       <c r="A161" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B161" s="3"/>
       <c r="C161" s="3"/>
@@ -12379,7 +12387,7 @@
       <c r="F161" s="3"/>
       <c r="G161" s="4"/>
       <c r="H161" s="57" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I161" s="2"/>
       <c r="J161" s="2"/>
@@ -12390,7 +12398,7 @@
     </row>
     <row r="162" spans="1:14" ht="15.75" thickBot="1">
       <c r="A162" s="57" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B162" s="2"/>
       <c r="C162" s="2"/>
@@ -12415,47 +12423,47 @@
       <c r="F163" s="4"/>
       <c r="G163" s="4"/>
       <c r="H163" s="44" t="s">
+        <v>261</v>
+      </c>
+      <c r="I163" s="45" t="s">
         <v>262</v>
       </c>
-      <c r="I163" s="45" t="s">
+      <c r="J163" s="45" t="s">
         <v>263</v>
       </c>
-      <c r="J163" s="45" t="s">
+      <c r="K163" s="45" t="s">
         <v>264</v>
       </c>
-      <c r="K163" s="45" t="s">
+      <c r="L163" s="45" t="s">
         <v>265</v>
       </c>
-      <c r="L163" s="45" t="s">
+      <c r="M163" s="45" t="s">
         <v>266</v>
-      </c>
-      <c r="M163" s="45" t="s">
-        <v>267</v>
       </c>
       <c r="N163" s="4"/>
     </row>
     <row r="164" spans="1:14" ht="39.75" thickBot="1">
       <c r="A164" s="44" t="s">
+        <v>273</v>
+      </c>
+      <c r="B164" s="45" t="s">
         <v>274</v>
       </c>
-      <c r="B164" s="45" t="s">
+      <c r="C164" s="45" t="s">
         <v>275</v>
       </c>
-      <c r="C164" s="45" t="s">
+      <c r="D164" s="45" t="s">
         <v>276</v>
       </c>
-      <c r="D164" s="45" t="s">
+      <c r="E164" s="45" t="s">
         <v>277</v>
       </c>
-      <c r="E164" s="45" t="s">
+      <c r="F164" s="45" t="s">
         <v>278</v>
-      </c>
-      <c r="F164" s="45" t="s">
-        <v>279</v>
       </c>
       <c r="G164" s="4"/>
       <c r="H164" s="51" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I164" s="3"/>
       <c r="J164" s="3"/>
@@ -12466,7 +12474,7 @@
     </row>
     <row r="165" spans="1:14" ht="15.75" thickBot="1">
       <c r="A165" s="51" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B165" s="3"/>
       <c r="C165" s="3"/>
@@ -12475,7 +12483,7 @@
       <c r="F165" s="3"/>
       <c r="G165" s="4"/>
       <c r="H165" s="51" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I165" s="3"/>
       <c r="J165" s="3"/>
@@ -12486,7 +12494,7 @@
     </row>
     <row r="166" spans="1:14" ht="15.75" thickBot="1">
       <c r="A166" s="51" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B166" s="3"/>
       <c r="C166" s="3"/>
@@ -12495,7 +12503,7 @@
       <c r="F166" s="3"/>
       <c r="G166" s="4"/>
       <c r="H166" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I166" s="3"/>
       <c r="J166" s="3"/>
@@ -12506,7 +12514,7 @@
     </row>
     <row r="167" spans="1:14" ht="15.75" thickBot="1">
       <c r="A167" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B167" s="3"/>
       <c r="C167" s="3"/>
@@ -12515,7 +12523,7 @@
       <c r="F167" s="3"/>
       <c r="G167" s="4"/>
       <c r="H167" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I167" s="3"/>
       <c r="J167" s="3"/>
@@ -12526,7 +12534,7 @@
     </row>
     <row r="168" spans="1:14" ht="15.75" thickBot="1">
       <c r="A168" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B168" s="3"/>
       <c r="C168" s="3"/>
@@ -12535,7 +12543,7 @@
       <c r="F168" s="3"/>
       <c r="G168" s="4"/>
       <c r="H168" s="57" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I168" s="2"/>
       <c r="J168" s="2"/>
@@ -12546,7 +12554,7 @@
     </row>
     <row r="169" spans="1:14" ht="15.75" thickBot="1">
       <c r="A169" s="57" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B169" s="2"/>
       <c r="C169" s="2"/>
@@ -12581,19 +12589,19 @@
     <row r="171" spans="1:14" ht="27" thickBot="1">
       <c r="A171" s="4"/>
       <c r="B171" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="C171" s="45" t="s">
         <v>280</v>
       </c>
-      <c r="C171" s="45" t="s">
+      <c r="D171" s="45" t="s">
         <v>281</v>
       </c>
-      <c r="D171" s="45" t="s">
+      <c r="E171" s="45" t="s">
         <v>282</v>
       </c>
-      <c r="E171" s="45" t="s">
+      <c r="F171" s="45" t="s">
         <v>283</v>
-      </c>
-      <c r="F171" s="45" t="s">
-        <v>284</v>
       </c>
       <c r="G171" s="4"/>
       <c r="H171" s="4"/>
@@ -12607,7 +12615,7 @@
     <row r="172" spans="1:14" ht="15.75" thickBot="1">
       <c r="A172" s="4"/>
       <c r="B172" s="51" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C172" s="3"/>
       <c r="D172" s="3"/>
@@ -12625,7 +12633,7 @@
     <row r="173" spans="1:14" ht="15.75" thickBot="1">
       <c r="A173" s="4"/>
       <c r="B173" s="51" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C173" s="3"/>
       <c r="D173" s="3"/>
@@ -12643,7 +12651,7 @@
     <row r="174" spans="1:14" ht="15.75" thickBot="1">
       <c r="A174" s="4"/>
       <c r="B174" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C174" s="3"/>
       <c r="D174" s="3"/>
@@ -12661,7 +12669,7 @@
     <row r="175" spans="1:14" ht="15.75" thickBot="1">
       <c r="A175" s="4"/>
       <c r="B175" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C175" s="3"/>
       <c r="D175" s="3"/>
@@ -12679,7 +12687,7 @@
     <row r="176" spans="1:14" ht="15.75" thickBot="1">
       <c r="A176" s="4"/>
       <c r="B176" s="57" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C176" s="2"/>
       <c r="D176" s="2"/>

</xml_diff>

<commit_message>
some more items done
</commit_message>
<xml_diff>
--- a/check list.xlsx
+++ b/check list.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="328">
   <si>
     <t>ARMOR</t>
   </si>
@@ -998,6 +998,9 @@
   </si>
   <si>
     <t>Suicide Note</t>
+  </si>
+  <si>
+    <t>In For The Kill</t>
   </si>
 </sst>
 </file>
@@ -9200,8 +9203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G36" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F121" sqref="F121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9499,7 +9502,7 @@
       <c r="C14" s="73"/>
       <c r="D14" s="73"/>
       <c r="E14" s="73"/>
-      <c r="F14" s="20"/>
+      <c r="F14" s="73"/>
       <c r="G14" s="58"/>
       <c r="H14" s="19" t="s">
         <v>155</v>
@@ -9618,7 +9621,7 @@
       <c r="H20" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="I20" s="20"/>
+      <c r="I20" s="73"/>
       <c r="J20" s="73"/>
       <c r="K20" s="73"/>
       <c r="L20" s="73"/>
@@ -10054,7 +10057,9 @@
       <c r="H42" s="75" t="s">
         <v>305</v>
       </c>
-      <c r="I42" s="20"/>
+      <c r="I42" s="75" t="s">
+        <v>327</v>
+      </c>
       <c r="J42" s="20"/>
       <c r="K42" s="20"/>
       <c r="L42" s="20"/>
@@ -10087,7 +10092,7 @@
       <c r="C44" s="73"/>
       <c r="D44" s="73"/>
       <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
+      <c r="F44" s="73"/>
       <c r="G44" s="58"/>
       <c r="H44" s="75" t="s">
         <v>309</v>
@@ -10124,8 +10129,8 @@
       </c>
       <c r="C46" s="73"/>
       <c r="D46" s="73"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="62"/>
+      <c r="E46" s="73"/>
+      <c r="F46" s="87"/>
       <c r="G46" s="58"/>
       <c r="H46" s="75" t="s">
         <v>318</v>
@@ -10927,7 +10932,7 @@
         <v>189</v>
       </c>
       <c r="I88" s="20"/>
-      <c r="J88" s="20"/>
+      <c r="J88" s="73"/>
       <c r="K88" s="73"/>
       <c r="L88" s="20"/>
       <c r="M88" s="58"/>
@@ -11110,7 +11115,7 @@
       </c>
       <c r="C98" s="20"/>
       <c r="D98" s="73"/>
-      <c r="E98" s="20"/>
+      <c r="E98" s="73"/>
       <c r="F98" s="20"/>
       <c r="G98" s="58"/>
       <c r="H98" s="19" t="s">
@@ -11165,7 +11170,7 @@
       <c r="B101" s="19" t="s">
         <v>297</v>
       </c>
-      <c r="C101" s="20"/>
+      <c r="C101" s="73"/>
       <c r="D101" s="73"/>
       <c r="E101" s="20"/>
       <c r="F101" s="20"/>
@@ -11563,10 +11568,10 @@
       <c r="B121" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="C121" s="20"/>
+      <c r="C121" s="73"/>
       <c r="D121" s="73"/>
       <c r="E121" s="73"/>
-      <c r="F121" s="20"/>
+      <c r="F121" s="73"/>
       <c r="G121" s="58"/>
       <c r="H121" s="19" t="s">
         <v>218</v>
@@ -11582,7 +11587,7 @@
       <c r="B122" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="C122" s="20"/>
+      <c r="C122" s="73"/>
       <c r="D122" s="73"/>
       <c r="E122" s="20"/>
       <c r="F122" s="73"/>
@@ -11658,7 +11663,7 @@
       <c r="B126" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="C126" s="20"/>
+      <c r="C126" s="73"/>
       <c r="D126" s="73"/>
       <c r="E126" s="73"/>
       <c r="F126" s="20"/>
@@ -12220,7 +12225,7 @@
       <c r="B153" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="C153" s="20"/>
+      <c r="C153" s="73"/>
       <c r="D153" s="73"/>
       <c r="E153" s="73"/>
       <c r="F153" s="73"/>

</xml_diff>

<commit_message>
much items, such updates
wow
</commit_message>
<xml_diff>
--- a/check list.xlsx
+++ b/check list.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="335">
   <si>
     <t>ARMOR</t>
   </si>
@@ -1001,6 +1001,27 @@
   </si>
   <si>
     <t>In For The Kill</t>
+  </si>
+  <si>
+    <t>Plague Gland</t>
+  </si>
+  <si>
+    <t>Phase Crystal</t>
+  </si>
+  <si>
+    <t>Farsight Globe</t>
+  </si>
+  <si>
+    <t>Xepera Xeper Xeperu</t>
+  </si>
+  <si>
+    <t>The Seal of Kharos</t>
+  </si>
+  <si>
+    <t>Bucket of Love</t>
+  </si>
+  <si>
+    <t>Scarab of Death</t>
   </si>
 </sst>
 </file>
@@ -1368,7 +1389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1648,12 +1669,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1661,6 +1676,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -9203,8 +9221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F121" sqref="F121"/>
+    <sheetView tabSelected="1" topLeftCell="B29" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9224,40 +9242,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="23.25" customHeight="1">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="97" t="s">
         <v>284</v>
       </c>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
-      <c r="G1" s="99"/>
-      <c r="H1" s="99"/>
-      <c r="I1" s="99"/>
-      <c r="J1" s="99"/>
-      <c r="K1" s="99"/>
-      <c r="L1" s="99"/>
-      <c r="M1" s="99"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
+      <c r="L1" s="97"/>
+      <c r="M1" s="97"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1">
-      <c r="A2" s="99"/>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
-      <c r="K2" s="99"/>
-      <c r="L2" s="99"/>
-      <c r="M2" s="99"/>
+      <c r="A2" s="97"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
       <c r="N2" s="1"/>
       <c r="O2" s="69"/>
       <c r="P2" s="70" t="s">
@@ -9266,19 +9284,19 @@
       <c r="Q2" s="1"/>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1">
-      <c r="A3" s="99"/>
-      <c r="B3" s="99"/>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="99"/>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99"/>
-      <c r="M3" s="99"/>
+      <c r="A3" s="97"/>
+      <c r="B3" s="97"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -9385,7 +9403,7 @@
       <c r="B8" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="20"/>
+      <c r="C8" s="100"/>
       <c r="D8" s="73"/>
       <c r="E8" s="73"/>
       <c r="F8" s="73"/>
@@ -9461,7 +9479,7 @@
       <c r="B12" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="20"/>
+      <c r="C12" s="73"/>
       <c r="D12" s="73"/>
       <c r="E12" s="73"/>
       <c r="F12" s="20"/>
@@ -9557,7 +9575,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="73"/>
-      <c r="D17" s="20"/>
+      <c r="D17" s="73"/>
       <c r="E17" s="73"/>
       <c r="F17" s="73"/>
       <c r="G17" s="58"/>
@@ -9597,7 +9615,7 @@
       <c r="C19" s="20"/>
       <c r="D19" s="73"/>
       <c r="E19" s="73"/>
-      <c r="F19" s="20"/>
+      <c r="F19" s="73"/>
       <c r="G19" s="58"/>
       <c r="H19" s="19" t="s">
         <v>160</v>
@@ -9736,7 +9754,7 @@
       <c r="I26" s="73"/>
       <c r="J26" s="73"/>
       <c r="K26" s="73"/>
-      <c r="L26" s="20"/>
+      <c r="L26" s="73"/>
       <c r="M26" s="58"/>
     </row>
     <row r="27" spans="1:13" ht="18" thickBot="1">
@@ -9829,7 +9847,7 @@
         <v>27</v>
       </c>
       <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
+      <c r="D31" s="73"/>
       <c r="E31" s="73"/>
       <c r="F31" s="20"/>
       <c r="G31" s="58"/>
@@ -9943,17 +9961,19 @@
       <c r="L36" s="20"/>
       <c r="M36" s="58"/>
     </row>
-    <row r="37" spans="1:13" ht="15.75" thickBot="1">
+    <row r="37" spans="1:13" ht="26.25" thickBot="1">
       <c r="A37" s="58"/>
       <c r="B37" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="20"/>
+      <c r="C37" s="100"/>
       <c r="D37" s="73"/>
       <c r="E37" s="73"/>
       <c r="F37" s="20"/>
       <c r="G37" s="58"/>
-      <c r="H37" s="20"/>
+      <c r="H37" s="75" t="s">
+        <v>332</v>
+      </c>
       <c r="I37" s="20"/>
       <c r="J37" s="20"/>
       <c r="K37" s="20"/>
@@ -10078,7 +10098,9 @@
       <c r="H43" s="75" t="s">
         <v>307</v>
       </c>
-      <c r="I43" s="20"/>
+      <c r="I43" s="75" t="s">
+        <v>334</v>
+      </c>
       <c r="J43" s="20"/>
       <c r="K43" s="20"/>
       <c r="L43" s="20"/>
@@ -10196,7 +10218,9 @@
       <c r="H49" s="76" t="s">
         <v>301</v>
       </c>
-      <c r="I49" s="63"/>
+      <c r="I49" s="76" t="s">
+        <v>329</v>
+      </c>
       <c r="J49" s="63"/>
       <c r="K49" s="63"/>
       <c r="L49" s="63"/>
@@ -10215,13 +10239,15 @@
       <c r="H50" s="76" t="s">
         <v>304</v>
       </c>
-      <c r="I50" s="63"/>
+      <c r="I50" s="76" t="s">
+        <v>330</v>
+      </c>
       <c r="J50" s="63"/>
       <c r="K50" s="63"/>
       <c r="L50" s="63"/>
       <c r="M50" s="58"/>
     </row>
-    <row r="51" spans="1:13" ht="15.75" thickBot="1">
+    <row r="51" spans="1:13" ht="26.25" thickBot="1">
       <c r="A51" s="58"/>
       <c r="B51" s="19" t="s">
         <v>44</v>
@@ -10234,7 +10260,9 @@
       <c r="H51" s="75" t="s">
         <v>306</v>
       </c>
-      <c r="I51" s="20"/>
+      <c r="I51" s="75" t="s">
+        <v>331</v>
+      </c>
       <c r="J51" s="20"/>
       <c r="K51" s="20"/>
       <c r="L51" s="20"/>
@@ -10459,7 +10487,7 @@
       <c r="B64" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="C64" s="20"/>
+      <c r="C64" s="73"/>
       <c r="D64" s="73"/>
       <c r="E64" s="73"/>
       <c r="F64" s="20"/>
@@ -10494,7 +10522,7 @@
         <v>59</v>
       </c>
       <c r="C66" s="73"/>
-      <c r="D66" s="80"/>
+      <c r="D66" s="73"/>
       <c r="E66" s="73"/>
       <c r="F66" s="73"/>
       <c r="G66" s="58"/>
@@ -10522,10 +10550,10 @@
       </c>
       <c r="I67" s="63"/>
       <c r="J67" s="63"/>
-      <c r="K67" s="100" t="s">
+      <c r="K67" s="98" t="s">
         <v>290</v>
       </c>
-      <c r="L67" s="101"/>
+      <c r="L67" s="99"/>
       <c r="M67" s="58"/>
     </row>
     <row r="68" spans="1:13" ht="15.75" thickBot="1">
@@ -10533,7 +10561,7 @@
       <c r="B68" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C68" s="20"/>
+      <c r="C68" s="73"/>
       <c r="D68" s="73"/>
       <c r="E68" s="73"/>
       <c r="F68" s="73"/>
@@ -10543,10 +10571,10 @@
       </c>
       <c r="I68" s="63"/>
       <c r="J68" s="63"/>
-      <c r="K68" s="100" t="s">
+      <c r="K68" s="98" t="s">
         <v>291</v>
       </c>
-      <c r="L68" s="101"/>
+      <c r="L68" s="99"/>
       <c r="M68" s="58"/>
     </row>
     <row r="69" spans="1:13" ht="15.75" thickBot="1">
@@ -10601,7 +10629,9 @@
       <c r="E71" s="73"/>
       <c r="F71" s="73"/>
       <c r="G71" s="58"/>
-      <c r="H71" s="20"/>
+      <c r="H71" s="75" t="s">
+        <v>333</v>
+      </c>
       <c r="I71" s="20"/>
       <c r="J71" s="20"/>
       <c r="K71" s="95" t="s">
@@ -10623,8 +10653,10 @@
       <c r="H72" s="20"/>
       <c r="I72" s="20"/>
       <c r="J72" s="20"/>
-      <c r="K72" s="97"/>
-      <c r="L72" s="98"/>
+      <c r="K72" s="95" t="s">
+        <v>328</v>
+      </c>
+      <c r="L72" s="96"/>
       <c r="M72" s="58"/>
     </row>
     <row r="73" spans="1:13" ht="15.75" thickBot="1">
@@ -10697,7 +10729,7 @@
       </c>
       <c r="C76" s="20"/>
       <c r="D76" s="73"/>
-      <c r="E76" s="20"/>
+      <c r="E76" s="73"/>
       <c r="F76" s="20"/>
       <c r="G76" s="58"/>
       <c r="H76" s="19" t="s">
@@ -10706,7 +10738,7 @@
       <c r="I76" s="20"/>
       <c r="J76" s="73"/>
       <c r="K76" s="73"/>
-      <c r="L76" s="20"/>
+      <c r="L76" s="73"/>
       <c r="M76" s="58"/>
     </row>
     <row r="77" spans="1:13" ht="15.75" thickBot="1">
@@ -10722,7 +10754,7 @@
       <c r="H77" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="I77" s="20"/>
+      <c r="I77" s="73"/>
       <c r="J77" s="73"/>
       <c r="K77" s="73"/>
       <c r="L77" s="73"/>
@@ -10779,9 +10811,9 @@
       <c r="H80" s="19" t="s">
         <v>181</v>
       </c>
-      <c r="I80" s="20"/>
+      <c r="I80" s="100"/>
       <c r="J80" s="73"/>
-      <c r="K80" s="20"/>
+      <c r="K80" s="73"/>
       <c r="L80" s="20"/>
       <c r="M80" s="58"/>
     </row>
@@ -10855,7 +10887,7 @@
       <c r="H84" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="I84" s="20"/>
+      <c r="I84" s="100"/>
       <c r="J84" s="73"/>
       <c r="K84" s="20"/>
       <c r="L84" s="73"/>
@@ -10907,7 +10939,7 @@
       <c r="C87" s="73"/>
       <c r="D87" s="73"/>
       <c r="E87" s="73"/>
-      <c r="F87" s="20"/>
+      <c r="F87" s="73"/>
       <c r="G87" s="58"/>
       <c r="H87" s="19" t="s">
         <v>188</v>
@@ -10982,7 +11014,7 @@
       </c>
       <c r="C91" s="20"/>
       <c r="D91" s="73"/>
-      <c r="E91" s="20"/>
+      <c r="E91" s="73"/>
       <c r="F91" s="73"/>
       <c r="G91" s="58"/>
       <c r="H91" s="19" t="s">
@@ -11001,7 +11033,7 @@
       </c>
       <c r="C92" s="73"/>
       <c r="D92" s="73"/>
-      <c r="E92" s="20"/>
+      <c r="E92" s="73"/>
       <c r="F92" s="20"/>
       <c r="G92" s="58"/>
       <c r="H92" s="19" t="s">
@@ -11056,7 +11088,7 @@
       <c r="B95" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="C95" s="20"/>
+      <c r="C95" s="73"/>
       <c r="D95" s="73"/>
       <c r="E95" s="73"/>
       <c r="F95" s="73"/>
@@ -11140,7 +11172,7 @@
       <c r="H99" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="I99" s="20"/>
+      <c r="I99" s="73"/>
       <c r="J99" s="73"/>
       <c r="K99" s="73"/>
       <c r="L99" s="20"/>
@@ -11189,7 +11221,7 @@
       <c r="B102" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="C102" s="20"/>
+      <c r="C102" s="73"/>
       <c r="D102" s="73"/>
       <c r="E102" s="73"/>
       <c r="F102" s="73"/>
@@ -11280,7 +11312,7 @@
       <c r="C106" s="20"/>
       <c r="D106" s="73"/>
       <c r="E106" s="73"/>
-      <c r="F106" s="20"/>
+      <c r="F106" s="73"/>
       <c r="G106" s="58"/>
       <c r="H106" s="19" t="s">
         <v>203</v>
@@ -11324,7 +11356,7 @@
         <v>205</v>
       </c>
       <c r="I108" s="72"/>
-      <c r="J108" s="20"/>
+      <c r="J108" s="73"/>
       <c r="K108" s="73"/>
       <c r="L108" s="73"/>
       <c r="M108" s="58"/>
@@ -11336,7 +11368,7 @@
       </c>
       <c r="C109" s="20"/>
       <c r="D109" s="73"/>
-      <c r="E109" s="20"/>
+      <c r="E109" s="73"/>
       <c r="F109" s="73"/>
       <c r="G109" s="58"/>
       <c r="H109" s="19" t="s">
@@ -11355,7 +11387,7 @@
       </c>
       <c r="C110" s="73"/>
       <c r="D110" s="73"/>
-      <c r="E110" s="20"/>
+      <c r="E110" s="73"/>
       <c r="F110" s="20"/>
       <c r="G110" s="58"/>
       <c r="H110" s="19" t="s">
@@ -11433,7 +11465,7 @@
         <v>300</v>
       </c>
       <c r="D114" s="73"/>
-      <c r="E114" s="20"/>
+      <c r="E114" s="73"/>
       <c r="F114" s="20"/>
       <c r="G114" s="58"/>
       <c r="H114" s="19" t="s">
@@ -11450,7 +11482,7 @@
       <c r="B115" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="C115" s="20"/>
+      <c r="C115" s="100"/>
       <c r="D115" s="73"/>
       <c r="E115" s="73"/>
       <c r="F115" s="20"/>
@@ -11481,7 +11513,7 @@
         <v>286</v>
       </c>
       <c r="J116" s="73"/>
-      <c r="K116" s="20"/>
+      <c r="K116" s="73"/>
       <c r="L116" s="73"/>
       <c r="M116" s="58"/>
     </row>
@@ -11514,7 +11546,7 @@
       <c r="C118" s="20"/>
       <c r="D118" s="73"/>
       <c r="E118" s="73"/>
-      <c r="F118" s="20"/>
+      <c r="F118" s="73"/>
       <c r="G118" s="58"/>
       <c r="H118" s="19" t="s">
         <v>215</v>
@@ -11578,7 +11610,7 @@
       </c>
       <c r="I121" s="73"/>
       <c r="J121" s="73"/>
-      <c r="K121" s="20"/>
+      <c r="K121" s="73"/>
       <c r="L121" s="73"/>
       <c r="M121" s="58"/>
     </row>
@@ -11682,7 +11714,7 @@
       <c r="B127" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="C127" s="20"/>
+      <c r="C127" s="100"/>
       <c r="D127" s="73"/>
       <c r="E127" s="20"/>
       <c r="F127" s="73"/>
@@ -11728,7 +11760,7 @@
       <c r="H129" s="19" t="s">
         <v>225</v>
       </c>
-      <c r="I129" s="20"/>
+      <c r="I129" s="73"/>
       <c r="J129" s="73"/>
       <c r="K129" s="73"/>
       <c r="L129" s="20"/>
@@ -11797,7 +11829,7 @@
         <v>124</v>
       </c>
       <c r="C133" s="73"/>
-      <c r="D133" s="20"/>
+      <c r="D133" s="73"/>
       <c r="E133" s="73"/>
       <c r="F133" s="20"/>
       <c r="G133" s="58"/>
@@ -11943,7 +11975,7 @@
       <c r="B140" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="C140" s="20"/>
+      <c r="C140" s="100"/>
       <c r="D140" s="73"/>
       <c r="E140" s="20"/>
       <c r="F140" s="73"/>
@@ -12137,7 +12169,7 @@
       </c>
       <c r="C149" s="73"/>
       <c r="D149" s="73"/>
-      <c r="E149" s="20"/>
+      <c r="E149" s="73"/>
       <c r="F149" s="73"/>
       <c r="G149" s="4"/>
       <c r="H149" s="44" t="s">

</xml_diff>

<commit_message>
the number of items needing fixing is too damn high
*meme-rised*
</commit_message>
<xml_diff>
--- a/check list.xlsx
+++ b/check list.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="337">
   <si>
     <t>ARMOR</t>
   </si>
@@ -1022,6 +1022,12 @@
   </si>
   <si>
     <t>Scarab of Death</t>
+  </si>
+  <si>
+    <t>Ras Algethi</t>
+  </si>
+  <si>
+    <t>The Idiot Ball</t>
   </si>
 </sst>
 </file>
@@ -1389,7 +1395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1648,6 +1654,9 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1678,7 +1687,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2517,13 +2526,13 @@
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
       <c r="G27" s="7"/>
-      <c r="H27" s="91" t="s">
+      <c r="H27" s="92" t="s">
         <v>170</v>
       </c>
-      <c r="I27" s="91"/>
-      <c r="J27" s="91"/>
-      <c r="K27" s="91"/>
-      <c r="L27" s="91"/>
+      <c r="I27" s="92"/>
+      <c r="J27" s="92"/>
+      <c r="K27" s="92"/>
+      <c r="L27" s="92"/>
       <c r="M27" s="7"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1">
@@ -2678,13 +2687,13 @@
       <c r="E36" s="20"/>
       <c r="F36" s="29"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="91" t="s">
+      <c r="H36" s="92" t="s">
         <v>171</v>
       </c>
-      <c r="I36" s="91"/>
-      <c r="J36" s="91"/>
-      <c r="K36" s="91"/>
-      <c r="L36" s="91"/>
+      <c r="I36" s="92"/>
+      <c r="J36" s="92"/>
+      <c r="K36" s="92"/>
+      <c r="L36" s="92"/>
       <c r="M36" s="7"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
@@ -2845,13 +2854,13 @@
         <v>3</v>
       </c>
       <c r="G45" s="7"/>
-      <c r="H45" s="91" t="s">
+      <c r="H45" s="92" t="s">
         <v>172</v>
       </c>
-      <c r="I45" s="91"/>
-      <c r="J45" s="91"/>
-      <c r="K45" s="91"/>
-      <c r="L45" s="91"/>
+      <c r="I45" s="92"/>
+      <c r="J45" s="92"/>
+      <c r="K45" s="92"/>
+      <c r="L45" s="92"/>
       <c r="M45" s="7"/>
     </row>
     <row r="46" spans="1:13" ht="15.75" thickBot="1">
@@ -3000,13 +3009,13 @@
       <c r="E54" s="39"/>
       <c r="F54" s="39"/>
       <c r="G54" s="7"/>
-      <c r="H54" s="91" t="s">
+      <c r="H54" s="92" t="s">
         <v>173</v>
       </c>
-      <c r="I54" s="91"/>
-      <c r="J54" s="91"/>
-      <c r="K54" s="91"/>
-      <c r="L54" s="91"/>
+      <c r="I54" s="92"/>
+      <c r="J54" s="92"/>
+      <c r="K54" s="92"/>
+      <c r="L54" s="92"/>
       <c r="M54" s="7"/>
     </row>
     <row r="55" spans="1:13" ht="15.75" thickBot="1">
@@ -3155,13 +3164,13 @@
       <c r="E63" s="20"/>
       <c r="F63" s="20"/>
       <c r="G63" s="7"/>
-      <c r="H63" s="91" t="s">
+      <c r="H63" s="92" t="s">
         <v>174</v>
       </c>
-      <c r="I63" s="91"/>
-      <c r="J63" s="91"/>
-      <c r="K63" s="91"/>
-      <c r="L63" s="91"/>
+      <c r="I63" s="92"/>
+      <c r="J63" s="92"/>
+      <c r="K63" s="92"/>
+      <c r="L63" s="92"/>
       <c r="M63" s="7"/>
     </row>
     <row r="64" spans="1:13" ht="15.75" thickBot="1">
@@ -4470,11 +4479,11 @@
       <c r="E132" s="20"/>
       <c r="F132" s="20"/>
       <c r="G132" s="7"/>
-      <c r="H132" s="90"/>
-      <c r="I132" s="90"/>
-      <c r="J132" s="90"/>
-      <c r="K132" s="90"/>
-      <c r="L132" s="90"/>
+      <c r="H132" s="91"/>
+      <c r="I132" s="91"/>
+      <c r="J132" s="91"/>
+      <c r="K132" s="91"/>
+      <c r="L132" s="91"/>
       <c r="M132" s="7"/>
     </row>
     <row r="133" spans="1:14" ht="18" thickBot="1">
@@ -6220,13 +6229,13 @@
       <c r="E30" s="20"/>
       <c r="F30" s="20"/>
       <c r="G30" s="58"/>
-      <c r="H30" s="92" t="s">
+      <c r="H30" s="93" t="s">
         <v>170</v>
       </c>
-      <c r="I30" s="93"/>
-      <c r="J30" s="93"/>
-      <c r="K30" s="93"/>
-      <c r="L30" s="94"/>
+      <c r="I30" s="94"/>
+      <c r="J30" s="94"/>
+      <c r="K30" s="94"/>
+      <c r="L30" s="95"/>
       <c r="M30" s="58"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1">
@@ -6381,13 +6390,13 @@
       <c r="E39" s="20"/>
       <c r="F39" s="62"/>
       <c r="G39" s="58"/>
-      <c r="H39" s="92" t="s">
+      <c r="H39" s="93" t="s">
         <v>171</v>
       </c>
-      <c r="I39" s="93"/>
-      <c r="J39" s="93"/>
-      <c r="K39" s="93"/>
-      <c r="L39" s="94"/>
+      <c r="I39" s="94"/>
+      <c r="J39" s="94"/>
+      <c r="K39" s="94"/>
+      <c r="L39" s="95"/>
       <c r="M39" s="58"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" thickBot="1">
@@ -6548,13 +6557,13 @@
         <v>3</v>
       </c>
       <c r="G48" s="58"/>
-      <c r="H48" s="92" t="s">
+      <c r="H48" s="93" t="s">
         <v>172</v>
       </c>
-      <c r="I48" s="93"/>
-      <c r="J48" s="93"/>
-      <c r="K48" s="93"/>
-      <c r="L48" s="94"/>
+      <c r="I48" s="94"/>
+      <c r="J48" s="94"/>
+      <c r="K48" s="94"/>
+      <c r="L48" s="95"/>
       <c r="M48" s="58"/>
     </row>
     <row r="49" spans="1:13" ht="15.75" thickBot="1">
@@ -6703,13 +6712,13 @@
       <c r="E57" s="39"/>
       <c r="F57" s="39"/>
       <c r="G57" s="58"/>
-      <c r="H57" s="92" t="s">
+      <c r="H57" s="93" t="s">
         <v>173</v>
       </c>
-      <c r="I57" s="93"/>
-      <c r="J57" s="93"/>
-      <c r="K57" s="93"/>
-      <c r="L57" s="94"/>
+      <c r="I57" s="94"/>
+      <c r="J57" s="94"/>
+      <c r="K57" s="94"/>
+      <c r="L57" s="95"/>
       <c r="M57" s="58"/>
     </row>
     <row r="58" spans="1:13" ht="15.75" thickBot="1">
@@ -6858,13 +6867,13 @@
       <c r="E66" s="20"/>
       <c r="F66" s="20"/>
       <c r="G66" s="58"/>
-      <c r="H66" s="92" t="s">
+      <c r="H66" s="93" t="s">
         <v>174</v>
       </c>
-      <c r="I66" s="93"/>
-      <c r="J66" s="93"/>
-      <c r="K66" s="93"/>
-      <c r="L66" s="94"/>
+      <c r="I66" s="94"/>
+      <c r="J66" s="94"/>
+      <c r="K66" s="94"/>
+      <c r="L66" s="95"/>
       <c r="M66" s="58"/>
     </row>
     <row r="67" spans="1:13" ht="15.75" thickBot="1">
@@ -9221,8 +9230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B29" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView tabSelected="1" topLeftCell="G7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I115" sqref="I115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9242,40 +9251,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="23.25" customHeight="1">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="98" t="s">
         <v>284</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97"/>
-      <c r="L1" s="97"/>
-      <c r="M1" s="97"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1">
-      <c r="A2" s="97"/>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
+      <c r="A2" s="98"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
       <c r="N2" s="1"/>
       <c r="O2" s="69"/>
       <c r="P2" s="70" t="s">
@@ -9284,19 +9293,19 @@
       <c r="Q2" s="1"/>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1">
-      <c r="A3" s="97"/>
-      <c r="B3" s="97"/>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
+      <c r="A3" s="98"/>
+      <c r="B3" s="98"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -9384,7 +9393,7 @@
       <c r="B7" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="39"/>
+      <c r="C7" s="101"/>
       <c r="D7" s="74"/>
       <c r="E7" s="74"/>
       <c r="F7" s="74"/>
@@ -9394,7 +9403,7 @@
       </c>
       <c r="I7" s="20"/>
       <c r="J7" s="73"/>
-      <c r="K7" s="20"/>
+      <c r="K7" s="73"/>
       <c r="L7" s="73"/>
       <c r="M7" s="58"/>
     </row>
@@ -9403,7 +9412,7 @@
       <c r="B8" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="100"/>
+      <c r="C8" s="73"/>
       <c r="D8" s="73"/>
       <c r="E8" s="73"/>
       <c r="F8" s="73"/>
@@ -9726,7 +9735,7 @@
       <c r="B25" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="80"/>
+      <c r="C25" s="73"/>
       <c r="D25" s="73"/>
       <c r="E25" s="20"/>
       <c r="F25" s="20"/>
@@ -9808,7 +9817,7 @@
       <c r="B29" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="20"/>
+      <c r="C29" s="73"/>
       <c r="D29" s="20"/>
       <c r="E29" s="73"/>
       <c r="F29" s="20"/>
@@ -9832,13 +9841,13 @@
       <c r="E30" s="73"/>
       <c r="F30" s="73"/>
       <c r="G30" s="58"/>
-      <c r="H30" s="92" t="s">
+      <c r="H30" s="93" t="s">
         <v>170</v>
       </c>
-      <c r="I30" s="93"/>
-      <c r="J30" s="93"/>
-      <c r="K30" s="93"/>
-      <c r="L30" s="94"/>
+      <c r="I30" s="94"/>
+      <c r="J30" s="94"/>
+      <c r="K30" s="94"/>
+      <c r="L30" s="95"/>
       <c r="M30" s="58"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1">
@@ -9846,7 +9855,7 @@
       <c r="B31" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="20"/>
+      <c r="C31" s="73"/>
       <c r="D31" s="73"/>
       <c r="E31" s="73"/>
       <c r="F31" s="20"/>
@@ -9854,7 +9863,9 @@
       <c r="H31" s="76" t="s">
         <v>294</v>
       </c>
-      <c r="I31" s="63"/>
+      <c r="I31" s="76" t="s">
+        <v>335</v>
+      </c>
       <c r="J31" s="63"/>
       <c r="K31" s="63"/>
       <c r="L31" s="63"/>
@@ -9873,7 +9884,9 @@
       <c r="H32" s="76" t="s">
         <v>308</v>
       </c>
-      <c r="I32" s="63"/>
+      <c r="I32" s="76" t="s">
+        <v>336</v>
+      </c>
       <c r="J32" s="63"/>
       <c r="K32" s="63"/>
       <c r="L32" s="63"/>
@@ -9928,7 +9941,7 @@
       <c r="B35" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C35" s="20"/>
+      <c r="C35" s="73"/>
       <c r="D35" s="73"/>
       <c r="E35" s="20"/>
       <c r="F35" s="20"/>
@@ -9966,7 +9979,7 @@
       <c r="B37" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="100"/>
+      <c r="C37" s="73"/>
       <c r="D37" s="73"/>
       <c r="E37" s="73"/>
       <c r="F37" s="20"/>
@@ -10007,13 +10020,13 @@
       <c r="E39" s="73"/>
       <c r="F39" s="62"/>
       <c r="G39" s="58"/>
-      <c r="H39" s="92" t="s">
+      <c r="H39" s="93" t="s">
         <v>171</v>
       </c>
-      <c r="I39" s="93"/>
-      <c r="J39" s="93"/>
-      <c r="K39" s="93"/>
-      <c r="L39" s="94"/>
+      <c r="I39" s="94"/>
+      <c r="J39" s="94"/>
+      <c r="K39" s="94"/>
+      <c r="L39" s="95"/>
       <c r="M39" s="58"/>
     </row>
     <row r="40" spans="1:13" ht="30.75" thickBot="1">
@@ -10125,14 +10138,14 @@
       <c r="L44" s="20"/>
       <c r="M44" s="58"/>
     </row>
-    <row r="45" spans="1:13" ht="15.75" thickBot="1">
+    <row r="45" spans="1:13" ht="24" customHeight="1" thickBot="1">
       <c r="A45" s="58"/>
       <c r="B45" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="C45" s="20"/>
+      <c r="C45" s="73"/>
       <c r="D45" s="73"/>
-      <c r="E45" s="20"/>
+      <c r="E45" s="73"/>
       <c r="F45" s="73"/>
       <c r="G45" s="58"/>
       <c r="H45" s="75" t="s">
@@ -10196,13 +10209,13 @@
         <v>3</v>
       </c>
       <c r="G48" s="58"/>
-      <c r="H48" s="92" t="s">
+      <c r="H48" s="93" t="s">
         <v>172</v>
       </c>
-      <c r="I48" s="93"/>
-      <c r="J48" s="93"/>
-      <c r="K48" s="93"/>
-      <c r="L48" s="94"/>
+      <c r="I48" s="94"/>
+      <c r="J48" s="94"/>
+      <c r="K48" s="94"/>
+      <c r="L48" s="95"/>
       <c r="M48" s="58"/>
     </row>
     <row r="49" spans="1:13" ht="15.75" thickBot="1">
@@ -10371,13 +10384,13 @@
       <c r="E57" s="74"/>
       <c r="F57" s="74"/>
       <c r="G57" s="58"/>
-      <c r="H57" s="92" t="s">
+      <c r="H57" s="93" t="s">
         <v>173</v>
       </c>
-      <c r="I57" s="93"/>
-      <c r="J57" s="93"/>
-      <c r="K57" s="93"/>
-      <c r="L57" s="94"/>
+      <c r="I57" s="94"/>
+      <c r="J57" s="94"/>
+      <c r="K57" s="94"/>
+      <c r="L57" s="95"/>
       <c r="M57" s="58"/>
     </row>
     <row r="58" spans="1:13" ht="15.75" thickBot="1">
@@ -10526,13 +10539,13 @@
       <c r="E66" s="73"/>
       <c r="F66" s="73"/>
       <c r="G66" s="58"/>
-      <c r="H66" s="92" t="s">
+      <c r="H66" s="93" t="s">
         <v>174</v>
       </c>
-      <c r="I66" s="93"/>
-      <c r="J66" s="93"/>
-      <c r="K66" s="93"/>
-      <c r="L66" s="94"/>
+      <c r="I66" s="94"/>
+      <c r="J66" s="94"/>
+      <c r="K66" s="94"/>
+      <c r="L66" s="95"/>
       <c r="M66" s="58"/>
     </row>
     <row r="67" spans="1:13" ht="15.75" thickBot="1">
@@ -10550,10 +10563,10 @@
       </c>
       <c r="I67" s="63"/>
       <c r="J67" s="63"/>
-      <c r="K67" s="98" t="s">
+      <c r="K67" s="99" t="s">
         <v>290</v>
       </c>
-      <c r="L67" s="99"/>
+      <c r="L67" s="100"/>
       <c r="M67" s="58"/>
     </row>
     <row r="68" spans="1:13" ht="15.75" thickBot="1">
@@ -10571,10 +10584,10 @@
       </c>
       <c r="I68" s="63"/>
       <c r="J68" s="63"/>
-      <c r="K68" s="98" t="s">
+      <c r="K68" s="99" t="s">
         <v>291</v>
       </c>
-      <c r="L68" s="99"/>
+      <c r="L68" s="100"/>
       <c r="M68" s="58"/>
     </row>
     <row r="69" spans="1:13" ht="15.75" thickBot="1">
@@ -10592,10 +10605,10 @@
       </c>
       <c r="I69" s="20"/>
       <c r="J69" s="20"/>
-      <c r="K69" s="95" t="s">
+      <c r="K69" s="96" t="s">
         <v>298</v>
       </c>
-      <c r="L69" s="96"/>
+      <c r="L69" s="97"/>
       <c r="M69" s="58"/>
     </row>
     <row r="70" spans="1:13" ht="15.75" thickBot="1">
@@ -10613,10 +10626,10 @@
       </c>
       <c r="I70" s="20"/>
       <c r="J70" s="20"/>
-      <c r="K70" s="95" t="s">
+      <c r="K70" s="96" t="s">
         <v>299</v>
       </c>
-      <c r="L70" s="96"/>
+      <c r="L70" s="97"/>
       <c r="M70" s="58"/>
     </row>
     <row r="71" spans="1:13" ht="15.75" thickBot="1">
@@ -10634,10 +10647,10 @@
       </c>
       <c r="I71" s="20"/>
       <c r="J71" s="20"/>
-      <c r="K71" s="95" t="s">
+      <c r="K71" s="96" t="s">
         <v>314</v>
       </c>
-      <c r="L71" s="96"/>
+      <c r="L71" s="97"/>
       <c r="M71" s="58"/>
     </row>
     <row r="72" spans="1:13" ht="15.75" thickBot="1">
@@ -10653,10 +10666,10 @@
       <c r="H72" s="20"/>
       <c r="I72" s="20"/>
       <c r="J72" s="20"/>
-      <c r="K72" s="95" t="s">
+      <c r="K72" s="96" t="s">
         <v>328</v>
       </c>
-      <c r="L72" s="96"/>
+      <c r="L72" s="97"/>
       <c r="M72" s="58"/>
     </row>
     <row r="73" spans="1:13" ht="15.75" thickBot="1">
@@ -10683,7 +10696,7 @@
       </c>
       <c r="C74" s="73"/>
       <c r="D74" s="73"/>
-      <c r="E74" s="20"/>
+      <c r="E74" s="73"/>
       <c r="F74" s="73"/>
       <c r="G74" s="58"/>
       <c r="H74" s="13" t="s">
@@ -10735,7 +10748,7 @@
       <c r="H76" s="19" t="s">
         <v>177</v>
       </c>
-      <c r="I76" s="20"/>
+      <c r="I76" s="73"/>
       <c r="J76" s="73"/>
       <c r="K76" s="73"/>
       <c r="L76" s="73"/>
@@ -10811,7 +10824,7 @@
       <c r="H80" s="19" t="s">
         <v>181</v>
       </c>
-      <c r="I80" s="100"/>
+      <c r="I80" s="90"/>
       <c r="J80" s="73"/>
       <c r="K80" s="73"/>
       <c r="L80" s="20"/>
@@ -10887,7 +10900,7 @@
       <c r="H84" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="I84" s="100"/>
+      <c r="I84" s="73"/>
       <c r="J84" s="73"/>
       <c r="K84" s="20"/>
       <c r="L84" s="73"/>
@@ -10898,7 +10911,7 @@
       <c r="B85" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="C85" s="20"/>
+      <c r="C85" s="73"/>
       <c r="D85" s="73"/>
       <c r="E85" s="20"/>
       <c r="F85" s="73"/>
@@ -11001,7 +11014,7 @@
       <c r="H90" s="19" t="s">
         <v>191</v>
       </c>
-      <c r="I90" s="20"/>
+      <c r="I90" s="90"/>
       <c r="J90" s="20"/>
       <c r="K90" s="73"/>
       <c r="L90" s="20"/>
@@ -11431,7 +11444,7 @@
       <c r="H112" s="19" t="s">
         <v>209</v>
       </c>
-      <c r="I112" s="20"/>
+      <c r="I112" s="90"/>
       <c r="J112" s="73"/>
       <c r="K112" s="73"/>
       <c r="L112" s="20"/>
@@ -11442,7 +11455,7 @@
       <c r="B113" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="C113" s="20"/>
+      <c r="C113" s="90"/>
       <c r="D113" s="73"/>
       <c r="E113" s="20"/>
       <c r="F113" s="73"/>
@@ -11482,7 +11495,7 @@
       <c r="B115" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="C115" s="100"/>
+      <c r="C115" s="73"/>
       <c r="D115" s="73"/>
       <c r="E115" s="73"/>
       <c r="F115" s="20"/>
@@ -11543,7 +11556,7 @@
       <c r="B118" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="C118" s="20"/>
+      <c r="C118" s="90"/>
       <c r="D118" s="73"/>
       <c r="E118" s="73"/>
       <c r="F118" s="73"/>
@@ -11551,7 +11564,7 @@
       <c r="H118" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="I118" s="20"/>
+      <c r="I118" s="90"/>
       <c r="J118" s="20"/>
       <c r="K118" s="73"/>
       <c r="L118" s="73"/>
@@ -11714,7 +11727,7 @@
       <c r="B127" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="C127" s="100"/>
+      <c r="C127" s="73"/>
       <c r="D127" s="73"/>
       <c r="E127" s="20"/>
       <c r="F127" s="73"/>
@@ -11955,7 +11968,7 @@
       <c r="B139" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="C139" s="20"/>
+      <c r="C139" s="73"/>
       <c r="D139" s="73"/>
       <c r="E139" s="73"/>
       <c r="F139" s="20"/>
@@ -11975,7 +11988,7 @@
       <c r="B140" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="C140" s="100"/>
+      <c r="C140" s="73"/>
       <c r="D140" s="73"/>
       <c r="E140" s="20"/>
       <c r="F140" s="73"/>
@@ -12109,7 +12122,7 @@
       <c r="B146" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="C146" s="20"/>
+      <c r="C146" s="90"/>
       <c r="D146" s="73"/>
       <c r="E146" s="73"/>
       <c r="F146" s="73"/>
@@ -12129,7 +12142,7 @@
       <c r="B147" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="C147" s="20"/>
+      <c r="C147" s="90"/>
       <c r="D147" s="73"/>
       <c r="E147" s="73"/>
       <c r="F147" s="73"/>

</xml_diff>

<commit_message>
items updated/ umo updated
i have started work on umo page, already done many umos.
</commit_message>
<xml_diff>
--- a/check list.xlsx
+++ b/check list.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="356">
   <si>
     <t>ARMOR</t>
   </si>
@@ -1028,13 +1028,70 @@
   </si>
   <si>
     <t>The Idiot Ball</t>
+  </si>
+  <si>
+    <t>Elemental Band</t>
+  </si>
+  <si>
+    <t>Evenstar</t>
+  </si>
+  <si>
+    <t>Ten Pin Striker</t>
+  </si>
+  <si>
+    <t>Solitude</t>
+  </si>
+  <si>
+    <t>Marksman's Eye</t>
+  </si>
+  <si>
+    <t>Essence of Itherael</t>
+  </si>
+  <si>
+    <t>Heart of Frost</t>
+  </si>
+  <si>
+    <t>Periapt of Life</t>
+  </si>
+  <si>
+    <t>Wrathspirit</t>
+  </si>
+  <si>
+    <t>Larzuk's Round Shot</t>
+  </si>
+  <si>
+    <t>Farnham's Lost Marble</t>
+  </si>
+  <si>
+    <t>The Moon Crystal</t>
+  </si>
+  <si>
+    <t>The Demon Core</t>
+  </si>
+  <si>
+    <t>Uldyssian's Spirit</t>
+  </si>
+  <si>
+    <t>Relic of Yaerius</t>
+  </si>
+  <si>
+    <t>Nor Tiraj's Flaming Sphere</t>
+  </si>
+  <si>
+    <t>Crystal of Tears</t>
+  </si>
+  <si>
+    <t>Zayl's Soul Orb</t>
+  </si>
+  <si>
+    <t>The Endless Light</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="23">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1196,6 +1253,19 @@
       <color rgb="FF111111"/>
       <name val="Verdana"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1395,7 +1465,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1657,6 +1727,9 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1687,7 +1760,10 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2526,13 +2602,13 @@
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
       <c r="G27" s="7"/>
-      <c r="H27" s="92" t="s">
+      <c r="H27" s="93" t="s">
         <v>170</v>
       </c>
-      <c r="I27" s="92"/>
-      <c r="J27" s="92"/>
-      <c r="K27" s="92"/>
-      <c r="L27" s="92"/>
+      <c r="I27" s="93"/>
+      <c r="J27" s="93"/>
+      <c r="K27" s="93"/>
+      <c r="L27" s="93"/>
       <c r="M27" s="7"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1">
@@ -2687,13 +2763,13 @@
       <c r="E36" s="20"/>
       <c r="F36" s="29"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="92" t="s">
+      <c r="H36" s="93" t="s">
         <v>171</v>
       </c>
-      <c r="I36" s="92"/>
-      <c r="J36" s="92"/>
-      <c r="K36" s="92"/>
-      <c r="L36" s="92"/>
+      <c r="I36" s="93"/>
+      <c r="J36" s="93"/>
+      <c r="K36" s="93"/>
+      <c r="L36" s="93"/>
       <c r="M36" s="7"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
@@ -2854,13 +2930,13 @@
         <v>3</v>
       </c>
       <c r="G45" s="7"/>
-      <c r="H45" s="92" t="s">
+      <c r="H45" s="93" t="s">
         <v>172</v>
       </c>
-      <c r="I45" s="92"/>
-      <c r="J45" s="92"/>
-      <c r="K45" s="92"/>
-      <c r="L45" s="92"/>
+      <c r="I45" s="93"/>
+      <c r="J45" s="93"/>
+      <c r="K45" s="93"/>
+      <c r="L45" s="93"/>
       <c r="M45" s="7"/>
     </row>
     <row r="46" spans="1:13" ht="15.75" thickBot="1">
@@ -3009,13 +3085,13 @@
       <c r="E54" s="39"/>
       <c r="F54" s="39"/>
       <c r="G54" s="7"/>
-      <c r="H54" s="92" t="s">
+      <c r="H54" s="93" t="s">
         <v>173</v>
       </c>
-      <c r="I54" s="92"/>
-      <c r="J54" s="92"/>
-      <c r="K54" s="92"/>
-      <c r="L54" s="92"/>
+      <c r="I54" s="93"/>
+      <c r="J54" s="93"/>
+      <c r="K54" s="93"/>
+      <c r="L54" s="93"/>
       <c r="M54" s="7"/>
     </row>
     <row r="55" spans="1:13" ht="15.75" thickBot="1">
@@ -3164,13 +3240,13 @@
       <c r="E63" s="20"/>
       <c r="F63" s="20"/>
       <c r="G63" s="7"/>
-      <c r="H63" s="92" t="s">
+      <c r="H63" s="93" t="s">
         <v>174</v>
       </c>
-      <c r="I63" s="92"/>
-      <c r="J63" s="92"/>
-      <c r="K63" s="92"/>
-      <c r="L63" s="92"/>
+      <c r="I63" s="93"/>
+      <c r="J63" s="93"/>
+      <c r="K63" s="93"/>
+      <c r="L63" s="93"/>
       <c r="M63" s="7"/>
     </row>
     <row r="64" spans="1:13" ht="15.75" thickBot="1">
@@ -4479,11 +4555,11 @@
       <c r="E132" s="20"/>
       <c r="F132" s="20"/>
       <c r="G132" s="7"/>
-      <c r="H132" s="91"/>
-      <c r="I132" s="91"/>
-      <c r="J132" s="91"/>
-      <c r="K132" s="91"/>
-      <c r="L132" s="91"/>
+      <c r="H132" s="92"/>
+      <c r="I132" s="92"/>
+      <c r="J132" s="92"/>
+      <c r="K132" s="92"/>
+      <c r="L132" s="92"/>
       <c r="M132" s="7"/>
     </row>
     <row r="133" spans="1:14" ht="18" thickBot="1">
@@ -6229,13 +6305,13 @@
       <c r="E30" s="20"/>
       <c r="F30" s="20"/>
       <c r="G30" s="58"/>
-      <c r="H30" s="93" t="s">
+      <c r="H30" s="94" t="s">
         <v>170</v>
       </c>
-      <c r="I30" s="94"/>
-      <c r="J30" s="94"/>
-      <c r="K30" s="94"/>
-      <c r="L30" s="95"/>
+      <c r="I30" s="95"/>
+      <c r="J30" s="95"/>
+      <c r="K30" s="95"/>
+      <c r="L30" s="96"/>
       <c r="M30" s="58"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1">
@@ -6390,13 +6466,13 @@
       <c r="E39" s="20"/>
       <c r="F39" s="62"/>
       <c r="G39" s="58"/>
-      <c r="H39" s="93" t="s">
+      <c r="H39" s="94" t="s">
         <v>171</v>
       </c>
-      <c r="I39" s="94"/>
-      <c r="J39" s="94"/>
-      <c r="K39" s="94"/>
-      <c r="L39" s="95"/>
+      <c r="I39" s="95"/>
+      <c r="J39" s="95"/>
+      <c r="K39" s="95"/>
+      <c r="L39" s="96"/>
       <c r="M39" s="58"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" thickBot="1">
@@ -6557,13 +6633,13 @@
         <v>3</v>
       </c>
       <c r="G48" s="58"/>
-      <c r="H48" s="93" t="s">
+      <c r="H48" s="94" t="s">
         <v>172</v>
       </c>
-      <c r="I48" s="94"/>
-      <c r="J48" s="94"/>
-      <c r="K48" s="94"/>
-      <c r="L48" s="95"/>
+      <c r="I48" s="95"/>
+      <c r="J48" s="95"/>
+      <c r="K48" s="95"/>
+      <c r="L48" s="96"/>
       <c r="M48" s="58"/>
     </row>
     <row r="49" spans="1:13" ht="15.75" thickBot="1">
@@ -6712,13 +6788,13 @@
       <c r="E57" s="39"/>
       <c r="F57" s="39"/>
       <c r="G57" s="58"/>
-      <c r="H57" s="93" t="s">
+      <c r="H57" s="94" t="s">
         <v>173</v>
       </c>
-      <c r="I57" s="94"/>
-      <c r="J57" s="94"/>
-      <c r="K57" s="94"/>
-      <c r="L57" s="95"/>
+      <c r="I57" s="95"/>
+      <c r="J57" s="95"/>
+      <c r="K57" s="95"/>
+      <c r="L57" s="96"/>
       <c r="M57" s="58"/>
     </row>
     <row r="58" spans="1:13" ht="15.75" thickBot="1">
@@ -6867,13 +6943,13 @@
       <c r="E66" s="20"/>
       <c r="F66" s="20"/>
       <c r="G66" s="58"/>
-      <c r="H66" s="93" t="s">
+      <c r="H66" s="94" t="s">
         <v>174</v>
       </c>
-      <c r="I66" s="94"/>
-      <c r="J66" s="94"/>
-      <c r="K66" s="94"/>
-      <c r="L66" s="95"/>
+      <c r="I66" s="95"/>
+      <c r="J66" s="95"/>
+      <c r="K66" s="95"/>
+      <c r="L66" s="96"/>
       <c r="M66" s="58"/>
     </row>
     <row r="67" spans="1:13" ht="15.75" thickBot="1">
@@ -9230,8 +9306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I115" sqref="I115"/>
+    <sheetView tabSelected="1" topLeftCell="G48" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I67" sqref="I67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9251,40 +9327,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="23.25" customHeight="1">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="99" t="s">
         <v>284</v>
       </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
-      <c r="H1" s="98"/>
-      <c r="I1" s="98"/>
-      <c r="J1" s="98"/>
-      <c r="K1" s="98"/>
-      <c r="L1" s="98"/>
-      <c r="M1" s="98"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
+      <c r="L1" s="99"/>
+      <c r="M1" s="99"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1">
-      <c r="A2" s="98"/>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
+      <c r="A2" s="99"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
       <c r="N2" s="1"/>
       <c r="O2" s="69"/>
       <c r="P2" s="70" t="s">
@@ -9293,19 +9369,19 @@
       <c r="Q2" s="1"/>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1">
-      <c r="A3" s="98"/>
-      <c r="B3" s="98"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
+      <c r="A3" s="99"/>
+      <c r="B3" s="99"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="99"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -9393,7 +9469,7 @@
       <c r="B7" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="101"/>
+      <c r="C7" s="91"/>
       <c r="D7" s="74"/>
       <c r="E7" s="74"/>
       <c r="F7" s="74"/>
@@ -9667,7 +9743,7 @@
       <c r="H21" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="I21" s="80"/>
+      <c r="I21" s="73"/>
       <c r="J21" s="73"/>
       <c r="K21" s="73"/>
       <c r="L21" s="73"/>
@@ -9726,7 +9802,7 @@
       </c>
       <c r="I24" s="20"/>
       <c r="J24" s="73"/>
-      <c r="K24" s="20"/>
+      <c r="K24" s="73"/>
       <c r="L24" s="20"/>
       <c r="M24" s="58"/>
     </row>
@@ -9737,7 +9813,7 @@
       </c>
       <c r="C25" s="73"/>
       <c r="D25" s="73"/>
-      <c r="E25" s="20"/>
+      <c r="E25" s="73"/>
       <c r="F25" s="20"/>
       <c r="G25" s="58"/>
       <c r="H25" s="19" t="s">
@@ -9841,13 +9917,13 @@
       <c r="E30" s="73"/>
       <c r="F30" s="73"/>
       <c r="G30" s="58"/>
-      <c r="H30" s="93" t="s">
+      <c r="H30" s="94" t="s">
         <v>170</v>
       </c>
-      <c r="I30" s="94"/>
-      <c r="J30" s="94"/>
-      <c r="K30" s="94"/>
-      <c r="L30" s="95"/>
+      <c r="I30" s="95"/>
+      <c r="J30" s="95"/>
+      <c r="K30" s="95"/>
+      <c r="L30" s="96"/>
       <c r="M30" s="58"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1">
@@ -9903,7 +9979,9 @@
       <c r="H33" s="75" t="s">
         <v>310</v>
       </c>
-      <c r="I33" s="20"/>
+      <c r="I33" s="75" t="s">
+        <v>337</v>
+      </c>
       <c r="J33" s="20"/>
       <c r="K33" s="20"/>
       <c r="L33" s="20"/>
@@ -9943,7 +10021,7 @@
       </c>
       <c r="C35" s="73"/>
       <c r="D35" s="73"/>
-      <c r="E35" s="20"/>
+      <c r="E35" s="73"/>
       <c r="F35" s="20"/>
       <c r="G35" s="58"/>
       <c r="H35" s="75" t="s">
@@ -10020,13 +10098,13 @@
       <c r="E39" s="73"/>
       <c r="F39" s="62"/>
       <c r="G39" s="58"/>
-      <c r="H39" s="93" t="s">
+      <c r="H39" s="94" t="s">
         <v>171</v>
       </c>
-      <c r="I39" s="94"/>
-      <c r="J39" s="94"/>
-      <c r="K39" s="94"/>
-      <c r="L39" s="95"/>
+      <c r="I39" s="95"/>
+      <c r="J39" s="95"/>
+      <c r="K39" s="95"/>
+      <c r="L39" s="96"/>
       <c r="M39" s="58"/>
     </row>
     <row r="40" spans="1:13" ht="30.75" thickBot="1">
@@ -10132,7 +10210,9 @@
       <c r="H44" s="75" t="s">
         <v>309</v>
       </c>
-      <c r="I44" s="20"/>
+      <c r="I44" s="75" t="s">
+        <v>338</v>
+      </c>
       <c r="J44" s="20"/>
       <c r="K44" s="20"/>
       <c r="L44" s="20"/>
@@ -10209,13 +10289,13 @@
         <v>3</v>
       </c>
       <c r="G48" s="58"/>
-      <c r="H48" s="93" t="s">
+      <c r="H48" s="94" t="s">
         <v>172</v>
       </c>
-      <c r="I48" s="94"/>
-      <c r="J48" s="94"/>
-      <c r="K48" s="94"/>
-      <c r="L48" s="95"/>
+      <c r="I48" s="95"/>
+      <c r="J48" s="95"/>
+      <c r="K48" s="95"/>
+      <c r="L48" s="96"/>
       <c r="M48" s="58"/>
     </row>
     <row r="49" spans="1:13" ht="15.75" thickBot="1">
@@ -10260,7 +10340,7 @@
       <c r="L50" s="63"/>
       <c r="M50" s="58"/>
     </row>
-    <row r="51" spans="1:13" ht="26.25" thickBot="1">
+    <row r="51" spans="1:13" ht="23.25" thickBot="1">
       <c r="A51" s="58"/>
       <c r="B51" s="19" t="s">
         <v>44</v>
@@ -10273,7 +10353,7 @@
       <c r="H51" s="75" t="s">
         <v>306</v>
       </c>
-      <c r="I51" s="75" t="s">
+      <c r="I51" s="102" t="s">
         <v>331</v>
       </c>
       <c r="J51" s="20"/>
@@ -10384,13 +10464,13 @@
       <c r="E57" s="74"/>
       <c r="F57" s="74"/>
       <c r="G57" s="58"/>
-      <c r="H57" s="93" t="s">
+      <c r="H57" s="94" t="s">
         <v>173</v>
       </c>
-      <c r="I57" s="94"/>
-      <c r="J57" s="94"/>
-      <c r="K57" s="94"/>
-      <c r="L57" s="95"/>
+      <c r="I57" s="95"/>
+      <c r="J57" s="95"/>
+      <c r="K57" s="95"/>
+      <c r="L57" s="96"/>
       <c r="M57" s="58"/>
     </row>
     <row r="58" spans="1:13" ht="15.75" thickBot="1">
@@ -10398,19 +10478,25 @@
       <c r="B58" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="C58" s="20"/>
+      <c r="C58" s="73"/>
       <c r="D58" s="73"/>
       <c r="E58" s="73"/>
       <c r="F58" s="20"/>
       <c r="G58" s="58"/>
-      <c r="H58" s="63"/>
-      <c r="I58" s="63"/>
-      <c r="J58" s="63"/>
+      <c r="H58" s="76" t="s">
+        <v>339</v>
+      </c>
+      <c r="I58" s="103" t="s">
+        <v>346</v>
+      </c>
+      <c r="J58" s="76" t="s">
+        <v>353</v>
+      </c>
       <c r="K58" s="63"/>
       <c r="L58" s="63"/>
       <c r="M58" s="58"/>
     </row>
-    <row r="59" spans="1:13" ht="15.75" thickBot="1">
+    <row r="59" spans="1:13" ht="24.75" thickBot="1">
       <c r="A59" s="58"/>
       <c r="B59" s="38" t="s">
         <v>52</v>
@@ -10420,14 +10506,20 @@
       <c r="E59" s="74"/>
       <c r="F59" s="74"/>
       <c r="G59" s="58"/>
-      <c r="H59" s="63"/>
-      <c r="I59" s="63"/>
-      <c r="J59" s="63"/>
+      <c r="H59" s="76" t="s">
+        <v>340</v>
+      </c>
+      <c r="I59" s="103" t="s">
+        <v>347</v>
+      </c>
+      <c r="J59" s="76" t="s">
+        <v>354</v>
+      </c>
       <c r="K59" s="63"/>
       <c r="L59" s="63"/>
       <c r="M59" s="58"/>
     </row>
-    <row r="60" spans="1:13" ht="15.75" thickBot="1">
+    <row r="60" spans="1:13" ht="23.25" thickBot="1">
       <c r="A60" s="58"/>
       <c r="B60" s="19" t="s">
         <v>53</v>
@@ -10437,9 +10529,15 @@
       <c r="E60" s="20"/>
       <c r="F60" s="20"/>
       <c r="G60" s="58"/>
-      <c r="H60" s="20"/>
-      <c r="I60" s="20"/>
-      <c r="J60" s="20"/>
+      <c r="H60" s="75" t="s">
+        <v>341</v>
+      </c>
+      <c r="I60" s="102" t="s">
+        <v>348</v>
+      </c>
+      <c r="J60" s="102" t="s">
+        <v>355</v>
+      </c>
       <c r="K60" s="20"/>
       <c r="L60" s="20"/>
       <c r="M60" s="58"/>
@@ -10454,8 +10552,12 @@
       <c r="E61" s="73"/>
       <c r="F61" s="73"/>
       <c r="G61" s="58"/>
-      <c r="H61" s="20"/>
-      <c r="I61" s="20"/>
+      <c r="H61" s="102" t="s">
+        <v>342</v>
+      </c>
+      <c r="I61" s="75" t="s">
+        <v>349</v>
+      </c>
       <c r="J61" s="20"/>
       <c r="K61" s="20"/>
       <c r="L61" s="20"/>
@@ -10471,8 +10573,12 @@
       <c r="E62" s="73"/>
       <c r="F62" s="73"/>
       <c r="G62" s="58"/>
-      <c r="H62" s="20"/>
-      <c r="I62" s="20"/>
+      <c r="H62" s="75" t="s">
+        <v>343</v>
+      </c>
+      <c r="I62" s="75" t="s">
+        <v>350</v>
+      </c>
       <c r="J62" s="20"/>
       <c r="K62" s="20"/>
       <c r="L62" s="20"/>
@@ -10488,14 +10594,18 @@
       <c r="E63" s="73"/>
       <c r="F63" s="20"/>
       <c r="G63" s="58"/>
-      <c r="H63" s="20"/>
-      <c r="I63" s="20"/>
+      <c r="H63" s="75" t="s">
+        <v>344</v>
+      </c>
+      <c r="I63" s="75" t="s">
+        <v>351</v>
+      </c>
       <c r="J63" s="20"/>
       <c r="K63" s="20"/>
       <c r="L63" s="20"/>
       <c r="M63" s="58"/>
     </row>
-    <row r="64" spans="1:13" ht="15.75" thickBot="1">
+    <row r="64" spans="1:13" ht="23.25" thickBot="1">
       <c r="A64" s="58"/>
       <c r="B64" s="19" t="s">
         <v>57</v>
@@ -10505,8 +10615,12 @@
       <c r="E64" s="73"/>
       <c r="F64" s="20"/>
       <c r="G64" s="58"/>
-      <c r="H64" s="20"/>
-      <c r="I64" s="20"/>
+      <c r="H64" s="75" t="s">
+        <v>345</v>
+      </c>
+      <c r="I64" s="102" t="s">
+        <v>352</v>
+      </c>
       <c r="J64" s="20"/>
       <c r="K64" s="20"/>
       <c r="L64" s="20"/>
@@ -10539,13 +10653,13 @@
       <c r="E66" s="73"/>
       <c r="F66" s="73"/>
       <c r="G66" s="58"/>
-      <c r="H66" s="93" t="s">
+      <c r="H66" s="94" t="s">
         <v>174</v>
       </c>
-      <c r="I66" s="94"/>
-      <c r="J66" s="94"/>
-      <c r="K66" s="94"/>
-      <c r="L66" s="95"/>
+      <c r="I66" s="95"/>
+      <c r="J66" s="95"/>
+      <c r="K66" s="95"/>
+      <c r="L66" s="96"/>
       <c r="M66" s="58"/>
     </row>
     <row r="67" spans="1:13" ht="15.75" thickBot="1">
@@ -10563,10 +10677,10 @@
       </c>
       <c r="I67" s="63"/>
       <c r="J67" s="63"/>
-      <c r="K67" s="99" t="s">
+      <c r="K67" s="100" t="s">
         <v>290</v>
       </c>
-      <c r="L67" s="100"/>
+      <c r="L67" s="101"/>
       <c r="M67" s="58"/>
     </row>
     <row r="68" spans="1:13" ht="15.75" thickBot="1">
@@ -10584,10 +10698,10 @@
       </c>
       <c r="I68" s="63"/>
       <c r="J68" s="63"/>
-      <c r="K68" s="99" t="s">
+      <c r="K68" s="100" t="s">
         <v>291</v>
       </c>
-      <c r="L68" s="100"/>
+      <c r="L68" s="101"/>
       <c r="M68" s="58"/>
     </row>
     <row r="69" spans="1:13" ht="15.75" thickBot="1">
@@ -10605,10 +10719,10 @@
       </c>
       <c r="I69" s="20"/>
       <c r="J69" s="20"/>
-      <c r="K69" s="96" t="s">
+      <c r="K69" s="97" t="s">
         <v>298</v>
       </c>
-      <c r="L69" s="97"/>
+      <c r="L69" s="98"/>
       <c r="M69" s="58"/>
     </row>
     <row r="70" spans="1:13" ht="15.75" thickBot="1">
@@ -10626,10 +10740,10 @@
       </c>
       <c r="I70" s="20"/>
       <c r="J70" s="20"/>
-      <c r="K70" s="96" t="s">
+      <c r="K70" s="97" t="s">
         <v>299</v>
       </c>
-      <c r="L70" s="97"/>
+      <c r="L70" s="98"/>
       <c r="M70" s="58"/>
     </row>
     <row r="71" spans="1:13" ht="15.75" thickBot="1">
@@ -10647,10 +10761,10 @@
       </c>
       <c r="I71" s="20"/>
       <c r="J71" s="20"/>
-      <c r="K71" s="96" t="s">
+      <c r="K71" s="97" t="s">
         <v>314</v>
       </c>
-      <c r="L71" s="97"/>
+      <c r="L71" s="98"/>
       <c r="M71" s="58"/>
     </row>
     <row r="72" spans="1:13" ht="15.75" thickBot="1">
@@ -10666,10 +10780,10 @@
       <c r="H72" s="20"/>
       <c r="I72" s="20"/>
       <c r="J72" s="20"/>
-      <c r="K72" s="96" t="s">
+      <c r="K72" s="97" t="s">
         <v>328</v>
       </c>
-      <c r="L72" s="97"/>
+      <c r="L72" s="98"/>
       <c r="M72" s="58"/>
     </row>
     <row r="73" spans="1:13" ht="15.75" thickBot="1">
@@ -10876,7 +10990,7 @@
       <c r="C83" s="73"/>
       <c r="D83" s="73"/>
       <c r="E83" s="73"/>
-      <c r="F83" s="20"/>
+      <c r="F83" s="73"/>
       <c r="G83" s="58"/>
       <c r="H83" s="19" t="s">
         <v>184</v>
@@ -10976,7 +11090,7 @@
       <c r="H88" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="I88" s="20"/>
+      <c r="I88" s="73"/>
       <c r="J88" s="73"/>
       <c r="K88" s="73"/>
       <c r="L88" s="20"/>
@@ -10998,7 +11112,7 @@
       <c r="I89" s="20"/>
       <c r="J89" s="73"/>
       <c r="K89" s="73"/>
-      <c r="L89" s="20"/>
+      <c r="L89" s="73"/>
       <c r="M89" s="58"/>
     </row>
     <row r="90" spans="1:13" ht="15.75" thickBot="1">
@@ -11014,7 +11128,7 @@
       <c r="H90" s="19" t="s">
         <v>191</v>
       </c>
-      <c r="I90" s="90"/>
+      <c r="I90" s="73"/>
       <c r="J90" s="20"/>
       <c r="K90" s="73"/>
       <c r="L90" s="20"/>
@@ -11085,7 +11199,7 @@
       <c r="C94" s="73"/>
       <c r="D94" s="73"/>
       <c r="E94" s="73"/>
-      <c r="F94" s="20"/>
+      <c r="F94" s="73"/>
       <c r="G94" s="58"/>
       <c r="H94" s="19" t="s">
         <v>195</v>
@@ -11130,7 +11244,7 @@
       </c>
       <c r="I96" s="20"/>
       <c r="J96" s="20"/>
-      <c r="K96" s="20"/>
+      <c r="K96" s="73"/>
       <c r="L96" s="20"/>
       <c r="M96" s="58"/>
     </row>
@@ -11161,7 +11275,7 @@
       <c r="C98" s="20"/>
       <c r="D98" s="73"/>
       <c r="E98" s="73"/>
-      <c r="F98" s="20"/>
+      <c r="F98" s="73"/>
       <c r="G98" s="58"/>
       <c r="H98" s="19" t="s">
         <v>195</v>
@@ -11217,7 +11331,7 @@
       </c>
       <c r="C101" s="73"/>
       <c r="D101" s="73"/>
-      <c r="E101" s="20"/>
+      <c r="E101" s="73"/>
       <c r="F101" s="20"/>
       <c r="G101" s="58"/>
       <c r="H101" s="19" t="s">
@@ -11390,7 +11504,7 @@
       <c r="I109" s="73"/>
       <c r="J109" s="20"/>
       <c r="K109" s="73"/>
-      <c r="L109" s="20"/>
+      <c r="L109" s="73"/>
       <c r="M109" s="58"/>
     </row>
     <row r="110" spans="1:13" ht="15.75" thickBot="1">
@@ -11444,7 +11558,7 @@
       <c r="H112" s="19" t="s">
         <v>209</v>
       </c>
-      <c r="I112" s="90"/>
+      <c r="I112" s="73"/>
       <c r="J112" s="73"/>
       <c r="K112" s="73"/>
       <c r="L112" s="20"/>
@@ -11455,7 +11569,7 @@
       <c r="B113" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="C113" s="90"/>
+      <c r="C113" s="73"/>
       <c r="D113" s="73"/>
       <c r="E113" s="20"/>
       <c r="F113" s="73"/>
@@ -11503,7 +11617,7 @@
       <c r="H115" s="19" t="s">
         <v>212</v>
       </c>
-      <c r="I115" s="20"/>
+      <c r="I115" s="73"/>
       <c r="J115" s="73"/>
       <c r="K115" s="73"/>
       <c r="L115" s="73"/>
@@ -11548,7 +11662,7 @@
       <c r="I117" s="73"/>
       <c r="J117" s="73"/>
       <c r="K117" s="73"/>
-      <c r="L117" s="20"/>
+      <c r="L117" s="73"/>
       <c r="M117" s="58"/>
     </row>
     <row r="118" spans="1:13" ht="15.75" thickBot="1">
@@ -11556,7 +11670,7 @@
       <c r="B118" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="C118" s="90"/>
+      <c r="C118" s="73"/>
       <c r="D118" s="73"/>
       <c r="E118" s="73"/>
       <c r="F118" s="73"/>
@@ -11564,7 +11678,7 @@
       <c r="H118" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="I118" s="90"/>
+      <c r="I118" s="73"/>
       <c r="J118" s="20"/>
       <c r="K118" s="73"/>
       <c r="L118" s="73"/>
@@ -11583,7 +11697,7 @@
       <c r="H119" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="I119" s="80"/>
+      <c r="I119" s="73"/>
       <c r="J119" s="73"/>
       <c r="K119" s="20"/>
       <c r="L119" s="73"/>
@@ -11717,7 +11831,7 @@
         <v>222</v>
       </c>
       <c r="I126" s="20"/>
-      <c r="J126" s="20"/>
+      <c r="J126" s="73"/>
       <c r="K126" s="20"/>
       <c r="L126" s="20"/>
       <c r="M126" s="58"/>
@@ -11749,7 +11863,7 @@
       <c r="C128" s="83"/>
       <c r="D128" s="82"/>
       <c r="E128" s="74"/>
-      <c r="F128" s="39"/>
+      <c r="F128" s="74"/>
       <c r="G128" s="58"/>
       <c r="H128" s="19" t="s">
         <v>224</v>
@@ -11787,7 +11901,7 @@
       <c r="C130" s="73"/>
       <c r="D130" s="73"/>
       <c r="E130" s="73"/>
-      <c r="F130" s="20"/>
+      <c r="F130" s="73"/>
       <c r="G130" s="58"/>
       <c r="H130" s="19" t="s">
         <v>226</v>
@@ -11814,7 +11928,7 @@
       <c r="I131" s="20"/>
       <c r="J131" s="73"/>
       <c r="K131" s="73"/>
-      <c r="L131" s="20"/>
+      <c r="L131" s="73"/>
       <c r="M131" s="58"/>
     </row>
     <row r="132" spans="1:14" ht="15.75" thickBot="1">
@@ -11844,7 +11958,7 @@
       <c r="C133" s="73"/>
       <c r="D133" s="73"/>
       <c r="E133" s="73"/>
-      <c r="F133" s="20"/>
+      <c r="F133" s="73"/>
       <c r="G133" s="58"/>
       <c r="H133" s="19" t="s">
         <v>229</v>
@@ -12122,7 +12236,7 @@
       <c r="B146" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="C146" s="90"/>
+      <c r="C146" s="73"/>
       <c r="D146" s="73"/>
       <c r="E146" s="73"/>
       <c r="F146" s="73"/>
@@ -12142,7 +12256,7 @@
       <c r="B147" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="C147" s="90"/>
+      <c r="C147" s="73"/>
       <c r="D147" s="73"/>
       <c r="E147" s="73"/>
       <c r="F147" s="73"/>
@@ -12231,7 +12345,7 @@
         <v>141</v>
       </c>
       <c r="C151" s="73"/>
-      <c r="D151" s="20"/>
+      <c r="D151" s="73"/>
       <c r="E151" s="73"/>
       <c r="F151" s="73"/>
       <c r="G151" s="4"/>

</xml_diff>

<commit_message>
many more items done
now fewer items r left, this should be done soon
</commit_message>
<xml_diff>
--- a/check list.xlsx
+++ b/check list.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="381">
   <si>
     <t>ARMOR</t>
   </si>
@@ -1091,6 +1091,75 @@
   </si>
   <si>
     <t>Vizjerei's Necklace</t>
+  </si>
+  <si>
+    <t>Quiv tsin's talisman</t>
+  </si>
+  <si>
+    <t>Der Nebelring</t>
+  </si>
+  <si>
+    <t>Ring of Truth</t>
+  </si>
+  <si>
+    <t>Teganze Pendant</t>
+  </si>
+  <si>
+    <t>Angel Heart</t>
+  </si>
+  <si>
+    <t>Empyrean Band</t>
+  </si>
+  <si>
+    <t>Zakarum Stoning Rock</t>
+  </si>
+  <si>
+    <t>Earth Rouser</t>
+  </si>
+  <si>
+    <t>Eye of the Storm</t>
+  </si>
+  <si>
+    <t>Xorine's Ring</t>
+  </si>
+  <si>
+    <t>Ring of Disengagement</t>
+  </si>
+  <si>
+    <t>Pandemonium</t>
+  </si>
+  <si>
+    <t>Sigil of Tur Dulra</t>
+  </si>
+  <si>
+    <t>Warbringer</t>
+  </si>
+  <si>
+    <t>Explorer's Globe</t>
+  </si>
+  <si>
+    <t>Athulua's Oracle</t>
+  </si>
+  <si>
+    <t>Ripstar</t>
+  </si>
+  <si>
+    <t>The Dreamcatcher</t>
+  </si>
+  <si>
+    <t>Witchmoon</t>
+  </si>
+  <si>
+    <t>Fren Slairea</t>
+  </si>
+  <si>
+    <t>The Boulder</t>
+  </si>
+  <si>
+    <t>Bloodbond</t>
+  </si>
+  <si>
+    <t>Felblood</t>
   </si>
 </sst>
 </file>
@@ -1718,9 +1787,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1764,6 +1830,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2602,13 +2671,13 @@
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
       <c r="G27" s="7"/>
-      <c r="H27" s="93" t="s">
+      <c r="H27" s="92" t="s">
         <v>170</v>
       </c>
-      <c r="I27" s="93"/>
-      <c r="J27" s="93"/>
-      <c r="K27" s="93"/>
-      <c r="L27" s="93"/>
+      <c r="I27" s="92"/>
+      <c r="J27" s="92"/>
+      <c r="K27" s="92"/>
+      <c r="L27" s="92"/>
       <c r="M27" s="7"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1">
@@ -2763,13 +2832,13 @@
       <c r="E36" s="20"/>
       <c r="F36" s="29"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="93" t="s">
+      <c r="H36" s="92" t="s">
         <v>171</v>
       </c>
-      <c r="I36" s="93"/>
-      <c r="J36" s="93"/>
-      <c r="K36" s="93"/>
-      <c r="L36" s="93"/>
+      <c r="I36" s="92"/>
+      <c r="J36" s="92"/>
+      <c r="K36" s="92"/>
+      <c r="L36" s="92"/>
       <c r="M36" s="7"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
@@ -2930,13 +2999,13 @@
         <v>3</v>
       </c>
       <c r="G45" s="7"/>
-      <c r="H45" s="93" t="s">
+      <c r="H45" s="92" t="s">
         <v>172</v>
       </c>
-      <c r="I45" s="93"/>
-      <c r="J45" s="93"/>
-      <c r="K45" s="93"/>
-      <c r="L45" s="93"/>
+      <c r="I45" s="92"/>
+      <c r="J45" s="92"/>
+      <c r="K45" s="92"/>
+      <c r="L45" s="92"/>
       <c r="M45" s="7"/>
     </row>
     <row r="46" spans="1:13" ht="15.75" thickBot="1">
@@ -3085,13 +3154,13 @@
       <c r="E54" s="39"/>
       <c r="F54" s="39"/>
       <c r="G54" s="7"/>
-      <c r="H54" s="93" t="s">
+      <c r="H54" s="92" t="s">
         <v>173</v>
       </c>
-      <c r="I54" s="93"/>
-      <c r="J54" s="93"/>
-      <c r="K54" s="93"/>
-      <c r="L54" s="93"/>
+      <c r="I54" s="92"/>
+      <c r="J54" s="92"/>
+      <c r="K54" s="92"/>
+      <c r="L54" s="92"/>
       <c r="M54" s="7"/>
     </row>
     <row r="55" spans="1:13" ht="15.75" thickBot="1">
@@ -3240,13 +3309,13 @@
       <c r="E63" s="20"/>
       <c r="F63" s="20"/>
       <c r="G63" s="7"/>
-      <c r="H63" s="93" t="s">
+      <c r="H63" s="92" t="s">
         <v>174</v>
       </c>
-      <c r="I63" s="93"/>
-      <c r="J63" s="93"/>
-      <c r="K63" s="93"/>
-      <c r="L63" s="93"/>
+      <c r="I63" s="92"/>
+      <c r="J63" s="92"/>
+      <c r="K63" s="92"/>
+      <c r="L63" s="92"/>
       <c r="M63" s="7"/>
     </row>
     <row r="64" spans="1:13" ht="15.75" thickBot="1">
@@ -4555,11 +4624,11 @@
       <c r="E132" s="20"/>
       <c r="F132" s="20"/>
       <c r="G132" s="7"/>
-      <c r="H132" s="92"/>
-      <c r="I132" s="92"/>
-      <c r="J132" s="92"/>
-      <c r="K132" s="92"/>
-      <c r="L132" s="92"/>
+      <c r="H132" s="91"/>
+      <c r="I132" s="91"/>
+      <c r="J132" s="91"/>
+      <c r="K132" s="91"/>
+      <c r="L132" s="91"/>
       <c r="M132" s="7"/>
     </row>
     <row r="133" spans="1:14" ht="18" thickBot="1">
@@ -6305,13 +6374,13 @@
       <c r="E30" s="20"/>
       <c r="F30" s="20"/>
       <c r="G30" s="58"/>
-      <c r="H30" s="94" t="s">
+      <c r="H30" s="93" t="s">
         <v>170</v>
       </c>
-      <c r="I30" s="95"/>
-      <c r="J30" s="95"/>
-      <c r="K30" s="95"/>
-      <c r="L30" s="96"/>
+      <c r="I30" s="94"/>
+      <c r="J30" s="94"/>
+      <c r="K30" s="94"/>
+      <c r="L30" s="95"/>
       <c r="M30" s="58"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1">
@@ -6466,13 +6535,13 @@
       <c r="E39" s="20"/>
       <c r="F39" s="62"/>
       <c r="G39" s="58"/>
-      <c r="H39" s="94" t="s">
+      <c r="H39" s="93" t="s">
         <v>171</v>
       </c>
-      <c r="I39" s="95"/>
-      <c r="J39" s="95"/>
-      <c r="K39" s="95"/>
-      <c r="L39" s="96"/>
+      <c r="I39" s="94"/>
+      <c r="J39" s="94"/>
+      <c r="K39" s="94"/>
+      <c r="L39" s="95"/>
       <c r="M39" s="58"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" thickBot="1">
@@ -6633,13 +6702,13 @@
         <v>3</v>
       </c>
       <c r="G48" s="58"/>
-      <c r="H48" s="94" t="s">
+      <c r="H48" s="93" t="s">
         <v>172</v>
       </c>
-      <c r="I48" s="95"/>
-      <c r="J48" s="95"/>
-      <c r="K48" s="95"/>
-      <c r="L48" s="96"/>
+      <c r="I48" s="94"/>
+      <c r="J48" s="94"/>
+      <c r="K48" s="94"/>
+      <c r="L48" s="95"/>
       <c r="M48" s="58"/>
     </row>
     <row r="49" spans="1:13" ht="15.75" thickBot="1">
@@ -6788,13 +6857,13 @@
       <c r="E57" s="39"/>
       <c r="F57" s="39"/>
       <c r="G57" s="58"/>
-      <c r="H57" s="94" t="s">
+      <c r="H57" s="93" t="s">
         <v>173</v>
       </c>
-      <c r="I57" s="95"/>
-      <c r="J57" s="95"/>
-      <c r="K57" s="95"/>
-      <c r="L57" s="96"/>
+      <c r="I57" s="94"/>
+      <c r="J57" s="94"/>
+      <c r="K57" s="94"/>
+      <c r="L57" s="95"/>
       <c r="M57" s="58"/>
     </row>
     <row r="58" spans="1:13" ht="15.75" thickBot="1">
@@ -6943,13 +7012,13 @@
       <c r="E66" s="20"/>
       <c r="F66" s="20"/>
       <c r="G66" s="58"/>
-      <c r="H66" s="94" t="s">
+      <c r="H66" s="93" t="s">
         <v>174</v>
       </c>
-      <c r="I66" s="95"/>
-      <c r="J66" s="95"/>
-      <c r="K66" s="95"/>
-      <c r="L66" s="96"/>
+      <c r="I66" s="94"/>
+      <c r="J66" s="94"/>
+      <c r="K66" s="94"/>
+      <c r="L66" s="95"/>
       <c r="M66" s="58"/>
     </row>
     <row r="67" spans="1:13" ht="15.75" thickBot="1">
@@ -9306,8 +9375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A117" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D129" sqref="D129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9327,40 +9396,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="23.25" customHeight="1">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="98" t="s">
         <v>284</v>
       </c>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
-      <c r="G1" s="99"/>
-      <c r="H1" s="99"/>
-      <c r="I1" s="99"/>
-      <c r="J1" s="99"/>
-      <c r="K1" s="99"/>
-      <c r="L1" s="99"/>
-      <c r="M1" s="99"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1">
-      <c r="A2" s="99"/>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
-      <c r="K2" s="99"/>
-      <c r="L2" s="99"/>
-      <c r="M2" s="99"/>
+      <c r="A2" s="98"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
       <c r="N2" s="1"/>
       <c r="O2" s="69"/>
       <c r="P2" s="70" t="s">
@@ -9369,19 +9438,19 @@
       <c r="Q2" s="1"/>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1">
-      <c r="A3" s="99"/>
-      <c r="B3" s="99"/>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="99"/>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99"/>
-      <c r="M3" s="99"/>
+      <c r="A3" s="98"/>
+      <c r="B3" s="98"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -9548,14 +9617,14 @@
       <c r="C11" s="73"/>
       <c r="D11" s="73"/>
       <c r="E11" s="73"/>
-      <c r="F11" s="20"/>
+      <c r="F11" s="73"/>
       <c r="G11" s="58"/>
       <c r="H11" s="19" t="s">
         <v>152</v>
       </c>
       <c r="I11" s="73"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="73"/>
       <c r="L11" s="73"/>
       <c r="M11" s="58"/>
     </row>
@@ -9583,7 +9652,7 @@
       <c r="B13" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="20"/>
+      <c r="C13" s="73"/>
       <c r="D13" s="73"/>
       <c r="E13" s="73"/>
       <c r="F13" s="73"/>
@@ -9592,7 +9661,7 @@
         <v>154</v>
       </c>
       <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
+      <c r="J13" s="73"/>
       <c r="K13" s="73"/>
       <c r="L13" s="73"/>
       <c r="M13" s="58"/>
@@ -9629,7 +9698,7 @@
       <c r="H15" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="I15" s="20"/>
+      <c r="I15" s="73"/>
       <c r="J15" s="73"/>
       <c r="K15" s="73"/>
       <c r="L15" s="73"/>
@@ -9716,7 +9785,7 @@
       <c r="B20" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="20"/>
+      <c r="C20" s="73"/>
       <c r="D20" s="73"/>
       <c r="E20" s="73"/>
       <c r="F20" s="73"/>
@@ -9736,7 +9805,7 @@
         <v>18</v>
       </c>
       <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
+      <c r="D21" s="73"/>
       <c r="E21" s="73"/>
       <c r="F21" s="20"/>
       <c r="G21" s="58"/>
@@ -9775,13 +9844,13 @@
       </c>
       <c r="C23" s="80"/>
       <c r="D23" s="73"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
+      <c r="E23" s="80"/>
+      <c r="F23" s="73"/>
       <c r="G23" s="58"/>
       <c r="H23" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="I23" s="20"/>
+      <c r="I23" s="73"/>
       <c r="J23" s="73"/>
       <c r="K23" s="73"/>
       <c r="L23" s="20"/>
@@ -9792,7 +9861,7 @@
       <c r="B24" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="20"/>
+      <c r="C24" s="73"/>
       <c r="D24" s="73"/>
       <c r="E24" s="73"/>
       <c r="F24" s="73"/>
@@ -9800,7 +9869,7 @@
       <c r="H24" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="I24" s="20"/>
+      <c r="I24" s="73"/>
       <c r="J24" s="73"/>
       <c r="K24" s="73"/>
       <c r="L24" s="20"/>
@@ -9894,7 +9963,7 @@
         <v>25</v>
       </c>
       <c r="C29" s="73"/>
-      <c r="D29" s="20"/>
+      <c r="D29" s="73"/>
       <c r="E29" s="73"/>
       <c r="F29" s="20"/>
       <c r="G29" s="58"/>
@@ -9917,13 +9986,13 @@
       <c r="E30" s="73"/>
       <c r="F30" s="73"/>
       <c r="G30" s="58"/>
-      <c r="H30" s="94" t="s">
+      <c r="H30" s="93" t="s">
         <v>170</v>
       </c>
-      <c r="I30" s="95"/>
-      <c r="J30" s="95"/>
-      <c r="K30" s="95"/>
-      <c r="L30" s="96"/>
+      <c r="I30" s="94"/>
+      <c r="J30" s="94"/>
+      <c r="K30" s="94"/>
+      <c r="L30" s="95"/>
       <c r="M30" s="58"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1">
@@ -9942,12 +10011,14 @@
       <c r="I31" s="76" t="s">
         <v>335</v>
       </c>
-      <c r="J31" s="63"/>
+      <c r="J31" s="76" t="s">
+        <v>367</v>
+      </c>
       <c r="K31" s="63"/>
       <c r="L31" s="63"/>
       <c r="M31" s="58"/>
     </row>
-    <row r="32" spans="1:13" ht="15.75" thickBot="1">
+    <row r="32" spans="1:13" ht="30.75" thickBot="1">
       <c r="A32" s="58"/>
       <c r="B32" s="19" t="s">
         <v>28</v>
@@ -9955,7 +10026,7 @@
       <c r="C32" s="73"/>
       <c r="D32" s="73"/>
       <c r="E32" s="73"/>
-      <c r="F32" s="20"/>
+      <c r="F32" s="73"/>
       <c r="G32" s="58"/>
       <c r="H32" s="76" t="s">
         <v>308</v>
@@ -9963,7 +10034,9 @@
       <c r="I32" s="76" t="s">
         <v>336</v>
       </c>
-      <c r="J32" s="63"/>
+      <c r="J32" s="76" t="s">
+        <v>368</v>
+      </c>
       <c r="K32" s="63"/>
       <c r="L32" s="63"/>
       <c r="M32" s="58"/>
@@ -9982,7 +10055,9 @@
       <c r="I33" s="75" t="s">
         <v>337</v>
       </c>
-      <c r="J33" s="20"/>
+      <c r="J33" s="89" t="s">
+        <v>332</v>
+      </c>
       <c r="K33" s="20"/>
       <c r="L33" s="20"/>
       <c r="M33" s="58"/>
@@ -10008,8 +10083,12 @@
       <c r="H34" s="75" t="s">
         <v>313</v>
       </c>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
+      <c r="I34" s="75" t="s">
+        <v>359</v>
+      </c>
+      <c r="J34" s="75" t="s">
+        <v>374</v>
+      </c>
       <c r="K34" s="20"/>
       <c r="L34" s="20"/>
       <c r="M34" s="58"/>
@@ -10027,8 +10106,12 @@
       <c r="H35" s="75" t="s">
         <v>316</v>
       </c>
-      <c r="I35" s="20"/>
-      <c r="J35" s="20"/>
+      <c r="I35" s="75" t="s">
+        <v>360</v>
+      </c>
+      <c r="J35" s="75" t="s">
+        <v>379</v>
+      </c>
       <c r="K35" s="20"/>
       <c r="L35" s="20"/>
       <c r="M35" s="58"/>
@@ -10046,7 +10129,9 @@
       <c r="H36" s="75" t="s">
         <v>325</v>
       </c>
-      <c r="I36" s="20"/>
+      <c r="I36" s="75" t="s">
+        <v>363</v>
+      </c>
       <c r="J36" s="20"/>
       <c r="K36" s="20"/>
       <c r="L36" s="20"/>
@@ -10065,7 +10150,9 @@
       <c r="H37" s="75" t="s">
         <v>332</v>
       </c>
-      <c r="I37" s="20"/>
+      <c r="I37" s="75" t="s">
+        <v>365</v>
+      </c>
       <c r="J37" s="20"/>
       <c r="K37" s="20"/>
       <c r="L37" s="20"/>
@@ -10076,7 +10163,7 @@
       <c r="B38" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C38" s="20"/>
+      <c r="C38" s="73"/>
       <c r="D38" s="73"/>
       <c r="E38" s="73"/>
       <c r="F38" s="73"/>
@@ -10096,15 +10183,15 @@
       <c r="C39" s="73"/>
       <c r="D39" s="73"/>
       <c r="E39" s="73"/>
-      <c r="F39" s="62"/>
+      <c r="F39" s="86"/>
       <c r="G39" s="58"/>
-      <c r="H39" s="94" t="s">
+      <c r="H39" s="93" t="s">
         <v>171</v>
       </c>
-      <c r="I39" s="95"/>
-      <c r="J39" s="95"/>
-      <c r="K39" s="95"/>
-      <c r="L39" s="96"/>
+      <c r="I39" s="94"/>
+      <c r="J39" s="94"/>
+      <c r="K39" s="94"/>
+      <c r="L39" s="95"/>
       <c r="M39" s="58"/>
     </row>
     <row r="40" spans="1:13" ht="30.75" thickBot="1">
@@ -10121,8 +10208,12 @@
       <c r="I40" s="76" t="s">
         <v>323</v>
       </c>
-      <c r="J40" s="63"/>
-      <c r="K40" s="63"/>
+      <c r="J40" s="76" t="s">
+        <v>361</v>
+      </c>
+      <c r="K40" s="76" t="s">
+        <v>377</v>
+      </c>
       <c r="L40" s="63"/>
       <c r="M40" s="58"/>
     </row>
@@ -10150,8 +10241,12 @@
       <c r="I41" s="76" t="s">
         <v>324</v>
       </c>
-      <c r="J41" s="63"/>
-      <c r="K41" s="63"/>
+      <c r="J41" s="76" t="s">
+        <v>362</v>
+      </c>
+      <c r="K41" s="76" t="s">
+        <v>380</v>
+      </c>
       <c r="L41" s="63"/>
       <c r="M41" s="58"/>
     </row>
@@ -10171,7 +10266,9 @@
       <c r="I42" s="75" t="s">
         <v>327</v>
       </c>
-      <c r="J42" s="20"/>
+      <c r="J42" s="75" t="s">
+        <v>369</v>
+      </c>
       <c r="K42" s="20"/>
       <c r="L42" s="20"/>
       <c r="M42" s="58"/>
@@ -10181,9 +10278,9 @@
       <c r="B43" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C43" s="20"/>
+      <c r="C43" s="73"/>
       <c r="D43" s="73"/>
-      <c r="E43" s="20"/>
+      <c r="E43" s="73"/>
       <c r="F43" s="20"/>
       <c r="G43" s="58"/>
       <c r="H43" s="75" t="s">
@@ -10192,7 +10289,9 @@
       <c r="I43" s="75" t="s">
         <v>334</v>
       </c>
-      <c r="J43" s="20"/>
+      <c r="J43" s="75" t="s">
+        <v>370</v>
+      </c>
       <c r="K43" s="20"/>
       <c r="L43" s="20"/>
       <c r="M43" s="58"/>
@@ -10204,7 +10303,7 @@
       </c>
       <c r="C44" s="73"/>
       <c r="D44" s="73"/>
-      <c r="E44" s="20"/>
+      <c r="E44" s="73"/>
       <c r="F44" s="73"/>
       <c r="G44" s="58"/>
       <c r="H44" s="75" t="s">
@@ -10213,7 +10312,9 @@
       <c r="I44" s="75" t="s">
         <v>338</v>
       </c>
-      <c r="J44" s="20"/>
+      <c r="J44" s="89" t="s">
+        <v>373</v>
+      </c>
       <c r="K44" s="20"/>
       <c r="L44" s="20"/>
       <c r="M44" s="58"/>
@@ -10234,12 +10335,14 @@
       <c r="I45" s="75" t="s">
         <v>357</v>
       </c>
-      <c r="J45" s="20"/>
+      <c r="J45" s="75" t="s">
+        <v>375</v>
+      </c>
       <c r="K45" s="20"/>
       <c r="L45" s="20"/>
       <c r="M45" s="58"/>
     </row>
-    <row r="46" spans="1:13" ht="15.75" thickBot="1">
+    <row r="46" spans="1:13" ht="26.25" thickBot="1">
       <c r="A46" s="58"/>
       <c r="B46" s="19" t="s">
         <v>40</v>
@@ -10247,13 +10350,17 @@
       <c r="C46" s="73"/>
       <c r="D46" s="73"/>
       <c r="E46" s="73"/>
-      <c r="F46" s="87"/>
+      <c r="F46" s="86"/>
       <c r="G46" s="58"/>
       <c r="H46" s="75" t="s">
         <v>318</v>
       </c>
-      <c r="I46" s="20"/>
-      <c r="J46" s="20"/>
+      <c r="I46" s="75" t="s">
+        <v>358</v>
+      </c>
+      <c r="J46" s="75" t="s">
+        <v>376</v>
+      </c>
       <c r="K46" s="20"/>
       <c r="L46" s="20"/>
       <c r="M46" s="58"/>
@@ -10291,13 +10398,13 @@
         <v>3</v>
       </c>
       <c r="G48" s="58"/>
-      <c r="H48" s="94" t="s">
+      <c r="H48" s="93" t="s">
         <v>172</v>
       </c>
-      <c r="I48" s="95"/>
-      <c r="J48" s="95"/>
-      <c r="K48" s="95"/>
-      <c r="L48" s="96"/>
+      <c r="I48" s="94"/>
+      <c r="J48" s="94"/>
+      <c r="K48" s="94"/>
+      <c r="L48" s="95"/>
       <c r="M48" s="58"/>
     </row>
     <row r="49" spans="1:13" ht="15.75" thickBot="1">
@@ -10329,7 +10436,7 @@
       <c r="C50" s="73"/>
       <c r="D50" s="73"/>
       <c r="E50" s="73"/>
-      <c r="F50" s="20"/>
+      <c r="F50" s="73"/>
       <c r="G50" s="58"/>
       <c r="H50" s="76" t="s">
         <v>304</v>
@@ -10350,12 +10457,12 @@
       <c r="C51" s="73"/>
       <c r="D51" s="73"/>
       <c r="E51" s="73"/>
-      <c r="F51" s="20"/>
+      <c r="F51" s="73"/>
       <c r="G51" s="58"/>
       <c r="H51" s="75" t="s">
         <v>306</v>
       </c>
-      <c r="I51" s="90" t="s">
+      <c r="I51" s="89" t="s">
         <v>331</v>
       </c>
       <c r="J51" s="20"/>
@@ -10384,7 +10491,7 @@
       <c r="L52" s="20"/>
       <c r="M52" s="58"/>
     </row>
-    <row r="53" spans="1:13" ht="15.75" thickBot="1">
+    <row r="53" spans="1:13" ht="23.25" thickBot="1">
       <c r="A53" s="58"/>
       <c r="B53" s="19" t="s">
         <v>46</v>
@@ -10392,12 +10499,14 @@
       <c r="C53" s="73"/>
       <c r="D53" s="73"/>
       <c r="E53" s="73"/>
-      <c r="F53" s="20"/>
+      <c r="F53" s="73"/>
       <c r="G53" s="58"/>
       <c r="H53" s="75" t="s">
         <v>320</v>
       </c>
-      <c r="I53" s="20"/>
+      <c r="I53" s="89" t="s">
+        <v>364</v>
+      </c>
       <c r="J53" s="20"/>
       <c r="K53" s="20"/>
       <c r="L53" s="20"/>
@@ -10416,7 +10525,9 @@
       <c r="H54" s="75" t="s">
         <v>321</v>
       </c>
-      <c r="I54" s="20"/>
+      <c r="I54" s="75" t="s">
+        <v>366</v>
+      </c>
       <c r="J54" s="20"/>
       <c r="K54" s="20"/>
       <c r="L54" s="20"/>
@@ -10429,13 +10540,15 @@
       </c>
       <c r="C55" s="73"/>
       <c r="D55" s="73"/>
-      <c r="E55" s="20"/>
-      <c r="F55" s="20"/>
+      <c r="E55" s="73"/>
+      <c r="F55" s="73"/>
       <c r="G55" s="58"/>
       <c r="H55" s="75" t="s">
         <v>326</v>
       </c>
-      <c r="I55" s="20"/>
+      <c r="I55" s="75" t="s">
+        <v>378</v>
+      </c>
       <c r="J55" s="20"/>
       <c r="K55" s="20"/>
       <c r="L55" s="20"/>
@@ -10446,7 +10559,7 @@
       <c r="B56" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="C56" s="20"/>
+      <c r="C56" s="73"/>
       <c r="D56" s="73"/>
       <c r="E56" s="73"/>
       <c r="F56" s="20"/>
@@ -10468,13 +10581,13 @@
       <c r="E57" s="74"/>
       <c r="F57" s="74"/>
       <c r="G57" s="58"/>
-      <c r="H57" s="94" t="s">
+      <c r="H57" s="93" t="s">
         <v>173</v>
       </c>
-      <c r="I57" s="95"/>
-      <c r="J57" s="95"/>
-      <c r="K57" s="95"/>
-      <c r="L57" s="96"/>
+      <c r="I57" s="94"/>
+      <c r="J57" s="94"/>
+      <c r="K57" s="94"/>
+      <c r="L57" s="95"/>
       <c r="M57" s="58"/>
     </row>
     <row r="58" spans="1:13" ht="15.75" thickBot="1">
@@ -10490,7 +10603,7 @@
       <c r="H58" s="76" t="s">
         <v>339</v>
       </c>
-      <c r="I58" s="91" t="s">
+      <c r="I58" s="90" t="s">
         <v>346</v>
       </c>
       <c r="J58" s="76" t="s">
@@ -10513,7 +10626,7 @@
       <c r="H59" s="76" t="s">
         <v>340</v>
       </c>
-      <c r="I59" s="91" t="s">
+      <c r="I59" s="90" t="s">
         <v>347</v>
       </c>
       <c r="J59" s="76" t="s">
@@ -10529,17 +10642,17 @@
         <v>53</v>
       </c>
       <c r="C60" s="73"/>
-      <c r="D60" s="20"/>
+      <c r="D60" s="73"/>
       <c r="E60" s="20"/>
       <c r="F60" s="20"/>
       <c r="G60" s="58"/>
       <c r="H60" s="75" t="s">
         <v>341</v>
       </c>
-      <c r="I60" s="90" t="s">
+      <c r="I60" s="89" t="s">
         <v>348</v>
       </c>
-      <c r="J60" s="90" t="s">
+      <c r="J60" s="89" t="s">
         <v>355</v>
       </c>
       <c r="K60" s="20"/>
@@ -10556,13 +10669,15 @@
       <c r="E61" s="73"/>
       <c r="F61" s="73"/>
       <c r="G61" s="58"/>
-      <c r="H61" s="90" t="s">
+      <c r="H61" s="89" t="s">
         <v>342</v>
       </c>
       <c r="I61" s="75" t="s">
         <v>349</v>
       </c>
-      <c r="J61" s="20"/>
+      <c r="J61" s="75" t="s">
+        <v>371</v>
+      </c>
       <c r="K61" s="20"/>
       <c r="L61" s="20"/>
       <c r="M61" s="58"/>
@@ -10583,7 +10698,9 @@
       <c r="I62" s="75" t="s">
         <v>350</v>
       </c>
-      <c r="J62" s="20"/>
+      <c r="J62" s="89" t="s">
+        <v>372</v>
+      </c>
       <c r="K62" s="20"/>
       <c r="L62" s="20"/>
       <c r="M62" s="58"/>
@@ -10622,7 +10739,7 @@
       <c r="H64" s="75" t="s">
         <v>345</v>
       </c>
-      <c r="I64" s="90" t="s">
+      <c r="I64" s="89" t="s">
         <v>352</v>
       </c>
       <c r="J64" s="20"/>
@@ -10657,13 +10774,13 @@
       <c r="E66" s="73"/>
       <c r="F66" s="73"/>
       <c r="G66" s="58"/>
-      <c r="H66" s="94" t="s">
+      <c r="H66" s="93" t="s">
         <v>174</v>
       </c>
-      <c r="I66" s="95"/>
-      <c r="J66" s="95"/>
-      <c r="K66" s="95"/>
-      <c r="L66" s="96"/>
+      <c r="I66" s="94"/>
+      <c r="J66" s="94"/>
+      <c r="K66" s="94"/>
+      <c r="L66" s="95"/>
       <c r="M66" s="58"/>
     </row>
     <row r="67" spans="1:13" ht="15.75" thickBot="1">
@@ -10681,10 +10798,10 @@
       </c>
       <c r="I67" s="63"/>
       <c r="J67" s="63"/>
-      <c r="K67" s="100" t="s">
+      <c r="K67" s="99" t="s">
         <v>290</v>
       </c>
-      <c r="L67" s="101"/>
+      <c r="L67" s="100"/>
       <c r="M67" s="58"/>
     </row>
     <row r="68" spans="1:13" ht="15.75" thickBot="1">
@@ -10702,10 +10819,10 @@
       </c>
       <c r="I68" s="63"/>
       <c r="J68" s="63"/>
-      <c r="K68" s="100" t="s">
+      <c r="K68" s="99" t="s">
         <v>291</v>
       </c>
-      <c r="L68" s="101"/>
+      <c r="L68" s="100"/>
       <c r="M68" s="58"/>
     </row>
     <row r="69" spans="1:13" ht="15.75" thickBot="1">
@@ -10713,7 +10830,7 @@
       <c r="B69" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="C69" s="20"/>
+      <c r="C69" s="73"/>
       <c r="D69" s="73"/>
       <c r="E69" s="73"/>
       <c r="F69" s="73"/>
@@ -10723,10 +10840,10 @@
       </c>
       <c r="I69" s="20"/>
       <c r="J69" s="20"/>
-      <c r="K69" s="97" t="s">
+      <c r="K69" s="96" t="s">
         <v>298</v>
       </c>
-      <c r="L69" s="98"/>
+      <c r="L69" s="97"/>
       <c r="M69" s="58"/>
     </row>
     <row r="70" spans="1:13" ht="15.75" thickBot="1">
@@ -10744,10 +10861,10 @@
       </c>
       <c r="I70" s="20"/>
       <c r="J70" s="20"/>
-      <c r="K70" s="97" t="s">
+      <c r="K70" s="96" t="s">
         <v>299</v>
       </c>
-      <c r="L70" s="98"/>
+      <c r="L70" s="97"/>
       <c r="M70" s="58"/>
     </row>
     <row r="71" spans="1:13" ht="15.75" thickBot="1">
@@ -10765,10 +10882,10 @@
       </c>
       <c r="I71" s="20"/>
       <c r="J71" s="20"/>
-      <c r="K71" s="97" t="s">
+      <c r="K71" s="96" t="s">
         <v>314</v>
       </c>
-      <c r="L71" s="98"/>
+      <c r="L71" s="97"/>
       <c r="M71" s="58"/>
     </row>
     <row r="72" spans="1:13" ht="15.75" thickBot="1">
@@ -10784,10 +10901,10 @@
       <c r="H72" s="20"/>
       <c r="I72" s="20"/>
       <c r="J72" s="20"/>
-      <c r="K72" s="97" t="s">
+      <c r="K72" s="96" t="s">
         <v>328</v>
       </c>
-      <c r="L72" s="98"/>
+      <c r="L72" s="97"/>
       <c r="M72" s="58"/>
     </row>
     <row r="73" spans="1:13" ht="15.75" thickBot="1">
@@ -10847,7 +10964,7 @@
       <c r="H75" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="I75" s="20"/>
+      <c r="I75" s="73"/>
       <c r="J75" s="73"/>
       <c r="K75" s="73"/>
       <c r="L75" s="73"/>
@@ -10858,7 +10975,7 @@
       <c r="B76" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="C76" s="20"/>
+      <c r="C76" s="73"/>
       <c r="D76" s="73"/>
       <c r="E76" s="73"/>
       <c r="F76" s="20"/>
@@ -10899,7 +11016,7 @@
       <c r="C78" s="20"/>
       <c r="D78" s="73"/>
       <c r="E78" s="73"/>
-      <c r="F78" s="20"/>
+      <c r="F78" s="73"/>
       <c r="G78" s="58"/>
       <c r="H78" s="19" t="s">
         <v>179</v>
@@ -10945,7 +11062,7 @@
       <c r="I80" s="73"/>
       <c r="J80" s="73"/>
       <c r="K80" s="73"/>
-      <c r="L80" s="20"/>
+      <c r="L80" s="73"/>
       <c r="M80" s="58"/>
     </row>
     <row r="81" spans="1:13" ht="15.75" thickBot="1">
@@ -10973,7 +11090,7 @@
         <v>75</v>
       </c>
       <c r="C82" s="73"/>
-      <c r="D82" s="20"/>
+      <c r="D82" s="73"/>
       <c r="E82" s="73"/>
       <c r="F82" s="20"/>
       <c r="G82" s="58"/>
@@ -11011,7 +11128,7 @@
         <v>77</v>
       </c>
       <c r="C84" s="73"/>
-      <c r="D84" s="20"/>
+      <c r="D84" s="73"/>
       <c r="E84" s="73"/>
       <c r="F84" s="20"/>
       <c r="G84" s="58"/>
@@ -11020,7 +11137,7 @@
       </c>
       <c r="I84" s="73"/>
       <c r="J84" s="73"/>
-      <c r="K84" s="20"/>
+      <c r="K84" s="73"/>
       <c r="L84" s="73"/>
       <c r="M84" s="58"/>
     </row>
@@ -11031,7 +11148,7 @@
       </c>
       <c r="C85" s="73"/>
       <c r="D85" s="73"/>
-      <c r="E85" s="20"/>
+      <c r="E85" s="73"/>
       <c r="F85" s="73"/>
       <c r="G85" s="58"/>
       <c r="H85" s="19" t="s">
@@ -11075,7 +11192,7 @@
       <c r="H87" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="I87" s="20"/>
+      <c r="I87" s="73"/>
       <c r="J87" s="73"/>
       <c r="K87" s="73"/>
       <c r="L87" s="20"/>
@@ -11105,7 +11222,7 @@
       <c r="B89" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="C89" s="20"/>
+      <c r="C89" s="73"/>
       <c r="D89" s="78"/>
       <c r="E89" s="73"/>
       <c r="F89" s="73"/>
@@ -11154,7 +11271,7 @@
       <c r="I91" s="73"/>
       <c r="J91" s="73"/>
       <c r="K91" s="73"/>
-      <c r="L91" s="20"/>
+      <c r="L91" s="73"/>
       <c r="M91" s="58"/>
     </row>
     <row r="92" spans="1:13" ht="15.75" thickBot="1">
@@ -11184,7 +11301,7 @@
       <c r="C93" s="73"/>
       <c r="D93" s="20"/>
       <c r="E93" s="73"/>
-      <c r="F93" s="20"/>
+      <c r="F93" s="73"/>
       <c r="G93" s="58"/>
       <c r="H93" s="19" t="s">
         <v>194</v>
@@ -11208,7 +11325,7 @@
       <c r="H94" s="19" t="s">
         <v>195</v>
       </c>
-      <c r="I94" s="20"/>
+      <c r="I94" s="73"/>
       <c r="J94" s="73"/>
       <c r="K94" s="20"/>
       <c r="L94" s="20"/>
@@ -11247,7 +11364,7 @@
         <v>196</v>
       </c>
       <c r="I96" s="73"/>
-      <c r="J96" s="20"/>
+      <c r="J96" s="73"/>
       <c r="K96" s="73"/>
       <c r="L96" s="20"/>
       <c r="M96" s="58"/>
@@ -11276,7 +11393,7 @@
       <c r="B98" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="C98" s="20"/>
+      <c r="C98" s="73"/>
       <c r="D98" s="73"/>
       <c r="E98" s="73"/>
       <c r="F98" s="73"/>
@@ -11284,7 +11401,7 @@
       <c r="H98" s="19" t="s">
         <v>195</v>
       </c>
-      <c r="I98" s="20"/>
+      <c r="I98" s="73"/>
       <c r="J98" s="20"/>
       <c r="K98" s="73"/>
       <c r="L98" s="20"/>
@@ -11374,7 +11491,7 @@
       <c r="C103" s="73"/>
       <c r="D103" s="73"/>
       <c r="E103" s="73"/>
-      <c r="F103" s="87"/>
+      <c r="F103" s="86"/>
       <c r="G103" s="58"/>
       <c r="H103" s="19" t="s">
         <v>202</v>
@@ -11467,10 +11584,10 @@
       <c r="H107" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="I107" s="20"/>
+      <c r="I107" s="73"/>
       <c r="J107" s="73"/>
       <c r="K107" s="73"/>
-      <c r="L107" s="20"/>
+      <c r="L107" s="73"/>
       <c r="M107" s="58"/>
     </row>
     <row r="108" spans="1:13" ht="15.75" thickBot="1">
@@ -11535,7 +11652,7 @@
       <c r="B111" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="C111" s="20"/>
+      <c r="C111" s="73"/>
       <c r="D111" s="20"/>
       <c r="E111" s="73"/>
       <c r="F111" s="73"/>
@@ -11554,7 +11671,7 @@
       <c r="B112" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="C112" s="20"/>
+      <c r="C112" s="73"/>
       <c r="D112" s="73"/>
       <c r="E112" s="73"/>
       <c r="F112" s="73"/>
@@ -11565,7 +11682,7 @@
       <c r="I112" s="73"/>
       <c r="J112" s="73"/>
       <c r="K112" s="73"/>
-      <c r="L112" s="20"/>
+      <c r="L112" s="73"/>
       <c r="M112" s="58"/>
     </row>
     <row r="113" spans="1:13" ht="15.75" thickBot="1">
@@ -11640,7 +11757,7 @@
       <c r="H116" s="19" t="s">
         <v>213</v>
       </c>
-      <c r="I116" s="75" t="s">
+      <c r="I116" s="72" t="s">
         <v>286</v>
       </c>
       <c r="J116" s="73"/>
@@ -11656,7 +11773,7 @@
       <c r="C117" s="84" t="s">
         <v>287</v>
       </c>
-      <c r="D117" s="41"/>
+      <c r="D117" s="83"/>
       <c r="E117" s="74"/>
       <c r="F117" s="74"/>
       <c r="G117" s="58"/>
@@ -11683,7 +11800,7 @@
         <v>215</v>
       </c>
       <c r="I118" s="73"/>
-      <c r="J118" s="20"/>
+      <c r="J118" s="73"/>
       <c r="K118" s="73"/>
       <c r="L118" s="73"/>
       <c r="M118" s="58"/>
@@ -11703,7 +11820,7 @@
       </c>
       <c r="I119" s="73"/>
       <c r="J119" s="73"/>
-      <c r="K119" s="20"/>
+      <c r="K119" s="73"/>
       <c r="L119" s="73"/>
       <c r="M119" s="58"/>
     </row>
@@ -11720,9 +11837,9 @@
       <c r="H120" s="19" t="s">
         <v>217</v>
       </c>
-      <c r="I120" s="80"/>
+      <c r="I120" s="73"/>
       <c r="J120" s="73"/>
-      <c r="K120" s="89"/>
+      <c r="K120" s="88"/>
       <c r="L120" s="73"/>
       <c r="M120" s="58"/>
     </row>
@@ -11761,7 +11878,7 @@
       <c r="I122" s="73"/>
       <c r="J122" s="73"/>
       <c r="K122" s="73"/>
-      <c r="L122" s="20"/>
+      <c r="L122" s="73"/>
       <c r="M122" s="58"/>
     </row>
     <row r="123" spans="1:13" ht="15.75" thickBot="1">
@@ -11778,7 +11895,7 @@
         <v>220</v>
       </c>
       <c r="I123" s="73"/>
-      <c r="J123" s="20"/>
+      <c r="J123" s="73"/>
       <c r="K123" s="73"/>
       <c r="L123" s="20"/>
       <c r="M123" s="58"/>
@@ -11798,8 +11915,8 @@
       </c>
       <c r="I124" s="73"/>
       <c r="J124" s="73"/>
-      <c r="K124" s="20"/>
-      <c r="L124" s="20"/>
+      <c r="K124" s="73"/>
+      <c r="L124" s="73"/>
       <c r="M124" s="58"/>
     </row>
     <row r="125" spans="1:13" ht="15.75" thickBot="1">
@@ -11834,9 +11951,9 @@
       <c r="H126" s="19" t="s">
         <v>222</v>
       </c>
-      <c r="I126" s="20"/>
+      <c r="I126" s="73"/>
       <c r="J126" s="73"/>
-      <c r="K126" s="20"/>
+      <c r="K126" s="73"/>
       <c r="L126" s="20"/>
       <c r="M126" s="58"/>
     </row>
@@ -11847,13 +11964,13 @@
       </c>
       <c r="C127" s="73"/>
       <c r="D127" s="73"/>
-      <c r="E127" s="20"/>
+      <c r="E127" s="73"/>
       <c r="F127" s="73"/>
       <c r="G127" s="58"/>
       <c r="H127" s="19" t="s">
         <v>223</v>
       </c>
-      <c r="I127" s="20"/>
+      <c r="I127" s="73"/>
       <c r="J127" s="73"/>
       <c r="K127" s="73"/>
       <c r="L127" s="73"/>
@@ -11872,7 +11989,7 @@
       <c r="H128" s="19" t="s">
         <v>224</v>
       </c>
-      <c r="I128" s="20"/>
+      <c r="I128" s="73"/>
       <c r="J128" s="73"/>
       <c r="K128" s="73"/>
       <c r="L128" s="20"/>
@@ -11912,7 +12029,7 @@
       </c>
       <c r="I130" s="73"/>
       <c r="J130" s="73"/>
-      <c r="K130" s="85"/>
+      <c r="K130" s="73"/>
       <c r="L130" s="73"/>
       <c r="M130" s="58"/>
     </row>
@@ -11921,7 +12038,7 @@
       <c r="B131" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="C131" s="86"/>
+      <c r="C131" s="101"/>
       <c r="D131" s="74"/>
       <c r="E131" s="74"/>
       <c r="F131" s="83"/>
@@ -11997,7 +12114,7 @@
         <v>126</v>
       </c>
       <c r="C135" s="43"/>
-      <c r="D135" s="88"/>
+      <c r="D135" s="87"/>
       <c r="E135" s="73"/>
       <c r="F135" s="20"/>
       <c r="G135" s="4"/>
@@ -12047,9 +12164,9 @@
         <v>128</v>
       </c>
       <c r="C137" s="73"/>
-      <c r="D137" s="20"/>
+      <c r="D137" s="73"/>
       <c r="E137" s="73"/>
-      <c r="F137" s="20"/>
+      <c r="F137" s="73"/>
       <c r="G137" s="4"/>
       <c r="H137" s="51" t="s">
         <v>238</v>
@@ -12126,7 +12243,7 @@
       <c r="B141" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="C141" s="20"/>
+      <c r="C141" s="73"/>
       <c r="D141" s="73"/>
       <c r="E141" s="20"/>
       <c r="F141" s="73"/>
@@ -12144,10 +12261,10 @@
       <c r="B142" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="C142" s="20"/>
+      <c r="C142" s="73"/>
       <c r="D142" s="73"/>
       <c r="E142" s="73"/>
-      <c r="F142" s="87"/>
+      <c r="F142" s="86"/>
       <c r="G142" s="4"/>
       <c r="H142" s="44" t="s">
         <v>243</v>
@@ -12370,7 +12487,7 @@
       </c>
       <c r="C152" s="73"/>
       <c r="D152" s="73"/>
-      <c r="E152" s="20"/>
+      <c r="E152" s="73"/>
       <c r="F152" s="73"/>
       <c r="G152" s="4"/>
       <c r="H152" s="51" t="s">
@@ -12431,7 +12548,7 @@
       <c r="C155" s="73"/>
       <c r="D155" s="73"/>
       <c r="E155" s="73"/>
-      <c r="F155" s="87"/>
+      <c r="F155" s="86"/>
       <c r="G155" s="4"/>
       <c r="H155" s="4"/>
       <c r="I155" s="4"/>

</xml_diff>

<commit_message>
Achievement Unlocked: All TU done
also, only 56 su left, rest all done
</commit_message>
<xml_diff>
--- a/check list.xlsx
+++ b/check list.xlsx
@@ -1540,7 +1540,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1784,9 +1784,6 @@
     <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1830,9 +1827,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2671,13 +2665,13 @@
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
       <c r="G27" s="7"/>
-      <c r="H27" s="92" t="s">
+      <c r="H27" s="91" t="s">
         <v>170</v>
       </c>
-      <c r="I27" s="92"/>
-      <c r="J27" s="92"/>
-      <c r="K27" s="92"/>
-      <c r="L27" s="92"/>
+      <c r="I27" s="91"/>
+      <c r="J27" s="91"/>
+      <c r="K27" s="91"/>
+      <c r="L27" s="91"/>
       <c r="M27" s="7"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1">
@@ -2832,13 +2826,13 @@
       <c r="E36" s="20"/>
       <c r="F36" s="29"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="92" t="s">
+      <c r="H36" s="91" t="s">
         <v>171</v>
       </c>
-      <c r="I36" s="92"/>
-      <c r="J36" s="92"/>
-      <c r="K36" s="92"/>
-      <c r="L36" s="92"/>
+      <c r="I36" s="91"/>
+      <c r="J36" s="91"/>
+      <c r="K36" s="91"/>
+      <c r="L36" s="91"/>
       <c r="M36" s="7"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
@@ -2999,13 +2993,13 @@
         <v>3</v>
       </c>
       <c r="G45" s="7"/>
-      <c r="H45" s="92" t="s">
+      <c r="H45" s="91" t="s">
         <v>172</v>
       </c>
-      <c r="I45" s="92"/>
-      <c r="J45" s="92"/>
-      <c r="K45" s="92"/>
-      <c r="L45" s="92"/>
+      <c r="I45" s="91"/>
+      <c r="J45" s="91"/>
+      <c r="K45" s="91"/>
+      <c r="L45" s="91"/>
       <c r="M45" s="7"/>
     </row>
     <row r="46" spans="1:13" ht="15.75" thickBot="1">
@@ -3154,13 +3148,13 @@
       <c r="E54" s="39"/>
       <c r="F54" s="39"/>
       <c r="G54" s="7"/>
-      <c r="H54" s="92" t="s">
+      <c r="H54" s="91" t="s">
         <v>173</v>
       </c>
-      <c r="I54" s="92"/>
-      <c r="J54" s="92"/>
-      <c r="K54" s="92"/>
-      <c r="L54" s="92"/>
+      <c r="I54" s="91"/>
+      <c r="J54" s="91"/>
+      <c r="K54" s="91"/>
+      <c r="L54" s="91"/>
       <c r="M54" s="7"/>
     </row>
     <row r="55" spans="1:13" ht="15.75" thickBot="1">
@@ -3309,13 +3303,13 @@
       <c r="E63" s="20"/>
       <c r="F63" s="20"/>
       <c r="G63" s="7"/>
-      <c r="H63" s="92" t="s">
+      <c r="H63" s="91" t="s">
         <v>174</v>
       </c>
-      <c r="I63" s="92"/>
-      <c r="J63" s="92"/>
-      <c r="K63" s="92"/>
-      <c r="L63" s="92"/>
+      <c r="I63" s="91"/>
+      <c r="J63" s="91"/>
+      <c r="K63" s="91"/>
+      <c r="L63" s="91"/>
       <c r="M63" s="7"/>
     </row>
     <row r="64" spans="1:13" ht="15.75" thickBot="1">
@@ -4624,11 +4618,11 @@
       <c r="E132" s="20"/>
       <c r="F132" s="20"/>
       <c r="G132" s="7"/>
-      <c r="H132" s="91"/>
-      <c r="I132" s="91"/>
-      <c r="J132" s="91"/>
-      <c r="K132" s="91"/>
-      <c r="L132" s="91"/>
+      <c r="H132" s="90"/>
+      <c r="I132" s="90"/>
+      <c r="J132" s="90"/>
+      <c r="K132" s="90"/>
+      <c r="L132" s="90"/>
       <c r="M132" s="7"/>
     </row>
     <row r="133" spans="1:14" ht="18" thickBot="1">
@@ -6374,13 +6368,13 @@
       <c r="E30" s="20"/>
       <c r="F30" s="20"/>
       <c r="G30" s="58"/>
-      <c r="H30" s="93" t="s">
+      <c r="H30" s="92" t="s">
         <v>170</v>
       </c>
-      <c r="I30" s="94"/>
-      <c r="J30" s="94"/>
-      <c r="K30" s="94"/>
-      <c r="L30" s="95"/>
+      <c r="I30" s="93"/>
+      <c r="J30" s="93"/>
+      <c r="K30" s="93"/>
+      <c r="L30" s="94"/>
       <c r="M30" s="58"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1">
@@ -6535,13 +6529,13 @@
       <c r="E39" s="20"/>
       <c r="F39" s="62"/>
       <c r="G39" s="58"/>
-      <c r="H39" s="93" t="s">
+      <c r="H39" s="92" t="s">
         <v>171</v>
       </c>
-      <c r="I39" s="94"/>
-      <c r="J39" s="94"/>
-      <c r="K39" s="94"/>
-      <c r="L39" s="95"/>
+      <c r="I39" s="93"/>
+      <c r="J39" s="93"/>
+      <c r="K39" s="93"/>
+      <c r="L39" s="94"/>
       <c r="M39" s="58"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" thickBot="1">
@@ -6702,13 +6696,13 @@
         <v>3</v>
       </c>
       <c r="G48" s="58"/>
-      <c r="H48" s="93" t="s">
+      <c r="H48" s="92" t="s">
         <v>172</v>
       </c>
-      <c r="I48" s="94"/>
-      <c r="J48" s="94"/>
-      <c r="K48" s="94"/>
-      <c r="L48" s="95"/>
+      <c r="I48" s="93"/>
+      <c r="J48" s="93"/>
+      <c r="K48" s="93"/>
+      <c r="L48" s="94"/>
       <c r="M48" s="58"/>
     </row>
     <row r="49" spans="1:13" ht="15.75" thickBot="1">
@@ -6857,13 +6851,13 @@
       <c r="E57" s="39"/>
       <c r="F57" s="39"/>
       <c r="G57" s="58"/>
-      <c r="H57" s="93" t="s">
+      <c r="H57" s="92" t="s">
         <v>173</v>
       </c>
-      <c r="I57" s="94"/>
-      <c r="J57" s="94"/>
-      <c r="K57" s="94"/>
-      <c r="L57" s="95"/>
+      <c r="I57" s="93"/>
+      <c r="J57" s="93"/>
+      <c r="K57" s="93"/>
+      <c r="L57" s="94"/>
       <c r="M57" s="58"/>
     </row>
     <row r="58" spans="1:13" ht="15.75" thickBot="1">
@@ -7012,13 +7006,13 @@
       <c r="E66" s="20"/>
       <c r="F66" s="20"/>
       <c r="G66" s="58"/>
-      <c r="H66" s="93" t="s">
+      <c r="H66" s="92" t="s">
         <v>174</v>
       </c>
-      <c r="I66" s="94"/>
-      <c r="J66" s="94"/>
-      <c r="K66" s="94"/>
-      <c r="L66" s="95"/>
+      <c r="I66" s="93"/>
+      <c r="J66" s="93"/>
+      <c r="K66" s="93"/>
+      <c r="L66" s="94"/>
       <c r="M66" s="58"/>
     </row>
     <row r="67" spans="1:13" ht="15.75" thickBot="1">
@@ -9375,8 +9369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D129" sqref="D129"/>
+    <sheetView tabSelected="1" topLeftCell="B116" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C124" sqref="C124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9396,40 +9390,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="23.25" customHeight="1">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="97" t="s">
         <v>284</v>
       </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
-      <c r="H1" s="98"/>
-      <c r="I1" s="98"/>
-      <c r="J1" s="98"/>
-      <c r="K1" s="98"/>
-      <c r="L1" s="98"/>
-      <c r="M1" s="98"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
+      <c r="L1" s="97"/>
+      <c r="M1" s="97"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1">
-      <c r="A2" s="98"/>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
+      <c r="A2" s="97"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
       <c r="N2" s="1"/>
       <c r="O2" s="69"/>
       <c r="P2" s="70" t="s">
@@ -9438,19 +9432,19 @@
       <c r="Q2" s="1"/>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1">
-      <c r="A3" s="98"/>
-      <c r="B3" s="98"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
+      <c r="A3" s="97"/>
+      <c r="B3" s="97"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -9660,7 +9654,7 @@
       <c r="H13" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="I13" s="20"/>
+      <c r="I13" s="73"/>
       <c r="J13" s="73"/>
       <c r="K13" s="73"/>
       <c r="L13" s="73"/>
@@ -9736,10 +9730,10 @@
       <c r="H17" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="I17" s="20"/>
+      <c r="I17" s="73"/>
       <c r="J17" s="73"/>
       <c r="K17" s="20"/>
-      <c r="L17" s="20"/>
+      <c r="L17" s="73"/>
       <c r="M17" s="58"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1">
@@ -9755,7 +9749,7 @@
       <c r="H18" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="I18" s="80"/>
+      <c r="I18" s="73"/>
       <c r="J18" s="73"/>
       <c r="K18" s="73"/>
       <c r="L18" s="73"/>
@@ -9766,7 +9760,7 @@
       <c r="B19" s="19" t="s">
         <v>315</v>
       </c>
-      <c r="C19" s="20"/>
+      <c r="C19" s="73"/>
       <c r="D19" s="73"/>
       <c r="E19" s="73"/>
       <c r="F19" s="73"/>
@@ -9774,7 +9768,7 @@
       <c r="H19" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="I19" s="20"/>
+      <c r="I19" s="73"/>
       <c r="J19" s="73"/>
       <c r="K19" s="73"/>
       <c r="L19" s="20"/>
@@ -9804,7 +9798,7 @@
       <c r="B21" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="20"/>
+      <c r="C21" s="73"/>
       <c r="D21" s="73"/>
       <c r="E21" s="73"/>
       <c r="F21" s="20"/>
@@ -9842,9 +9836,9 @@
       <c r="B23" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="80"/>
+      <c r="C23" s="73"/>
       <c r="D23" s="73"/>
-      <c r="E23" s="80"/>
+      <c r="E23" s="73"/>
       <c r="F23" s="73"/>
       <c r="G23" s="58"/>
       <c r="H23" s="19" t="s">
@@ -9951,10 +9945,10 @@
       <c r="H28" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="I28" s="20"/>
+      <c r="I28" s="73"/>
       <c r="J28" s="73"/>
       <c r="K28" s="20"/>
-      <c r="L28" s="62"/>
+      <c r="L28" s="85"/>
       <c r="M28" s="58"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1">
@@ -9986,13 +9980,13 @@
       <c r="E30" s="73"/>
       <c r="F30" s="73"/>
       <c r="G30" s="58"/>
-      <c r="H30" s="93" t="s">
+      <c r="H30" s="92" t="s">
         <v>170</v>
       </c>
-      <c r="I30" s="94"/>
-      <c r="J30" s="94"/>
-      <c r="K30" s="94"/>
-      <c r="L30" s="95"/>
+      <c r="I30" s="93"/>
+      <c r="J30" s="93"/>
+      <c r="K30" s="93"/>
+      <c r="L30" s="94"/>
       <c r="M30" s="58"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1">
@@ -10055,7 +10049,7 @@
       <c r="I33" s="75" t="s">
         <v>337</v>
       </c>
-      <c r="J33" s="89" t="s">
+      <c r="J33" s="88" t="s">
         <v>332</v>
       </c>
       <c r="K33" s="20"/>
@@ -10183,15 +10177,15 @@
       <c r="C39" s="73"/>
       <c r="D39" s="73"/>
       <c r="E39" s="73"/>
-      <c r="F39" s="86"/>
+      <c r="F39" s="85"/>
       <c r="G39" s="58"/>
-      <c r="H39" s="93" t="s">
+      <c r="H39" s="92" t="s">
         <v>171</v>
       </c>
-      <c r="I39" s="94"/>
-      <c r="J39" s="94"/>
-      <c r="K39" s="94"/>
-      <c r="L39" s="95"/>
+      <c r="I39" s="93"/>
+      <c r="J39" s="93"/>
+      <c r="K39" s="93"/>
+      <c r="L39" s="94"/>
       <c r="M39" s="58"/>
     </row>
     <row r="40" spans="1:13" ht="30.75" thickBot="1">
@@ -10312,7 +10306,7 @@
       <c r="I44" s="75" t="s">
         <v>338</v>
       </c>
-      <c r="J44" s="89" t="s">
+      <c r="J44" s="88" t="s">
         <v>373</v>
       </c>
       <c r="K44" s="20"/>
@@ -10350,7 +10344,7 @@
       <c r="C46" s="73"/>
       <c r="D46" s="73"/>
       <c r="E46" s="73"/>
-      <c r="F46" s="86"/>
+      <c r="F46" s="85"/>
       <c r="G46" s="58"/>
       <c r="H46" s="75" t="s">
         <v>318</v>
@@ -10398,13 +10392,13 @@
         <v>3</v>
       </c>
       <c r="G48" s="58"/>
-      <c r="H48" s="93" t="s">
+      <c r="H48" s="92" t="s">
         <v>172</v>
       </c>
-      <c r="I48" s="94"/>
-      <c r="J48" s="94"/>
-      <c r="K48" s="94"/>
-      <c r="L48" s="95"/>
+      <c r="I48" s="93"/>
+      <c r="J48" s="93"/>
+      <c r="K48" s="93"/>
+      <c r="L48" s="94"/>
       <c r="M48" s="58"/>
     </row>
     <row r="49" spans="1:13" ht="15.75" thickBot="1">
@@ -10462,7 +10456,7 @@
       <c r="H51" s="75" t="s">
         <v>306</v>
       </c>
-      <c r="I51" s="89" t="s">
+      <c r="I51" s="88" t="s">
         <v>331</v>
       </c>
       <c r="J51" s="20"/>
@@ -10504,7 +10498,7 @@
       <c r="H53" s="75" t="s">
         <v>320</v>
       </c>
-      <c r="I53" s="89" t="s">
+      <c r="I53" s="88" t="s">
         <v>364</v>
       </c>
       <c r="J53" s="20"/>
@@ -10562,7 +10556,7 @@
       <c r="C56" s="73"/>
       <c r="D56" s="73"/>
       <c r="E56" s="73"/>
-      <c r="F56" s="20"/>
+      <c r="F56" s="73"/>
       <c r="G56" s="58"/>
       <c r="H56" s="58"/>
       <c r="I56" s="58"/>
@@ -10581,13 +10575,13 @@
       <c r="E57" s="74"/>
       <c r="F57" s="74"/>
       <c r="G57" s="58"/>
-      <c r="H57" s="93" t="s">
+      <c r="H57" s="92" t="s">
         <v>173</v>
       </c>
-      <c r="I57" s="94"/>
-      <c r="J57" s="94"/>
-      <c r="K57" s="94"/>
-      <c r="L57" s="95"/>
+      <c r="I57" s="93"/>
+      <c r="J57" s="93"/>
+      <c r="K57" s="93"/>
+      <c r="L57" s="94"/>
       <c r="M57" s="58"/>
     </row>
     <row r="58" spans="1:13" ht="15.75" thickBot="1">
@@ -10603,7 +10597,7 @@
       <c r="H58" s="76" t="s">
         <v>339</v>
       </c>
-      <c r="I58" s="90" t="s">
+      <c r="I58" s="89" t="s">
         <v>346</v>
       </c>
       <c r="J58" s="76" t="s">
@@ -10618,7 +10612,7 @@
       <c r="B59" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="C59" s="39"/>
+      <c r="C59" s="74"/>
       <c r="D59" s="74"/>
       <c r="E59" s="74"/>
       <c r="F59" s="74"/>
@@ -10626,7 +10620,7 @@
       <c r="H59" s="76" t="s">
         <v>340</v>
       </c>
-      <c r="I59" s="90" t="s">
+      <c r="I59" s="89" t="s">
         <v>347</v>
       </c>
       <c r="J59" s="76" t="s">
@@ -10649,10 +10643,10 @@
       <c r="H60" s="75" t="s">
         <v>341</v>
       </c>
-      <c r="I60" s="89" t="s">
+      <c r="I60" s="88" t="s">
         <v>348</v>
       </c>
-      <c r="J60" s="89" t="s">
+      <c r="J60" s="88" t="s">
         <v>355</v>
       </c>
       <c r="K60" s="20"/>
@@ -10669,7 +10663,7 @@
       <c r="E61" s="73"/>
       <c r="F61" s="73"/>
       <c r="G61" s="58"/>
-      <c r="H61" s="89" t="s">
+      <c r="H61" s="88" t="s">
         <v>342</v>
       </c>
       <c r="I61" s="75" t="s">
@@ -10698,7 +10692,7 @@
       <c r="I62" s="75" t="s">
         <v>350</v>
       </c>
-      <c r="J62" s="89" t="s">
+      <c r="J62" s="88" t="s">
         <v>372</v>
       </c>
       <c r="K62" s="20"/>
@@ -10734,12 +10728,12 @@
       <c r="C64" s="73"/>
       <c r="D64" s="73"/>
       <c r="E64" s="73"/>
-      <c r="F64" s="20"/>
+      <c r="F64" s="73"/>
       <c r="G64" s="58"/>
       <c r="H64" s="75" t="s">
         <v>345</v>
       </c>
-      <c r="I64" s="89" t="s">
+      <c r="I64" s="88" t="s">
         <v>352</v>
       </c>
       <c r="J64" s="20"/>
@@ -10774,13 +10768,13 @@
       <c r="E66" s="73"/>
       <c r="F66" s="73"/>
       <c r="G66" s="58"/>
-      <c r="H66" s="93" t="s">
+      <c r="H66" s="92" t="s">
         <v>174</v>
       </c>
-      <c r="I66" s="94"/>
-      <c r="J66" s="94"/>
-      <c r="K66" s="94"/>
-      <c r="L66" s="95"/>
+      <c r="I66" s="93"/>
+      <c r="J66" s="93"/>
+      <c r="K66" s="93"/>
+      <c r="L66" s="94"/>
       <c r="M66" s="58"/>
     </row>
     <row r="67" spans="1:13" ht="15.75" thickBot="1">
@@ -10798,10 +10792,10 @@
       </c>
       <c r="I67" s="63"/>
       <c r="J67" s="63"/>
-      <c r="K67" s="99" t="s">
+      <c r="K67" s="98" t="s">
         <v>290</v>
       </c>
-      <c r="L67" s="100"/>
+      <c r="L67" s="99"/>
       <c r="M67" s="58"/>
     </row>
     <row r="68" spans="1:13" ht="15.75" thickBot="1">
@@ -10819,10 +10813,10 @@
       </c>
       <c r="I68" s="63"/>
       <c r="J68" s="63"/>
-      <c r="K68" s="99" t="s">
+      <c r="K68" s="98" t="s">
         <v>291</v>
       </c>
-      <c r="L68" s="100"/>
+      <c r="L68" s="99"/>
       <c r="M68" s="58"/>
     </row>
     <row r="69" spans="1:13" ht="15.75" thickBot="1">
@@ -10840,10 +10834,10 @@
       </c>
       <c r="I69" s="20"/>
       <c r="J69" s="20"/>
-      <c r="K69" s="96" t="s">
+      <c r="K69" s="95" t="s">
         <v>298</v>
       </c>
-      <c r="L69" s="97"/>
+      <c r="L69" s="96"/>
       <c r="M69" s="58"/>
     </row>
     <row r="70" spans="1:13" ht="15.75" thickBot="1">
@@ -10854,17 +10848,17 @@
       <c r="C70" s="73"/>
       <c r="D70" s="73"/>
       <c r="E70" s="77"/>
-      <c r="F70" s="20"/>
+      <c r="F70" s="73"/>
       <c r="G70" s="58"/>
       <c r="H70" s="75" t="s">
         <v>317</v>
       </c>
       <c r="I70" s="20"/>
       <c r="J70" s="20"/>
-      <c r="K70" s="96" t="s">
+      <c r="K70" s="95" t="s">
         <v>299</v>
       </c>
-      <c r="L70" s="97"/>
+      <c r="L70" s="96"/>
       <c r="M70" s="58"/>
     </row>
     <row r="71" spans="1:13" ht="15.75" thickBot="1">
@@ -10882,10 +10876,10 @@
       </c>
       <c r="I71" s="20"/>
       <c r="J71" s="20"/>
-      <c r="K71" s="96" t="s">
+      <c r="K71" s="95" t="s">
         <v>314</v>
       </c>
-      <c r="L71" s="97"/>
+      <c r="L71" s="96"/>
       <c r="M71" s="58"/>
     </row>
     <row r="72" spans="1:13" ht="15.75" thickBot="1">
@@ -10896,15 +10890,15 @@
       <c r="C72" s="73"/>
       <c r="D72" s="73"/>
       <c r="E72" s="73"/>
-      <c r="F72" s="85"/>
+      <c r="F72" s="80"/>
       <c r="G72" s="58"/>
       <c r="H72" s="20"/>
       <c r="I72" s="20"/>
       <c r="J72" s="20"/>
-      <c r="K72" s="96" t="s">
+      <c r="K72" s="95" t="s">
         <v>328</v>
       </c>
-      <c r="L72" s="97"/>
+      <c r="L72" s="96"/>
       <c r="M72" s="58"/>
     </row>
     <row r="73" spans="1:13" ht="15.75" thickBot="1">
@@ -10956,7 +10950,7 @@
       <c r="B75" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="C75" s="20"/>
+      <c r="C75" s="73"/>
       <c r="D75" s="73"/>
       <c r="E75" s="73"/>
       <c r="F75" s="73"/>
@@ -10978,7 +10972,7 @@
       <c r="C76" s="73"/>
       <c r="D76" s="73"/>
       <c r="E76" s="73"/>
-      <c r="F76" s="20"/>
+      <c r="F76" s="73"/>
       <c r="G76" s="58"/>
       <c r="H76" s="19" t="s">
         <v>177</v>
@@ -11013,7 +11007,7 @@
       <c r="B78" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="C78" s="20"/>
+      <c r="C78" s="73"/>
       <c r="D78" s="73"/>
       <c r="E78" s="73"/>
       <c r="F78" s="73"/>
@@ -11032,7 +11026,7 @@
       <c r="B79" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="C79" s="20"/>
+      <c r="C79" s="73"/>
       <c r="D79" s="73"/>
       <c r="E79" s="73"/>
       <c r="F79" s="73"/>
@@ -11116,7 +11110,7 @@
       <c r="H83" s="19" t="s">
         <v>184</v>
       </c>
-      <c r="I83" s="20"/>
+      <c r="I83" s="73"/>
       <c r="J83" s="73"/>
       <c r="K83" s="73"/>
       <c r="L83" s="73"/>
@@ -11154,7 +11148,7 @@
       <c r="H85" s="19" t="s">
         <v>186</v>
       </c>
-      <c r="I85" s="20"/>
+      <c r="I85" s="73"/>
       <c r="J85" s="73"/>
       <c r="K85" s="73"/>
       <c r="L85" s="20"/>
@@ -11173,7 +11167,7 @@
       <c r="H86" s="19" t="s">
         <v>187</v>
       </c>
-      <c r="I86" s="20"/>
+      <c r="I86" s="73"/>
       <c r="J86" s="73"/>
       <c r="K86" s="73"/>
       <c r="L86" s="73"/>
@@ -11230,7 +11224,7 @@
       <c r="H89" s="19" t="s">
         <v>190</v>
       </c>
-      <c r="I89" s="20"/>
+      <c r="I89" s="73"/>
       <c r="J89" s="73"/>
       <c r="K89" s="73"/>
       <c r="L89" s="73"/>
@@ -11260,7 +11254,7 @@
       <c r="B91" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="C91" s="20"/>
+      <c r="C91" s="73"/>
       <c r="D91" s="73"/>
       <c r="E91" s="73"/>
       <c r="F91" s="73"/>
@@ -11299,14 +11293,14 @@
         <v>86</v>
       </c>
       <c r="C93" s="73"/>
-      <c r="D93" s="20"/>
+      <c r="D93" s="73"/>
       <c r="E93" s="73"/>
       <c r="F93" s="73"/>
       <c r="G93" s="58"/>
       <c r="H93" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="I93" s="20"/>
+      <c r="I93" s="73"/>
       <c r="J93" s="73"/>
       <c r="K93" s="73"/>
       <c r="L93" s="20"/>
@@ -11382,7 +11376,7 @@
       <c r="H97" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="I97" s="20"/>
+      <c r="I97" s="73"/>
       <c r="J97" s="73"/>
       <c r="K97" s="73"/>
       <c r="L97" s="73"/>
@@ -11433,7 +11427,7 @@
       </c>
       <c r="C100" s="74"/>
       <c r="D100" s="74"/>
-      <c r="E100" s="39"/>
+      <c r="E100" s="74"/>
       <c r="F100" s="83"/>
       <c r="G100" s="58"/>
       <c r="H100" s="19" t="s">
@@ -11453,7 +11447,7 @@
       <c r="C101" s="73"/>
       <c r="D101" s="73"/>
       <c r="E101" s="73"/>
-      <c r="F101" s="20"/>
+      <c r="F101" s="73"/>
       <c r="G101" s="58"/>
       <c r="H101" s="19" t="s">
         <v>200</v>
@@ -11491,12 +11485,12 @@
       <c r="C103" s="73"/>
       <c r="D103" s="73"/>
       <c r="E103" s="73"/>
-      <c r="F103" s="86"/>
+      <c r="F103" s="85"/>
       <c r="G103" s="58"/>
       <c r="H103" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="I103" s="20"/>
+      <c r="I103" s="73"/>
       <c r="J103" s="73"/>
       <c r="K103" s="73"/>
       <c r="L103" s="62"/>
@@ -11576,7 +11570,7 @@
       <c r="B107" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="C107" s="20"/>
+      <c r="C107" s="73"/>
       <c r="D107" s="73"/>
       <c r="E107" s="73"/>
       <c r="F107" s="73"/>
@@ -11595,7 +11589,7 @@
       <c r="B108" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="C108" s="20"/>
+      <c r="C108" s="73"/>
       <c r="D108" s="73"/>
       <c r="E108" s="73"/>
       <c r="F108" s="73"/>
@@ -11614,7 +11608,7 @@
       <c r="B109" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="C109" s="20"/>
+      <c r="C109" s="73"/>
       <c r="D109" s="73"/>
       <c r="E109" s="73"/>
       <c r="F109" s="73"/>
@@ -11660,10 +11654,10 @@
       <c r="H111" s="19" t="s">
         <v>208</v>
       </c>
-      <c r="I111" s="20"/>
+      <c r="I111" s="73"/>
       <c r="J111" s="73"/>
       <c r="K111" s="73"/>
-      <c r="L111" s="20"/>
+      <c r="L111" s="73"/>
       <c r="M111" s="58"/>
     </row>
     <row r="112" spans="1:13" ht="15.75" thickBot="1">
@@ -11699,7 +11693,7 @@
         <v>210</v>
       </c>
       <c r="I113" s="73"/>
-      <c r="J113" s="20"/>
+      <c r="J113" s="73"/>
       <c r="K113" s="73"/>
       <c r="L113" s="20"/>
       <c r="M113" s="58"/>
@@ -11733,7 +11727,7 @@
       <c r="C115" s="73"/>
       <c r="D115" s="73"/>
       <c r="E115" s="73"/>
-      <c r="F115" s="20"/>
+      <c r="F115" s="73"/>
       <c r="G115" s="58"/>
       <c r="H115" s="19" t="s">
         <v>212</v>
@@ -11749,7 +11743,7 @@
       <c r="B116" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="C116" s="20"/>
+      <c r="C116" s="73"/>
       <c r="D116" s="73"/>
       <c r="E116" s="73"/>
       <c r="F116" s="73"/>
@@ -11839,7 +11833,7 @@
       </c>
       <c r="I120" s="73"/>
       <c r="J120" s="73"/>
-      <c r="K120" s="88"/>
+      <c r="K120" s="87"/>
       <c r="L120" s="73"/>
       <c r="M120" s="58"/>
     </row>
@@ -11908,7 +11902,7 @@
       <c r="C124" s="73"/>
       <c r="D124" s="73"/>
       <c r="E124" s="73"/>
-      <c r="F124" s="20"/>
+      <c r="F124" s="73"/>
       <c r="G124" s="58"/>
       <c r="H124" s="19" t="s">
         <v>221</v>
@@ -11946,7 +11940,7 @@
       <c r="C126" s="73"/>
       <c r="D126" s="73"/>
       <c r="E126" s="73"/>
-      <c r="F126" s="20"/>
+      <c r="F126" s="80"/>
       <c r="G126" s="58"/>
       <c r="H126" s="19" t="s">
         <v>222</v>
@@ -12038,7 +12032,7 @@
       <c r="B131" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="C131" s="101"/>
+      <c r="C131" s="74"/>
       <c r="D131" s="74"/>
       <c r="E131" s="74"/>
       <c r="F131" s="83"/>
@@ -12113,8 +12107,8 @@
       <c r="B135" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="C135" s="43"/>
-      <c r="D135" s="87"/>
+      <c r="C135" s="86"/>
+      <c r="D135" s="86"/>
       <c r="E135" s="73"/>
       <c r="F135" s="20"/>
       <c r="G135" s="4"/>
@@ -12206,7 +12200,7 @@
       <c r="C139" s="73"/>
       <c r="D139" s="73"/>
       <c r="E139" s="73"/>
-      <c r="F139" s="20"/>
+      <c r="F139" s="73"/>
       <c r="G139" s="4"/>
       <c r="H139" s="52" t="s">
         <v>240</v>
@@ -12245,7 +12239,7 @@
       </c>
       <c r="C141" s="73"/>
       <c r="D141" s="73"/>
-      <c r="E141" s="20"/>
+      <c r="E141" s="73"/>
       <c r="F141" s="73"/>
       <c r="G141" s="4"/>
       <c r="H141" s="4"/>
@@ -12264,7 +12258,7 @@
       <c r="C142" s="73"/>
       <c r="D142" s="73"/>
       <c r="E142" s="73"/>
-      <c r="F142" s="86"/>
+      <c r="F142" s="85"/>
       <c r="G142" s="4"/>
       <c r="H142" s="44" t="s">
         <v>243</v>
@@ -12525,7 +12519,7 @@
       <c r="B154" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="C154" s="20"/>
+      <c r="C154" s="73"/>
       <c r="D154" s="73"/>
       <c r="E154" s="73"/>
       <c r="F154" s="20"/>
@@ -12548,7 +12542,7 @@
       <c r="C155" s="73"/>
       <c r="D155" s="73"/>
       <c r="E155" s="73"/>
-      <c r="F155" s="86"/>
+      <c r="F155" s="85"/>
       <c r="G155" s="4"/>
       <c r="H155" s="4"/>
       <c r="I155" s="4"/>

</xml_diff>

<commit_message>
4 items upped / missing items names added
added names of missing items to help finding them easily
</commit_message>
<xml_diff>
--- a/check list.xlsx
+++ b/check list.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1246" uniqueCount="454">
   <si>
     <t>ARMOR</t>
   </si>
@@ -1160,13 +1160,244 @@
   </si>
   <si>
     <t>Felblood</t>
+  </si>
+  <si>
+    <r>
+      <t>Amulets</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13.5"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>(All done)</t>
+    </r>
+  </si>
+  <si>
+    <t>Ouroboros</t>
+  </si>
+  <si>
+    <t>QQ</t>
+  </si>
+  <si>
+    <t>Witchcraft</t>
+  </si>
+  <si>
+    <t>Bad Mood Ring</t>
+  </si>
+  <si>
+    <t>Assur's bane</t>
+  </si>
+  <si>
+    <t>Sigil of the 7 deadly sin</t>
+  </si>
+  <si>
+    <t>Zann Esu's Stone</t>
+  </si>
+  <si>
+    <t>kekeke</t>
+  </si>
+  <si>
+    <t>Arkenstone</t>
+  </si>
+  <si>
+    <t>Bag of tricks</t>
+  </si>
+  <si>
+    <t>Arrowsider</t>
+  </si>
+  <si>
+    <t>Devils's dance</t>
+  </si>
+  <si>
+    <t>Idol of stars</t>
+  </si>
+  <si>
+    <t>Vizjun's Ball Bearing</t>
+  </si>
+  <si>
+    <t>Nagapearl</t>
+  </si>
+  <si>
+    <t>Auriel's Focus</t>
+  </si>
+  <si>
+    <t>orb of annihilation</t>
+  </si>
+  <si>
+    <t>Lodestone</t>
+  </si>
+  <si>
+    <t>Kara's Trinket</t>
+  </si>
+  <si>
+    <t>Monsterball</t>
+  </si>
+  <si>
+    <t>Eye of malic</t>
+  </si>
+  <si>
+    <t>Apple of discord</t>
+  </si>
+  <si>
+    <t>The perfect sphere</t>
+  </si>
+  <si>
+    <t>Wizard's Cloak</t>
+  </si>
+  <si>
+    <t>Lunar Eclipse</t>
+  </si>
+  <si>
+    <t>Titan's Steps</t>
+  </si>
+  <si>
+    <t>Frigid Chopper</t>
+  </si>
+  <si>
+    <t>Klonk</t>
+  </si>
+  <si>
+    <t>Heaven's Bite</t>
+  </si>
+  <si>
+    <t>The Dark Descent</t>
+  </si>
+  <si>
+    <t>Gonnagal's Dirk</t>
+  </si>
+  <si>
+    <t>Scream of Nature</t>
+  </si>
+  <si>
+    <t>Gladiator's Rage</t>
+  </si>
+  <si>
+    <t>The Might of the Ancients</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skeid's Battlesong </t>
+  </si>
+  <si>
+    <t>Peace Warder</t>
+  </si>
+  <si>
+    <t>Dark Talon</t>
+  </si>
+  <si>
+    <t>Feltongue</t>
+  </si>
+  <si>
+    <t>Roflchopper</t>
+  </si>
+  <si>
+    <t>Hellslayer</t>
+  </si>
+  <si>
+    <t>Staff of Shadows</t>
+  </si>
+  <si>
+    <t>Hovering Dame</t>
+  </si>
+  <si>
+    <t>Dragonclaw</t>
+  </si>
+  <si>
+    <t>Chober Chaber</t>
+  </si>
+  <si>
+    <t>Plague Bolter</t>
+  </si>
+  <si>
+    <t>Mons Meg</t>
+  </si>
+  <si>
+    <t>Ranger's Path</t>
+  </si>
+  <si>
+    <t>Dragonfly</t>
+  </si>
+  <si>
+    <t>Wrath of Nature</t>
+  </si>
+  <si>
+    <t>Washi Bai Ron</t>
+  </si>
+  <si>
+    <t>Golden Chariot</t>
+  </si>
+  <si>
+    <t>Soul Harvest</t>
+  </si>
+  <si>
+    <t>Uldyssian's Awakening</t>
+  </si>
+  <si>
+    <t>Gathering Storm</t>
+  </si>
+  <si>
+    <t>Eerie Flash</t>
+  </si>
+  <si>
+    <t>Dark Guardian</t>
+  </si>
+  <si>
+    <t>Sentry of Death</t>
+  </si>
+  <si>
+    <t>Sinwar</t>
+  </si>
+  <si>
+    <t>Grim Silhouette</t>
+  </si>
+  <si>
+    <t>Mark of the Que-Hagan</t>
+  </si>
+  <si>
+    <t>Phoenix Ash</t>
+  </si>
+  <si>
+    <t>Tobio's Key</t>
+  </si>
+  <si>
+    <t>The Vanquisher</t>
+  </si>
+  <si>
+    <t>Sculptor of Pain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ironhood </t>
+  </si>
+  <si>
+    <t>Warlock's Brilliance</t>
+  </si>
+  <si>
+    <t>Wolf Teeth</t>
+  </si>
+  <si>
+    <t>Lilith's Legion</t>
+  </si>
+  <si>
+    <t>Wisdom of Scosglen</t>
+  </si>
+  <si>
+    <t>Forest Defender</t>
+  </si>
+  <si>
+    <t>Blessed Wrath</t>
+  </si>
+  <si>
+    <t>Fauztin's Shadow</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="25">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1338,6 +1569,25 @@
     <font>
       <sz val="9"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1540,7 +1790,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1797,6 +2047,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2665,13 +2924,13 @@
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
       <c r="G27" s="7"/>
-      <c r="H27" s="91" t="s">
+      <c r="H27" s="94" t="s">
         <v>170</v>
       </c>
-      <c r="I27" s="91"/>
-      <c r="J27" s="91"/>
-      <c r="K27" s="91"/>
-      <c r="L27" s="91"/>
+      <c r="I27" s="94"/>
+      <c r="J27" s="94"/>
+      <c r="K27" s="94"/>
+      <c r="L27" s="94"/>
       <c r="M27" s="7"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1">
@@ -2826,13 +3085,13 @@
       <c r="E36" s="20"/>
       <c r="F36" s="29"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="91" t="s">
+      <c r="H36" s="94" t="s">
         <v>171</v>
       </c>
-      <c r="I36" s="91"/>
-      <c r="J36" s="91"/>
-      <c r="K36" s="91"/>
-      <c r="L36" s="91"/>
+      <c r="I36" s="94"/>
+      <c r="J36" s="94"/>
+      <c r="K36" s="94"/>
+      <c r="L36" s="94"/>
       <c r="M36" s="7"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
@@ -2993,13 +3252,13 @@
         <v>3</v>
       </c>
       <c r="G45" s="7"/>
-      <c r="H45" s="91" t="s">
+      <c r="H45" s="94" t="s">
         <v>172</v>
       </c>
-      <c r="I45" s="91"/>
-      <c r="J45" s="91"/>
-      <c r="K45" s="91"/>
-      <c r="L45" s="91"/>
+      <c r="I45" s="94"/>
+      <c r="J45" s="94"/>
+      <c r="K45" s="94"/>
+      <c r="L45" s="94"/>
       <c r="M45" s="7"/>
     </row>
     <row r="46" spans="1:13" ht="15.75" thickBot="1">
@@ -3148,13 +3407,13 @@
       <c r="E54" s="39"/>
       <c r="F54" s="39"/>
       <c r="G54" s="7"/>
-      <c r="H54" s="91" t="s">
+      <c r="H54" s="94" t="s">
         <v>173</v>
       </c>
-      <c r="I54" s="91"/>
-      <c r="J54" s="91"/>
-      <c r="K54" s="91"/>
-      <c r="L54" s="91"/>
+      <c r="I54" s="94"/>
+      <c r="J54" s="94"/>
+      <c r="K54" s="94"/>
+      <c r="L54" s="94"/>
       <c r="M54" s="7"/>
     </row>
     <row r="55" spans="1:13" ht="15.75" thickBot="1">
@@ -3303,13 +3562,13 @@
       <c r="E63" s="20"/>
       <c r="F63" s="20"/>
       <c r="G63" s="7"/>
-      <c r="H63" s="91" t="s">
+      <c r="H63" s="94" t="s">
         <v>174</v>
       </c>
-      <c r="I63" s="91"/>
-      <c r="J63" s="91"/>
-      <c r="K63" s="91"/>
-      <c r="L63" s="91"/>
+      <c r="I63" s="94"/>
+      <c r="J63" s="94"/>
+      <c r="K63" s="94"/>
+      <c r="L63" s="94"/>
       <c r="M63" s="7"/>
     </row>
     <row r="64" spans="1:13" ht="15.75" thickBot="1">
@@ -4618,11 +4877,11 @@
       <c r="E132" s="20"/>
       <c r="F132" s="20"/>
       <c r="G132" s="7"/>
-      <c r="H132" s="90"/>
-      <c r="I132" s="90"/>
-      <c r="J132" s="90"/>
-      <c r="K132" s="90"/>
-      <c r="L132" s="90"/>
+      <c r="H132" s="93"/>
+      <c r="I132" s="93"/>
+      <c r="J132" s="93"/>
+      <c r="K132" s="93"/>
+      <c r="L132" s="93"/>
       <c r="M132" s="7"/>
     </row>
     <row r="133" spans="1:14" ht="18" thickBot="1">
@@ -6368,13 +6627,13 @@
       <c r="E30" s="20"/>
       <c r="F30" s="20"/>
       <c r="G30" s="58"/>
-      <c r="H30" s="92" t="s">
+      <c r="H30" s="95" t="s">
         <v>170</v>
       </c>
-      <c r="I30" s="93"/>
-      <c r="J30" s="93"/>
-      <c r="K30" s="93"/>
-      <c r="L30" s="94"/>
+      <c r="I30" s="96"/>
+      <c r="J30" s="96"/>
+      <c r="K30" s="96"/>
+      <c r="L30" s="97"/>
       <c r="M30" s="58"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1">
@@ -6529,13 +6788,13 @@
       <c r="E39" s="20"/>
       <c r="F39" s="62"/>
       <c r="G39" s="58"/>
-      <c r="H39" s="92" t="s">
+      <c r="H39" s="95" t="s">
         <v>171</v>
       </c>
-      <c r="I39" s="93"/>
-      <c r="J39" s="93"/>
-      <c r="K39" s="93"/>
-      <c r="L39" s="94"/>
+      <c r="I39" s="96"/>
+      <c r="J39" s="96"/>
+      <c r="K39" s="96"/>
+      <c r="L39" s="97"/>
       <c r="M39" s="58"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" thickBot="1">
@@ -6696,13 +6955,13 @@
         <v>3</v>
       </c>
       <c r="G48" s="58"/>
-      <c r="H48" s="92" t="s">
+      <c r="H48" s="95" t="s">
         <v>172</v>
       </c>
-      <c r="I48" s="93"/>
-      <c r="J48" s="93"/>
-      <c r="K48" s="93"/>
-      <c r="L48" s="94"/>
+      <c r="I48" s="96"/>
+      <c r="J48" s="96"/>
+      <c r="K48" s="96"/>
+      <c r="L48" s="97"/>
       <c r="M48" s="58"/>
     </row>
     <row r="49" spans="1:13" ht="15.75" thickBot="1">
@@ -6851,13 +7110,13 @@
       <c r="E57" s="39"/>
       <c r="F57" s="39"/>
       <c r="G57" s="58"/>
-      <c r="H57" s="92" t="s">
+      <c r="H57" s="95" t="s">
         <v>173</v>
       </c>
-      <c r="I57" s="93"/>
-      <c r="J57" s="93"/>
-      <c r="K57" s="93"/>
-      <c r="L57" s="94"/>
+      <c r="I57" s="96"/>
+      <c r="J57" s="96"/>
+      <c r="K57" s="96"/>
+      <c r="L57" s="97"/>
       <c r="M57" s="58"/>
     </row>
     <row r="58" spans="1:13" ht="15.75" thickBot="1">
@@ -7006,13 +7265,13 @@
       <c r="E66" s="20"/>
       <c r="F66" s="20"/>
       <c r="G66" s="58"/>
-      <c r="H66" s="92" t="s">
+      <c r="H66" s="95" t="s">
         <v>174</v>
       </c>
-      <c r="I66" s="93"/>
-      <c r="J66" s="93"/>
-      <c r="K66" s="93"/>
-      <c r="L66" s="94"/>
+      <c r="I66" s="96"/>
+      <c r="J66" s="96"/>
+      <c r="K66" s="96"/>
+      <c r="L66" s="97"/>
       <c r="M66" s="58"/>
     </row>
     <row r="67" spans="1:13" ht="15.75" thickBot="1">
@@ -9369,8 +9628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B116" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C124" sqref="C124"/>
+    <sheetView tabSelected="1" topLeftCell="H92" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J98" sqref="J98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9390,40 +9649,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="23.25" customHeight="1">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="100" t="s">
         <v>284</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97"/>
-      <c r="L1" s="97"/>
-      <c r="M1" s="97"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
+      <c r="J1" s="100"/>
+      <c r="K1" s="100"/>
+      <c r="L1" s="100"/>
+      <c r="M1" s="100"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1">
-      <c r="A2" s="97"/>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
+      <c r="A2" s="100"/>
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="100"/>
+      <c r="L2" s="100"/>
+      <c r="M2" s="100"/>
       <c r="N2" s="1"/>
       <c r="O2" s="69"/>
       <c r="P2" s="70" t="s">
@@ -9432,19 +9691,19 @@
       <c r="Q2" s="1"/>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1">
-      <c r="A3" s="97"/>
-      <c r="B3" s="97"/>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
+      <c r="A3" s="100"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -9660,7 +9919,7 @@
       <c r="L13" s="73"/>
       <c r="M13" s="58"/>
     </row>
-    <row r="14" spans="1:17" ht="15.75" thickBot="1">
+    <row r="14" spans="1:17" ht="26.25" thickBot="1">
       <c r="A14" s="58"/>
       <c r="B14" s="19" t="s">
         <v>12</v>
@@ -9676,7 +9935,9 @@
       <c r="I14" s="73"/>
       <c r="J14" s="73"/>
       <c r="K14" s="73"/>
-      <c r="L14" s="20"/>
+      <c r="L14" s="20" t="s">
+        <v>426</v>
+      </c>
       <c r="M14" s="58"/>
     </row>
     <row r="15" spans="1:17" ht="15.75" thickBot="1">
@@ -9732,7 +9993,9 @@
       </c>
       <c r="I17" s="73"/>
       <c r="J17" s="73"/>
-      <c r="K17" s="20"/>
+      <c r="K17" s="20" t="s">
+        <v>427</v>
+      </c>
       <c r="L17" s="73"/>
       <c r="M17" s="58"/>
     </row>
@@ -9755,7 +10018,7 @@
       <c r="L18" s="73"/>
       <c r="M18" s="58"/>
     </row>
-    <row r="19" spans="1:13" ht="15.75" thickBot="1">
+    <row r="19" spans="1:13" ht="26.25" thickBot="1">
       <c r="A19" s="58"/>
       <c r="B19" s="19" t="s">
         <v>315</v>
@@ -9771,7 +10034,9 @@
       <c r="I19" s="73"/>
       <c r="J19" s="73"/>
       <c r="K19" s="73"/>
-      <c r="L19" s="20"/>
+      <c r="L19" s="20" t="s">
+        <v>428</v>
+      </c>
       <c r="M19" s="58"/>
     </row>
     <row r="20" spans="1:13" ht="15.75" thickBot="1">
@@ -9793,7 +10058,7 @@
       <c r="L20" s="73"/>
       <c r="M20" s="58"/>
     </row>
-    <row r="21" spans="1:13" ht="15.75" thickBot="1">
+    <row r="21" spans="1:13" ht="26.25" thickBot="1">
       <c r="A21" s="58"/>
       <c r="B21" s="19" t="s">
         <v>18</v>
@@ -9801,7 +10066,9 @@
       <c r="C21" s="73"/>
       <c r="D21" s="73"/>
       <c r="E21" s="73"/>
-      <c r="F21" s="20"/>
+      <c r="F21" s="20" t="s">
+        <v>405</v>
+      </c>
       <c r="G21" s="58"/>
       <c r="H21" s="19" t="s">
         <v>162</v>
@@ -9847,10 +10114,12 @@
       <c r="I23" s="73"/>
       <c r="J23" s="73"/>
       <c r="K23" s="73"/>
-      <c r="L23" s="20"/>
+      <c r="L23" s="20" t="s">
+        <v>429</v>
+      </c>
       <c r="M23" s="58"/>
     </row>
-    <row r="24" spans="1:13" ht="15.75" thickBot="1">
+    <row r="24" spans="1:13" ht="26.25" thickBot="1">
       <c r="A24" s="58"/>
       <c r="B24" s="19" t="s">
         <v>21</v>
@@ -9866,7 +10135,9 @@
       <c r="I24" s="73"/>
       <c r="J24" s="73"/>
       <c r="K24" s="73"/>
-      <c r="L24" s="20"/>
+      <c r="L24" s="20" t="s">
+        <v>430</v>
+      </c>
       <c r="M24" s="58"/>
     </row>
     <row r="25" spans="1:13" ht="15.75" thickBot="1">
@@ -9932,7 +10203,7 @@
       <c r="L27" s="73"/>
       <c r="M27" s="58"/>
     </row>
-    <row r="28" spans="1:13" ht="15.75" thickBot="1">
+    <row r="28" spans="1:13" ht="26.25" thickBot="1">
       <c r="A28" s="58"/>
       <c r="B28" s="19" t="s">
         <v>24</v>
@@ -9947,11 +10218,13 @@
       </c>
       <c r="I28" s="73"/>
       <c r="J28" s="73"/>
-      <c r="K28" s="20"/>
+      <c r="K28" s="20" t="s">
+        <v>431</v>
+      </c>
       <c r="L28" s="85"/>
       <c r="M28" s="58"/>
     </row>
-    <row r="29" spans="1:13" ht="15.75" thickBot="1">
+    <row r="29" spans="1:13" ht="26.25" thickBot="1">
       <c r="A29" s="58"/>
       <c r="B29" s="19" t="s">
         <v>25</v>
@@ -9959,7 +10232,9 @@
       <c r="C29" s="73"/>
       <c r="D29" s="73"/>
       <c r="E29" s="73"/>
-      <c r="F29" s="20"/>
+      <c r="F29" s="20" t="s">
+        <v>406</v>
+      </c>
       <c r="G29" s="58"/>
       <c r="H29" s="58"/>
       <c r="I29" s="58"/>
@@ -9980,13 +10255,13 @@
       <c r="E30" s="73"/>
       <c r="F30" s="73"/>
       <c r="G30" s="58"/>
-      <c r="H30" s="92" t="s">
+      <c r="H30" s="95" t="s">
         <v>170</v>
       </c>
-      <c r="I30" s="93"/>
-      <c r="J30" s="93"/>
-      <c r="K30" s="93"/>
-      <c r="L30" s="94"/>
+      <c r="I30" s="96"/>
+      <c r="J30" s="96"/>
+      <c r="K30" s="96"/>
+      <c r="L30" s="97"/>
       <c r="M30" s="58"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1">
@@ -10008,7 +10283,9 @@
       <c r="J31" s="76" t="s">
         <v>367</v>
       </c>
-      <c r="K31" s="63"/>
+      <c r="K31" s="76" t="s">
+        <v>383</v>
+      </c>
       <c r="L31" s="63"/>
       <c r="M31" s="58"/>
     </row>
@@ -10031,7 +10308,9 @@
       <c r="J32" s="76" t="s">
         <v>368</v>
       </c>
-      <c r="K32" s="63"/>
+      <c r="K32" s="92" t="s">
+        <v>384</v>
+      </c>
       <c r="L32" s="63"/>
       <c r="M32" s="58"/>
     </row>
@@ -10052,11 +10331,13 @@
       <c r="J33" s="88" t="s">
         <v>332</v>
       </c>
-      <c r="K33" s="20"/>
+      <c r="K33" s="91" t="s">
+        <v>385</v>
+      </c>
       <c r="L33" s="20"/>
       <c r="M33" s="58"/>
     </row>
-    <row r="34" spans="1:13" ht="18" thickBot="1">
+    <row r="34" spans="1:13" ht="26.25" thickBot="1">
       <c r="A34" s="58"/>
       <c r="B34" s="33" t="s">
         <v>29</v>
@@ -10083,11 +10364,13 @@
       <c r="J34" s="75" t="s">
         <v>374</v>
       </c>
-      <c r="K34" s="20"/>
+      <c r="K34" s="91" t="s">
+        <v>386</v>
+      </c>
       <c r="L34" s="20"/>
       <c r="M34" s="58"/>
     </row>
-    <row r="35" spans="1:13" ht="15.75" thickBot="1">
+    <row r="35" spans="1:13" ht="26.25" thickBot="1">
       <c r="A35" s="58"/>
       <c r="B35" s="19" t="s">
         <v>30</v>
@@ -10106,18 +10389,20 @@
       <c r="J35" s="75" t="s">
         <v>379</v>
       </c>
-      <c r="K35" s="20"/>
+      <c r="K35" s="91" t="s">
+        <v>387</v>
+      </c>
       <c r="L35" s="20"/>
       <c r="M35" s="58"/>
     </row>
-    <row r="36" spans="1:13" ht="15.75" thickBot="1">
+    <row r="36" spans="1:13" ht="26.25" thickBot="1">
       <c r="A36" s="58"/>
       <c r="B36" s="19" t="s">
         <v>31</v>
       </c>
       <c r="C36" s="73"/>
       <c r="D36" s="73"/>
-      <c r="E36" s="20"/>
+      <c r="E36" s="73"/>
       <c r="F36" s="73"/>
       <c r="G36" s="58"/>
       <c r="H36" s="75" t="s">
@@ -10126,7 +10411,9 @@
       <c r="I36" s="75" t="s">
         <v>363</v>
       </c>
-      <c r="J36" s="20"/>
+      <c r="J36" s="91" t="s">
+        <v>370</v>
+      </c>
       <c r="K36" s="20"/>
       <c r="L36" s="20"/>
       <c r="M36" s="58"/>
@@ -10139,7 +10426,7 @@
       <c r="C37" s="73"/>
       <c r="D37" s="73"/>
       <c r="E37" s="73"/>
-      <c r="F37" s="20"/>
+      <c r="F37" s="73"/>
       <c r="G37" s="58"/>
       <c r="H37" s="75" t="s">
         <v>332</v>
@@ -10147,7 +10434,9 @@
       <c r="I37" s="75" t="s">
         <v>365</v>
       </c>
-      <c r="J37" s="20"/>
+      <c r="J37" s="91" t="s">
+        <v>382</v>
+      </c>
       <c r="K37" s="20"/>
       <c r="L37" s="20"/>
       <c r="M37" s="58"/>
@@ -10179,13 +10468,13 @@
       <c r="E39" s="73"/>
       <c r="F39" s="85"/>
       <c r="G39" s="58"/>
-      <c r="H39" s="92" t="s">
-        <v>171</v>
-      </c>
-      <c r="I39" s="93"/>
-      <c r="J39" s="93"/>
-      <c r="K39" s="93"/>
-      <c r="L39" s="94"/>
+      <c r="H39" s="95" t="s">
+        <v>381</v>
+      </c>
+      <c r="I39" s="96"/>
+      <c r="J39" s="96"/>
+      <c r="K39" s="96"/>
+      <c r="L39" s="97"/>
       <c r="M39" s="58"/>
     </row>
     <row r="40" spans="1:13" ht="30.75" thickBot="1">
@@ -10263,7 +10552,7 @@
       <c r="J42" s="75" t="s">
         <v>369</v>
       </c>
-      <c r="K42" s="20"/>
+      <c r="K42" s="90"/>
       <c r="L42" s="20"/>
       <c r="M42" s="58"/>
     </row>
@@ -10275,7 +10564,9 @@
       <c r="C43" s="73"/>
       <c r="D43" s="73"/>
       <c r="E43" s="73"/>
-      <c r="F43" s="20"/>
+      <c r="F43" s="20" t="s">
+        <v>407</v>
+      </c>
       <c r="G43" s="58"/>
       <c r="H43" s="75" t="s">
         <v>307</v>
@@ -10392,13 +10683,13 @@
         <v>3</v>
       </c>
       <c r="G48" s="58"/>
-      <c r="H48" s="92" t="s">
+      <c r="H48" s="95" t="s">
         <v>172</v>
       </c>
-      <c r="I48" s="93"/>
-      <c r="J48" s="93"/>
-      <c r="K48" s="93"/>
-      <c r="L48" s="94"/>
+      <c r="I48" s="96"/>
+      <c r="J48" s="96"/>
+      <c r="K48" s="96"/>
+      <c r="L48" s="97"/>
       <c r="M48" s="58"/>
     </row>
     <row r="49" spans="1:13" ht="15.75" thickBot="1">
@@ -10417,7 +10708,9 @@
       <c r="I49" s="76" t="s">
         <v>329</v>
       </c>
-      <c r="J49" s="63"/>
+      <c r="J49" s="92" t="s">
+        <v>388</v>
+      </c>
       <c r="K49" s="63"/>
       <c r="L49" s="63"/>
       <c r="M49" s="58"/>
@@ -10438,7 +10731,9 @@
       <c r="I50" s="76" t="s">
         <v>330</v>
       </c>
-      <c r="J50" s="63"/>
+      <c r="J50" s="92" t="s">
+        <v>389</v>
+      </c>
       <c r="K50" s="63"/>
       <c r="L50" s="63"/>
       <c r="M50" s="58"/>
@@ -10459,7 +10754,9 @@
       <c r="I51" s="88" t="s">
         <v>331</v>
       </c>
-      <c r="J51" s="20"/>
+      <c r="J51" s="91" t="s">
+        <v>390</v>
+      </c>
       <c r="K51" s="20"/>
       <c r="L51" s="20"/>
       <c r="M51" s="58"/>
@@ -10575,16 +10872,16 @@
       <c r="E57" s="74"/>
       <c r="F57" s="74"/>
       <c r="G57" s="58"/>
-      <c r="H57" s="92" t="s">
+      <c r="H57" s="95" t="s">
         <v>173</v>
       </c>
-      <c r="I57" s="93"/>
-      <c r="J57" s="93"/>
-      <c r="K57" s="93"/>
-      <c r="L57" s="94"/>
+      <c r="I57" s="96"/>
+      <c r="J57" s="96"/>
+      <c r="K57" s="96"/>
+      <c r="L57" s="97"/>
       <c r="M57" s="58"/>
     </row>
-    <row r="58" spans="1:13" ht="15.75" thickBot="1">
+    <row r="58" spans="1:13" ht="30.75" thickBot="1">
       <c r="A58" s="58"/>
       <c r="B58" s="19" t="s">
         <v>51</v>
@@ -10592,7 +10889,9 @@
       <c r="C58" s="73"/>
       <c r="D58" s="73"/>
       <c r="E58" s="73"/>
-      <c r="F58" s="20"/>
+      <c r="F58" s="20" t="s">
+        <v>408</v>
+      </c>
       <c r="G58" s="58"/>
       <c r="H58" s="76" t="s">
         <v>339</v>
@@ -10603,11 +10902,15 @@
       <c r="J58" s="76" t="s">
         <v>353</v>
       </c>
-      <c r="K58" s="63"/>
-      <c r="L58" s="63"/>
+      <c r="K58" s="63" t="s">
+        <v>396</v>
+      </c>
+      <c r="L58" s="63" t="s">
+        <v>403</v>
+      </c>
       <c r="M58" s="58"/>
     </row>
-    <row r="59" spans="1:13" ht="24.75" thickBot="1">
+    <row r="59" spans="1:13" ht="45.75" thickBot="1">
       <c r="A59" s="58"/>
       <c r="B59" s="38" t="s">
         <v>52</v>
@@ -10626,19 +10929,27 @@
       <c r="J59" s="76" t="s">
         <v>354</v>
       </c>
-      <c r="K59" s="63"/>
-      <c r="L59" s="63"/>
+      <c r="K59" s="63" t="s">
+        <v>397</v>
+      </c>
+      <c r="L59" s="63" t="s">
+        <v>404</v>
+      </c>
       <c r="M59" s="58"/>
     </row>
-    <row r="60" spans="1:13" ht="23.25" thickBot="1">
+    <row r="60" spans="1:13" ht="26.25" thickBot="1">
       <c r="A60" s="58"/>
       <c r="B60" s="19" t="s">
         <v>53</v>
       </c>
       <c r="C60" s="73"/>
       <c r="D60" s="73"/>
-      <c r="E60" s="20"/>
-      <c r="F60" s="20"/>
+      <c r="E60" s="20" t="s">
+        <v>409</v>
+      </c>
+      <c r="F60" s="20" t="s">
+        <v>410</v>
+      </c>
       <c r="G60" s="58"/>
       <c r="H60" s="75" t="s">
         <v>341</v>
@@ -10649,7 +10960,9 @@
       <c r="J60" s="88" t="s">
         <v>355</v>
       </c>
-      <c r="K60" s="20"/>
+      <c r="K60" s="20" t="s">
+        <v>398</v>
+      </c>
       <c r="L60" s="20"/>
       <c r="M60" s="58"/>
     </row>
@@ -10672,11 +10985,13 @@
       <c r="J61" s="75" t="s">
         <v>371</v>
       </c>
-      <c r="K61" s="20"/>
+      <c r="K61" s="20" t="s">
+        <v>399</v>
+      </c>
       <c r="L61" s="20"/>
       <c r="M61" s="58"/>
     </row>
-    <row r="62" spans="1:13" ht="15.75" thickBot="1">
+    <row r="62" spans="1:13" ht="26.25" thickBot="1">
       <c r="A62" s="58"/>
       <c r="B62" s="19" t="s">
         <v>55</v>
@@ -10695,11 +11010,13 @@
       <c r="J62" s="88" t="s">
         <v>372</v>
       </c>
-      <c r="K62" s="20"/>
+      <c r="K62" s="20" t="s">
+        <v>400</v>
+      </c>
       <c r="L62" s="20"/>
       <c r="M62" s="58"/>
     </row>
-    <row r="63" spans="1:13" ht="15.75" thickBot="1">
+    <row r="63" spans="1:13" ht="26.25" thickBot="1">
       <c r="A63" s="58"/>
       <c r="B63" s="19" t="s">
         <v>56</v>
@@ -10707,7 +11024,9 @@
       <c r="C63" s="73"/>
       <c r="D63" s="73"/>
       <c r="E63" s="73"/>
-      <c r="F63" s="20"/>
+      <c r="F63" s="20" t="s">
+        <v>411</v>
+      </c>
       <c r="G63" s="58"/>
       <c r="H63" s="75" t="s">
         <v>344</v>
@@ -10715,12 +11034,16 @@
       <c r="I63" s="75" t="s">
         <v>351</v>
       </c>
-      <c r="J63" s="20"/>
-      <c r="K63" s="20"/>
+      <c r="J63" s="20" t="s">
+        <v>394</v>
+      </c>
+      <c r="K63" s="20" t="s">
+        <v>401</v>
+      </c>
       <c r="L63" s="20"/>
       <c r="M63" s="58"/>
     </row>
-    <row r="64" spans="1:13" ht="23.25" thickBot="1">
+    <row r="64" spans="1:13" ht="26.25" thickBot="1">
       <c r="A64" s="58"/>
       <c r="B64" s="19" t="s">
         <v>57</v>
@@ -10736,8 +11059,12 @@
       <c r="I64" s="88" t="s">
         <v>352</v>
       </c>
-      <c r="J64" s="20"/>
-      <c r="K64" s="20"/>
+      <c r="J64" s="20" t="s">
+        <v>395</v>
+      </c>
+      <c r="K64" s="20" t="s">
+        <v>402</v>
+      </c>
       <c r="L64" s="20"/>
       <c r="M64" s="58"/>
     </row>
@@ -10768,13 +11095,13 @@
       <c r="E66" s="73"/>
       <c r="F66" s="73"/>
       <c r="G66" s="58"/>
-      <c r="H66" s="92" t="s">
+      <c r="H66" s="95" t="s">
         <v>174</v>
       </c>
-      <c r="I66" s="93"/>
-      <c r="J66" s="93"/>
-      <c r="K66" s="93"/>
-      <c r="L66" s="94"/>
+      <c r="I66" s="96"/>
+      <c r="J66" s="96"/>
+      <c r="K66" s="96"/>
+      <c r="L66" s="97"/>
       <c r="M66" s="58"/>
     </row>
     <row r="67" spans="1:13" ht="15.75" thickBot="1">
@@ -10790,12 +11117,16 @@
       <c r="H67" s="76" t="s">
         <v>288</v>
       </c>
-      <c r="I67" s="63"/>
-      <c r="J67" s="63"/>
-      <c r="K67" s="98" t="s">
+      <c r="I67" s="92" t="s">
+        <v>392</v>
+      </c>
+      <c r="J67" s="92" t="s">
+        <v>393</v>
+      </c>
+      <c r="K67" s="101" t="s">
         <v>290</v>
       </c>
-      <c r="L67" s="99"/>
+      <c r="L67" s="102"/>
       <c r="M67" s="58"/>
     </row>
     <row r="68" spans="1:13" ht="15.75" thickBot="1">
@@ -10813,10 +11144,10 @@
       </c>
       <c r="I68" s="63"/>
       <c r="J68" s="63"/>
-      <c r="K68" s="98" t="s">
+      <c r="K68" s="101" t="s">
         <v>291</v>
       </c>
-      <c r="L68" s="99"/>
+      <c r="L68" s="102"/>
       <c r="M68" s="58"/>
     </row>
     <row r="69" spans="1:13" ht="15.75" thickBot="1">
@@ -10834,10 +11165,10 @@
       </c>
       <c r="I69" s="20"/>
       <c r="J69" s="20"/>
-      <c r="K69" s="95" t="s">
+      <c r="K69" s="98" t="s">
         <v>298</v>
       </c>
-      <c r="L69" s="96"/>
+      <c r="L69" s="99"/>
       <c r="M69" s="58"/>
     </row>
     <row r="70" spans="1:13" ht="15.75" thickBot="1">
@@ -10855,10 +11186,10 @@
       </c>
       <c r="I70" s="20"/>
       <c r="J70" s="20"/>
-      <c r="K70" s="95" t="s">
+      <c r="K70" s="98" t="s">
         <v>299</v>
       </c>
-      <c r="L70" s="96"/>
+      <c r="L70" s="99"/>
       <c r="M70" s="58"/>
     </row>
     <row r="71" spans="1:13" ht="15.75" thickBot="1">
@@ -10876,13 +11207,13 @@
       </c>
       <c r="I71" s="20"/>
       <c r="J71" s="20"/>
-      <c r="K71" s="95" t="s">
+      <c r="K71" s="98" t="s">
         <v>314</v>
       </c>
-      <c r="L71" s="96"/>
+      <c r="L71" s="99"/>
       <c r="M71" s="58"/>
     </row>
-    <row r="72" spans="1:13" ht="15.75" thickBot="1">
+    <row r="72" spans="1:13" ht="26.25" thickBot="1">
       <c r="A72" s="58"/>
       <c r="B72" s="19" t="s">
         <v>65</v>
@@ -10890,15 +11221,19 @@
       <c r="C72" s="73"/>
       <c r="D72" s="73"/>
       <c r="E72" s="73"/>
-      <c r="F72" s="80"/>
+      <c r="F72" s="80" t="s">
+        <v>412</v>
+      </c>
       <c r="G72" s="58"/>
-      <c r="H72" s="20"/>
+      <c r="H72" s="91" t="s">
+        <v>391</v>
+      </c>
       <c r="I72" s="20"/>
       <c r="J72" s="20"/>
-      <c r="K72" s="95" t="s">
+      <c r="K72" s="98" t="s">
         <v>328</v>
       </c>
-      <c r="L72" s="96"/>
+      <c r="L72" s="99"/>
       <c r="M72" s="58"/>
     </row>
     <row r="73" spans="1:13" ht="15.75" thickBot="1">
@@ -11040,7 +11375,7 @@
       <c r="L79" s="73"/>
       <c r="M79" s="58"/>
     </row>
-    <row r="80" spans="1:13" ht="15.75" thickBot="1">
+    <row r="80" spans="1:13" ht="26.25" thickBot="1">
       <c r="A80" s="58"/>
       <c r="B80" s="19" t="s">
         <v>73</v>
@@ -11048,7 +11383,9 @@
       <c r="C80" s="73"/>
       <c r="D80" s="73"/>
       <c r="E80" s="73"/>
-      <c r="F80" s="20"/>
+      <c r="F80" s="20" t="s">
+        <v>413</v>
+      </c>
       <c r="G80" s="58"/>
       <c r="H80" s="19" t="s">
         <v>181</v>
@@ -11078,7 +11415,7 @@
       <c r="L81" s="73"/>
       <c r="M81" s="58"/>
     </row>
-    <row r="82" spans="1:13" ht="15.75" thickBot="1">
+    <row r="82" spans="1:13" ht="26.25" thickBot="1">
       <c r="A82" s="58"/>
       <c r="B82" s="19" t="s">
         <v>75</v>
@@ -11086,7 +11423,9 @@
       <c r="C82" s="73"/>
       <c r="D82" s="73"/>
       <c r="E82" s="73"/>
-      <c r="F82" s="20"/>
+      <c r="F82" s="20" t="s">
+        <v>414</v>
+      </c>
       <c r="G82" s="58"/>
       <c r="H82" s="19" t="s">
         <v>183</v>
@@ -11116,7 +11455,7 @@
       <c r="L83" s="73"/>
       <c r="M83" s="58"/>
     </row>
-    <row r="84" spans="1:13" ht="15.75" thickBot="1">
+    <row r="84" spans="1:13" ht="39" thickBot="1">
       <c r="A84" s="58"/>
       <c r="B84" s="19" t="s">
         <v>77</v>
@@ -11124,7 +11463,9 @@
       <c r="C84" s="73"/>
       <c r="D84" s="73"/>
       <c r="E84" s="73"/>
-      <c r="F84" s="20"/>
+      <c r="F84" s="20" t="s">
+        <v>415</v>
+      </c>
       <c r="G84" s="58"/>
       <c r="H84" s="19" t="s">
         <v>185</v>
@@ -11135,7 +11476,7 @@
       <c r="L84" s="73"/>
       <c r="M84" s="58"/>
     </row>
-    <row r="85" spans="1:13" ht="15.75" thickBot="1">
+    <row r="85" spans="1:13" ht="26.25" thickBot="1">
       <c r="A85" s="58"/>
       <c r="B85" s="19" t="s">
         <v>78</v>
@@ -11151,16 +11492,20 @@
       <c r="I85" s="73"/>
       <c r="J85" s="73"/>
       <c r="K85" s="73"/>
-      <c r="L85" s="20"/>
+      <c r="L85" s="20" t="s">
+        <v>432</v>
+      </c>
       <c r="M85" s="58"/>
     </row>
-    <row r="86" spans="1:13" ht="15.75" thickBot="1">
+    <row r="86" spans="1:13" ht="26.25" thickBot="1">
       <c r="A86" s="58"/>
       <c r="B86" s="19" t="s">
         <v>79</v>
       </c>
       <c r="C86" s="73"/>
-      <c r="D86" s="20"/>
+      <c r="D86" s="20" t="s">
+        <v>416</v>
+      </c>
       <c r="E86" s="73"/>
       <c r="F86" s="73"/>
       <c r="G86" s="58"/>
@@ -11173,7 +11518,7 @@
       <c r="L86" s="73"/>
       <c r="M86" s="58"/>
     </row>
-    <row r="87" spans="1:13" ht="15.75" thickBot="1">
+    <row r="87" spans="1:13" ht="26.25" thickBot="1">
       <c r="A87" s="58"/>
       <c r="B87" s="19" t="s">
         <v>80</v>
@@ -11189,16 +11534,20 @@
       <c r="I87" s="73"/>
       <c r="J87" s="73"/>
       <c r="K87" s="73"/>
-      <c r="L87" s="20"/>
+      <c r="L87" s="20" t="s">
+        <v>433</v>
+      </c>
       <c r="M87" s="58"/>
     </row>
-    <row r="88" spans="1:13" ht="15.75" thickBot="1">
+    <row r="88" spans="1:13" ht="26.25" thickBot="1">
       <c r="A88" s="58"/>
       <c r="B88" s="19" t="s">
         <v>81</v>
       </c>
       <c r="C88" s="73"/>
-      <c r="D88" s="80"/>
+      <c r="D88" s="80" t="s">
+        <v>417</v>
+      </c>
       <c r="E88" s="73"/>
       <c r="F88" s="73"/>
       <c r="G88" s="58"/>
@@ -11230,7 +11579,7 @@
       <c r="L89" s="73"/>
       <c r="M89" s="58"/>
     </row>
-    <row r="90" spans="1:13" ht="15.75" thickBot="1">
+    <row r="90" spans="1:13" ht="26.25" thickBot="1">
       <c r="A90" s="58"/>
       <c r="B90" s="38" t="s">
         <v>83</v>
@@ -11238,15 +11587,21 @@
       <c r="C90" s="74"/>
       <c r="D90" s="74"/>
       <c r="E90" s="74"/>
-      <c r="F90" s="41"/>
+      <c r="F90" s="41" t="s">
+        <v>418</v>
+      </c>
       <c r="G90" s="58"/>
       <c r="H90" s="19" t="s">
         <v>191</v>
       </c>
       <c r="I90" s="73"/>
-      <c r="J90" s="20"/>
+      <c r="J90" s="20" t="s">
+        <v>434</v>
+      </c>
       <c r="K90" s="73"/>
-      <c r="L90" s="20"/>
+      <c r="L90" s="20" t="s">
+        <v>435</v>
+      </c>
       <c r="M90" s="58"/>
     </row>
     <row r="91" spans="1:13" ht="15.75" thickBot="1">
@@ -11276,7 +11631,7 @@
       <c r="C92" s="73"/>
       <c r="D92" s="73"/>
       <c r="E92" s="73"/>
-      <c r="F92" s="20"/>
+      <c r="F92" s="73"/>
       <c r="G92" s="58"/>
       <c r="H92" s="19" t="s">
         <v>193</v>
@@ -11287,7 +11642,7 @@
       <c r="L92" s="73"/>
       <c r="M92" s="58"/>
     </row>
-    <row r="93" spans="1:13" ht="15.75" thickBot="1">
+    <row r="93" spans="1:13" ht="26.25" thickBot="1">
       <c r="A93" s="58"/>
       <c r="B93" s="19" t="s">
         <v>86</v>
@@ -11303,10 +11658,12 @@
       <c r="I93" s="73"/>
       <c r="J93" s="73"/>
       <c r="K93" s="73"/>
-      <c r="L93" s="20"/>
+      <c r="L93" s="20" t="s">
+        <v>436</v>
+      </c>
       <c r="M93" s="58"/>
     </row>
-    <row r="94" spans="1:13" ht="15.75" thickBot="1">
+    <row r="94" spans="1:13" ht="26.25" thickBot="1">
       <c r="A94" s="58"/>
       <c r="B94" s="19" t="s">
         <v>87</v>
@@ -11317,15 +11674,17 @@
       <c r="F94" s="73"/>
       <c r="G94" s="58"/>
       <c r="H94" s="19" t="s">
-        <v>195</v>
+        <v>322</v>
       </c>
       <c r="I94" s="73"/>
       <c r="J94" s="73"/>
-      <c r="K94" s="20"/>
-      <c r="L94" s="20"/>
+      <c r="K94" s="73"/>
+      <c r="L94" s="20" t="s">
+        <v>437</v>
+      </c>
       <c r="M94" s="58"/>
     </row>
-    <row r="95" spans="1:13" ht="15.75" thickBot="1">
+    <row r="95" spans="1:13" ht="26.25" thickBot="1">
       <c r="A95" s="58"/>
       <c r="B95" s="19" t="s">
         <v>88</v>
@@ -11336,12 +11695,14 @@
       <c r="F95" s="73"/>
       <c r="G95" s="58"/>
       <c r="H95" s="19" t="s">
-        <v>322</v>
+        <v>196</v>
       </c>
       <c r="I95" s="73"/>
       <c r="J95" s="73"/>
       <c r="K95" s="73"/>
-      <c r="L95" s="73"/>
+      <c r="L95" s="20" t="s">
+        <v>438</v>
+      </c>
       <c r="M95" s="58"/>
     </row>
     <row r="96" spans="1:13" ht="15.75" thickBot="1">
@@ -11355,15 +11716,15 @@
       <c r="F96" s="73"/>
       <c r="G96" s="58"/>
       <c r="H96" s="19" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="I96" s="73"/>
       <c r="J96" s="73"/>
       <c r="K96" s="73"/>
-      <c r="L96" s="20"/>
+      <c r="L96" s="73"/>
       <c r="M96" s="58"/>
     </row>
-    <row r="97" spans="1:13" ht="15.75" thickBot="1">
+    <row r="97" spans="1:13" ht="39" thickBot="1">
       <c r="A97" s="58"/>
       <c r="B97" s="19" t="s">
         <v>293</v>
@@ -11374,15 +11735,19 @@
       <c r="F97" s="73"/>
       <c r="G97" s="58"/>
       <c r="H97" s="19" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I97" s="73"/>
-      <c r="J97" s="73"/>
+      <c r="J97" s="20" t="s">
+        <v>439</v>
+      </c>
       <c r="K97" s="73"/>
-      <c r="L97" s="73"/>
+      <c r="L97" s="20" t="s">
+        <v>440</v>
+      </c>
       <c r="M97" s="58"/>
     </row>
-    <row r="98" spans="1:13" ht="15.75" thickBot="1">
+    <row r="98" spans="1:13" ht="39" thickBot="1">
       <c r="A98" s="58"/>
       <c r="B98" s="19" t="s">
         <v>90</v>
@@ -11393,15 +11758,17 @@
       <c r="F98" s="73"/>
       <c r="G98" s="58"/>
       <c r="H98" s="19" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="I98" s="73"/>
-      <c r="J98" s="20"/>
+      <c r="J98" s="73"/>
       <c r="K98" s="73"/>
-      <c r="L98" s="20"/>
+      <c r="L98" s="20" t="s">
+        <v>441</v>
+      </c>
       <c r="M98" s="58"/>
     </row>
-    <row r="99" spans="1:13" ht="15.75" thickBot="1">
+    <row r="99" spans="1:13" ht="26.25" thickBot="1">
       <c r="A99" s="58"/>
       <c r="B99" s="19" t="s">
         <v>91</v>
@@ -11412,12 +11779,14 @@
       <c r="F99" s="73"/>
       <c r="G99" s="58"/>
       <c r="H99" s="19" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="I99" s="73"/>
       <c r="J99" s="73"/>
       <c r="K99" s="73"/>
-      <c r="L99" s="20"/>
+      <c r="L99" s="20" t="s">
+        <v>442</v>
+      </c>
       <c r="M99" s="58"/>
     </row>
     <row r="100" spans="1:13" ht="15.75" thickBot="1">
@@ -11431,15 +11800,15 @@
       <c r="F100" s="83"/>
       <c r="G100" s="58"/>
       <c r="H100" s="19" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="I100" s="73"/>
       <c r="J100" s="73"/>
       <c r="K100" s="73"/>
-      <c r="L100" s="20"/>
+      <c r="L100" s="73"/>
       <c r="M100" s="58"/>
     </row>
-    <row r="101" spans="1:13" ht="15.75" thickBot="1">
+    <row r="101" spans="1:13" ht="39" thickBot="1">
       <c r="A101" s="58"/>
       <c r="B101" s="19" t="s">
         <v>297</v>
@@ -11450,15 +11819,19 @@
       <c r="F101" s="73"/>
       <c r="G101" s="58"/>
       <c r="H101" s="19" t="s">
-        <v>200</v>
-      </c>
-      <c r="I101" s="73"/>
+        <v>201</v>
+      </c>
+      <c r="I101" s="72"/>
       <c r="J101" s="73"/>
-      <c r="K101" s="73"/>
-      <c r="L101" s="73"/>
+      <c r="K101" s="20" t="s">
+        <v>443</v>
+      </c>
+      <c r="L101" s="20" t="s">
+        <v>444</v>
+      </c>
       <c r="M101" s="58"/>
     </row>
-    <row r="102" spans="1:13" ht="15.75" thickBot="1">
+    <row r="102" spans="1:13" ht="30.75" thickBot="1">
       <c r="A102" s="58"/>
       <c r="B102" s="19" t="s">
         <v>94</v>
@@ -11469,12 +11842,14 @@
       <c r="F102" s="73"/>
       <c r="G102" s="58"/>
       <c r="H102" s="19" t="s">
-        <v>201</v>
-      </c>
-      <c r="I102" s="72"/>
+        <v>202</v>
+      </c>
+      <c r="I102" s="73"/>
       <c r="J102" s="73"/>
-      <c r="K102" s="20"/>
-      <c r="L102" s="20"/>
+      <c r="K102" s="73"/>
+      <c r="L102" s="62" t="s">
+        <v>445</v>
+      </c>
       <c r="M102" s="58"/>
     </row>
     <row r="103" spans="1:13" ht="15.75" thickBot="1">
@@ -11487,16 +11862,14 @@
       <c r="E103" s="73"/>
       <c r="F103" s="85"/>
       <c r="G103" s="58"/>
-      <c r="H103" s="19" t="s">
-        <v>202</v>
-      </c>
-      <c r="I103" s="73"/>
-      <c r="J103" s="73"/>
-      <c r="K103" s="73"/>
-      <c r="L103" s="62"/>
+      <c r="H103" s="58"/>
+      <c r="I103" s="58"/>
+      <c r="J103" s="58"/>
+      <c r="K103" s="58"/>
+      <c r="L103" s="58"/>
       <c r="M103" s="58"/>
     </row>
-    <row r="104" spans="1:13" ht="15.75" thickBot="1">
+    <row r="104" spans="1:13" ht="18" thickBot="1">
       <c r="A104" s="58"/>
       <c r="B104" s="58"/>
       <c r="C104" s="58"/>
@@ -11504,11 +11877,21 @@
       <c r="E104" s="58"/>
       <c r="F104" s="58"/>
       <c r="G104" s="58"/>
-      <c r="H104" s="58"/>
-      <c r="I104" s="58"/>
-      <c r="J104" s="58"/>
-      <c r="K104" s="58"/>
-      <c r="L104" s="58"/>
+      <c r="H104" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="I104" s="59" t="s">
+        <v>242</v>
+      </c>
+      <c r="J104" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="K104" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="L104" s="16" t="s">
+        <v>3</v>
+      </c>
       <c r="M104" s="58"/>
     </row>
     <row r="105" spans="1:13" ht="35.25" thickBot="1">
@@ -11529,21 +11912,13 @@
         <v>3</v>
       </c>
       <c r="G105" s="58"/>
-      <c r="H105" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="I105" s="59" t="s">
-        <v>242</v>
-      </c>
-      <c r="J105" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="K105" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="L105" s="16" t="s">
-        <v>3</v>
-      </c>
+      <c r="H105" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="I105" s="73"/>
+      <c r="J105" s="73"/>
+      <c r="K105" s="73"/>
+      <c r="L105" s="73"/>
       <c r="M105" s="58"/>
     </row>
     <row r="106" spans="1:13" ht="26.25" thickBot="1">
@@ -11557,7 +11932,7 @@
       <c r="F106" s="73"/>
       <c r="G106" s="58"/>
       <c r="H106" s="19" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="I106" s="73"/>
       <c r="J106" s="73"/>
@@ -11576,9 +11951,9 @@
       <c r="F107" s="73"/>
       <c r="G107" s="58"/>
       <c r="H107" s="19" t="s">
-        <v>204</v>
-      </c>
-      <c r="I107" s="73"/>
+        <v>205</v>
+      </c>
+      <c r="I107" s="72"/>
       <c r="J107" s="73"/>
       <c r="K107" s="73"/>
       <c r="L107" s="73"/>
@@ -11595,10 +11970,12 @@
       <c r="F108" s="73"/>
       <c r="G108" s="58"/>
       <c r="H108" s="19" t="s">
-        <v>205</v>
-      </c>
-      <c r="I108" s="72"/>
-      <c r="J108" s="73"/>
+        <v>206</v>
+      </c>
+      <c r="I108" s="73"/>
+      <c r="J108" s="20" t="s">
+        <v>446</v>
+      </c>
       <c r="K108" s="73"/>
       <c r="L108" s="73"/>
       <c r="M108" s="58"/>
@@ -11614,10 +11991,10 @@
       <c r="F109" s="73"/>
       <c r="G109" s="58"/>
       <c r="H109" s="19" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="I109" s="73"/>
-      <c r="J109" s="20"/>
+      <c r="J109" s="81"/>
       <c r="K109" s="73"/>
       <c r="L109" s="73"/>
       <c r="M109" s="58"/>
@@ -11633,10 +12010,10 @@
       <c r="F110" s="73"/>
       <c r="G110" s="58"/>
       <c r="H110" s="19" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="I110" s="73"/>
-      <c r="J110" s="81"/>
+      <c r="J110" s="73"/>
       <c r="K110" s="73"/>
       <c r="L110" s="73"/>
       <c r="M110" s="58"/>
@@ -11647,12 +12024,14 @@
         <v>102</v>
       </c>
       <c r="C111" s="73"/>
-      <c r="D111" s="20"/>
+      <c r="D111" s="20" t="s">
+        <v>419</v>
+      </c>
       <c r="E111" s="73"/>
       <c r="F111" s="73"/>
       <c r="G111" s="58"/>
       <c r="H111" s="19" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="I111" s="73"/>
       <c r="J111" s="73"/>
@@ -11660,7 +12039,7 @@
       <c r="L111" s="73"/>
       <c r="M111" s="58"/>
     </row>
-    <row r="112" spans="1:13" ht="15.75" thickBot="1">
+    <row r="112" spans="1:13" ht="26.25" thickBot="1">
       <c r="A112" s="58"/>
       <c r="B112" s="19" t="s">
         <v>103</v>
@@ -11671,12 +12050,14 @@
       <c r="F112" s="73"/>
       <c r="G112" s="58"/>
       <c r="H112" s="19" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="I112" s="73"/>
       <c r="J112" s="73"/>
       <c r="K112" s="73"/>
-      <c r="L112" s="73"/>
+      <c r="L112" s="20" t="s">
+        <v>447</v>
+      </c>
       <c r="M112" s="58"/>
     </row>
     <row r="113" spans="1:13" ht="15.75" thickBot="1">
@@ -11686,16 +12067,18 @@
       </c>
       <c r="C113" s="73"/>
       <c r="D113" s="73"/>
-      <c r="E113" s="20"/>
+      <c r="E113" s="20" t="s">
+        <v>420</v>
+      </c>
       <c r="F113" s="73"/>
       <c r="G113" s="58"/>
       <c r="H113" s="19" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="I113" s="73"/>
       <c r="J113" s="73"/>
       <c r="K113" s="73"/>
-      <c r="L113" s="20"/>
+      <c r="L113" s="73"/>
       <c r="M113" s="58"/>
     </row>
     <row r="114" spans="1:13" ht="15.75" thickBot="1">
@@ -11708,10 +12091,12 @@
       </c>
       <c r="D114" s="73"/>
       <c r="E114" s="73"/>
-      <c r="F114" s="20"/>
+      <c r="F114" s="20" t="s">
+        <v>421</v>
+      </c>
       <c r="G114" s="58"/>
       <c r="H114" s="19" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I114" s="73"/>
       <c r="J114" s="73"/>
@@ -11730,9 +12115,11 @@
       <c r="F115" s="73"/>
       <c r="G115" s="58"/>
       <c r="H115" s="19" t="s">
-        <v>212</v>
-      </c>
-      <c r="I115" s="73"/>
+        <v>213</v>
+      </c>
+      <c r="I115" s="72" t="s">
+        <v>286</v>
+      </c>
       <c r="J115" s="73"/>
       <c r="K115" s="73"/>
       <c r="L115" s="73"/>
@@ -11749,11 +12136,9 @@
       <c r="F116" s="73"/>
       <c r="G116" s="58"/>
       <c r="H116" s="19" t="s">
-        <v>213</v>
-      </c>
-      <c r="I116" s="72" t="s">
-        <v>286</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="I116" s="73"/>
       <c r="J116" s="73"/>
       <c r="K116" s="73"/>
       <c r="L116" s="73"/>
@@ -11772,7 +12157,7 @@
       <c r="F117" s="74"/>
       <c r="G117" s="58"/>
       <c r="H117" s="19" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="I117" s="73"/>
       <c r="J117" s="73"/>
@@ -11791,7 +12176,7 @@
       <c r="F118" s="73"/>
       <c r="G118" s="58"/>
       <c r="H118" s="19" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="I118" s="73"/>
       <c r="J118" s="73"/>
@@ -11810,11 +12195,11 @@
       <c r="F119" s="73"/>
       <c r="G119" s="58"/>
       <c r="H119" s="19" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="I119" s="73"/>
       <c r="J119" s="73"/>
-      <c r="K119" s="73"/>
+      <c r="K119" s="87"/>
       <c r="L119" s="73"/>
       <c r="M119" s="58"/>
     </row>
@@ -11829,11 +12214,11 @@
       <c r="F120" s="73"/>
       <c r="G120" s="58"/>
       <c r="H120" s="19" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="I120" s="73"/>
       <c r="J120" s="73"/>
-      <c r="K120" s="87"/>
+      <c r="K120" s="73"/>
       <c r="L120" s="73"/>
       <c r="M120" s="58"/>
     </row>
@@ -11848,7 +12233,7 @@
       <c r="F121" s="73"/>
       <c r="G121" s="58"/>
       <c r="H121" s="19" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="I121" s="73"/>
       <c r="J121" s="73"/>
@@ -11856,23 +12241,25 @@
       <c r="L121" s="73"/>
       <c r="M121" s="58"/>
     </row>
-    <row r="122" spans="1:13" ht="15.75" thickBot="1">
+    <row r="122" spans="1:13" ht="26.25" thickBot="1">
       <c r="A122" s="58"/>
       <c r="B122" s="19" t="s">
         <v>113</v>
       </c>
       <c r="C122" s="73"/>
       <c r="D122" s="73"/>
-      <c r="E122" s="20"/>
+      <c r="E122" s="73"/>
       <c r="F122" s="73"/>
       <c r="G122" s="58"/>
       <c r="H122" s="19" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="I122" s="73"/>
       <c r="J122" s="73"/>
       <c r="K122" s="73"/>
-      <c r="L122" s="73"/>
+      <c r="L122" s="20" t="s">
+        <v>448</v>
+      </c>
       <c r="M122" s="58"/>
     </row>
     <row r="123" spans="1:13" ht="15.75" thickBot="1">
@@ -11886,12 +12273,12 @@
       <c r="F123" s="73"/>
       <c r="G123" s="58"/>
       <c r="H123" s="19" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I123" s="73"/>
       <c r="J123" s="73"/>
       <c r="K123" s="73"/>
-      <c r="L123" s="20"/>
+      <c r="L123" s="73"/>
       <c r="M123" s="58"/>
     </row>
     <row r="124" spans="1:13" ht="15.75" thickBot="1">
@@ -11905,7 +12292,7 @@
       <c r="F124" s="73"/>
       <c r="G124" s="58"/>
       <c r="H124" s="19" t="s">
-        <v>221</v>
+        <v>295</v>
       </c>
       <c r="I124" s="73"/>
       <c r="J124" s="73"/>
@@ -11913,7 +12300,7 @@
       <c r="L124" s="73"/>
       <c r="M124" s="58"/>
     </row>
-    <row r="125" spans="1:13" ht="15.75" thickBot="1">
+    <row r="125" spans="1:13" ht="26.25" thickBot="1">
       <c r="A125" s="58"/>
       <c r="B125" s="19" t="s">
         <v>116</v>
@@ -11924,15 +12311,17 @@
       <c r="F125" s="73"/>
       <c r="G125" s="58"/>
       <c r="H125" s="19" t="s">
-        <v>295</v>
+        <v>222</v>
       </c>
       <c r="I125" s="73"/>
       <c r="J125" s="73"/>
       <c r="K125" s="73"/>
-      <c r="L125" s="20"/>
+      <c r="L125" s="20" t="s">
+        <v>449</v>
+      </c>
       <c r="M125" s="58"/>
     </row>
-    <row r="126" spans="1:13" ht="15.75" thickBot="1">
+    <row r="126" spans="1:13" ht="26.25" thickBot="1">
       <c r="A126" s="58"/>
       <c r="B126" s="19" t="s">
         <v>117</v>
@@ -11940,18 +12329,20 @@
       <c r="C126" s="73"/>
       <c r="D126" s="73"/>
       <c r="E126" s="73"/>
-      <c r="F126" s="80"/>
+      <c r="F126" s="80" t="s">
+        <v>422</v>
+      </c>
       <c r="G126" s="58"/>
       <c r="H126" s="19" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="I126" s="73"/>
       <c r="J126" s="73"/>
       <c r="K126" s="73"/>
-      <c r="L126" s="20"/>
+      <c r="L126" s="73"/>
       <c r="M126" s="58"/>
     </row>
-    <row r="127" spans="1:13" ht="15.75" thickBot="1">
+    <row r="127" spans="1:13" ht="39" thickBot="1">
       <c r="A127" s="58"/>
       <c r="B127" s="19" t="s">
         <v>118</v>
@@ -11962,15 +12353,17 @@
       <c r="F127" s="73"/>
       <c r="G127" s="58"/>
       <c r="H127" s="19" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I127" s="73"/>
       <c r="J127" s="73"/>
       <c r="K127" s="73"/>
-      <c r="L127" s="73"/>
+      <c r="L127" s="20" t="s">
+        <v>450</v>
+      </c>
       <c r="M127" s="58"/>
     </row>
-    <row r="128" spans="1:13" ht="15.75" thickBot="1">
+    <row r="128" spans="1:13" ht="26.25" thickBot="1">
       <c r="A128" s="58"/>
       <c r="B128" s="38" t="s">
         <v>119</v>
@@ -11981,12 +12374,14 @@
       <c r="F128" s="74"/>
       <c r="G128" s="58"/>
       <c r="H128" s="19" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="I128" s="73"/>
       <c r="J128" s="73"/>
       <c r="K128" s="73"/>
-      <c r="L128" s="20"/>
+      <c r="L128" s="20" t="s">
+        <v>451</v>
+      </c>
       <c r="M128" s="58"/>
     </row>
     <row r="129" spans="1:14" ht="15.75" thickBot="1">
@@ -12000,12 +12395,12 @@
       <c r="F129" s="73"/>
       <c r="G129" s="58"/>
       <c r="H129" s="19" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="I129" s="73"/>
       <c r="J129" s="73"/>
       <c r="K129" s="73"/>
-      <c r="L129" s="20"/>
+      <c r="L129" s="73"/>
       <c r="M129" s="58"/>
     </row>
     <row r="130" spans="1:14" ht="15.75" thickBot="1">
@@ -12019,7 +12414,7 @@
       <c r="F130" s="73"/>
       <c r="G130" s="58"/>
       <c r="H130" s="19" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="I130" s="73"/>
       <c r="J130" s="73"/>
@@ -12027,7 +12422,7 @@
       <c r="L130" s="73"/>
       <c r="M130" s="58"/>
     </row>
-    <row r="131" spans="1:14" ht="15.75" thickBot="1">
+    <row r="131" spans="1:14" ht="26.25" thickBot="1">
       <c r="A131" s="58"/>
       <c r="B131" s="38" t="s">
         <v>122</v>
@@ -12038,15 +12433,17 @@
       <c r="F131" s="83"/>
       <c r="G131" s="58"/>
       <c r="H131" s="19" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="I131" s="73"/>
       <c r="J131" s="73"/>
       <c r="K131" s="73"/>
-      <c r="L131" s="73"/>
+      <c r="L131" s="20" t="s">
+        <v>452</v>
+      </c>
       <c r="M131" s="58"/>
     </row>
-    <row r="132" spans="1:14" ht="15.75" thickBot="1">
+    <row r="132" spans="1:14" ht="30.75" thickBot="1">
       <c r="A132" s="58"/>
       <c r="B132" s="19" t="s">
         <v>123</v>
@@ -12054,15 +12451,19 @@
       <c r="C132" s="73"/>
       <c r="D132" s="73"/>
       <c r="E132" s="73"/>
-      <c r="F132" s="20"/>
+      <c r="F132" s="20" t="s">
+        <v>423</v>
+      </c>
       <c r="G132" s="58"/>
       <c r="H132" s="19" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="I132" s="73"/>
       <c r="J132" s="73"/>
       <c r="K132" s="73"/>
-      <c r="L132" s="20"/>
+      <c r="L132" s="62" t="s">
+        <v>453</v>
+      </c>
       <c r="M132" s="58"/>
     </row>
     <row r="133" spans="1:14" ht="15.75" thickBot="1">
@@ -12075,16 +12476,14 @@
       <c r="E133" s="73"/>
       <c r="F133" s="73"/>
       <c r="G133" s="58"/>
-      <c r="H133" s="19" t="s">
-        <v>229</v>
-      </c>
-      <c r="I133" s="73"/>
-      <c r="J133" s="73"/>
-      <c r="K133" s="73"/>
-      <c r="L133" s="62"/>
-      <c r="M133" s="58"/>
-    </row>
-    <row r="134" spans="1:14" ht="15.75" thickBot="1">
+      <c r="H133" s="4"/>
+      <c r="I133" s="4"/>
+      <c r="J133" s="4"/>
+      <c r="K133" s="4"/>
+      <c r="L133" s="4"/>
+      <c r="M133" s="4"/>
+    </row>
+    <row r="134" spans="1:14" ht="27" thickBot="1">
       <c r="A134" s="58"/>
       <c r="B134" s="19" t="s">
         <v>125</v>
@@ -12092,17 +12491,31 @@
       <c r="C134" s="73"/>
       <c r="D134" s="73"/>
       <c r="E134" s="73"/>
-      <c r="F134" s="20"/>
+      <c r="F134" s="20" t="s">
+        <v>424</v>
+      </c>
       <c r="G134" s="4"/>
-      <c r="H134" s="4"/>
-      <c r="I134" s="4"/>
-      <c r="J134" s="4"/>
-      <c r="K134" s="4"/>
-      <c r="L134" s="4"/>
-      <c r="M134" s="4"/>
+      <c r="H134" s="44" t="s">
+        <v>231</v>
+      </c>
+      <c r="I134" s="45" t="s">
+        <v>232</v>
+      </c>
+      <c r="J134" s="45" t="s">
+        <v>233</v>
+      </c>
+      <c r="K134" s="45" t="s">
+        <v>234</v>
+      </c>
+      <c r="L134" s="45" t="s">
+        <v>235</v>
+      </c>
+      <c r="M134" s="45" t="s">
+        <v>236</v>
+      </c>
       <c r="N134" s="4"/>
     </row>
-    <row r="135" spans="1:14" ht="27" thickBot="1">
+    <row r="135" spans="1:14" ht="15.75" thickBot="1">
       <c r="A135" s="58"/>
       <c r="B135" s="19" t="s">
         <v>126</v>
@@ -12110,26 +12523,16 @@
       <c r="C135" s="86"/>
       <c r="D135" s="86"/>
       <c r="E135" s="73"/>
-      <c r="F135" s="20"/>
+      <c r="F135" s="73"/>
       <c r="G135" s="4"/>
-      <c r="H135" s="44" t="s">
-        <v>231</v>
-      </c>
-      <c r="I135" s="45" t="s">
-        <v>232</v>
-      </c>
-      <c r="J135" s="45" t="s">
-        <v>233</v>
-      </c>
-      <c r="K135" s="45" t="s">
-        <v>234</v>
-      </c>
-      <c r="L135" s="45" t="s">
-        <v>235</v>
-      </c>
-      <c r="M135" s="45" t="s">
-        <v>236</v>
-      </c>
+      <c r="H135" s="51" t="s">
+        <v>237</v>
+      </c>
+      <c r="I135" s="3"/>
+      <c r="J135" s="3"/>
+      <c r="K135" s="3"/>
+      <c r="L135" s="3"/>
+      <c r="M135" s="3"/>
       <c r="N135" s="4"/>
     </row>
     <row r="136" spans="1:14" ht="15.75" thickBot="1">
@@ -12143,7 +12546,7 @@
       <c r="F136" s="77"/>
       <c r="G136" s="4"/>
       <c r="H136" s="51" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="I136" s="3"/>
       <c r="J136" s="3"/>
@@ -12163,7 +12566,7 @@
       <c r="F137" s="73"/>
       <c r="G137" s="4"/>
       <c r="H137" s="51" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="I137" s="3"/>
       <c r="J137" s="3"/>
@@ -12182,14 +12585,14 @@
       <c r="E138" s="73"/>
       <c r="F138" s="73"/>
       <c r="G138" s="4"/>
-      <c r="H138" s="51" t="s">
-        <v>239</v>
-      </c>
-      <c r="I138" s="3"/>
-      <c r="J138" s="3"/>
-      <c r="K138" s="3"/>
-      <c r="L138" s="3"/>
-      <c r="M138" s="3"/>
+      <c r="H138" s="52" t="s">
+        <v>240</v>
+      </c>
+      <c r="I138" s="54"/>
+      <c r="J138" s="54"/>
+      <c r="K138" s="54"/>
+      <c r="L138" s="54"/>
+      <c r="M138" s="54"/>
       <c r="N138" s="4"/>
     </row>
     <row r="139" spans="1:14" ht="15.75" thickBot="1">
@@ -12202,8 +12605,8 @@
       <c r="E139" s="73"/>
       <c r="F139" s="73"/>
       <c r="G139" s="4"/>
-      <c r="H139" s="52" t="s">
-        <v>240</v>
+      <c r="H139" s="53" t="s">
+        <v>241</v>
       </c>
       <c r="I139" s="54"/>
       <c r="J139" s="54"/>
@@ -12212,27 +12615,27 @@
       <c r="M139" s="54"/>
       <c r="N139" s="4"/>
     </row>
-    <row r="140" spans="1:14" ht="15.75" thickBot="1">
+    <row r="140" spans="1:14" ht="26.25" thickBot="1">
       <c r="A140" s="58"/>
       <c r="B140" s="19" t="s">
         <v>131</v>
       </c>
       <c r="C140" s="73"/>
       <c r="D140" s="73"/>
-      <c r="E140" s="20"/>
+      <c r="E140" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="F140" s="73"/>
       <c r="G140" s="4"/>
-      <c r="H140" s="53" t="s">
-        <v>241</v>
-      </c>
-      <c r="I140" s="54"/>
-      <c r="J140" s="54"/>
-      <c r="K140" s="54"/>
-      <c r="L140" s="54"/>
-      <c r="M140" s="54"/>
+      <c r="H140" s="4"/>
+      <c r="I140" s="4"/>
+      <c r="J140" s="4"/>
+      <c r="K140" s="4"/>
+      <c r="L140" s="4"/>
+      <c r="M140" s="4"/>
       <c r="N140" s="4"/>
     </row>
-    <row r="141" spans="1:14" ht="15.75" thickBot="1">
+    <row r="141" spans="1:14" ht="27" thickBot="1">
       <c r="A141" s="58"/>
       <c r="B141" s="19" t="s">
         <v>132</v>
@@ -12242,15 +12645,27 @@
       <c r="E141" s="73"/>
       <c r="F141" s="73"/>
       <c r="G141" s="4"/>
-      <c r="H141" s="4"/>
-      <c r="I141" s="4"/>
-      <c r="J141" s="4"/>
-      <c r="K141" s="4"/>
-      <c r="L141" s="4"/>
-      <c r="M141" s="4"/>
+      <c r="H141" s="44" t="s">
+        <v>243</v>
+      </c>
+      <c r="I141" s="45" t="s">
+        <v>244</v>
+      </c>
+      <c r="J141" s="45" t="s">
+        <v>245</v>
+      </c>
+      <c r="K141" s="45" t="s">
+        <v>246</v>
+      </c>
+      <c r="L141" s="45" t="s">
+        <v>247</v>
+      </c>
+      <c r="M141" s="45" t="s">
+        <v>248</v>
+      </c>
       <c r="N141" s="4"/>
     </row>
-    <row r="142" spans="1:14" ht="27" thickBot="1">
+    <row r="142" spans="1:14" ht="15.75" thickBot="1">
       <c r="A142" s="58"/>
       <c r="B142" s="19" t="s">
         <v>133</v>
@@ -12260,24 +12675,14 @@
       <c r="E142" s="73"/>
       <c r="F142" s="85"/>
       <c r="G142" s="4"/>
-      <c r="H142" s="44" t="s">
-        <v>243</v>
-      </c>
-      <c r="I142" s="45" t="s">
-        <v>244</v>
-      </c>
-      <c r="J142" s="45" t="s">
-        <v>245</v>
-      </c>
-      <c r="K142" s="45" t="s">
-        <v>246</v>
-      </c>
-      <c r="L142" s="45" t="s">
-        <v>247</v>
-      </c>
-      <c r="M142" s="45" t="s">
-        <v>248</v>
-      </c>
+      <c r="H142" s="51" t="s">
+        <v>237</v>
+      </c>
+      <c r="I142" s="3"/>
+      <c r="J142" s="3"/>
+      <c r="K142" s="3"/>
+      <c r="L142" s="3"/>
+      <c r="M142" s="3"/>
       <c r="N142" s="4"/>
     </row>
     <row r="143" spans="1:14" ht="15.75" thickBot="1">
@@ -12289,7 +12694,7 @@
       <c r="F143" s="58"/>
       <c r="G143" s="4"/>
       <c r="H143" s="51" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="I143" s="3"/>
       <c r="J143" s="3"/>
@@ -12317,7 +12722,7 @@
       </c>
       <c r="G144" s="4"/>
       <c r="H144" s="51" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="I144" s="3"/>
       <c r="J144" s="3"/>
@@ -12337,7 +12742,7 @@
       <c r="F145" s="73"/>
       <c r="G145" s="4"/>
       <c r="H145" s="51" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="I145" s="3"/>
       <c r="J145" s="3"/>
@@ -12356,14 +12761,14 @@
       <c r="E146" s="73"/>
       <c r="F146" s="73"/>
       <c r="G146" s="4"/>
-      <c r="H146" s="51" t="s">
-        <v>240</v>
-      </c>
-      <c r="I146" s="3"/>
-      <c r="J146" s="3"/>
-      <c r="K146" s="3"/>
-      <c r="L146" s="3"/>
-      <c r="M146" s="3"/>
+      <c r="H146" s="57" t="s">
+        <v>241</v>
+      </c>
+      <c r="I146" s="2"/>
+      <c r="J146" s="2"/>
+      <c r="K146" s="2"/>
+      <c r="L146" s="2"/>
+      <c r="M146" s="2"/>
       <c r="N146" s="4"/>
     </row>
     <row r="147" spans="1:14" ht="15.75" thickBot="1">
@@ -12376,17 +12781,15 @@
       <c r="E147" s="73"/>
       <c r="F147" s="73"/>
       <c r="G147" s="4"/>
-      <c r="H147" s="57" t="s">
-        <v>241</v>
-      </c>
-      <c r="I147" s="2"/>
-      <c r="J147" s="2"/>
-      <c r="K147" s="2"/>
-      <c r="L147" s="2"/>
-      <c r="M147" s="2"/>
+      <c r="H147" s="4"/>
+      <c r="I147" s="4"/>
+      <c r="J147" s="4"/>
+      <c r="K147" s="4"/>
+      <c r="L147" s="4"/>
+      <c r="M147" s="4"/>
       <c r="N147" s="4"/>
     </row>
-    <row r="148" spans="1:14" ht="15.75" thickBot="1">
+    <row r="148" spans="1:14" ht="27" thickBot="1">
       <c r="A148" s="58"/>
       <c r="B148" s="19" t="s">
         <v>138</v>
@@ -12396,15 +12799,27 @@
       <c r="E148" s="73"/>
       <c r="F148" s="73"/>
       <c r="G148" s="4"/>
-      <c r="H148" s="4"/>
-      <c r="I148" s="4"/>
-      <c r="J148" s="4"/>
-      <c r="K148" s="4"/>
-      <c r="L148" s="4"/>
-      <c r="M148" s="4"/>
+      <c r="H148" s="44" t="s">
+        <v>249</v>
+      </c>
+      <c r="I148" s="45" t="s">
+        <v>250</v>
+      </c>
+      <c r="J148" s="45" t="s">
+        <v>251</v>
+      </c>
+      <c r="K148" s="45" t="s">
+        <v>252</v>
+      </c>
+      <c r="L148" s="45" t="s">
+        <v>253</v>
+      </c>
+      <c r="M148" s="45" t="s">
+        <v>254</v>
+      </c>
       <c r="N148" s="4"/>
     </row>
-    <row r="149" spans="1:14" ht="27" thickBot="1">
+    <row r="149" spans="1:14" ht="15.75" thickBot="1">
       <c r="A149" s="58"/>
       <c r="B149" s="19" t="s">
         <v>139</v>
@@ -12414,24 +12829,14 @@
       <c r="E149" s="73"/>
       <c r="F149" s="73"/>
       <c r="G149" s="4"/>
-      <c r="H149" s="44" t="s">
-        <v>249</v>
-      </c>
-      <c r="I149" s="45" t="s">
-        <v>250</v>
-      </c>
-      <c r="J149" s="45" t="s">
-        <v>251</v>
-      </c>
-      <c r="K149" s="45" t="s">
-        <v>252</v>
-      </c>
-      <c r="L149" s="45" t="s">
-        <v>253</v>
-      </c>
-      <c r="M149" s="45" t="s">
-        <v>254</v>
-      </c>
+      <c r="H149" s="51" t="s">
+        <v>237</v>
+      </c>
+      <c r="I149" s="3"/>
+      <c r="J149" s="3"/>
+      <c r="K149" s="3"/>
+      <c r="L149" s="3"/>
+      <c r="M149" s="3"/>
       <c r="N149" s="4"/>
     </row>
     <row r="150" spans="1:14" ht="15.75" thickBot="1">
@@ -12445,7 +12850,7 @@
       <c r="F150" s="73"/>
       <c r="G150" s="4"/>
       <c r="H150" s="51" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="I150" s="3"/>
       <c r="J150" s="3"/>
@@ -12465,7 +12870,7 @@
       <c r="F151" s="73"/>
       <c r="G151" s="4"/>
       <c r="H151" s="51" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="I151" s="3"/>
       <c r="J151" s="3"/>
@@ -12485,7 +12890,7 @@
       <c r="F152" s="73"/>
       <c r="G152" s="4"/>
       <c r="H152" s="51" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="I152" s="3"/>
       <c r="J152" s="3"/>
@@ -12504,14 +12909,14 @@
       <c r="E153" s="73"/>
       <c r="F153" s="73"/>
       <c r="G153" s="4"/>
-      <c r="H153" s="51" t="s">
-        <v>240</v>
-      </c>
-      <c r="I153" s="3"/>
-      <c r="J153" s="3"/>
-      <c r="K153" s="3"/>
-      <c r="L153" s="3"/>
-      <c r="M153" s="3"/>
+      <c r="H153" s="57" t="s">
+        <v>241</v>
+      </c>
+      <c r="I153" s="2"/>
+      <c r="J153" s="2"/>
+      <c r="K153" s="2"/>
+      <c r="L153" s="2"/>
+      <c r="M153" s="2"/>
       <c r="N153" s="4"/>
     </row>
     <row r="154" spans="1:14" ht="15.75" thickBot="1">
@@ -12522,19 +12927,17 @@
       <c r="C154" s="73"/>
       <c r="D154" s="73"/>
       <c r="E154" s="73"/>
-      <c r="F154" s="20"/>
+      <c r="F154" s="73"/>
       <c r="G154" s="4"/>
-      <c r="H154" s="57" t="s">
-        <v>241</v>
-      </c>
-      <c r="I154" s="2"/>
-      <c r="J154" s="2"/>
-      <c r="K154" s="2"/>
-      <c r="L154" s="2"/>
-      <c r="M154" s="2"/>
+      <c r="H154" s="4"/>
+      <c r="I154" s="4"/>
+      <c r="J154" s="4"/>
+      <c r="K154" s="4"/>
+      <c r="L154" s="4"/>
+      <c r="M154" s="4"/>
       <c r="N154" s="4"/>
     </row>
-    <row r="155" spans="1:14" ht="15.75" thickBot="1">
+    <row r="155" spans="1:14" ht="27" thickBot="1">
       <c r="A155" s="58"/>
       <c r="B155" s="19" t="s">
         <v>145</v>
@@ -12544,15 +12947,27 @@
       <c r="E155" s="73"/>
       <c r="F155" s="85"/>
       <c r="G155" s="4"/>
-      <c r="H155" s="4"/>
-      <c r="I155" s="4"/>
-      <c r="J155" s="4"/>
-      <c r="K155" s="4"/>
-      <c r="L155" s="4"/>
-      <c r="M155" s="4"/>
+      <c r="H155" s="44" t="s">
+        <v>255</v>
+      </c>
+      <c r="I155" s="45" t="s">
+        <v>256</v>
+      </c>
+      <c r="J155" s="45" t="s">
+        <v>257</v>
+      </c>
+      <c r="K155" s="45" t="s">
+        <v>258</v>
+      </c>
+      <c r="L155" s="45" t="s">
+        <v>259</v>
+      </c>
+      <c r="M155" s="45" t="s">
+        <v>260</v>
+      </c>
       <c r="N155" s="4"/>
     </row>
-    <row r="156" spans="1:14" ht="27" thickBot="1">
+    <row r="156" spans="1:14" ht="15.75" thickBot="1">
       <c r="A156" s="58"/>
       <c r="B156" s="58"/>
       <c r="C156" s="58"/>
@@ -12560,24 +12975,14 @@
       <c r="E156" s="58"/>
       <c r="F156" s="58"/>
       <c r="G156" s="4"/>
-      <c r="H156" s="44" t="s">
-        <v>255</v>
-      </c>
-      <c r="I156" s="45" t="s">
-        <v>256</v>
-      </c>
-      <c r="J156" s="45" t="s">
-        <v>257</v>
-      </c>
-      <c r="K156" s="45" t="s">
-        <v>258</v>
-      </c>
-      <c r="L156" s="45" t="s">
-        <v>259</v>
-      </c>
-      <c r="M156" s="45" t="s">
-        <v>260</v>
-      </c>
+      <c r="H156" s="51" t="s">
+        <v>237</v>
+      </c>
+      <c r="I156" s="3"/>
+      <c r="J156" s="3"/>
+      <c r="K156" s="3"/>
+      <c r="L156" s="3"/>
+      <c r="M156" s="3"/>
       <c r="N156" s="4"/>
     </row>
     <row r="157" spans="1:14" ht="27" thickBot="1">
@@ -12601,7 +13006,7 @@
       </c>
       <c r="G157" s="4"/>
       <c r="H157" s="51" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="I157" s="3"/>
       <c r="J157" s="3"/>
@@ -12621,7 +13026,7 @@
       <c r="F158" s="3"/>
       <c r="G158" s="4"/>
       <c r="H158" s="51" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="I158" s="3"/>
       <c r="J158" s="3"/>
@@ -12641,7 +13046,7 @@
       <c r="F159" s="3"/>
       <c r="G159" s="4"/>
       <c r="H159" s="51" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="I159" s="3"/>
       <c r="J159" s="3"/>
@@ -12660,14 +13065,14 @@
       <c r="E160" s="3"/>
       <c r="F160" s="3"/>
       <c r="G160" s="4"/>
-      <c r="H160" s="51" t="s">
-        <v>240</v>
-      </c>
-      <c r="I160" s="3"/>
-      <c r="J160" s="3"/>
-      <c r="K160" s="3"/>
-      <c r="L160" s="3"/>
-      <c r="M160" s="3"/>
+      <c r="H160" s="57" t="s">
+        <v>241</v>
+      </c>
+      <c r="I160" s="2"/>
+      <c r="J160" s="2"/>
+      <c r="K160" s="2"/>
+      <c r="L160" s="2"/>
+      <c r="M160" s="2"/>
       <c r="N160" s="4"/>
     </row>
     <row r="161" spans="1:14" ht="15.75" thickBot="1">
@@ -12680,17 +13085,15 @@
       <c r="E161" s="3"/>
       <c r="F161" s="3"/>
       <c r="G161" s="4"/>
-      <c r="H161" s="57" t="s">
-        <v>241</v>
-      </c>
-      <c r="I161" s="2"/>
-      <c r="J161" s="2"/>
-      <c r="K161" s="2"/>
-      <c r="L161" s="2"/>
-      <c r="M161" s="2"/>
+      <c r="H161" s="4"/>
+      <c r="I161" s="4"/>
+      <c r="J161" s="4"/>
+      <c r="K161" s="4"/>
+      <c r="L161" s="4"/>
+      <c r="M161" s="4"/>
       <c r="N161" s="4"/>
     </row>
-    <row r="162" spans="1:14" ht="15.75" thickBot="1">
+    <row r="162" spans="1:14" ht="39.75" thickBot="1">
       <c r="A162" s="57" t="s">
         <v>241</v>
       </c>
@@ -12700,15 +13103,27 @@
       <c r="E162" s="2"/>
       <c r="F162" s="2"/>
       <c r="G162" s="4"/>
-      <c r="H162" s="4"/>
-      <c r="I162" s="4"/>
-      <c r="J162" s="4"/>
-      <c r="K162" s="4"/>
-      <c r="L162" s="4"/>
-      <c r="M162" s="4"/>
+      <c r="H162" s="44" t="s">
+        <v>261</v>
+      </c>
+      <c r="I162" s="45" t="s">
+        <v>262</v>
+      </c>
+      <c r="J162" s="45" t="s">
+        <v>263</v>
+      </c>
+      <c r="K162" s="45" t="s">
+        <v>264</v>
+      </c>
+      <c r="L162" s="45" t="s">
+        <v>265</v>
+      </c>
+      <c r="M162" s="45" t="s">
+        <v>266</v>
+      </c>
       <c r="N162" s="4"/>
     </row>
-    <row r="163" spans="1:14" ht="39.75" thickBot="1">
+    <row r="163" spans="1:14" ht="15.75" thickBot="1">
       <c r="A163" s="4"/>
       <c r="B163" s="4"/>
       <c r="C163" s="4"/>
@@ -12716,24 +13131,14 @@
       <c r="E163" s="4"/>
       <c r="F163" s="4"/>
       <c r="G163" s="4"/>
-      <c r="H163" s="44" t="s">
-        <v>261</v>
-      </c>
-      <c r="I163" s="45" t="s">
-        <v>262</v>
-      </c>
-      <c r="J163" s="45" t="s">
-        <v>263</v>
-      </c>
-      <c r="K163" s="45" t="s">
-        <v>264</v>
-      </c>
-      <c r="L163" s="45" t="s">
-        <v>265</v>
-      </c>
-      <c r="M163" s="45" t="s">
-        <v>266</v>
-      </c>
+      <c r="H163" s="51" t="s">
+        <v>237</v>
+      </c>
+      <c r="I163" s="3"/>
+      <c r="J163" s="3"/>
+      <c r="K163" s="3"/>
+      <c r="L163" s="3"/>
+      <c r="M163" s="3"/>
       <c r="N163" s="4"/>
     </row>
     <row r="164" spans="1:14" ht="39.75" thickBot="1">
@@ -12757,7 +13162,7 @@
       </c>
       <c r="G164" s="4"/>
       <c r="H164" s="51" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="I164" s="3"/>
       <c r="J164" s="3"/>
@@ -12777,7 +13182,7 @@
       <c r="F165" s="3"/>
       <c r="G165" s="4"/>
       <c r="H165" s="51" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="I165" s="3"/>
       <c r="J165" s="3"/>
@@ -12797,7 +13202,7 @@
       <c r="F166" s="3"/>
       <c r="G166" s="4"/>
       <c r="H166" s="51" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="I166" s="3"/>
       <c r="J166" s="3"/>
@@ -12816,14 +13221,14 @@
       <c r="E167" s="3"/>
       <c r="F167" s="3"/>
       <c r="G167" s="4"/>
-      <c r="H167" s="51" t="s">
-        <v>240</v>
-      </c>
-      <c r="I167" s="3"/>
-      <c r="J167" s="3"/>
-      <c r="K167" s="3"/>
-      <c r="L167" s="3"/>
-      <c r="M167" s="3"/>
+      <c r="H167" s="57" t="s">
+        <v>241</v>
+      </c>
+      <c r="I167" s="2"/>
+      <c r="J167" s="2"/>
+      <c r="K167" s="2"/>
+      <c r="L167" s="2"/>
+      <c r="M167" s="2"/>
       <c r="N167" s="4"/>
     </row>
     <row r="168" spans="1:14" ht="15.75" thickBot="1">
@@ -12836,14 +13241,6 @@
       <c r="E168" s="3"/>
       <c r="F168" s="3"/>
       <c r="G168" s="4"/>
-      <c r="H168" s="57" t="s">
-        <v>241</v>
-      </c>
-      <c r="I168" s="2"/>
-      <c r="J168" s="2"/>
-      <c r="K168" s="2"/>
-      <c r="L168" s="2"/>
-      <c r="M168" s="2"/>
       <c r="N168" s="4"/>
     </row>
     <row r="169" spans="1:14" ht="15.75" thickBot="1">

</xml_diff>

<commit_message>
few more items done / 1 umo done
</commit_message>
<xml_diff>
--- a/check list.xlsx
+++ b/check list.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1246" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1245" uniqueCount="453">
   <si>
     <t>ARMOR</t>
   </si>
@@ -1247,9 +1247,6 @@
   </si>
   <si>
     <t>Wizard's Cloak</t>
-  </si>
-  <si>
-    <t>Lunar Eclipse</t>
   </si>
   <si>
     <t>Titan's Steps</t>
@@ -9628,8 +9625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H92" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J98" sqref="J98"/>
+    <sheetView tabSelected="1" topLeftCell="G59" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I67" sqref="I67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9936,7 +9933,7 @@
       <c r="J14" s="73"/>
       <c r="K14" s="73"/>
       <c r="L14" s="20" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="M14" s="58"/>
     </row>
@@ -9994,7 +9991,7 @@
       <c r="I17" s="73"/>
       <c r="J17" s="73"/>
       <c r="K17" s="20" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="L17" s="73"/>
       <c r="M17" s="58"/>
@@ -10035,7 +10032,7 @@
       <c r="J19" s="73"/>
       <c r="K19" s="73"/>
       <c r="L19" s="20" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="M19" s="58"/>
     </row>
@@ -10115,7 +10112,7 @@
       <c r="J23" s="73"/>
       <c r="K23" s="73"/>
       <c r="L23" s="20" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="M23" s="58"/>
     </row>
@@ -10136,7 +10133,7 @@
       <c r="J24" s="73"/>
       <c r="K24" s="73"/>
       <c r="L24" s="20" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="M24" s="58"/>
     </row>
@@ -10219,12 +10216,12 @@
       <c r="I28" s="73"/>
       <c r="J28" s="73"/>
       <c r="K28" s="20" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L28" s="85"/>
       <c r="M28" s="58"/>
     </row>
-    <row r="29" spans="1:13" ht="26.25" thickBot="1">
+    <row r="29" spans="1:13" ht="15.75" thickBot="1">
       <c r="A29" s="58"/>
       <c r="B29" s="19" t="s">
         <v>25</v>
@@ -10232,9 +10229,7 @@
       <c r="C29" s="73"/>
       <c r="D29" s="73"/>
       <c r="E29" s="73"/>
-      <c r="F29" s="20" t="s">
-        <v>406</v>
-      </c>
+      <c r="F29" s="73"/>
       <c r="G29" s="58"/>
       <c r="H29" s="58"/>
       <c r="I29" s="58"/>
@@ -10364,7 +10359,7 @@
       <c r="J34" s="75" t="s">
         <v>374</v>
       </c>
-      <c r="K34" s="91" t="s">
+      <c r="K34" s="75" t="s">
         <v>386</v>
       </c>
       <c r="L34" s="20"/>
@@ -10411,7 +10406,7 @@
       <c r="I36" s="75" t="s">
         <v>363</v>
       </c>
-      <c r="J36" s="91" t="s">
+      <c r="J36" s="75" t="s">
         <v>370</v>
       </c>
       <c r="K36" s="20"/>
@@ -10565,7 +10560,7 @@
       <c r="D43" s="73"/>
       <c r="E43" s="73"/>
       <c r="F43" s="20" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G43" s="58"/>
       <c r="H43" s="75" t="s">
@@ -10890,7 +10885,7 @@
       <c r="D58" s="73"/>
       <c r="E58" s="73"/>
       <c r="F58" s="20" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G58" s="58"/>
       <c r="H58" s="76" t="s">
@@ -10945,10 +10940,10 @@
       <c r="C60" s="73"/>
       <c r="D60" s="73"/>
       <c r="E60" s="20" t="s">
+        <v>408</v>
+      </c>
+      <c r="F60" s="20" t="s">
         <v>409</v>
-      </c>
-      <c r="F60" s="20" t="s">
-        <v>410</v>
       </c>
       <c r="G60" s="58"/>
       <c r="H60" s="75" t="s">
@@ -10960,7 +10955,7 @@
       <c r="J60" s="88" t="s">
         <v>355</v>
       </c>
-      <c r="K60" s="20" t="s">
+      <c r="K60" s="75" t="s">
         <v>398</v>
       </c>
       <c r="L60" s="20"/>
@@ -11025,7 +11020,7 @@
       <c r="D63" s="73"/>
       <c r="E63" s="73"/>
       <c r="F63" s="20" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G63" s="58"/>
       <c r="H63" s="75" t="s">
@@ -11117,7 +11112,7 @@
       <c r="H67" s="76" t="s">
         <v>288</v>
       </c>
-      <c r="I67" s="92" t="s">
+      <c r="I67" s="76" t="s">
         <v>392</v>
       </c>
       <c r="J67" s="92" t="s">
@@ -11222,7 +11217,7 @@
       <c r="D72" s="73"/>
       <c r="E72" s="73"/>
       <c r="F72" s="80" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G72" s="58"/>
       <c r="H72" s="91" t="s">
@@ -11384,7 +11379,7 @@
       <c r="D80" s="73"/>
       <c r="E80" s="73"/>
       <c r="F80" s="20" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G80" s="58"/>
       <c r="H80" s="19" t="s">
@@ -11424,7 +11419,7 @@
       <c r="D82" s="73"/>
       <c r="E82" s="73"/>
       <c r="F82" s="20" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="G82" s="58"/>
       <c r="H82" s="19" t="s">
@@ -11464,7 +11459,7 @@
       <c r="D84" s="73"/>
       <c r="E84" s="73"/>
       <c r="F84" s="20" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G84" s="58"/>
       <c r="H84" s="19" t="s">
@@ -11493,7 +11488,7 @@
       <c r="J85" s="73"/>
       <c r="K85" s="73"/>
       <c r="L85" s="20" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="M85" s="58"/>
     </row>
@@ -11504,7 +11499,7 @@
       </c>
       <c r="C86" s="73"/>
       <c r="D86" s="20" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E86" s="73"/>
       <c r="F86" s="73"/>
@@ -11535,7 +11530,7 @@
       <c r="J87" s="73"/>
       <c r="K87" s="73"/>
       <c r="L87" s="20" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="M87" s="58"/>
     </row>
@@ -11546,7 +11541,7 @@
       </c>
       <c r="C88" s="73"/>
       <c r="D88" s="80" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E88" s="73"/>
       <c r="F88" s="73"/>
@@ -11588,7 +11583,7 @@
       <c r="D90" s="74"/>
       <c r="E90" s="74"/>
       <c r="F90" s="41" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G90" s="58"/>
       <c r="H90" s="19" t="s">
@@ -11596,11 +11591,11 @@
       </c>
       <c r="I90" s="73"/>
       <c r="J90" s="20" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="K90" s="73"/>
       <c r="L90" s="20" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="M90" s="58"/>
     </row>
@@ -11659,7 +11654,7 @@
       <c r="J93" s="73"/>
       <c r="K93" s="73"/>
       <c r="L93" s="20" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="M93" s="58"/>
     </row>
@@ -11680,7 +11675,7 @@
       <c r="J94" s="73"/>
       <c r="K94" s="73"/>
       <c r="L94" s="20" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="M94" s="58"/>
     </row>
@@ -11701,7 +11696,7 @@
       <c r="J95" s="73"/>
       <c r="K95" s="73"/>
       <c r="L95" s="20" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="M95" s="58"/>
     </row>
@@ -11739,11 +11734,11 @@
       </c>
       <c r="I97" s="73"/>
       <c r="J97" s="20" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="K97" s="73"/>
       <c r="L97" s="20" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="M97" s="58"/>
     </row>
@@ -11764,7 +11759,7 @@
       <c r="J98" s="73"/>
       <c r="K98" s="73"/>
       <c r="L98" s="20" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="M98" s="58"/>
     </row>
@@ -11785,7 +11780,7 @@
       <c r="J99" s="73"/>
       <c r="K99" s="73"/>
       <c r="L99" s="20" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="M99" s="58"/>
     </row>
@@ -11824,10 +11819,10 @@
       <c r="I101" s="72"/>
       <c r="J101" s="73"/>
       <c r="K101" s="20" t="s">
+        <v>442</v>
+      </c>
+      <c r="L101" s="20" t="s">
         <v>443</v>
-      </c>
-      <c r="L101" s="20" t="s">
-        <v>444</v>
       </c>
       <c r="M101" s="58"/>
     </row>
@@ -11848,7 +11843,7 @@
       <c r="J102" s="73"/>
       <c r="K102" s="73"/>
       <c r="L102" s="62" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="M102" s="58"/>
     </row>
@@ -11974,7 +11969,7 @@
       </c>
       <c r="I108" s="73"/>
       <c r="J108" s="20" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="K108" s="73"/>
       <c r="L108" s="73"/>
@@ -12025,7 +12020,7 @@
       </c>
       <c r="C111" s="73"/>
       <c r="D111" s="20" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E111" s="73"/>
       <c r="F111" s="73"/>
@@ -12056,7 +12051,7 @@
       <c r="J112" s="73"/>
       <c r="K112" s="73"/>
       <c r="L112" s="20" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="M112" s="58"/>
     </row>
@@ -12068,7 +12063,7 @@
       <c r="C113" s="73"/>
       <c r="D113" s="73"/>
       <c r="E113" s="20" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F113" s="73"/>
       <c r="G113" s="58"/>
@@ -12092,7 +12087,7 @@
       <c r="D114" s="73"/>
       <c r="E114" s="73"/>
       <c r="F114" s="20" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G114" s="58"/>
       <c r="H114" s="19" t="s">
@@ -12258,7 +12253,7 @@
       <c r="J122" s="73"/>
       <c r="K122" s="73"/>
       <c r="L122" s="20" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="M122" s="58"/>
     </row>
@@ -12317,7 +12312,7 @@
       <c r="J125" s="73"/>
       <c r="K125" s="73"/>
       <c r="L125" s="20" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="M125" s="58"/>
     </row>
@@ -12330,7 +12325,7 @@
       <c r="D126" s="73"/>
       <c r="E126" s="73"/>
       <c r="F126" s="80" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G126" s="58"/>
       <c r="H126" s="19" t="s">
@@ -12359,7 +12354,7 @@
       <c r="J127" s="73"/>
       <c r="K127" s="73"/>
       <c r="L127" s="20" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="M127" s="58"/>
     </row>
@@ -12380,7 +12375,7 @@
       <c r="J128" s="73"/>
       <c r="K128" s="73"/>
       <c r="L128" s="20" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="M128" s="58"/>
     </row>
@@ -12439,7 +12434,7 @@
       <c r="J131" s="73"/>
       <c r="K131" s="73"/>
       <c r="L131" s="20" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="M131" s="58"/>
     </row>
@@ -12452,7 +12447,7 @@
       <c r="D132" s="73"/>
       <c r="E132" s="73"/>
       <c r="F132" s="20" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G132" s="58"/>
       <c r="H132" s="19" t="s">
@@ -12462,7 +12457,7 @@
       <c r="J132" s="73"/>
       <c r="K132" s="73"/>
       <c r="L132" s="62" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="M132" s="58"/>
     </row>
@@ -12492,7 +12487,7 @@
       <c r="D134" s="73"/>
       <c r="E134" s="73"/>
       <c r="F134" s="20" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="G134" s="4"/>
       <c r="H134" s="44" t="s">
@@ -12623,7 +12618,7 @@
       <c r="C140" s="73"/>
       <c r="D140" s="73"/>
       <c r="E140" s="20" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F140" s="73"/>
       <c r="G140" s="4"/>

</xml_diff>

<commit_message>
Item list big update, 17 items missing
</commit_message>
<xml_diff>
--- a/check list.xlsx
+++ b/check list.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1258" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1265" uniqueCount="473">
   <si>
     <t>ARMOR</t>
   </si>
@@ -1384,9 +1384,6 @@
     <t>Fauztin's Shadow</t>
   </si>
   <si>
-    <t>check mf</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -1420,22 +1417,61 @@
     <t>proc forked lightning?</t>
   </si>
   <si>
-    <t>oskill?</t>
-  </si>
-  <si>
     <t>check searing glow, check +2 skills when apple</t>
+  </si>
+  <si>
+    <t>oskill fireboltbarrage</t>
+  </si>
+  <si>
+    <t>proc chickenlickin</t>
+  </si>
+  <si>
+    <t>kill-skill Mon Spinning Mind Flay
+ (535)</t>
+  </si>
+  <si>
+    <t>proc elementalrain (820)</t>
+  </si>
+  <si>
+    <t>pagan2 apple all skills 2</t>
+  </si>
+  <si>
+    <t>Blackguard Helm</t>
+  </si>
+  <si>
+    <t>Demonstring</t>
+  </si>
+  <si>
+    <t>absorb fire,cold,light, magic?</t>
+  </si>
+  <si>
+    <t>skill solistice and equinox?</t>
+  </si>
+  <si>
+    <t>3% Faster Cast Rate
++5% Bonus to Summoned Minion Attack Rating
++1 to Maximum Necromancer Minions
+3% Crushing Blow to Darklings?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="45">
+  <fonts count="46">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2245,63 +2281,89 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="32" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="33" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="34" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="8" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="9" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="37" fillId="9" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="39" fillId="10" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="35" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="36" fillId="8" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="9" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="9" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="10" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="43" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="44" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="44" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="44" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="44" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="44" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="44" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="44" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="44" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="44" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="44" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="44" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="44" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="43" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="43" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="43" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="43" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="43" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="43" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="43" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="43" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="43" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="43" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="43" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -2311,10 +2373,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2323,10 +2382,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2336,33 +2395,33 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2371,22 +2430,25 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2398,28 +2460,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2429,43 +2491,43 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2484,44 +2546,41 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2530,94 +2589,121 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="68">
     <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1 2" xfId="43" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1 3" xfId="53" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="22" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2 2" xfId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2 3" xfId="58" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="26" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3 2" xfId="48" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3 3" xfId="60" customBuiltin="1"/>
     <cellStyle name="20% - Accent4" xfId="30" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4 2" xfId="51" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4 3" xfId="62" customBuiltin="1"/>
     <cellStyle name="20% - Accent5" xfId="34" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5 2" xfId="54" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5 3" xfId="64" customBuiltin="1"/>
     <cellStyle name="20% - Accent6" xfId="38" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6 2" xfId="56" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6 3" xfId="66" customBuiltin="1"/>
     <cellStyle name="40% - Accent1" xfId="19" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1 2" xfId="44" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1 3" xfId="50" customBuiltin="1"/>
     <cellStyle name="40% - Accent2" xfId="23" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2 2" xfId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2 3" xfId="59" customBuiltin="1"/>
     <cellStyle name="40% - Accent3" xfId="27" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3 2" xfId="49" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3 3" xfId="61" customBuiltin="1"/>
     <cellStyle name="40% - Accent4" xfId="31" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4 2" xfId="52" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4 3" xfId="63" customBuiltin="1"/>
     <cellStyle name="40% - Accent5" xfId="35" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5 2" xfId="55" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5 3" xfId="65" customBuiltin="1"/>
     <cellStyle name="40% - Accent6" xfId="39" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6 2" xfId="57" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6 3" xfId="67" customBuiltin="1"/>
     <cellStyle name="60% - Accent1" xfId="20" builtinId="32" customBuiltin="1"/>
     <cellStyle name="60% - Accent2" xfId="24" builtinId="36" customBuiltin="1"/>
     <cellStyle name="60% - Accent3" xfId="28" builtinId="40" customBuiltin="1"/>
@@ -2643,7 +2729,9 @@
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note 2" xfId="41" customBuiltin="1"/>
+    <cellStyle name="Note 2" xfId="41"/>
+    <cellStyle name="Note 3" xfId="42" customBuiltin="1"/>
+    <cellStyle name="Note 4" xfId="45" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="16" builtinId="25" customBuiltin="1"/>
@@ -3481,13 +3569,13 @@
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
       <c r="G27" s="7"/>
-      <c r="H27" s="91" t="s">
+      <c r="H27" s="96" t="s">
         <v>170</v>
       </c>
-      <c r="I27" s="91"/>
-      <c r="J27" s="91"/>
-      <c r="K27" s="91"/>
-      <c r="L27" s="91"/>
+      <c r="I27" s="96"/>
+      <c r="J27" s="96"/>
+      <c r="K27" s="96"/>
+      <c r="L27" s="96"/>
       <c r="M27" s="7"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1">
@@ -3642,13 +3730,13 @@
       <c r="E36" s="20"/>
       <c r="F36" s="29"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="91" t="s">
+      <c r="H36" s="96" t="s">
         <v>171</v>
       </c>
-      <c r="I36" s="91"/>
-      <c r="J36" s="91"/>
-      <c r="K36" s="91"/>
-      <c r="L36" s="91"/>
+      <c r="I36" s="96"/>
+      <c r="J36" s="96"/>
+      <c r="K36" s="96"/>
+      <c r="L36" s="96"/>
       <c r="M36" s="7"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
@@ -3809,13 +3897,13 @@
         <v>3</v>
       </c>
       <c r="G45" s="7"/>
-      <c r="H45" s="91" t="s">
+      <c r="H45" s="96" t="s">
         <v>172</v>
       </c>
-      <c r="I45" s="91"/>
-      <c r="J45" s="91"/>
-      <c r="K45" s="91"/>
-      <c r="L45" s="91"/>
+      <c r="I45" s="96"/>
+      <c r="J45" s="96"/>
+      <c r="K45" s="96"/>
+      <c r="L45" s="96"/>
       <c r="M45" s="7"/>
     </row>
     <row r="46" spans="1:13" ht="15.75" thickBot="1">
@@ -3964,13 +4052,13 @@
       <c r="E54" s="39"/>
       <c r="F54" s="39"/>
       <c r="G54" s="7"/>
-      <c r="H54" s="91" t="s">
+      <c r="H54" s="96" t="s">
         <v>173</v>
       </c>
-      <c r="I54" s="91"/>
-      <c r="J54" s="91"/>
-      <c r="K54" s="91"/>
-      <c r="L54" s="91"/>
+      <c r="I54" s="96"/>
+      <c r="J54" s="96"/>
+      <c r="K54" s="96"/>
+      <c r="L54" s="96"/>
       <c r="M54" s="7"/>
     </row>
     <row r="55" spans="1:13" ht="15.75" thickBot="1">
@@ -4119,13 +4207,13 @@
       <c r="E63" s="20"/>
       <c r="F63" s="20"/>
       <c r="G63" s="7"/>
-      <c r="H63" s="91" t="s">
+      <c r="H63" s="96" t="s">
         <v>174</v>
       </c>
-      <c r="I63" s="91"/>
-      <c r="J63" s="91"/>
-      <c r="K63" s="91"/>
-      <c r="L63" s="91"/>
+      <c r="I63" s="96"/>
+      <c r="J63" s="96"/>
+      <c r="K63" s="96"/>
+      <c r="L63" s="96"/>
       <c r="M63" s="7"/>
     </row>
     <row r="64" spans="1:13" ht="15.75" thickBot="1">
@@ -5434,11 +5522,11 @@
       <c r="E132" s="20"/>
       <c r="F132" s="20"/>
       <c r="G132" s="7"/>
-      <c r="H132" s="90"/>
-      <c r="I132" s="90"/>
-      <c r="J132" s="90"/>
-      <c r="K132" s="90"/>
-      <c r="L132" s="90"/>
+      <c r="H132" s="95"/>
+      <c r="I132" s="95"/>
+      <c r="J132" s="95"/>
+      <c r="K132" s="95"/>
+      <c r="L132" s="95"/>
       <c r="M132" s="7"/>
     </row>
     <row r="133" spans="1:14" ht="18" thickBot="1">
@@ -7184,13 +7272,13 @@
       <c r="E30" s="20"/>
       <c r="F30" s="20"/>
       <c r="G30" s="58"/>
-      <c r="H30" s="92" t="s">
+      <c r="H30" s="97" t="s">
         <v>170</v>
       </c>
-      <c r="I30" s="93"/>
-      <c r="J30" s="93"/>
-      <c r="K30" s="93"/>
-      <c r="L30" s="94"/>
+      <c r="I30" s="98"/>
+      <c r="J30" s="98"/>
+      <c r="K30" s="98"/>
+      <c r="L30" s="99"/>
       <c r="M30" s="58"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1">
@@ -7345,13 +7433,13 @@
       <c r="E39" s="20"/>
       <c r="F39" s="62"/>
       <c r="G39" s="58"/>
-      <c r="H39" s="92" t="s">
+      <c r="H39" s="97" t="s">
         <v>171</v>
       </c>
-      <c r="I39" s="93"/>
-      <c r="J39" s="93"/>
-      <c r="K39" s="93"/>
-      <c r="L39" s="94"/>
+      <c r="I39" s="98"/>
+      <c r="J39" s="98"/>
+      <c r="K39" s="98"/>
+      <c r="L39" s="99"/>
       <c r="M39" s="58"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" thickBot="1">
@@ -7512,13 +7600,13 @@
         <v>3</v>
       </c>
       <c r="G48" s="58"/>
-      <c r="H48" s="92" t="s">
+      <c r="H48" s="97" t="s">
         <v>172</v>
       </c>
-      <c r="I48" s="93"/>
-      <c r="J48" s="93"/>
-      <c r="K48" s="93"/>
-      <c r="L48" s="94"/>
+      <c r="I48" s="98"/>
+      <c r="J48" s="98"/>
+      <c r="K48" s="98"/>
+      <c r="L48" s="99"/>
       <c r="M48" s="58"/>
     </row>
     <row r="49" spans="1:13" ht="15.75" thickBot="1">
@@ -7667,13 +7755,13 @@
       <c r="E57" s="39"/>
       <c r="F57" s="39"/>
       <c r="G57" s="58"/>
-      <c r="H57" s="92" t="s">
+      <c r="H57" s="97" t="s">
         <v>173</v>
       </c>
-      <c r="I57" s="93"/>
-      <c r="J57" s="93"/>
-      <c r="K57" s="93"/>
-      <c r="L57" s="94"/>
+      <c r="I57" s="98"/>
+      <c r="J57" s="98"/>
+      <c r="K57" s="98"/>
+      <c r="L57" s="99"/>
       <c r="M57" s="58"/>
     </row>
     <row r="58" spans="1:13" ht="15.75" thickBot="1">
@@ -7822,13 +7910,13 @@
       <c r="E66" s="20"/>
       <c r="F66" s="20"/>
       <c r="G66" s="58"/>
-      <c r="H66" s="92" t="s">
+      <c r="H66" s="97" t="s">
         <v>174</v>
       </c>
-      <c r="I66" s="93"/>
-      <c r="J66" s="93"/>
-      <c r="K66" s="93"/>
-      <c r="L66" s="94"/>
+      <c r="I66" s="98"/>
+      <c r="J66" s="98"/>
+      <c r="K66" s="98"/>
+      <c r="L66" s="99"/>
       <c r="M66" s="58"/>
     </row>
     <row r="67" spans="1:13" ht="15.75" thickBot="1">
@@ -10185,8 +10273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A148" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E140" sqref="E140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10206,40 +10294,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="23.25" customHeight="1">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="102" t="s">
         <v>284</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
-      <c r="J1" s="95"/>
-      <c r="K1" s="95"/>
-      <c r="L1" s="95"/>
-      <c r="M1" s="95"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="102"/>
+      <c r="F1" s="102"/>
+      <c r="G1" s="102"/>
+      <c r="H1" s="102"/>
+      <c r="I1" s="102"/>
+      <c r="J1" s="102"/>
+      <c r="K1" s="102"/>
+      <c r="L1" s="102"/>
+      <c r="M1" s="102"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1">
-      <c r="A2" s="95"/>
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
+      <c r="A2" s="102"/>
+      <c r="B2" s="102"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="102"/>
+      <c r="I2" s="102"/>
+      <c r="J2" s="102"/>
+      <c r="K2" s="102"/>
+      <c r="L2" s="102"/>
+      <c r="M2" s="102"/>
       <c r="N2" s="1"/>
       <c r="O2" s="69"/>
       <c r="P2" s="70" t="s">
@@ -10248,19 +10336,19 @@
       <c r="Q2" s="1"/>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1">
-      <c r="A3" s="95"/>
-      <c r="B3" s="95"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="95"/>
-      <c r="I3" s="95"/>
-      <c r="J3" s="95"/>
-      <c r="K3" s="95"/>
-      <c r="L3" s="95"/>
-      <c r="M3" s="95"/>
+      <c r="A3" s="102"/>
+      <c r="B3" s="102"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
+      <c r="G3" s="102"/>
+      <c r="H3" s="102"/>
+      <c r="I3" s="102"/>
+      <c r="J3" s="102"/>
+      <c r="K3" s="102"/>
+      <c r="L3" s="102"/>
+      <c r="M3" s="102"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -10342,11 +10430,11 @@
       <c r="K6" s="73"/>
       <c r="L6" s="73"/>
       <c r="M6" s="58"/>
-      <c r="O6" s="99" t="s">
+      <c r="O6" s="91" t="s">
+        <v>451</v>
+      </c>
+      <c r="P6" t="s">
         <v>452</v>
-      </c>
-      <c r="P6" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1">
@@ -10386,11 +10474,11 @@
       <c r="K8" s="73"/>
       <c r="L8" s="73"/>
       <c r="M8" s="58"/>
-      <c r="O8" s="98" t="s">
-        <v>452</v>
+      <c r="O8" s="90" t="s">
+        <v>451</v>
       </c>
       <c r="P8" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="15.75" thickBot="1">
@@ -10504,7 +10592,7 @@
       <c r="I14" s="73"/>
       <c r="J14" s="73"/>
       <c r="K14" s="73"/>
-      <c r="L14" s="89" t="s">
+      <c r="L14" s="105" t="s">
         <v>423</v>
       </c>
       <c r="M14" s="58"/>
@@ -10547,7 +10635,7 @@
       <c r="L16" s="73"/>
       <c r="M16" s="58"/>
     </row>
-    <row r="17" spans="1:13" ht="26.25" thickBot="1">
+    <row r="17" spans="1:13" ht="45.75" thickBot="1">
       <c r="A17" s="58"/>
       <c r="B17" s="19" t="s">
         <v>15</v>
@@ -10562,12 +10650,14 @@
       </c>
       <c r="I17" s="73"/>
       <c r="J17" s="73"/>
-      <c r="K17" s="75" t="s">
+      <c r="K17" s="105" t="s">
         <v>424</v>
       </c>
-      <c r="L17" s="73"/>
+      <c r="L17" s="89" t="s">
+        <v>469</v>
+      </c>
       <c r="M17" s="58" t="s">
-        <v>463</v>
+        <v>470</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1">
@@ -10605,7 +10695,7 @@
       <c r="I19" s="73"/>
       <c r="J19" s="73"/>
       <c r="K19" s="73"/>
-      <c r="L19" s="89" t="s">
+      <c r="L19" s="105" t="s">
         <v>425</v>
       </c>
       <c r="M19" s="58"/>
@@ -10637,7 +10727,7 @@
       <c r="C21" s="73"/>
       <c r="D21" s="73"/>
       <c r="E21" s="73"/>
-      <c r="F21" s="89" t="s">
+      <c r="F21" s="105" t="s">
         <v>405</v>
       </c>
       <c r="G21" s="58"/>
@@ -10685,7 +10775,7 @@
       <c r="I23" s="73"/>
       <c r="J23" s="73"/>
       <c r="K23" s="73"/>
-      <c r="L23" s="89" t="s">
+      <c r="L23" s="105" t="s">
         <v>426</v>
       </c>
       <c r="M23" s="58"/>
@@ -10706,12 +10796,10 @@
       <c r="I24" s="73"/>
       <c r="J24" s="73"/>
       <c r="K24" s="73"/>
-      <c r="L24" s="75" t="s">
+      <c r="L24" s="105" t="s">
         <v>427</v>
       </c>
-      <c r="M24" s="58" t="s">
-        <v>451</v>
-      </c>
+      <c r="M24" s="58"/>
     </row>
     <row r="25" spans="1:13" ht="15.75" thickBot="1">
       <c r="A25" s="58"/>
@@ -10791,10 +10879,10 @@
       </c>
       <c r="I28" s="73"/>
       <c r="J28" s="73"/>
-      <c r="K28" s="89" t="s">
+      <c r="K28" s="105" t="s">
         <v>428</v>
       </c>
-      <c r="L28" s="85"/>
+      <c r="L28" s="84"/>
       <c r="M28" s="58"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1">
@@ -10826,13 +10914,13 @@
       <c r="E30" s="73"/>
       <c r="F30" s="73"/>
       <c r="G30" s="58"/>
-      <c r="H30" s="92" t="s">
+      <c r="H30" s="97" t="s">
         <v>170</v>
       </c>
-      <c r="I30" s="93"/>
-      <c r="J30" s="93"/>
-      <c r="K30" s="93"/>
-      <c r="L30" s="94"/>
+      <c r="I30" s="98"/>
+      <c r="J30" s="98"/>
+      <c r="K30" s="98"/>
+      <c r="L30" s="99"/>
       <c r="M30" s="58"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1">
@@ -10845,16 +10933,16 @@
       <c r="E31" s="73"/>
       <c r="F31" s="73"/>
       <c r="G31" s="58"/>
-      <c r="H31" s="101" t="s">
+      <c r="H31" s="93" t="s">
         <v>294</v>
       </c>
-      <c r="I31" s="101" t="s">
+      <c r="I31" s="93" t="s">
         <v>335</v>
       </c>
-      <c r="J31" s="101" t="s">
+      <c r="J31" s="93" t="s">
         <v>367</v>
       </c>
-      <c r="K31" s="101" t="s">
+      <c r="K31" s="93" t="s">
         <v>383</v>
       </c>
       <c r="L31" s="63"/>
@@ -10870,16 +10958,16 @@
       <c r="E32" s="73"/>
       <c r="F32" s="73"/>
       <c r="G32" s="58"/>
-      <c r="H32" s="101" t="s">
+      <c r="H32" s="93" t="s">
         <v>308</v>
       </c>
-      <c r="I32" s="101" t="s">
+      <c r="I32" s="93" t="s">
         <v>336</v>
       </c>
-      <c r="J32" s="101" t="s">
+      <c r="J32" s="93" t="s">
         <v>368</v>
       </c>
-      <c r="K32" s="105" t="s">
+      <c r="K32" s="108" t="s">
         <v>384</v>
       </c>
       <c r="L32" s="63"/>
@@ -10899,10 +10987,10 @@
       <c r="I33" s="72" t="s">
         <v>337</v>
       </c>
-      <c r="J33" s="100" t="s">
+      <c r="J33" s="92" t="s">
         <v>332</v>
       </c>
-      <c r="K33" s="89" t="s">
+      <c r="K33" s="105" t="s">
         <v>385</v>
       </c>
       <c r="L33" s="20"/>
@@ -10960,7 +11048,7 @@
       <c r="J35" s="72" t="s">
         <v>379</v>
       </c>
-      <c r="K35" s="89" t="s">
+      <c r="K35" s="105" t="s">
         <v>387</v>
       </c>
       <c r="L35" s="20"/>
@@ -11005,7 +11093,7 @@
       <c r="I37" s="72" t="s">
         <v>365</v>
       </c>
-      <c r="J37" s="89" t="s">
+      <c r="J37" s="105" t="s">
         <v>382</v>
       </c>
       <c r="K37" s="20"/>
@@ -11037,15 +11125,15 @@
       <c r="C39" s="73"/>
       <c r="D39" s="73"/>
       <c r="E39" s="73"/>
-      <c r="F39" s="85"/>
+      <c r="F39" s="84"/>
       <c r="G39" s="58"/>
-      <c r="H39" s="92" t="s">
+      <c r="H39" s="97" t="s">
         <v>381</v>
       </c>
-      <c r="I39" s="93"/>
-      <c r="J39" s="93"/>
-      <c r="K39" s="93"/>
-      <c r="L39" s="94"/>
+      <c r="I39" s="98"/>
+      <c r="J39" s="98"/>
+      <c r="K39" s="98"/>
+      <c r="L39" s="99"/>
       <c r="M39" s="58"/>
     </row>
     <row r="40" spans="1:13" ht="30.75" thickBot="1">
@@ -11056,16 +11144,16 @@
       <c r="E40" s="65"/>
       <c r="F40" s="66"/>
       <c r="G40" s="58"/>
-      <c r="H40" s="101" t="s">
+      <c r="H40" s="93" t="s">
         <v>302</v>
       </c>
-      <c r="I40" s="101" t="s">
+      <c r="I40" s="93" t="s">
         <v>323</v>
       </c>
-      <c r="J40" s="101" t="s">
+      <c r="J40" s="93" t="s">
         <v>361</v>
       </c>
-      <c r="K40" s="101" t="s">
+      <c r="K40" s="93" t="s">
         <v>377</v>
       </c>
       <c r="L40" s="63"/>
@@ -11089,16 +11177,16 @@
         <v>3</v>
       </c>
       <c r="G41" s="58"/>
-      <c r="H41" s="101" t="s">
+      <c r="H41" s="93" t="s">
         <v>303</v>
       </c>
-      <c r="I41" s="101" t="s">
+      <c r="I41" s="93" t="s">
         <v>324</v>
       </c>
-      <c r="J41" s="101" t="s">
+      <c r="J41" s="93" t="s">
         <v>362</v>
       </c>
-      <c r="K41" s="101" t="s">
+      <c r="K41" s="93" t="s">
         <v>380</v>
       </c>
       <c r="L41" s="63"/>
@@ -11123,7 +11211,7 @@
       <c r="J42" s="72" t="s">
         <v>369</v>
       </c>
-      <c r="K42" s="88"/>
+      <c r="K42" s="87"/>
       <c r="L42" s="20"/>
       <c r="M42" s="58"/>
     </row>
@@ -11135,7 +11223,7 @@
       <c r="C43" s="73"/>
       <c r="D43" s="73"/>
       <c r="E43" s="73"/>
-      <c r="F43" s="89" t="s">
+      <c r="F43" s="105" t="s">
         <v>406</v>
       </c>
       <c r="G43" s="58"/>
@@ -11168,7 +11256,7 @@
       <c r="I44" s="72" t="s">
         <v>338</v>
       </c>
-      <c r="J44" s="100" t="s">
+      <c r="J44" s="92" t="s">
         <v>373</v>
       </c>
       <c r="K44" s="20"/>
@@ -11206,7 +11294,7 @@
       <c r="C46" s="73"/>
       <c r="D46" s="73"/>
       <c r="E46" s="73"/>
-      <c r="F46" s="85"/>
+      <c r="F46" s="84"/>
       <c r="G46" s="58"/>
       <c r="H46" s="72" t="s">
         <v>318</v>
@@ -11254,13 +11342,13 @@
         <v>3</v>
       </c>
       <c r="G48" s="58"/>
-      <c r="H48" s="92" t="s">
+      <c r="H48" s="97" t="s">
         <v>172</v>
       </c>
-      <c r="I48" s="93"/>
-      <c r="J48" s="93"/>
-      <c r="K48" s="93"/>
-      <c r="L48" s="94"/>
+      <c r="I48" s="98"/>
+      <c r="J48" s="98"/>
+      <c r="K48" s="98"/>
+      <c r="L48" s="99"/>
       <c r="M48" s="58"/>
     </row>
     <row r="49" spans="1:13" ht="15.75" thickBot="1">
@@ -11273,13 +11361,13 @@
       <c r="E49" s="73"/>
       <c r="F49" s="73"/>
       <c r="G49" s="58"/>
-      <c r="H49" s="101" t="s">
+      <c r="H49" s="93" t="s">
         <v>301</v>
       </c>
-      <c r="I49" s="101" t="s">
+      <c r="I49" s="93" t="s">
         <v>329</v>
       </c>
-      <c r="J49" s="105" t="s">
+      <c r="J49" s="108" t="s">
         <v>388</v>
       </c>
       <c r="K49" s="63"/>
@@ -11296,13 +11384,13 @@
       <c r="E50" s="73"/>
       <c r="F50" s="73"/>
       <c r="G50" s="58"/>
-      <c r="H50" s="101" t="s">
+      <c r="H50" s="93" t="s">
         <v>304</v>
       </c>
-      <c r="I50" s="101" t="s">
+      <c r="I50" s="93" t="s">
         <v>330</v>
       </c>
-      <c r="J50" s="105" t="s">
+      <c r="J50" s="108" t="s">
         <v>389</v>
       </c>
       <c r="K50" s="63"/>
@@ -11322,10 +11410,10 @@
       <c r="H51" s="72" t="s">
         <v>306</v>
       </c>
-      <c r="I51" s="100" t="s">
+      <c r="I51" s="92" t="s">
         <v>331</v>
       </c>
-      <c r="J51" s="89" t="s">
+      <c r="J51" s="88" t="s">
         <v>390</v>
       </c>
       <c r="K51" s="20"/>
@@ -11366,7 +11454,7 @@
       <c r="H53" s="72" t="s">
         <v>320</v>
       </c>
-      <c r="I53" s="100" t="s">
+      <c r="I53" s="92" t="s">
         <v>364</v>
       </c>
       <c r="J53" s="20"/>
@@ -11443,13 +11531,13 @@
       <c r="E57" s="74"/>
       <c r="F57" s="74"/>
       <c r="G57" s="58"/>
-      <c r="H57" s="92" t="s">
+      <c r="H57" s="97" t="s">
         <v>173</v>
       </c>
-      <c r="I57" s="93"/>
-      <c r="J57" s="93"/>
-      <c r="K57" s="93"/>
-      <c r="L57" s="94"/>
+      <c r="I57" s="98"/>
+      <c r="J57" s="98"/>
+      <c r="K57" s="98"/>
+      <c r="L57" s="99"/>
       <c r="M57" s="58"/>
     </row>
     <row r="58" spans="1:13" ht="30.75" thickBot="1">
@@ -11460,23 +11548,23 @@
       <c r="C58" s="73"/>
       <c r="D58" s="73"/>
       <c r="E58" s="73"/>
-      <c r="F58" s="89" t="s">
+      <c r="F58" s="105" t="s">
         <v>407</v>
       </c>
       <c r="G58" s="58"/>
-      <c r="H58" s="101" t="s">
+      <c r="H58" s="93" t="s">
         <v>339</v>
       </c>
-      <c r="I58" s="108" t="s">
+      <c r="I58" s="94" t="s">
         <v>346</v>
       </c>
-      <c r="J58" s="101" t="s">
+      <c r="J58" s="93" t="s">
         <v>353</v>
       </c>
-      <c r="K58" s="63" t="s">
+      <c r="K58" s="108" t="s">
         <v>396</v>
       </c>
-      <c r="L58" s="63" t="s">
+      <c r="L58" s="108" t="s">
         <v>403</v>
       </c>
       <c r="M58" s="58"/>
@@ -11491,19 +11579,19 @@
       <c r="E59" s="74"/>
       <c r="F59" s="74"/>
       <c r="G59" s="58"/>
-      <c r="H59" s="101" t="s">
+      <c r="H59" s="93" t="s">
         <v>340</v>
       </c>
-      <c r="I59" s="108" t="s">
+      <c r="I59" s="94" t="s">
         <v>347</v>
       </c>
-      <c r="J59" s="101" t="s">
+      <c r="J59" s="93" t="s">
         <v>354</v>
       </c>
-      <c r="K59" s="63" t="s">
+      <c r="K59" s="108" t="s">
         <v>397</v>
       </c>
-      <c r="L59" s="63" t="s">
+      <c r="L59" s="108" t="s">
         <v>404</v>
       </c>
       <c r="M59" s="58"/>
@@ -11520,15 +11608,15 @@
         <v>408</v>
       </c>
       <c r="G60" s="58" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="H60" s="72" t="s">
         <v>341</v>
       </c>
-      <c r="I60" s="100" t="s">
+      <c r="I60" s="92" t="s">
         <v>348</v>
       </c>
-      <c r="J60" s="100" t="s">
+      <c r="J60" s="92" t="s">
         <v>355</v>
       </c>
       <c r="K60" s="72" t="s">
@@ -11547,7 +11635,7 @@
       <c r="E61" s="73"/>
       <c r="F61" s="73"/>
       <c r="G61" s="58"/>
-      <c r="H61" s="100" t="s">
+      <c r="H61" s="92" t="s">
         <v>342</v>
       </c>
       <c r="I61" s="72" t="s">
@@ -11556,13 +11644,13 @@
       <c r="J61" s="72" t="s">
         <v>371</v>
       </c>
-      <c r="K61" s="20" t="s">
+      <c r="K61" s="105" t="s">
         <v>399</v>
       </c>
       <c r="L61" s="20"/>
       <c r="M61" s="58"/>
     </row>
-    <row r="62" spans="1:13" ht="26.25" thickBot="1">
+    <row r="62" spans="1:13" ht="195.75" thickBot="1">
       <c r="A62" s="58"/>
       <c r="B62" s="19" t="s">
         <v>55</v>
@@ -11578,14 +11666,16 @@
       <c r="I62" s="72" t="s">
         <v>350</v>
       </c>
-      <c r="J62" s="100" t="s">
+      <c r="J62" s="92" t="s">
         <v>372</v>
       </c>
-      <c r="K62" s="20" t="s">
+      <c r="K62" s="75" t="s">
         <v>400</v>
       </c>
       <c r="L62" s="20"/>
-      <c r="M62" s="58"/>
+      <c r="M62" s="58" t="s">
+        <v>472</v>
+      </c>
     </row>
     <row r="63" spans="1:13" ht="45.75" thickBot="1">
       <c r="A63" s="58"/>
@@ -11599,7 +11689,7 @@
         <v>409</v>
       </c>
       <c r="G63" s="58" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="H63" s="72" t="s">
         <v>344</v>
@@ -11607,10 +11697,10 @@
       <c r="I63" s="72" t="s">
         <v>351</v>
       </c>
-      <c r="J63" s="20" t="s">
+      <c r="J63" s="105" t="s">
         <v>394</v>
       </c>
-      <c r="K63" s="20" t="s">
+      <c r="K63" s="105" t="s">
         <v>401</v>
       </c>
       <c r="L63" s="20"/>
@@ -11629,13 +11719,13 @@
       <c r="H64" s="72" t="s">
         <v>345</v>
       </c>
-      <c r="I64" s="100" t="s">
+      <c r="I64" s="92" t="s">
         <v>352</v>
       </c>
-      <c r="J64" s="20" t="s">
+      <c r="J64" s="105" t="s">
         <v>395</v>
       </c>
-      <c r="K64" s="20" t="s">
+      <c r="K64" s="105" t="s">
         <v>402</v>
       </c>
       <c r="L64" s="20"/>
@@ -11668,13 +11758,13 @@
       <c r="E66" s="73"/>
       <c r="F66" s="73"/>
       <c r="G66" s="58"/>
-      <c r="H66" s="92" t="s">
+      <c r="H66" s="97" t="s">
         <v>174</v>
       </c>
-      <c r="I66" s="93"/>
-      <c r="J66" s="93"/>
-      <c r="K66" s="93"/>
-      <c r="L66" s="94"/>
+      <c r="I66" s="98"/>
+      <c r="J66" s="98"/>
+      <c r="K66" s="98"/>
+      <c r="L66" s="99"/>
       <c r="M66" s="58"/>
     </row>
     <row r="67" spans="1:13" ht="30.75" thickBot="1">
@@ -11687,21 +11777,21 @@
       <c r="E67" s="73"/>
       <c r="F67" s="73"/>
       <c r="G67" s="58"/>
-      <c r="H67" s="101" t="s">
+      <c r="H67" s="93" t="s">
         <v>288</v>
       </c>
-      <c r="I67" s="101" t="s">
+      <c r="I67" s="93" t="s">
         <v>392</v>
       </c>
       <c r="J67" s="76" t="s">
         <v>393</v>
       </c>
-      <c r="K67" s="107" t="s">
+      <c r="K67" s="103" t="s">
         <v>290</v>
       </c>
-      <c r="L67" s="106"/>
+      <c r="L67" s="104"/>
       <c r="M67" s="58" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="68" spans="1:13" ht="15.75" thickBot="1">
@@ -11714,15 +11804,15 @@
       <c r="E68" s="73"/>
       <c r="F68" s="73"/>
       <c r="G68" s="58"/>
-      <c r="H68" s="101" t="s">
+      <c r="H68" s="93" t="s">
         <v>289</v>
       </c>
       <c r="I68" s="63"/>
       <c r="J68" s="63"/>
-      <c r="K68" s="107" t="s">
+      <c r="K68" s="103" t="s">
         <v>291</v>
       </c>
-      <c r="L68" s="106"/>
+      <c r="L68" s="104"/>
       <c r="M68" s="58"/>
     </row>
     <row r="69" spans="1:13" ht="15.75" thickBot="1">
@@ -11740,10 +11830,10 @@
       </c>
       <c r="I69" s="20"/>
       <c r="J69" s="20"/>
-      <c r="K69" s="104" t="s">
+      <c r="K69" s="100" t="s">
         <v>298</v>
       </c>
-      <c r="L69" s="102"/>
+      <c r="L69" s="101"/>
       <c r="M69" s="58"/>
     </row>
     <row r="70" spans="1:13" ht="15.75" thickBot="1">
@@ -11761,10 +11851,10 @@
       </c>
       <c r="I70" s="20"/>
       <c r="J70" s="20"/>
-      <c r="K70" s="104" t="s">
+      <c r="K70" s="100" t="s">
         <v>299</v>
       </c>
-      <c r="L70" s="102"/>
+      <c r="L70" s="101"/>
       <c r="M70" s="58"/>
     </row>
     <row r="71" spans="1:13" ht="15.75" thickBot="1">
@@ -11782,10 +11872,10 @@
       </c>
       <c r="I71" s="20"/>
       <c r="J71" s="20"/>
-      <c r="K71" s="104" t="s">
+      <c r="K71" s="100" t="s">
         <v>314</v>
       </c>
-      <c r="L71" s="102"/>
+      <c r="L71" s="101"/>
       <c r="M71" s="58"/>
     </row>
     <row r="72" spans="1:13" ht="26.25" thickBot="1">
@@ -11796,19 +11886,19 @@
       <c r="C72" s="73"/>
       <c r="D72" s="73"/>
       <c r="E72" s="73"/>
-      <c r="F72" s="96" t="s">
+      <c r="F72" s="105" t="s">
         <v>410</v>
       </c>
       <c r="G72" s="58"/>
-      <c r="H72" s="89" t="s">
+      <c r="H72" s="105" t="s">
         <v>391</v>
       </c>
       <c r="I72" s="20"/>
       <c r="J72" s="20"/>
-      <c r="K72" s="104" t="s">
+      <c r="K72" s="100" t="s">
         <v>328</v>
       </c>
-      <c r="L72" s="102"/>
+      <c r="L72" s="101"/>
       <c r="M72" s="58"/>
     </row>
     <row r="73" spans="1:13" ht="15.75" thickBot="1">
@@ -11898,8 +11988,8 @@
       <c r="B77" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="C77" s="83"/>
-      <c r="D77" s="83"/>
+      <c r="C77" s="82"/>
+      <c r="D77" s="82"/>
       <c r="E77" s="74"/>
       <c r="F77" s="74"/>
       <c r="G77" s="58"/>
@@ -11962,7 +12052,7 @@
         <v>411</v>
       </c>
       <c r="G80" s="58" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="H80" s="19" t="s">
         <v>181</v>
@@ -12000,7 +12090,7 @@
       <c r="C82" s="73"/>
       <c r="D82" s="73"/>
       <c r="E82" s="73"/>
-      <c r="F82" s="89" t="s">
+      <c r="F82" s="105" t="s">
         <v>412</v>
       </c>
       <c r="G82" s="58"/>
@@ -12040,7 +12130,7 @@
       <c r="C84" s="73"/>
       <c r="D84" s="73"/>
       <c r="E84" s="73"/>
-      <c r="F84" s="89" t="s">
+      <c r="F84" s="105" t="s">
         <v>413</v>
       </c>
       <c r="G84" s="58"/>
@@ -12069,7 +12159,7 @@
       <c r="I85" s="73"/>
       <c r="J85" s="73"/>
       <c r="K85" s="73"/>
-      <c r="L85" s="89" t="s">
+      <c r="L85" s="105" t="s">
         <v>429</v>
       </c>
       <c r="M85" s="58"/>
@@ -12081,12 +12171,12 @@
       </c>
       <c r="C86" s="73"/>
       <c r="D86" s="75" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E86" s="73"/>
       <c r="F86" s="73"/>
       <c r="G86" s="58" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="H86" s="19" t="s">
         <v>187</v>
@@ -12113,7 +12203,7 @@
       <c r="I87" s="73"/>
       <c r="J87" s="73"/>
       <c r="K87" s="73"/>
-      <c r="L87" s="89" t="s">
+      <c r="L87" s="105" t="s">
         <v>430</v>
       </c>
       <c r="M87" s="58"/>
@@ -12124,13 +12214,13 @@
         <v>81</v>
       </c>
       <c r="C88" s="73"/>
-      <c r="D88" s="97" t="s">
+      <c r="D88" s="89" t="s">
         <v>414</v>
       </c>
       <c r="E88" s="73"/>
       <c r="F88" s="73"/>
       <c r="G88" s="58" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="H88" s="19" t="s">
         <v>189</v>
@@ -12168,7 +12258,7 @@
       <c r="C90" s="74"/>
       <c r="D90" s="74"/>
       <c r="E90" s="74"/>
-      <c r="F90" s="103" t="s">
+      <c r="F90" s="106" t="s">
         <v>415</v>
       </c>
       <c r="G90" s="58"/>
@@ -12176,11 +12266,11 @@
         <v>191</v>
       </c>
       <c r="I90" s="73"/>
-      <c r="J90" s="89" t="s">
+      <c r="J90" s="105" t="s">
         <v>431</v>
       </c>
       <c r="K90" s="73"/>
-      <c r="L90" s="89" t="s">
+      <c r="L90" s="105" t="s">
         <v>432</v>
       </c>
       <c r="M90" s="58"/>
@@ -12239,7 +12329,7 @@
       <c r="I93" s="73"/>
       <c r="J93" s="73"/>
       <c r="K93" s="73"/>
-      <c r="L93" s="89" t="s">
+      <c r="L93" s="105" t="s">
         <v>433</v>
       </c>
       <c r="M93" s="58"/>
@@ -12260,7 +12350,7 @@
       <c r="I94" s="73"/>
       <c r="J94" s="73"/>
       <c r="K94" s="73"/>
-      <c r="L94" s="89" t="s">
+      <c r="L94" s="105" t="s">
         <v>434</v>
       </c>
       <c r="M94" s="58"/>
@@ -12281,7 +12371,7 @@
       <c r="I95" s="73"/>
       <c r="J95" s="73"/>
       <c r="K95" s="73"/>
-      <c r="L95" s="89" t="s">
+      <c r="L95" s="105" t="s">
         <v>435</v>
       </c>
       <c r="M95" s="58"/>
@@ -12319,7 +12409,7 @@
         <v>195</v>
       </c>
       <c r="I97" s="73"/>
-      <c r="J97" s="89" t="s">
+      <c r="J97" s="105" t="s">
         <v>436</v>
       </c>
       <c r="K97" s="73"/>
@@ -12327,7 +12417,7 @@
         <v>437</v>
       </c>
       <c r="M97" s="58" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="98" spans="1:13" ht="39" thickBot="1">
@@ -12346,10 +12436,12 @@
       <c r="I98" s="73"/>
       <c r="J98" s="73"/>
       <c r="K98" s="73"/>
-      <c r="L98" s="89" t="s">
+      <c r="L98" s="75" t="s">
         <v>438</v>
       </c>
-      <c r="M98" s="58"/>
+      <c r="M98" s="58" t="s">
+        <v>471</v>
+      </c>
     </row>
     <row r="99" spans="1:13" ht="26.25" thickBot="1">
       <c r="A99" s="58"/>
@@ -12367,7 +12459,7 @@
       <c r="I99" s="73"/>
       <c r="J99" s="73"/>
       <c r="K99" s="73"/>
-      <c r="L99" s="89" t="s">
+      <c r="L99" s="105" t="s">
         <v>439</v>
       </c>
       <c r="M99" s="58"/>
@@ -12380,7 +12472,7 @@
       <c r="C100" s="74"/>
       <c r="D100" s="74"/>
       <c r="E100" s="74"/>
-      <c r="F100" s="83"/>
+      <c r="F100" s="82"/>
       <c r="G100" s="58"/>
       <c r="H100" s="19" t="s">
         <v>200</v>
@@ -12409,11 +12501,11 @@
       <c r="K101" s="75" t="s">
         <v>440</v>
       </c>
-      <c r="L101" s="89" t="s">
+      <c r="L101" s="105" t="s">
         <v>441</v>
       </c>
       <c r="M101" s="58" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="102" spans="1:13" ht="30.75" thickBot="1">
@@ -12445,7 +12537,7 @@
       <c r="C103" s="73"/>
       <c r="D103" s="73"/>
       <c r="E103" s="73"/>
-      <c r="F103" s="85"/>
+      <c r="F103" s="84"/>
       <c r="G103" s="58"/>
       <c r="H103" s="58"/>
       <c r="I103" s="58"/>
@@ -12558,7 +12650,7 @@
         <v>206</v>
       </c>
       <c r="I108" s="73"/>
-      <c r="J108" s="20" t="s">
+      <c r="J108" s="105" t="s">
         <v>443</v>
       </c>
       <c r="K108" s="73"/>
@@ -12579,7 +12671,7 @@
         <v>207</v>
       </c>
       <c r="I109" s="73"/>
-      <c r="J109" s="81"/>
+      <c r="J109" s="80"/>
       <c r="K109" s="73"/>
       <c r="L109" s="73"/>
       <c r="M109" s="58"/>
@@ -12603,18 +12695,20 @@
       <c r="L110" s="73"/>
       <c r="M110" s="58"/>
     </row>
-    <row r="111" spans="1:13" ht="15.75" thickBot="1">
+    <row r="111" spans="1:13" ht="45.75" thickBot="1">
       <c r="A111" s="58"/>
       <c r="B111" s="19" t="s">
         <v>102</v>
       </c>
       <c r="C111" s="73"/>
-      <c r="D111" s="20" t="s">
+      <c r="D111" s="75" t="s">
         <v>416</v>
       </c>
       <c r="E111" s="73"/>
       <c r="F111" s="73"/>
-      <c r="G111" s="58"/>
+      <c r="G111" s="58" t="s">
+        <v>463</v>
+      </c>
       <c r="H111" s="19" t="s">
         <v>209</v>
       </c>
@@ -12640,23 +12734,25 @@
       <c r="I112" s="73"/>
       <c r="J112" s="73"/>
       <c r="K112" s="73"/>
-      <c r="L112" s="20" t="s">
+      <c r="L112" s="105" t="s">
         <v>444</v>
       </c>
       <c r="M112" s="58"/>
     </row>
-    <row r="113" spans="1:13" ht="15.75" thickBot="1">
+    <row r="113" spans="1:13" ht="45.75" thickBot="1">
       <c r="A113" s="58"/>
       <c r="B113" s="19" t="s">
         <v>104</v>
       </c>
       <c r="C113" s="73"/>
       <c r="D113" s="73"/>
-      <c r="E113" s="20" t="s">
+      <c r="E113" s="75" t="s">
         <v>417</v>
       </c>
       <c r="F113" s="73"/>
-      <c r="G113" s="58"/>
+      <c r="G113" s="58" t="s">
+        <v>464</v>
+      </c>
       <c r="H113" s="19" t="s">
         <v>211</v>
       </c>
@@ -12666,7 +12762,7 @@
       <c r="L113" s="73"/>
       <c r="M113" s="58"/>
     </row>
-    <row r="114" spans="1:13" ht="15.75" thickBot="1">
+    <row r="114" spans="1:13" ht="90.75" thickBot="1">
       <c r="A114" s="58"/>
       <c r="B114" s="19" t="s">
         <v>105</v>
@@ -12676,10 +12772,12 @@
       </c>
       <c r="D114" s="73"/>
       <c r="E114" s="73"/>
-      <c r="F114" s="20" t="s">
+      <c r="F114" s="75" t="s">
         <v>418</v>
       </c>
-      <c r="G114" s="58"/>
+      <c r="G114" s="58" t="s">
+        <v>465</v>
+      </c>
       <c r="H114" s="19" t="s">
         <v>212</v>
       </c>
@@ -12734,10 +12832,10 @@
       <c r="B117" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="C117" s="84" t="s">
+      <c r="C117" s="83" t="s">
         <v>287</v>
       </c>
-      <c r="D117" s="83"/>
+      <c r="D117" s="82"/>
       <c r="E117" s="74"/>
       <c r="F117" s="74"/>
       <c r="G117" s="58"/>
@@ -12784,7 +12882,7 @@
       </c>
       <c r="I119" s="73"/>
       <c r="J119" s="73"/>
-      <c r="K119" s="87"/>
+      <c r="K119" s="86"/>
       <c r="L119" s="73"/>
       <c r="M119" s="58"/>
     </row>
@@ -12842,7 +12940,7 @@
       <c r="I122" s="73"/>
       <c r="J122" s="73"/>
       <c r="K122" s="73"/>
-      <c r="L122" s="20" t="s">
+      <c r="L122" s="105" t="s">
         <v>445</v>
       </c>
       <c r="M122" s="58"/>
@@ -12901,7 +12999,7 @@
       <c r="I125" s="73"/>
       <c r="J125" s="73"/>
       <c r="K125" s="73"/>
-      <c r="L125" s="20" t="s">
+      <c r="L125" s="105" t="s">
         <v>446</v>
       </c>
       <c r="M125" s="58"/>
@@ -12914,7 +13012,7 @@
       <c r="C126" s="73"/>
       <c r="D126" s="73"/>
       <c r="E126" s="73"/>
-      <c r="F126" s="80" t="s">
+      <c r="F126" s="105" t="s">
         <v>419</v>
       </c>
       <c r="G126" s="58"/>
@@ -12943,7 +13041,7 @@
       <c r="I127" s="73"/>
       <c r="J127" s="73"/>
       <c r="K127" s="73"/>
-      <c r="L127" s="20" t="s">
+      <c r="L127" s="105" t="s">
         <v>447</v>
       </c>
       <c r="M127" s="58"/>
@@ -12953,8 +13051,8 @@
       <c r="B128" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="C128" s="83"/>
-      <c r="D128" s="82"/>
+      <c r="C128" s="82"/>
+      <c r="D128" s="81"/>
       <c r="E128" s="74"/>
       <c r="F128" s="74"/>
       <c r="G128" s="58"/>
@@ -12964,7 +13062,7 @@
       <c r="I128" s="73"/>
       <c r="J128" s="73"/>
       <c r="K128" s="73"/>
-      <c r="L128" s="20" t="s">
+      <c r="L128" s="105" t="s">
         <v>448</v>
       </c>
       <c r="M128" s="58"/>
@@ -13015,7 +13113,7 @@
       <c r="C131" s="74"/>
       <c r="D131" s="74"/>
       <c r="E131" s="74"/>
-      <c r="F131" s="83"/>
+      <c r="F131" s="82"/>
       <c r="G131" s="58"/>
       <c r="H131" s="19" t="s">
         <v>228</v>
@@ -13023,7 +13121,7 @@
       <c r="I131" s="73"/>
       <c r="J131" s="73"/>
       <c r="K131" s="73"/>
-      <c r="L131" s="20" t="s">
+      <c r="L131" s="105" t="s">
         <v>449</v>
       </c>
       <c r="M131" s="58"/>
@@ -13036,17 +13134,17 @@
       <c r="C132" s="73"/>
       <c r="D132" s="73"/>
       <c r="E132" s="73"/>
-      <c r="F132" s="20" t="s">
+      <c r="F132" s="105" t="s">
         <v>420</v>
       </c>
       <c r="G132" s="58"/>
       <c r="H132" s="19" t="s">
-        <v>229</v>
+        <v>468</v>
       </c>
       <c r="I132" s="73"/>
       <c r="J132" s="73"/>
       <c r="K132" s="73"/>
-      <c r="L132" s="62" t="s">
+      <c r="L132" s="109" t="s">
         <v>450</v>
       </c>
       <c r="M132" s="58"/>
@@ -13068,7 +13166,7 @@
       <c r="L133" s="4"/>
       <c r="M133" s="4"/>
     </row>
-    <row r="134" spans="1:14" ht="27" thickBot="1">
+    <row r="134" spans="1:14" ht="60.75" thickBot="1">
       <c r="A134" s="58"/>
       <c r="B134" s="19" t="s">
         <v>125</v>
@@ -13076,10 +13174,12 @@
       <c r="C134" s="73"/>
       <c r="D134" s="73"/>
       <c r="E134" s="73"/>
-      <c r="F134" s="20" t="s">
+      <c r="F134" s="75" t="s">
         <v>421</v>
       </c>
-      <c r="G134" s="4"/>
+      <c r="G134" s="107" t="s">
+        <v>466</v>
+      </c>
       <c r="H134" s="44" t="s">
         <v>231</v>
       </c>
@@ -13105,8 +13205,8 @@
       <c r="B135" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="C135" s="86"/>
-      <c r="D135" s="86"/>
+      <c r="C135" s="85"/>
+      <c r="D135" s="85"/>
       <c r="E135" s="73"/>
       <c r="F135" s="73"/>
       <c r="G135" s="4"/>
@@ -13200,18 +13300,20 @@
       <c r="M139" s="54"/>
       <c r="N139" s="4"/>
     </row>
-    <row r="140" spans="1:14" ht="26.25" thickBot="1">
+    <row r="140" spans="1:14" ht="45.75" thickBot="1">
       <c r="A140" s="58"/>
       <c r="B140" s="19" t="s">
         <v>131</v>
       </c>
       <c r="C140" s="73"/>
       <c r="D140" s="73"/>
-      <c r="E140" s="20" t="s">
+      <c r="E140" s="75" t="s">
         <v>422</v>
       </c>
       <c r="F140" s="73"/>
-      <c r="G140" s="4"/>
+      <c r="G140" s="107" t="s">
+        <v>467</v>
+      </c>
       <c r="H140" s="4"/>
       <c r="I140" s="4"/>
       <c r="J140" s="4"/>
@@ -13258,7 +13360,7 @@
       <c r="C142" s="73"/>
       <c r="D142" s="73"/>
       <c r="E142" s="73"/>
-      <c r="F142" s="85"/>
+      <c r="F142" s="84"/>
       <c r="G142" s="4"/>
       <c r="H142" s="51" t="s">
         <v>237</v>
@@ -13530,7 +13632,7 @@
       <c r="C155" s="73"/>
       <c r="D155" s="73"/>
       <c r="E155" s="73"/>
-      <c r="F155" s="85"/>
+      <c r="F155" s="84"/>
       <c r="G155" s="4"/>
       <c r="H155" s="44" t="s">
         <v>255</v>

</xml_diff>

<commit_message>
Quest Ref change, 2 SU stat change, item list updat
</commit_message>
<xml_diff>
--- a/check list.xlsx
+++ b/check list.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1261" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1250" uniqueCount="458">
   <si>
     <t>ARMOR</t>
   </si>
@@ -1210,9 +1210,6 @@
     <t>Arrowsider</t>
   </si>
   <si>
-    <t>Devils's dance</t>
-  </si>
-  <si>
     <t>Idol of stars</t>
   </si>
   <si>
@@ -1396,50 +1393,19 @@
     <t xml:space="preserve">Skeld's Battlesong </t>
   </si>
   <si>
-    <t>proc Demonrend?</t>
-  </si>
-  <si>
-    <t>oskill Arcane Strike?</t>
-  </si>
-  <si>
-    <t>oskill Cold Blood?</t>
-  </si>
-  <si>
-    <t>oskill Ball Lightning?</t>
-  </si>
-  <si>
-    <t>add heal-melee 50-75?</t>
-  </si>
-  <si>
-    <t>proc forked lightning?</t>
-  </si>
-  <si>
-    <t>oskill fireboltbarrage</t>
-  </si>
-  <si>
-    <t>proc chickenlickin</t>
-  </si>
-  <si>
-    <t>kill-skill Mon Spinning Mind Flay
- (535)</t>
-  </si>
-  <si>
     <t>Blackguard Helm</t>
   </si>
   <si>
     <t>Demonstring</t>
-  </si>
-  <si>
-    <t>absorb fire,cold,light, magic?</t>
-  </si>
-  <si>
-    <t>skill solistice and equinox?</t>
   </si>
   <si>
     <t>3% Faster Cast Rate
 +5% Bonus to Summoned Minion Attack Rating
 +1 to Maximum Necromancer Minions
 3% Crushing Blow to Darklings?</t>
+  </si>
+  <si>
+    <t>Devil's dance</t>
   </si>
 </sst>
 </file>
@@ -2339,7 +2305,7 @@
     <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2556,9 +2522,6 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2593,9 +2556,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3557,13 +3517,13 @@
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
       <c r="G27" s="7"/>
-      <c r="H27" s="101" t="s">
+      <c r="H27" s="99" t="s">
         <v>170</v>
       </c>
-      <c r="I27" s="101"/>
-      <c r="J27" s="101"/>
-      <c r="K27" s="101"/>
-      <c r="L27" s="101"/>
+      <c r="I27" s="99"/>
+      <c r="J27" s="99"/>
+      <c r="K27" s="99"/>
+      <c r="L27" s="99"/>
       <c r="M27" s="7"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1">
@@ -3718,13 +3678,13 @@
       <c r="E36" s="20"/>
       <c r="F36" s="29"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="101" t="s">
+      <c r="H36" s="99" t="s">
         <v>171</v>
       </c>
-      <c r="I36" s="101"/>
-      <c r="J36" s="101"/>
-      <c r="K36" s="101"/>
-      <c r="L36" s="101"/>
+      <c r="I36" s="99"/>
+      <c r="J36" s="99"/>
+      <c r="K36" s="99"/>
+      <c r="L36" s="99"/>
       <c r="M36" s="7"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
@@ -3885,13 +3845,13 @@
         <v>3</v>
       </c>
       <c r="G45" s="7"/>
-      <c r="H45" s="101" t="s">
+      <c r="H45" s="99" t="s">
         <v>172</v>
       </c>
-      <c r="I45" s="101"/>
-      <c r="J45" s="101"/>
-      <c r="K45" s="101"/>
-      <c r="L45" s="101"/>
+      <c r="I45" s="99"/>
+      <c r="J45" s="99"/>
+      <c r="K45" s="99"/>
+      <c r="L45" s="99"/>
       <c r="M45" s="7"/>
     </row>
     <row r="46" spans="1:13" ht="15.75" thickBot="1">
@@ -4040,13 +4000,13 @@
       <c r="E54" s="39"/>
       <c r="F54" s="39"/>
       <c r="G54" s="7"/>
-      <c r="H54" s="101" t="s">
+      <c r="H54" s="99" t="s">
         <v>173</v>
       </c>
-      <c r="I54" s="101"/>
-      <c r="J54" s="101"/>
-      <c r="K54" s="101"/>
-      <c r="L54" s="101"/>
+      <c r="I54" s="99"/>
+      <c r="J54" s="99"/>
+      <c r="K54" s="99"/>
+      <c r="L54" s="99"/>
       <c r="M54" s="7"/>
     </row>
     <row r="55" spans="1:13" ht="15.75" thickBot="1">
@@ -4195,13 +4155,13 @@
       <c r="E63" s="20"/>
       <c r="F63" s="20"/>
       <c r="G63" s="7"/>
-      <c r="H63" s="101" t="s">
+      <c r="H63" s="99" t="s">
         <v>174</v>
       </c>
-      <c r="I63" s="101"/>
-      <c r="J63" s="101"/>
-      <c r="K63" s="101"/>
-      <c r="L63" s="101"/>
+      <c r="I63" s="99"/>
+      <c r="J63" s="99"/>
+      <c r="K63" s="99"/>
+      <c r="L63" s="99"/>
       <c r="M63" s="7"/>
     </row>
     <row r="64" spans="1:13" ht="15.75" thickBot="1">
@@ -5510,11 +5470,11 @@
       <c r="E132" s="20"/>
       <c r="F132" s="20"/>
       <c r="G132" s="7"/>
-      <c r="H132" s="100"/>
-      <c r="I132" s="100"/>
-      <c r="J132" s="100"/>
-      <c r="K132" s="100"/>
-      <c r="L132" s="100"/>
+      <c r="H132" s="98"/>
+      <c r="I132" s="98"/>
+      <c r="J132" s="98"/>
+      <c r="K132" s="98"/>
+      <c r="L132" s="98"/>
       <c r="M132" s="7"/>
     </row>
     <row r="133" spans="1:14" ht="18" thickBot="1">
@@ -7260,13 +7220,13 @@
       <c r="E30" s="20"/>
       <c r="F30" s="20"/>
       <c r="G30" s="58"/>
-      <c r="H30" s="102" t="s">
+      <c r="H30" s="100" t="s">
         <v>170</v>
       </c>
-      <c r="I30" s="103"/>
-      <c r="J30" s="103"/>
-      <c r="K30" s="103"/>
-      <c r="L30" s="104"/>
+      <c r="I30" s="101"/>
+      <c r="J30" s="101"/>
+      <c r="K30" s="101"/>
+      <c r="L30" s="102"/>
       <c r="M30" s="58"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1">
@@ -7421,13 +7381,13 @@
       <c r="E39" s="20"/>
       <c r="F39" s="62"/>
       <c r="G39" s="58"/>
-      <c r="H39" s="102" t="s">
+      <c r="H39" s="100" t="s">
         <v>171</v>
       </c>
-      <c r="I39" s="103"/>
-      <c r="J39" s="103"/>
-      <c r="K39" s="103"/>
-      <c r="L39" s="104"/>
+      <c r="I39" s="101"/>
+      <c r="J39" s="101"/>
+      <c r="K39" s="101"/>
+      <c r="L39" s="102"/>
       <c r="M39" s="58"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" thickBot="1">
@@ -7588,13 +7548,13 @@
         <v>3</v>
       </c>
       <c r="G48" s="58"/>
-      <c r="H48" s="102" t="s">
+      <c r="H48" s="100" t="s">
         <v>172</v>
       </c>
-      <c r="I48" s="103"/>
-      <c r="J48" s="103"/>
-      <c r="K48" s="103"/>
-      <c r="L48" s="104"/>
+      <c r="I48" s="101"/>
+      <c r="J48" s="101"/>
+      <c r="K48" s="101"/>
+      <c r="L48" s="102"/>
       <c r="M48" s="58"/>
     </row>
     <row r="49" spans="1:13" ht="15.75" thickBot="1">
@@ -7743,13 +7703,13 @@
       <c r="E57" s="39"/>
       <c r="F57" s="39"/>
       <c r="G57" s="58"/>
-      <c r="H57" s="102" t="s">
+      <c r="H57" s="100" t="s">
         <v>173</v>
       </c>
-      <c r="I57" s="103"/>
-      <c r="J57" s="103"/>
-      <c r="K57" s="103"/>
-      <c r="L57" s="104"/>
+      <c r="I57" s="101"/>
+      <c r="J57" s="101"/>
+      <c r="K57" s="101"/>
+      <c r="L57" s="102"/>
       <c r="M57" s="58"/>
     </row>
     <row r="58" spans="1:13" ht="15.75" thickBot="1">
@@ -7898,13 +7858,13 @@
       <c r="E66" s="20"/>
       <c r="F66" s="20"/>
       <c r="G66" s="58"/>
-      <c r="H66" s="102" t="s">
+      <c r="H66" s="100" t="s">
         <v>174</v>
       </c>
-      <c r="I66" s="103"/>
-      <c r="J66" s="103"/>
-      <c r="K66" s="103"/>
-      <c r="L66" s="104"/>
+      <c r="I66" s="101"/>
+      <c r="J66" s="101"/>
+      <c r="K66" s="101"/>
+      <c r="L66" s="102"/>
       <c r="M66" s="58"/>
     </row>
     <row r="67" spans="1:13" ht="15.75" thickBot="1">
@@ -10261,8 +10221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F134" sqref="F134"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10282,40 +10242,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="23.25" customHeight="1">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="105" t="s">
         <v>284</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="107"/>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="107"/>
-      <c r="I1" s="107"/>
-      <c r="J1" s="107"/>
-      <c r="K1" s="107"/>
-      <c r="L1" s="107"/>
-      <c r="M1" s="107"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
+      <c r="K1" s="105"/>
+      <c r="L1" s="105"/>
+      <c r="M1" s="105"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1">
-      <c r="A2" s="107"/>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="107"/>
-      <c r="H2" s="107"/>
-      <c r="I2" s="107"/>
-      <c r="J2" s="107"/>
-      <c r="K2" s="107"/>
-      <c r="L2" s="107"/>
-      <c r="M2" s="107"/>
+      <c r="A2" s="105"/>
+      <c r="B2" s="105"/>
+      <c r="C2" s="105"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="105"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="105"/>
+      <c r="J2" s="105"/>
+      <c r="K2" s="105"/>
+      <c r="L2" s="105"/>
+      <c r="M2" s="105"/>
       <c r="N2" s="1"/>
       <c r="O2" s="69"/>
       <c r="P2" s="70" t="s">
@@ -10324,19 +10284,19 @@
       <c r="Q2" s="1"/>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1">
-      <c r="A3" s="107"/>
-      <c r="B3" s="107"/>
-      <c r="C3" s="107"/>
-      <c r="D3" s="107"/>
-      <c r="E3" s="107"/>
-      <c r="F3" s="107"/>
-      <c r="G3" s="107"/>
-      <c r="H3" s="107"/>
-      <c r="I3" s="107"/>
-      <c r="J3" s="107"/>
-      <c r="K3" s="107"/>
-      <c r="L3" s="107"/>
-      <c r="M3" s="107"/>
+      <c r="A3" s="105"/>
+      <c r="B3" s="105"/>
+      <c r="C3" s="105"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="105"/>
+      <c r="F3" s="105"/>
+      <c r="G3" s="105"/>
+      <c r="H3" s="105"/>
+      <c r="I3" s="105"/>
+      <c r="J3" s="105"/>
+      <c r="K3" s="105"/>
+      <c r="L3" s="105"/>
+      <c r="M3" s="105"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -10418,11 +10378,11 @@
       <c r="K6" s="73"/>
       <c r="L6" s="73"/>
       <c r="M6" s="58"/>
-      <c r="O6" s="91" t="s">
+      <c r="O6" s="89" t="s">
+        <v>450</v>
+      </c>
+      <c r="P6" t="s">
         <v>451</v>
-      </c>
-      <c r="P6" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1">
@@ -10462,11 +10422,11 @@
       <c r="K8" s="73"/>
       <c r="L8" s="73"/>
       <c r="M8" s="58"/>
-      <c r="O8" s="90" t="s">
-        <v>451</v>
+      <c r="O8" s="88" t="s">
+        <v>450</v>
       </c>
       <c r="P8" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="15.75" thickBot="1">
@@ -10580,8 +10540,8 @@
       <c r="I14" s="73"/>
       <c r="J14" s="73"/>
       <c r="K14" s="73"/>
-      <c r="L14" s="95" t="s">
-        <v>423</v>
+      <c r="L14" s="93" t="s">
+        <v>422</v>
       </c>
       <c r="M14" s="58"/>
     </row>
@@ -10623,7 +10583,7 @@
       <c r="L16" s="73"/>
       <c r="M16" s="58"/>
     </row>
-    <row r="17" spans="1:13" ht="45.75" thickBot="1">
+    <row r="17" spans="1:13" ht="26.25" thickBot="1">
       <c r="A17" s="58"/>
       <c r="B17" s="19" t="s">
         <v>15</v>
@@ -10638,15 +10598,13 @@
       </c>
       <c r="I17" s="73"/>
       <c r="J17" s="73"/>
-      <c r="K17" s="95" t="s">
-        <v>424</v>
-      </c>
-      <c r="L17" s="89" t="s">
-        <v>465</v>
-      </c>
-      <c r="M17" s="58" t="s">
-        <v>466</v>
-      </c>
+      <c r="K17" s="93" t="s">
+        <v>423</v>
+      </c>
+      <c r="L17" s="93" t="s">
+        <v>455</v>
+      </c>
+      <c r="M17" s="58"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1">
       <c r="A18" s="58"/>
@@ -10683,8 +10641,8 @@
       <c r="I19" s="73"/>
       <c r="J19" s="73"/>
       <c r="K19" s="73"/>
-      <c r="L19" s="95" t="s">
-        <v>425</v>
+      <c r="L19" s="93" t="s">
+        <v>424</v>
       </c>
       <c r="M19" s="58"/>
     </row>
@@ -10715,8 +10673,8 @@
       <c r="C21" s="73"/>
       <c r="D21" s="73"/>
       <c r="E21" s="73"/>
-      <c r="F21" s="95" t="s">
-        <v>405</v>
+      <c r="F21" s="93" t="s">
+        <v>404</v>
       </c>
       <c r="G21" s="58"/>
       <c r="H21" s="19" t="s">
@@ -10763,8 +10721,8 @@
       <c r="I23" s="73"/>
       <c r="J23" s="73"/>
       <c r="K23" s="73"/>
-      <c r="L23" s="95" t="s">
-        <v>426</v>
+      <c r="L23" s="93" t="s">
+        <v>425</v>
       </c>
       <c r="M23" s="58"/>
     </row>
@@ -10784,8 +10742,8 @@
       <c r="I24" s="73"/>
       <c r="J24" s="73"/>
       <c r="K24" s="73"/>
-      <c r="L24" s="95" t="s">
-        <v>427</v>
+      <c r="L24" s="93" t="s">
+        <v>426</v>
       </c>
       <c r="M24" s="58"/>
     </row>
@@ -10867,10 +10825,10 @@
       </c>
       <c r="I28" s="73"/>
       <c r="J28" s="73"/>
-      <c r="K28" s="95" t="s">
-        <v>428</v>
-      </c>
-      <c r="L28" s="84"/>
+      <c r="K28" s="93" t="s">
+        <v>427</v>
+      </c>
+      <c r="L28" s="83"/>
       <c r="M28" s="58"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1">
@@ -10902,13 +10860,13 @@
       <c r="E30" s="73"/>
       <c r="F30" s="73"/>
       <c r="G30" s="58"/>
-      <c r="H30" s="102" t="s">
+      <c r="H30" s="100" t="s">
         <v>170</v>
       </c>
-      <c r="I30" s="103"/>
-      <c r="J30" s="103"/>
-      <c r="K30" s="103"/>
-      <c r="L30" s="104"/>
+      <c r="I30" s="101"/>
+      <c r="J30" s="101"/>
+      <c r="K30" s="101"/>
+      <c r="L30" s="102"/>
       <c r="M30" s="58"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1">
@@ -10921,16 +10879,16 @@
       <c r="E31" s="73"/>
       <c r="F31" s="73"/>
       <c r="G31" s="58"/>
-      <c r="H31" s="93" t="s">
+      <c r="H31" s="91" t="s">
         <v>294</v>
       </c>
-      <c r="I31" s="93" t="s">
+      <c r="I31" s="91" t="s">
         <v>335</v>
       </c>
-      <c r="J31" s="93" t="s">
+      <c r="J31" s="91" t="s">
         <v>367</v>
       </c>
-      <c r="K31" s="93" t="s">
+      <c r="K31" s="91" t="s">
         <v>383</v>
       </c>
       <c r="L31" s="63"/>
@@ -10946,16 +10904,16 @@
       <c r="E32" s="73"/>
       <c r="F32" s="73"/>
       <c r="G32" s="58"/>
-      <c r="H32" s="93" t="s">
+      <c r="H32" s="91" t="s">
         <v>308</v>
       </c>
-      <c r="I32" s="93" t="s">
+      <c r="I32" s="91" t="s">
         <v>336</v>
       </c>
-      <c r="J32" s="93" t="s">
+      <c r="J32" s="91" t="s">
         <v>368</v>
       </c>
-      <c r="K32" s="98" t="s">
+      <c r="K32" s="96" t="s">
         <v>384</v>
       </c>
       <c r="L32" s="63"/>
@@ -10975,10 +10933,10 @@
       <c r="I33" s="72" t="s">
         <v>337</v>
       </c>
-      <c r="J33" s="92" t="s">
+      <c r="J33" s="90" t="s">
         <v>332</v>
       </c>
-      <c r="K33" s="95" t="s">
+      <c r="K33" s="93" t="s">
         <v>385</v>
       </c>
       <c r="L33" s="20"/>
@@ -11036,7 +10994,7 @@
       <c r="J35" s="72" t="s">
         <v>379</v>
       </c>
-      <c r="K35" s="95" t="s">
+      <c r="K35" s="93" t="s">
         <v>387</v>
       </c>
       <c r="L35" s="20"/>
@@ -11081,7 +11039,7 @@
       <c r="I37" s="72" t="s">
         <v>365</v>
       </c>
-      <c r="J37" s="95" t="s">
+      <c r="J37" s="93" t="s">
         <v>382</v>
       </c>
       <c r="K37" s="20"/>
@@ -11113,15 +11071,15 @@
       <c r="C39" s="73"/>
       <c r="D39" s="73"/>
       <c r="E39" s="73"/>
-      <c r="F39" s="84"/>
+      <c r="F39" s="83"/>
       <c r="G39" s="58"/>
-      <c r="H39" s="102" t="s">
+      <c r="H39" s="100" t="s">
         <v>381</v>
       </c>
-      <c r="I39" s="103"/>
-      <c r="J39" s="103"/>
-      <c r="K39" s="103"/>
-      <c r="L39" s="104"/>
+      <c r="I39" s="101"/>
+      <c r="J39" s="101"/>
+      <c r="K39" s="101"/>
+      <c r="L39" s="102"/>
       <c r="M39" s="58"/>
     </row>
     <row r="40" spans="1:13" ht="30.75" thickBot="1">
@@ -11132,16 +11090,16 @@
       <c r="E40" s="65"/>
       <c r="F40" s="66"/>
       <c r="G40" s="58"/>
-      <c r="H40" s="93" t="s">
+      <c r="H40" s="91" t="s">
         <v>302</v>
       </c>
-      <c r="I40" s="93" t="s">
+      <c r="I40" s="91" t="s">
         <v>323</v>
       </c>
-      <c r="J40" s="93" t="s">
+      <c r="J40" s="91" t="s">
         <v>361</v>
       </c>
-      <c r="K40" s="93" t="s">
+      <c r="K40" s="91" t="s">
         <v>377</v>
       </c>
       <c r="L40" s="63"/>
@@ -11165,16 +11123,16 @@
         <v>3</v>
       </c>
       <c r="G41" s="58"/>
-      <c r="H41" s="93" t="s">
+      <c r="H41" s="91" t="s">
         <v>303</v>
       </c>
-      <c r="I41" s="93" t="s">
+      <c r="I41" s="91" t="s">
         <v>324</v>
       </c>
-      <c r="J41" s="93" t="s">
+      <c r="J41" s="91" t="s">
         <v>362</v>
       </c>
-      <c r="K41" s="93" t="s">
+      <c r="K41" s="91" t="s">
         <v>380</v>
       </c>
       <c r="L41" s="63"/>
@@ -11199,7 +11157,7 @@
       <c r="J42" s="72" t="s">
         <v>369</v>
       </c>
-      <c r="K42" s="87"/>
+      <c r="K42" s="86"/>
       <c r="L42" s="20"/>
       <c r="M42" s="58"/>
     </row>
@@ -11211,8 +11169,8 @@
       <c r="C43" s="73"/>
       <c r="D43" s="73"/>
       <c r="E43" s="73"/>
-      <c r="F43" s="95" t="s">
-        <v>406</v>
+      <c r="F43" s="93" t="s">
+        <v>405</v>
       </c>
       <c r="G43" s="58"/>
       <c r="H43" s="72" t="s">
@@ -11244,7 +11202,7 @@
       <c r="I44" s="72" t="s">
         <v>338</v>
       </c>
-      <c r="J44" s="92" t="s">
+      <c r="J44" s="90" t="s">
         <v>373</v>
       </c>
       <c r="K44" s="20"/>
@@ -11282,7 +11240,7 @@
       <c r="C46" s="73"/>
       <c r="D46" s="73"/>
       <c r="E46" s="73"/>
-      <c r="F46" s="84"/>
+      <c r="F46" s="83"/>
       <c r="G46" s="58"/>
       <c r="H46" s="72" t="s">
         <v>318</v>
@@ -11330,13 +11288,13 @@
         <v>3</v>
       </c>
       <c r="G48" s="58"/>
-      <c r="H48" s="102" t="s">
+      <c r="H48" s="100" t="s">
         <v>172</v>
       </c>
-      <c r="I48" s="103"/>
-      <c r="J48" s="103"/>
-      <c r="K48" s="103"/>
-      <c r="L48" s="104"/>
+      <c r="I48" s="101"/>
+      <c r="J48" s="101"/>
+      <c r="K48" s="101"/>
+      <c r="L48" s="102"/>
       <c r="M48" s="58"/>
     </row>
     <row r="49" spans="1:13" ht="15.75" thickBot="1">
@@ -11349,13 +11307,13 @@
       <c r="E49" s="73"/>
       <c r="F49" s="73"/>
       <c r="G49" s="58"/>
-      <c r="H49" s="93" t="s">
+      <c r="H49" s="91" t="s">
         <v>301</v>
       </c>
-      <c r="I49" s="93" t="s">
+      <c r="I49" s="91" t="s">
         <v>329</v>
       </c>
-      <c r="J49" s="98" t="s">
+      <c r="J49" s="96" t="s">
         <v>388</v>
       </c>
       <c r="K49" s="63"/>
@@ -11372,13 +11330,13 @@
       <c r="E50" s="73"/>
       <c r="F50" s="73"/>
       <c r="G50" s="58"/>
-      <c r="H50" s="93" t="s">
+      <c r="H50" s="91" t="s">
         <v>304</v>
       </c>
-      <c r="I50" s="93" t="s">
+      <c r="I50" s="91" t="s">
         <v>330</v>
       </c>
-      <c r="J50" s="98" t="s">
+      <c r="J50" s="96" t="s">
         <v>389</v>
       </c>
       <c r="K50" s="63"/>
@@ -11398,10 +11356,10 @@
       <c r="H51" s="72" t="s">
         <v>306</v>
       </c>
-      <c r="I51" s="92" t="s">
+      <c r="I51" s="90" t="s">
         <v>331</v>
       </c>
-      <c r="J51" s="88" t="s">
+      <c r="J51" s="87" t="s">
         <v>390</v>
       </c>
       <c r="K51" s="20"/>
@@ -11442,7 +11400,7 @@
       <c r="H53" s="72" t="s">
         <v>320</v>
       </c>
-      <c r="I53" s="92" t="s">
+      <c r="I53" s="90" t="s">
         <v>364</v>
       </c>
       <c r="J53" s="20"/>
@@ -11519,13 +11477,13 @@
       <c r="E57" s="74"/>
       <c r="F57" s="74"/>
       <c r="G57" s="58"/>
-      <c r="H57" s="102" t="s">
+      <c r="H57" s="100" t="s">
         <v>173</v>
       </c>
-      <c r="I57" s="103"/>
-      <c r="J57" s="103"/>
-      <c r="K57" s="103"/>
-      <c r="L57" s="104"/>
+      <c r="I57" s="101"/>
+      <c r="J57" s="101"/>
+      <c r="K57" s="101"/>
+      <c r="L57" s="102"/>
       <c r="M57" s="58"/>
     </row>
     <row r="58" spans="1:13" ht="30.75" thickBot="1">
@@ -11536,24 +11494,24 @@
       <c r="C58" s="73"/>
       <c r="D58" s="73"/>
       <c r="E58" s="73"/>
-      <c r="F58" s="95" t="s">
-        <v>407</v>
+      <c r="F58" s="93" t="s">
+        <v>406</v>
       </c>
       <c r="G58" s="58"/>
-      <c r="H58" s="93" t="s">
+      <c r="H58" s="91" t="s">
         <v>339</v>
       </c>
-      <c r="I58" s="94" t="s">
+      <c r="I58" s="92" t="s">
         <v>346</v>
       </c>
-      <c r="J58" s="93" t="s">
+      <c r="J58" s="91" t="s">
         <v>353</v>
       </c>
-      <c r="K58" s="98" t="s">
-        <v>396</v>
-      </c>
-      <c r="L58" s="98" t="s">
-        <v>403</v>
+      <c r="K58" s="96" t="s">
+        <v>395</v>
+      </c>
+      <c r="L58" s="96" t="s">
+        <v>402</v>
       </c>
       <c r="M58" s="58"/>
     </row>
@@ -11567,24 +11525,24 @@
       <c r="E59" s="74"/>
       <c r="F59" s="74"/>
       <c r="G59" s="58"/>
-      <c r="H59" s="93" t="s">
+      <c r="H59" s="91" t="s">
         <v>340</v>
       </c>
-      <c r="I59" s="94" t="s">
+      <c r="I59" s="92" t="s">
         <v>347</v>
       </c>
-      <c r="J59" s="93" t="s">
+      <c r="J59" s="91" t="s">
         <v>354</v>
       </c>
-      <c r="K59" s="98" t="s">
-        <v>397</v>
-      </c>
-      <c r="L59" s="98" t="s">
-        <v>404</v>
+      <c r="K59" s="96" t="s">
+        <v>396</v>
+      </c>
+      <c r="L59" s="96" t="s">
+        <v>403</v>
       </c>
       <c r="M59" s="58"/>
     </row>
-    <row r="60" spans="1:13" ht="60.75" thickBot="1">
+    <row r="60" spans="1:13" ht="26.25" thickBot="1">
       <c r="A60" s="58"/>
       <c r="B60" s="19" t="s">
         <v>53</v>
@@ -11592,23 +11550,21 @@
       <c r="C60" s="73"/>
       <c r="D60" s="73"/>
       <c r="E60" s="73"/>
-      <c r="F60" s="75" t="s">
-        <v>408</v>
-      </c>
-      <c r="G60" s="58" t="s">
-        <v>460</v>
-      </c>
+      <c r="F60" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="G60" s="58"/>
       <c r="H60" s="72" t="s">
         <v>341</v>
       </c>
-      <c r="I60" s="92" t="s">
+      <c r="I60" s="90" t="s">
         <v>348</v>
       </c>
-      <c r="J60" s="92" t="s">
+      <c r="J60" s="90" t="s">
         <v>355</v>
       </c>
       <c r="K60" s="72" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="L60" s="20"/>
       <c r="M60" s="58"/>
@@ -11623,7 +11579,7 @@
       <c r="E61" s="73"/>
       <c r="F61" s="73"/>
       <c r="G61" s="58"/>
-      <c r="H61" s="92" t="s">
+      <c r="H61" s="90" t="s">
         <v>342</v>
       </c>
       <c r="I61" s="72" t="s">
@@ -11632,8 +11588,8 @@
       <c r="J61" s="72" t="s">
         <v>371</v>
       </c>
-      <c r="K61" s="95" t="s">
-        <v>399</v>
+      <c r="K61" s="93" t="s">
+        <v>398</v>
       </c>
       <c r="L61" s="20"/>
       <c r="M61" s="58"/>
@@ -11654,18 +11610,18 @@
       <c r="I62" s="72" t="s">
         <v>350</v>
       </c>
-      <c r="J62" s="92" t="s">
+      <c r="J62" s="90" t="s">
         <v>372</v>
       </c>
       <c r="K62" s="75" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="L62" s="20"/>
       <c r="M62" s="58" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" ht="45.75" thickBot="1">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="26.25" thickBot="1">
       <c r="A63" s="58"/>
       <c r="B63" s="19" t="s">
         <v>56</v>
@@ -11673,23 +11629,21 @@
       <c r="C63" s="73"/>
       <c r="D63" s="73"/>
       <c r="E63" s="73"/>
-      <c r="F63" s="75" t="s">
-        <v>409</v>
-      </c>
-      <c r="G63" s="58" t="s">
-        <v>459</v>
-      </c>
+      <c r="F63" s="93" t="s">
+        <v>408</v>
+      </c>
+      <c r="G63" s="58"/>
       <c r="H63" s="72" t="s">
         <v>344</v>
       </c>
       <c r="I63" s="72" t="s">
         <v>351</v>
       </c>
-      <c r="J63" s="95" t="s">
-        <v>394</v>
-      </c>
-      <c r="K63" s="95" t="s">
-        <v>401</v>
+      <c r="J63" s="93" t="s">
+        <v>393</v>
+      </c>
+      <c r="K63" s="93" t="s">
+        <v>400</v>
       </c>
       <c r="L63" s="20"/>
       <c r="M63" s="58"/>
@@ -11707,14 +11661,14 @@
       <c r="H64" s="72" t="s">
         <v>345</v>
       </c>
-      <c r="I64" s="92" t="s">
+      <c r="I64" s="90" t="s">
         <v>352</v>
       </c>
-      <c r="J64" s="95" t="s">
-        <v>395</v>
-      </c>
-      <c r="K64" s="95" t="s">
-        <v>402</v>
+      <c r="J64" s="93" t="s">
+        <v>394</v>
+      </c>
+      <c r="K64" s="93" t="s">
+        <v>401</v>
       </c>
       <c r="L64" s="20"/>
       <c r="M64" s="58"/>
@@ -11746,16 +11700,16 @@
       <c r="E66" s="73"/>
       <c r="F66" s="73"/>
       <c r="G66" s="58"/>
-      <c r="H66" s="102" t="s">
+      <c r="H66" s="100" t="s">
         <v>174</v>
       </c>
-      <c r="I66" s="103"/>
-      <c r="J66" s="103"/>
-      <c r="K66" s="103"/>
-      <c r="L66" s="104"/>
+      <c r="I66" s="101"/>
+      <c r="J66" s="101"/>
+      <c r="K66" s="101"/>
+      <c r="L66" s="102"/>
       <c r="M66" s="58"/>
     </row>
-    <row r="67" spans="1:13" ht="30.75" thickBot="1">
+    <row r="67" spans="1:13" ht="15.75" thickBot="1">
       <c r="A67" s="58"/>
       <c r="B67" s="19" t="s">
         <v>60</v>
@@ -11765,22 +11719,20 @@
       <c r="E67" s="73"/>
       <c r="F67" s="73"/>
       <c r="G67" s="58"/>
-      <c r="H67" s="93" t="s">
+      <c r="H67" s="91" t="s">
         <v>288</v>
       </c>
-      <c r="I67" s="93" t="s">
+      <c r="I67" s="91" t="s">
         <v>392</v>
       </c>
-      <c r="J67" s="76" t="s">
-        <v>393</v>
-      </c>
-      <c r="K67" s="108" t="s">
+      <c r="J67" s="96" t="s">
+        <v>457</v>
+      </c>
+      <c r="K67" s="106" t="s">
         <v>290</v>
       </c>
-      <c r="L67" s="109"/>
-      <c r="M67" s="58" t="s">
-        <v>458</v>
-      </c>
+      <c r="L67" s="107"/>
+      <c r="M67" s="58"/>
     </row>
     <row r="68" spans="1:13" ht="15.75" thickBot="1">
       <c r="A68" s="58"/>
@@ -11792,15 +11744,15 @@
       <c r="E68" s="73"/>
       <c r="F68" s="73"/>
       <c r="G68" s="58"/>
-      <c r="H68" s="93" t="s">
+      <c r="H68" s="91" t="s">
         <v>289</v>
       </c>
       <c r="I68" s="63"/>
       <c r="J68" s="63"/>
-      <c r="K68" s="108" t="s">
+      <c r="K68" s="106" t="s">
         <v>291</v>
       </c>
-      <c r="L68" s="109"/>
+      <c r="L68" s="107"/>
       <c r="M68" s="58"/>
     </row>
     <row r="69" spans="1:13" ht="15.75" thickBot="1">
@@ -11818,10 +11770,10 @@
       </c>
       <c r="I69" s="20"/>
       <c r="J69" s="20"/>
-      <c r="K69" s="105" t="s">
+      <c r="K69" s="103" t="s">
         <v>298</v>
       </c>
-      <c r="L69" s="106"/>
+      <c r="L69" s="104"/>
       <c r="M69" s="58"/>
     </row>
     <row r="70" spans="1:13" ht="15.75" thickBot="1">
@@ -11831,7 +11783,7 @@
       </c>
       <c r="C70" s="73"/>
       <c r="D70" s="73"/>
-      <c r="E70" s="77"/>
+      <c r="E70" s="76"/>
       <c r="F70" s="73"/>
       <c r="G70" s="58"/>
       <c r="H70" s="72" t="s">
@@ -11839,10 +11791,10 @@
       </c>
       <c r="I70" s="20"/>
       <c r="J70" s="20"/>
-      <c r="K70" s="105" t="s">
+      <c r="K70" s="103" t="s">
         <v>299</v>
       </c>
-      <c r="L70" s="106"/>
+      <c r="L70" s="104"/>
       <c r="M70" s="58"/>
     </row>
     <row r="71" spans="1:13" ht="15.75" thickBot="1">
@@ -11860,10 +11812,10 @@
       </c>
       <c r="I71" s="20"/>
       <c r="J71" s="20"/>
-      <c r="K71" s="105" t="s">
+      <c r="K71" s="103" t="s">
         <v>314</v>
       </c>
-      <c r="L71" s="106"/>
+      <c r="L71" s="104"/>
       <c r="M71" s="58"/>
     </row>
     <row r="72" spans="1:13" ht="26.25" thickBot="1">
@@ -11874,19 +11826,19 @@
       <c r="C72" s="73"/>
       <c r="D72" s="73"/>
       <c r="E72" s="73"/>
-      <c r="F72" s="95" t="s">
-        <v>410</v>
+      <c r="F72" s="93" t="s">
+        <v>409</v>
       </c>
       <c r="G72" s="58"/>
-      <c r="H72" s="95" t="s">
+      <c r="H72" s="93" t="s">
         <v>391</v>
       </c>
       <c r="I72" s="20"/>
       <c r="J72" s="20"/>
-      <c r="K72" s="105" t="s">
+      <c r="K72" s="103" t="s">
         <v>328</v>
       </c>
-      <c r="L72" s="106"/>
+      <c r="L72" s="104"/>
       <c r="M72" s="58"/>
     </row>
     <row r="73" spans="1:13" ht="15.75" thickBot="1">
@@ -11976,8 +11928,8 @@
       <c r="B77" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="C77" s="82"/>
-      <c r="D77" s="82"/>
+      <c r="C77" s="81"/>
+      <c r="D77" s="81"/>
       <c r="E77" s="74"/>
       <c r="F77" s="74"/>
       <c r="G77" s="58"/>
@@ -12036,8 +11988,8 @@
       <c r="C80" s="73"/>
       <c r="D80" s="73"/>
       <c r="E80" s="73"/>
-      <c r="F80" s="95" t="s">
-        <v>411</v>
+      <c r="F80" s="93" t="s">
+        <v>410</v>
       </c>
       <c r="G80" s="58"/>
       <c r="H80" s="19" t="s">
@@ -12076,8 +12028,8 @@
       <c r="C82" s="73"/>
       <c r="D82" s="73"/>
       <c r="E82" s="73"/>
-      <c r="F82" s="95" t="s">
-        <v>412</v>
+      <c r="F82" s="93" t="s">
+        <v>411</v>
       </c>
       <c r="G82" s="58"/>
       <c r="H82" s="19" t="s">
@@ -12116,8 +12068,8 @@
       <c r="C84" s="73"/>
       <c r="D84" s="73"/>
       <c r="E84" s="73"/>
-      <c r="F84" s="95" t="s">
-        <v>413</v>
+      <c r="F84" s="93" t="s">
+        <v>412</v>
       </c>
       <c r="G84" s="58"/>
       <c r="H84" s="19" t="s">
@@ -12145,25 +12097,23 @@
       <c r="I85" s="73"/>
       <c r="J85" s="73"/>
       <c r="K85" s="73"/>
-      <c r="L85" s="95" t="s">
-        <v>429</v>
+      <c r="L85" s="93" t="s">
+        <v>428</v>
       </c>
       <c r="M85" s="58"/>
     </row>
-    <row r="86" spans="1:13" ht="45.75" thickBot="1">
+    <row r="86" spans="1:13" ht="26.25" thickBot="1">
       <c r="A86" s="58"/>
       <c r="B86" s="19" t="s">
         <v>79</v>
       </c>
       <c r="C86" s="73"/>
-      <c r="D86" s="75" t="s">
-        <v>454</v>
+      <c r="D86" s="93" t="s">
+        <v>453</v>
       </c>
       <c r="E86" s="73"/>
       <c r="F86" s="73"/>
-      <c r="G86" s="58" t="s">
-        <v>457</v>
-      </c>
+      <c r="G86" s="58"/>
       <c r="H86" s="19" t="s">
         <v>187</v>
       </c>
@@ -12189,25 +12139,23 @@
       <c r="I87" s="73"/>
       <c r="J87" s="73"/>
       <c r="K87" s="73"/>
-      <c r="L87" s="95" t="s">
-        <v>430</v>
+      <c r="L87" s="93" t="s">
+        <v>429</v>
       </c>
       <c r="M87" s="58"/>
     </row>
-    <row r="88" spans="1:13" ht="45.75" thickBot="1">
+    <row r="88" spans="1:13" ht="26.25" thickBot="1">
       <c r="A88" s="58"/>
       <c r="B88" s="19" t="s">
         <v>81</v>
       </c>
       <c r="C88" s="73"/>
-      <c r="D88" s="89" t="s">
-        <v>414</v>
+      <c r="D88" s="93" t="s">
+        <v>413</v>
       </c>
       <c r="E88" s="73"/>
       <c r="F88" s="73"/>
-      <c r="G88" s="58" t="s">
-        <v>456</v>
-      </c>
+      <c r="G88" s="58"/>
       <c r="H88" s="19" t="s">
         <v>189</v>
       </c>
@@ -12223,7 +12171,7 @@
         <v>82</v>
       </c>
       <c r="C89" s="73"/>
-      <c r="D89" s="78"/>
+      <c r="D89" s="77"/>
       <c r="E89" s="73"/>
       <c r="F89" s="73"/>
       <c r="G89" s="58"/>
@@ -12244,20 +12192,20 @@
       <c r="C90" s="74"/>
       <c r="D90" s="74"/>
       <c r="E90" s="74"/>
-      <c r="F90" s="96" t="s">
-        <v>415</v>
+      <c r="F90" s="94" t="s">
+        <v>414</v>
       </c>
       <c r="G90" s="58"/>
       <c r="H90" s="19" t="s">
         <v>191</v>
       </c>
       <c r="I90" s="73"/>
-      <c r="J90" s="95" t="s">
+      <c r="J90" s="93" t="s">
+        <v>430</v>
+      </c>
+      <c r="K90" s="73"/>
+      <c r="L90" s="93" t="s">
         <v>431</v>
-      </c>
-      <c r="K90" s="73"/>
-      <c r="L90" s="95" t="s">
-        <v>432</v>
       </c>
       <c r="M90" s="58"/>
     </row>
@@ -12315,8 +12263,8 @@
       <c r="I93" s="73"/>
       <c r="J93" s="73"/>
       <c r="K93" s="73"/>
-      <c r="L93" s="95" t="s">
-        <v>433</v>
+      <c r="L93" s="93" t="s">
+        <v>432</v>
       </c>
       <c r="M93" s="58"/>
     </row>
@@ -12336,8 +12284,8 @@
       <c r="I94" s="73"/>
       <c r="J94" s="73"/>
       <c r="K94" s="73"/>
-      <c r="L94" s="95" t="s">
-        <v>434</v>
+      <c r="L94" s="93" t="s">
+        <v>433</v>
       </c>
       <c r="M94" s="58"/>
     </row>
@@ -12357,8 +12305,8 @@
       <c r="I95" s="73"/>
       <c r="J95" s="73"/>
       <c r="K95" s="73"/>
-      <c r="L95" s="95" t="s">
-        <v>435</v>
+      <c r="L95" s="93" t="s">
+        <v>434</v>
       </c>
       <c r="M95" s="58"/>
     </row>
@@ -12395,16 +12343,14 @@
         <v>195</v>
       </c>
       <c r="I97" s="73"/>
-      <c r="J97" s="95" t="s">
+      <c r="J97" s="93" t="s">
+        <v>435</v>
+      </c>
+      <c r="K97" s="73"/>
+      <c r="L97" s="93" t="s">
         <v>436</v>
       </c>
-      <c r="K97" s="73"/>
-      <c r="L97" s="75" t="s">
-        <v>437</v>
-      </c>
-      <c r="M97" s="58" t="s">
-        <v>455</v>
-      </c>
+      <c r="M97" s="58"/>
     </row>
     <row r="98" spans="1:13" ht="39" thickBot="1">
       <c r="A98" s="58"/>
@@ -12422,12 +12368,10 @@
       <c r="I98" s="73"/>
       <c r="J98" s="73"/>
       <c r="K98" s="73"/>
-      <c r="L98" s="75" t="s">
-        <v>438</v>
-      </c>
-      <c r="M98" s="58" t="s">
-        <v>467</v>
-      </c>
+      <c r="L98" s="93" t="s">
+        <v>437</v>
+      </c>
+      <c r="M98" s="58"/>
     </row>
     <row r="99" spans="1:13" ht="26.25" thickBot="1">
       <c r="A99" s="58"/>
@@ -12445,8 +12389,8 @@
       <c r="I99" s="73"/>
       <c r="J99" s="73"/>
       <c r="K99" s="73"/>
-      <c r="L99" s="95" t="s">
-        <v>439</v>
+      <c r="L99" s="93" t="s">
+        <v>438</v>
       </c>
       <c r="M99" s="58"/>
     </row>
@@ -12458,7 +12402,7 @@
       <c r="C100" s="74"/>
       <c r="D100" s="74"/>
       <c r="E100" s="74"/>
-      <c r="F100" s="82"/>
+      <c r="F100" s="81"/>
       <c r="G100" s="58"/>
       <c r="H100" s="19" t="s">
         <v>200</v>
@@ -12484,11 +12428,11 @@
       </c>
       <c r="I101" s="72"/>
       <c r="J101" s="73"/>
-      <c r="K101" s="95" t="s">
+      <c r="K101" s="93" t="s">
+        <v>439</v>
+      </c>
+      <c r="L101" s="93" t="s">
         <v>440</v>
-      </c>
-      <c r="L101" s="95" t="s">
-        <v>441</v>
       </c>
       <c r="M101" s="58"/>
     </row>
@@ -12508,8 +12452,8 @@
       <c r="I102" s="73"/>
       <c r="J102" s="73"/>
       <c r="K102" s="73"/>
-      <c r="L102" s="99" t="s">
-        <v>442</v>
+      <c r="L102" s="97" t="s">
+        <v>441</v>
       </c>
       <c r="M102" s="58"/>
     </row>
@@ -12521,7 +12465,7 @@
       <c r="C103" s="73"/>
       <c r="D103" s="73"/>
       <c r="E103" s="73"/>
-      <c r="F103" s="84"/>
+      <c r="F103" s="83"/>
       <c r="G103" s="58"/>
       <c r="H103" s="58"/>
       <c r="I103" s="58"/>
@@ -12634,8 +12578,8 @@
         <v>206</v>
       </c>
       <c r="I108" s="73"/>
-      <c r="J108" s="95" t="s">
-        <v>443</v>
+      <c r="J108" s="93" t="s">
+        <v>442</v>
       </c>
       <c r="K108" s="73"/>
       <c r="L108" s="73"/>
@@ -12655,7 +12599,7 @@
         <v>207</v>
       </c>
       <c r="I109" s="73"/>
-      <c r="J109" s="80"/>
+      <c r="J109" s="79"/>
       <c r="K109" s="73"/>
       <c r="L109" s="73"/>
       <c r="M109" s="58"/>
@@ -12679,20 +12623,18 @@
       <c r="L110" s="73"/>
       <c r="M110" s="58"/>
     </row>
-    <row r="111" spans="1:13" ht="45.75" thickBot="1">
+    <row r="111" spans="1:13" ht="15.75" thickBot="1">
       <c r="A111" s="58"/>
       <c r="B111" s="19" t="s">
         <v>102</v>
       </c>
       <c r="C111" s="73"/>
-      <c r="D111" s="75" t="s">
-        <v>416</v>
+      <c r="D111" s="93" t="s">
+        <v>415</v>
       </c>
       <c r="E111" s="73"/>
       <c r="F111" s="73"/>
-      <c r="G111" s="58" t="s">
-        <v>461</v>
-      </c>
+      <c r="G111" s="58"/>
       <c r="H111" s="19" t="s">
         <v>209</v>
       </c>
@@ -12718,25 +12660,23 @@
       <c r="I112" s="73"/>
       <c r="J112" s="73"/>
       <c r="K112" s="73"/>
-      <c r="L112" s="95" t="s">
-        <v>444</v>
+      <c r="L112" s="93" t="s">
+        <v>443</v>
       </c>
       <c r="M112" s="58"/>
     </row>
-    <row r="113" spans="1:13" ht="45.75" thickBot="1">
+    <row r="113" spans="1:13" ht="15.75" thickBot="1">
       <c r="A113" s="58"/>
       <c r="B113" s="19" t="s">
         <v>104</v>
       </c>
       <c r="C113" s="73"/>
       <c r="D113" s="73"/>
-      <c r="E113" s="75" t="s">
-        <v>417</v>
+      <c r="E113" s="93" t="s">
+        <v>416</v>
       </c>
       <c r="F113" s="73"/>
-      <c r="G113" s="58" t="s">
-        <v>462</v>
-      </c>
+      <c r="G113" s="58"/>
       <c r="H113" s="19" t="s">
         <v>211</v>
       </c>
@@ -12746,7 +12686,7 @@
       <c r="L113" s="73"/>
       <c r="M113" s="58"/>
     </row>
-    <row r="114" spans="1:13" ht="90.75" thickBot="1">
+    <row r="114" spans="1:13" ht="15.75" thickBot="1">
       <c r="A114" s="58"/>
       <c r="B114" s="19" t="s">
         <v>105</v>
@@ -12756,12 +12696,10 @@
       </c>
       <c r="D114" s="73"/>
       <c r="E114" s="73"/>
-      <c r="F114" s="75" t="s">
-        <v>418</v>
-      </c>
-      <c r="G114" s="58" t="s">
-        <v>463</v>
-      </c>
+      <c r="F114" s="93" t="s">
+        <v>417</v>
+      </c>
+      <c r="G114" s="58"/>
       <c r="H114" s="19" t="s">
         <v>212</v>
       </c>
@@ -12816,10 +12754,10 @@
       <c r="B117" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="C117" s="83" t="s">
+      <c r="C117" s="82" t="s">
         <v>287</v>
       </c>
-      <c r="D117" s="82"/>
+      <c r="D117" s="81"/>
       <c r="E117" s="74"/>
       <c r="F117" s="74"/>
       <c r="G117" s="58"/>
@@ -12866,7 +12804,7 @@
       </c>
       <c r="I119" s="73"/>
       <c r="J119" s="73"/>
-      <c r="K119" s="86"/>
+      <c r="K119" s="85"/>
       <c r="L119" s="73"/>
       <c r="M119" s="58"/>
     </row>
@@ -12924,8 +12862,8 @@
       <c r="I122" s="73"/>
       <c r="J122" s="73"/>
       <c r="K122" s="73"/>
-      <c r="L122" s="95" t="s">
-        <v>445</v>
+      <c r="L122" s="93" t="s">
+        <v>444</v>
       </c>
       <c r="M122" s="58"/>
     </row>
@@ -12983,8 +12921,8 @@
       <c r="I125" s="73"/>
       <c r="J125" s="73"/>
       <c r="K125" s="73"/>
-      <c r="L125" s="95" t="s">
-        <v>446</v>
+      <c r="L125" s="93" t="s">
+        <v>445</v>
       </c>
       <c r="M125" s="58"/>
     </row>
@@ -12996,8 +12934,8 @@
       <c r="C126" s="73"/>
       <c r="D126" s="73"/>
       <c r="E126" s="73"/>
-      <c r="F126" s="95" t="s">
-        <v>419</v>
+      <c r="F126" s="93" t="s">
+        <v>418</v>
       </c>
       <c r="G126" s="58"/>
       <c r="H126" s="19" t="s">
@@ -13025,8 +12963,8 @@
       <c r="I127" s="73"/>
       <c r="J127" s="73"/>
       <c r="K127" s="73"/>
-      <c r="L127" s="95" t="s">
-        <v>447</v>
+      <c r="L127" s="93" t="s">
+        <v>446</v>
       </c>
       <c r="M127" s="58"/>
     </row>
@@ -13035,8 +12973,8 @@
       <c r="B128" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="C128" s="82"/>
-      <c r="D128" s="81"/>
+      <c r="C128" s="81"/>
+      <c r="D128" s="80"/>
       <c r="E128" s="74"/>
       <c r="F128" s="74"/>
       <c r="G128" s="58"/>
@@ -13046,8 +12984,8 @@
       <c r="I128" s="73"/>
       <c r="J128" s="73"/>
       <c r="K128" s="73"/>
-      <c r="L128" s="95" t="s">
-        <v>448</v>
+      <c r="L128" s="93" t="s">
+        <v>447</v>
       </c>
       <c r="M128" s="58"/>
     </row>
@@ -13097,7 +13035,7 @@
       <c r="C131" s="74"/>
       <c r="D131" s="74"/>
       <c r="E131" s="74"/>
-      <c r="F131" s="82"/>
+      <c r="F131" s="81"/>
       <c r="G131" s="58"/>
       <c r="H131" s="19" t="s">
         <v>228</v>
@@ -13105,8 +13043,8 @@
       <c r="I131" s="73"/>
       <c r="J131" s="73"/>
       <c r="K131" s="73"/>
-      <c r="L131" s="95" t="s">
-        <v>449</v>
+      <c r="L131" s="93" t="s">
+        <v>448</v>
       </c>
       <c r="M131" s="58"/>
     </row>
@@ -13118,18 +13056,18 @@
       <c r="C132" s="73"/>
       <c r="D132" s="73"/>
       <c r="E132" s="73"/>
-      <c r="F132" s="95" t="s">
-        <v>420</v>
+      <c r="F132" s="93" t="s">
+        <v>419</v>
       </c>
       <c r="G132" s="58"/>
       <c r="H132" s="19" t="s">
-        <v>464</v>
+        <v>454</v>
       </c>
       <c r="I132" s="73"/>
       <c r="J132" s="73"/>
       <c r="K132" s="73"/>
-      <c r="L132" s="99" t="s">
-        <v>450</v>
+      <c r="L132" s="97" t="s">
+        <v>449</v>
       </c>
       <c r="M132" s="58"/>
     </row>
@@ -13158,10 +13096,10 @@
       <c r="C134" s="73"/>
       <c r="D134" s="73"/>
       <c r="E134" s="73"/>
-      <c r="F134" s="95" t="s">
-        <v>421</v>
-      </c>
-      <c r="G134" s="97"/>
+      <c r="F134" s="93" t="s">
+        <v>420</v>
+      </c>
+      <c r="G134" s="95"/>
       <c r="H134" s="44" t="s">
         <v>231</v>
       </c>
@@ -13187,8 +13125,8 @@
       <c r="B135" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="C135" s="85"/>
-      <c r="D135" s="85"/>
+      <c r="C135" s="84"/>
+      <c r="D135" s="84"/>
       <c r="E135" s="73"/>
       <c r="F135" s="73"/>
       <c r="G135" s="4"/>
@@ -13210,7 +13148,7 @@
       <c r="C136" s="73"/>
       <c r="D136" s="73"/>
       <c r="E136" s="73"/>
-      <c r="F136" s="77"/>
+      <c r="F136" s="76"/>
       <c r="G136" s="4"/>
       <c r="H136" s="51" t="s">
         <v>238</v>
@@ -13289,11 +13227,11 @@
       </c>
       <c r="C140" s="73"/>
       <c r="D140" s="73"/>
-      <c r="E140" s="95" t="s">
-        <v>422</v>
+      <c r="E140" s="93" t="s">
+        <v>421</v>
       </c>
       <c r="F140" s="73"/>
-      <c r="G140" s="97"/>
+      <c r="G140" s="95"/>
       <c r="H140" s="4"/>
       <c r="I140" s="4"/>
       <c r="J140" s="4"/>
@@ -13340,7 +13278,7 @@
       <c r="C142" s="73"/>
       <c r="D142" s="73"/>
       <c r="E142" s="73"/>
-      <c r="F142" s="84"/>
+      <c r="F142" s="83"/>
       <c r="G142" s="4"/>
       <c r="H142" s="51" t="s">
         <v>237</v>
@@ -13612,7 +13550,7 @@
       <c r="C155" s="73"/>
       <c r="D155" s="73"/>
       <c r="E155" s="73"/>
-      <c r="F155" s="84"/>
+      <c r="F155" s="83"/>
       <c r="G155" s="4"/>
       <c r="H155" s="44" t="s">
         <v>255</v>
@@ -13653,7 +13591,7 @@
       <c r="N156" s="4"/>
     </row>
     <row r="157" spans="1:14" ht="27" thickBot="1">
-      <c r="A157" s="79" t="s">
+      <c r="A157" s="78" t="s">
         <v>267</v>
       </c>
       <c r="B157" s="45" t="s">

</xml_diff>

<commit_message>
started work on sets
checked very few items then internet started acting up so i guess i will
do more later
P.S.: Quiri: read the celestia weapon's note in excel file
</commit_message>
<xml_diff>
--- a/check list.xlsx
+++ b/check list.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="474" activeTab="3"/>
@@ -12,12 +12,46 @@
     <sheet name="Blank full" sheetId="4" r:id="rId3"/>
     <sheet name="Text arrangement" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="J149" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Check the max/min possible damage on it from docs, I have a spear with 1184 max damage while in docs it have 1124 as max possible</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1250" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="461">
   <si>
     <t>ARMOR</t>
   </si>
@@ -1407,12 +1441,21 @@
   <si>
     <t>Devil's dance</t>
   </si>
+  <si>
+    <t>Armor</t>
+  </si>
+  <si>
+    <t>Gloves</t>
+  </si>
+  <si>
+    <t>Weapon</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="46">
+  <fonts count="48">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1759,6 +1802,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="36">
@@ -2305,7 +2361,7 @@
     <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2613,6 +2669,12 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="68">
@@ -10221,8 +10283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q190"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J51" sqref="J51"/>
+    <sheetView tabSelected="1" topLeftCell="A135" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J151" sqref="J151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13437,11 +13499,13 @@
       <c r="H149" s="51" t="s">
         <v>237</v>
       </c>
-      <c r="I149" s="3"/>
-      <c r="J149" s="3"/>
-      <c r="K149" s="3"/>
-      <c r="L149" s="3"/>
-      <c r="M149" s="3"/>
+      <c r="I149" s="108"/>
+      <c r="J149" s="108" t="s">
+        <v>460</v>
+      </c>
+      <c r="K149" s="108"/>
+      <c r="L149" s="108"/>
+      <c r="M149" s="108"/>
       <c r="N149" s="4"/>
     </row>
     <row r="150" spans="1:14" ht="15.75" thickBot="1">
@@ -13457,11 +13521,13 @@
       <c r="H150" s="51" t="s">
         <v>238</v>
       </c>
-      <c r="I150" s="3"/>
-      <c r="J150" s="3"/>
-      <c r="K150" s="3"/>
-      <c r="L150" s="3"/>
-      <c r="M150" s="3"/>
+      <c r="I150" s="108" t="s">
+        <v>458</v>
+      </c>
+      <c r="J150" s="108"/>
+      <c r="K150" s="108"/>
+      <c r="L150" s="108"/>
+      <c r="M150" s="108"/>
       <c r="N150" s="4"/>
     </row>
     <row r="151" spans="1:14" ht="15.75" thickBot="1">
@@ -13477,11 +13543,13 @@
       <c r="H151" s="51" t="s">
         <v>239</v>
       </c>
-      <c r="I151" s="3"/>
-      <c r="J151" s="3"/>
-      <c r="K151" s="3"/>
-      <c r="L151" s="3"/>
-      <c r="M151" s="3"/>
+      <c r="I151" s="108" t="s">
+        <v>205</v>
+      </c>
+      <c r="J151" s="108"/>
+      <c r="K151" s="108"/>
+      <c r="L151" s="108"/>
+      <c r="M151" s="108"/>
       <c r="N151" s="4"/>
     </row>
     <row r="152" spans="1:14" ht="15.75" thickBot="1">
@@ -13497,11 +13565,13 @@
       <c r="H152" s="51" t="s">
         <v>240</v>
       </c>
-      <c r="I152" s="3"/>
-      <c r="J152" s="3"/>
-      <c r="K152" s="3"/>
-      <c r="L152" s="3"/>
-      <c r="M152" s="3"/>
+      <c r="I152" s="108" t="s">
+        <v>459</v>
+      </c>
+      <c r="J152" s="108"/>
+      <c r="K152" s="108"/>
+      <c r="L152" s="108"/>
+      <c r="M152" s="108"/>
       <c r="N152" s="4"/>
     </row>
     <row r="153" spans="1:14" ht="15.75" thickBot="1">
@@ -13517,11 +13587,11 @@
       <c r="H153" s="57" t="s">
         <v>241</v>
       </c>
-      <c r="I153" s="2"/>
-      <c r="J153" s="2"/>
-      <c r="K153" s="2"/>
-      <c r="L153" s="2"/>
-      <c r="M153" s="2"/>
+      <c r="I153" s="109"/>
+      <c r="J153" s="109"/>
+      <c r="K153" s="109"/>
+      <c r="L153" s="109"/>
+      <c r="M153" s="109"/>
       <c r="N153" s="4"/>
     </row>
     <row r="154" spans="1:14" ht="15.75" thickBot="1">
@@ -14161,5 +14231,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>